<commit_message>
Update Modelling Pipeline, minor changes, calculation of atmospheric conditions
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -506,10 +506,10 @@
         <v>8.519418801836229</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.3314515207352832</v>
+        <v>-0.2744830222869237</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.885861091554528</v>
+        <v>-2.942829590002887</v>
       </c>
       <c r="F2" t="n">
         <v>8.500794589519501</v>
@@ -521,13 +521,13 @@
         <v>8.198146171346439</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.318952275842719</v>
+        <v>-0.2641320952288594</v>
       </c>
       <c r="J2" t="n">
         <v>-1.904283142004869</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.374214554427509</v>
+        <v>-3.429034735041368</v>
       </c>
       <c r="L2" t="n">
         <v>5.678760051727295</v>
@@ -544,10 +544,10 @@
         <v>16.28675076265056</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.732074944040755</v>
+        <v>-0.6249356946155221</v>
       </c>
       <c r="E3" t="n">
-        <v>-5.181641113629794</v>
+        <v>-5.288780363055024</v>
       </c>
       <c r="F3" t="n">
         <v>16.65613877773285</v>
@@ -559,13 +559,13 @@
         <v>15.52078963302567</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.6976456733237593</v>
+        <v>-0.5955451514945248</v>
       </c>
       <c r="J3" t="n">
         <v>-8.600137381010331</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.6684668900386992</v>
+        <v>-0.7705674118679333</v>
       </c>
       <c r="L3" t="n">
         <v>11.54215121269226</v>
@@ -582,10 +582,10 @@
         <v>23.38054526910285</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.191437047810165</v>
+        <v>-1.041910225050692</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.954525040365922</v>
+        <v>-7.104051863125395</v>
       </c>
       <c r="F4" t="n">
         <v>24.46634137630463</v>
@@ -597,13 +597,13 @@
         <v>22.13806674011207</v>
       </c>
       <c r="I4" t="n">
-        <v>-1.128122230576003</v>
+        <v>-0.9865414956707068</v>
       </c>
       <c r="J4" t="n">
         <v>-11.86663873428929</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.3350481456860628</v>
+        <v>-0.4766288805913597</v>
       </c>
       <c r="L4" t="n">
         <v>17.54942584037781</v>
@@ -620,10 +620,10 @@
         <v>29.86034637456686</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.697601672301151</v>
+        <v>-1.514198222601659</v>
       </c>
       <c r="E5" t="n">
-        <v>-8.260437843580602</v>
+        <v>-8.4438412932801</v>
       </c>
       <c r="F5" t="n">
         <v>31.93238091468811</v>
@@ -635,13 +635,13 @@
         <v>28.16527622615067</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.601234608017194</v>
+        <v>-1.428242347417871</v>
       </c>
       <c r="J5" t="n">
         <v>-11.93580062186216</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.313332253713913</v>
+        <v>-2.486324514313235</v>
       </c>
       <c r="L5" t="n">
         <v>23.66207647323608</v>
@@ -658,10 +658,10 @@
         <v>35.77376767348272</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.237455391285378</v>
+        <v>-2.029197988747954</v>
       </c>
       <c r="E6" t="n">
-        <v>-9.149007092401687</v>
+        <v>-9.357264494939114</v>
       </c>
       <c r="F6" t="n">
         <v>39.05590730905533</v>
@@ -673,13 +673,13 @@
         <v>33.68297082770759</v>
       </c>
       <c r="I6" t="n">
-        <v>-2.106687373855399</v>
+        <v>-1.910601569353406</v>
       </c>
       <c r="J6" t="n">
         <v>-8.107255176350909</v>
       </c>
       <c r="K6" t="n">
-        <v>-7.436495441808955</v>
+        <v>-7.632581246310945</v>
       </c>
       <c r="L6" t="n">
         <v>29.84382891654968</v>
@@ -696,10 +696,10 @@
         <v>41.16063799466459</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.79700200880756</v>
+        <v>-2.573234069733215</v>
       </c>
       <c r="E7" t="n">
-        <v>-9.66617973176464</v>
+        <v>-9.889947670838982</v>
       </c>
       <c r="F7" t="n">
         <v>45.83923888206482</v>
@@ -711,13 +711,13 @@
         <v>38.74906475579328</v>
       </c>
       <c r="I7" t="n">
-        <v>-2.633127600583277</v>
+        <v>-2.422470069896165</v>
       </c>
       <c r="J7" t="n">
         <v>-8.235904593435361</v>
       </c>
       <c r="K7" t="n">
-        <v>-7.956839444791608</v>
+        <v>-8.167496975478723</v>
       </c>
       <c r="L7" t="n">
         <v>36.06065058708191</v>
@@ -734,10 +734,10 @@
         <v>46.05555277051322</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.361634027789704</v>
+        <v>-3.131849799973255</v>
       </c>
       <c r="E8" t="n">
-        <v>-9.855617818620853</v>
+        <v>-10.08540204643731</v>
       </c>
       <c r="F8" t="n">
         <v>52.28536695241928</v>
@@ -749,13 +749,13 @@
         <v>43.40644178271985</v>
       </c>
       <c r="I8" t="n">
-        <v>-3.168273160223277</v>
+        <v>-2.95170609920023</v>
       </c>
       <c r="J8" t="n">
         <v>-5.130172176490072</v>
       </c>
       <c r="K8" t="n">
-        <v>-11.15572859798328</v>
+        <v>-11.37229565900633</v>
       </c>
       <c r="L8" t="n">
         <v>42.28074049949646</v>
@@ -772,10 +772,10 @@
         <v>50.48951225182122</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.916391809269403</v>
+        <v>-3.690078256473666</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.759436532509731</v>
+        <v>-9.985750085305469</v>
       </c>
       <c r="F9" t="n">
         <v>58.39795076847076</v>
@@ -787,13 +787,13 @@
         <v>47.68791001341147</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.699075943657273</v>
+        <v>-3.485320257392959</v>
       </c>
       <c r="J9" t="n">
         <v>-6.586913857908061</v>
       </c>
       <c r="K9" t="n">
-        <v>-9.313964481773095</v>
+        <v>-9.527720168037408</v>
       </c>
       <c r="L9" t="n">
         <v>48.47453761100769</v>
@@ -810,10 +810,10 @@
         <v>54.4910019001033</v>
       </c>
       <c r="D10" t="n">
-        <v>-4.446210147663738</v>
+        <v>-4.23270384904053</v>
       </c>
       <c r="E10" t="n">
-        <v>-9.418550854812565</v>
+        <v>-9.632057153435767</v>
       </c>
       <c r="F10" t="n">
         <v>64.18132090568542</v>
@@ -825,13 +825,13 @@
         <v>51.61950795466915</v>
       </c>
       <c r="I10" t="n">
-        <v>-4.211909711372438</v>
+        <v>-4.009654482144734</v>
       </c>
       <c r="J10" t="n">
         <v>-14.00656624087751</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.100118275946704</v>
+        <v>-1.302373505174407</v>
       </c>
       <c r="L10" t="n">
         <v>54.61471962928772</v>
@@ -848,10 +848,10 @@
         <v>58.08672636119757</v>
       </c>
       <c r="D11" t="n">
-        <v>-4.936154690177836</v>
+        <v>-4.744508420970917</v>
       </c>
       <c r="E11" t="n">
-        <v>-8.872801807488724</v>
+        <v>-9.064448076695637</v>
       </c>
       <c r="F11" t="n">
         <v>69.6404789686203</v>
@@ -863,13 +863,13 @@
         <v>55.22276170171533</v>
       </c>
       <c r="I11" t="n">
-        <v>-4.692777700768937</v>
+        <v>-4.510580546299819</v>
       </c>
       <c r="J11" t="n">
         <v>-17.54095608369634</v>
       </c>
       <c r="K11" t="n">
-        <v>3.574966128962153</v>
+        <v>3.39276897449303</v>
       </c>
       <c r="L11" t="n">
         <v>60.6761953830719</v>
@@ -886,10 +886,10 @@
         <v>61.3021172310517</v>
       </c>
       <c r="D12" t="n">
-        <v>-5.371652179191798</v>
+        <v>-5.210510624263786</v>
       </c>
       <c r="E12" t="n">
-        <v>-8.160945424134162</v>
+        <v>-8.322086979062171</v>
       </c>
       <c r="F12" t="n">
         <v>74.78109574317932</v>
@@ -901,13 +901,13 @@
         <v>58.51625578601728</v>
       </c>
       <c r="I12" t="n">
-        <v>-5.127538608925659</v>
+        <v>-4.973720097072566</v>
       </c>
       <c r="J12" t="n">
         <v>-11.6382355191162</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.8984055636363326</v>
+        <v>-1.052224075489422</v>
       </c>
       <c r="L12" t="n">
         <v>66.63611698150635</v>
@@ -924,10 +924,10 @@
         <v>64.16168483293919</v>
       </c>
       <c r="D13" t="n">
-        <v>-5.738710948095909</v>
+        <v>-5.616195136702888</v>
       </c>
       <c r="E13" t="n">
-        <v>-7.32054791941491</v>
+        <v>-7.443063730807939</v>
       </c>
       <c r="F13" t="n">
         <v>79.60951280593872</v>
@@ -939,13 +939,13 @@
         <v>61.5167289199957</v>
       </c>
       <c r="I13" t="n">
-        <v>-5.502142387055763</v>
+        <v>-5.38467708081417</v>
       </c>
       <c r="J13" t="n">
         <v>-13.57224390272271</v>
       </c>
       <c r="K13" t="n">
-        <v>2.699597029479968</v>
+        <v>2.582131723238383</v>
       </c>
       <c r="L13" t="n">
         <v>72.47387051582336</v>
@@ -962,10 +962,10 @@
         <v>66.68926621238614</v>
       </c>
       <c r="D14" t="n">
-        <v>-6.024121334438571</v>
+        <v>-5.947729212459708</v>
       </c>
       <c r="E14" t="n">
-        <v>-6.38784419694257</v>
+        <v>-6.46423631892144</v>
       </c>
       <c r="F14" t="n">
         <v>84.1327423453331</v>
@@ -977,13 +977,13 @@
         <v>64.23985083952782</v>
       </c>
       <c r="I14" t="n">
-        <v>-5.802862708536985</v>
+        <v>-5.72927637598373</v>
       </c>
       <c r="J14" t="n">
         <v>-7.089600779399854</v>
       </c>
       <c r="K14" t="n">
-        <v>-1.935196868483532</v>
+        <v>-2.008783201036794</v>
       </c>
       <c r="L14" t="n">
         <v>78.17107820510864</v>
@@ -1000,10 +1000,10 @@
         <v>68.90819396895697</v>
       </c>
       <c r="D15" t="n">
-        <v>-6.215653150541376</v>
+        <v>-6.192167984703453</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.397550190622276</v>
+        <v>-5.421035356460202</v>
       </c>
       <c r="F15" t="n">
         <v>88.3584668636322</v>
@@ -1015,13 +1015,13 @@
         <v>66.70076722045951</v>
       </c>
       <c r="I15" t="n">
-        <v>-6.016538963481581</v>
+        <v>-5.993806128829219</v>
       </c>
       <c r="J15" t="n">
         <v>-6.066499763697654</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.9745063085287482</v>
+        <v>-0.9972391431811074</v>
       </c>
       <c r="L15" t="n">
         <v>83.71160125732422</v>
@@ -1038,10 +1038,10 @@
         <v>70.84140964315219</v>
       </c>
       <c r="D16" t="n">
-        <v>-6.302226728836977</v>
+        <v>-6.337640022479033</v>
       </c>
       <c r="E16" t="n">
-        <v>-4.382672011811373</v>
+        <v>-4.347258718169307</v>
       </c>
       <c r="F16" t="n">
         <v>92.29503816366196</v>
@@ -1053,13 +1053,13 @@
         <v>68.91447847586318</v>
       </c>
       <c r="I16" t="n">
-        <v>-6.130802174070347</v>
+        <v>-6.165252203717531</v>
       </c>
       <c r="J16" t="n">
         <v>-2.60624493392778</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.36023286670153</v>
+        <v>-2.325782837054341</v>
       </c>
       <c r="L16" t="n">
         <v>89.08153748512268</v>
@@ -1076,10 +1076,10 @@
         <v>72.51153859695562</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.27406576108109</v>
+        <v>-6.373516906645429</v>
       </c>
       <c r="E17" t="n">
-        <v>-3.374309622980604</v>
+        <v>-3.274858477416259</v>
       </c>
       <c r="F17" t="n">
         <v>95.95148026943207</v>
@@ -1091,13 +1091,13 @@
         <v>70.89609960692228</v>
       </c>
       <c r="I17" t="n">
-        <v>-6.134289793661345</v>
+        <v>-6.231525329665376</v>
       </c>
       <c r="J17" t="n">
         <v>-2.913684595265906</v>
       </c>
       <c r="K17" t="n">
-        <v>0.06993165669588564</v>
+        <v>0.167167192699921</v>
       </c>
       <c r="L17" t="n">
         <v>94.26922011375427</v>
@@ -1114,10 +1114,10 @@
         <v>73.94092447897175</v>
       </c>
       <c r="D18" t="n">
-        <v>-6.122827292803419</v>
+        <v>-6.290555581382483</v>
       </c>
       <c r="E18" t="n">
-        <v>-2.401462780845065</v>
+        <v>-2.233734492266009</v>
       </c>
       <c r="F18" t="n">
         <v>99.33748608827591</v>
@@ -1129,13 +1129,13 @@
         <v>72.66102300905231</v>
       </c>
       <c r="I18" t="n">
-        <v>-6.016842471713568</v>
+        <v>-6.181667419759469</v>
       </c>
       <c r="J18" t="n">
         <v>-0.7549633027352296</v>
       </c>
       <c r="K18" t="n">
-        <v>0.04231316579787392</v>
+        <v>0.207138113843764</v>
       </c>
       <c r="L18" t="n">
         <v>99.26521944999695</v>
@@ -1152,10 +1152,10 @@
         <v>75.15164310911429</v>
       </c>
       <c r="D19" t="n">
-        <v>-5.841702331955064</v>
+        <v>-6.081019874168324</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.490853372702233</v>
+        <v>-1.251535830488976</v>
       </c>
       <c r="F19" t="n">
         <v>102.4634192585945</v>
@@ -1167,13 +1167,13 @@
         <v>74.22501584891296</v>
       </c>
       <c r="I19" t="n">
-        <v>-5.769673559158815</v>
+        <v>-6.006040292191001</v>
       </c>
       <c r="J19" t="n">
         <v>0.6365219879492631</v>
       </c>
       <c r="K19" t="n">
-        <v>0.7533179192680376</v>
+        <v>0.9896846523002222</v>
       </c>
       <c r="L19" t="n">
         <v>104.0623459815979</v>
@@ -1190,10 +1190,10 @@
         <v>76.16549611589225</v>
       </c>
       <c r="D20" t="n">
-        <v>-5.425489534931232</v>
+        <v>-5.738769058438906</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.6667651214767503</v>
+        <v>-0.3534855979690761</v>
       </c>
       <c r="F20" t="n">
         <v>105.3403136730194</v>
@@ -1205,13 +1205,13 @@
         <v>75.60426222175262</v>
       </c>
       <c r="I20" t="n">
-        <v>-5.385511214371617</v>
+        <v>-5.696482303011815</v>
       </c>
       <c r="J20" t="n">
         <v>8.71675703956166</v>
       </c>
       <c r="K20" t="n">
-        <v>-5.287068184849776</v>
+        <v>-4.976097096209575</v>
       </c>
       <c r="L20" t="n">
         <v>108.655642747879</v>
@@ -1228,10 +1228,10 @@
         <v>77.00398172655416</v>
       </c>
       <c r="D21" t="n">
-        <v>-4.870637774407634</v>
+        <v>-5.259317683109761</v>
       </c>
       <c r="E21" t="n">
-        <v>0.04910079508902498</v>
+        <v>0.437780703791141</v>
       </c>
       <c r="F21" t="n">
         <v>107.979874253273</v>
@@ -1243,13 +1243,13 @@
         <v>76.8153602954406</v>
       </c>
       <c r="I21" t="n">
-        <v>-4.858707135928356</v>
+        <v>-5.24643497229629</v>
       </c>
       <c r="J21" t="n">
         <v>11.85815534527128</v>
       </c>
       <c r="K21" t="n">
-        <v>-6.48215939384324</v>
+        <v>-6.094431557475311</v>
       </c>
       <c r="L21" t="n">
         <v>113.0423927307129</v>
@@ -1266,10 +1266,10 @@
         <v>77.68825976289256</v>
       </c>
       <c r="D22" t="n">
-        <v>-4.175256461227399</v>
+        <v>-4.639864327902043</v>
       </c>
       <c r="E22" t="n">
-        <v>0.6377363210498359</v>
+        <v>1.102344187724476</v>
       </c>
       <c r="F22" t="n">
         <v>110.3944753408432</v>
@@ -1281,13 +1281,13 @@
         <v>77.87529240910662</v>
       </c>
       <c r="I22" t="n">
-        <v>-4.185308292314221</v>
+        <v>-4.651034691428917</v>
       </c>
       <c r="J22" t="n">
         <v>6.012469489304225</v>
       </c>
       <c r="K22" t="n">
-        <v>1.188670256718074</v>
+        <v>1.654396655832775</v>
       </c>
       <c r="L22" t="n">
         <v>117.2221155166626</v>
@@ -1304,10 +1304,10 @@
         <v>78.23909919556851</v>
       </c>
       <c r="D23" t="n">
-        <v>-3.339095519254112</v>
+        <v>-3.879287611332589</v>
       </c>
       <c r="E23" t="n">
-        <v>1.082918697450118</v>
+        <v>1.623110789528589</v>
       </c>
       <c r="F23" t="n">
         <v>112.5971618890762</v>
@@ -1319,13 +1319,13 @@
         <v>78.80136285198196</v>
       </c>
       <c r="I23" t="n">
-        <v>-3.36309185963984</v>
+        <v>-3.907166030934215</v>
       </c>
       <c r="J23" t="n">
         <v>7.249452761779999</v>
       </c>
       <c r="K23" t="n">
-        <v>1.631475365962899</v>
+        <v>2.175549537257282</v>
       </c>
       <c r="L23" t="n">
         <v>121.1965661048889</v>
@@ -1342,10 +1342,10 @@
         <v>78.67681847309071</v>
       </c>
       <c r="D24" t="n">
-        <v>-2.363496317036779</v>
+        <v>-2.978107617795396</v>
       </c>
       <c r="E24" t="n">
-        <v>1.371276684286528</v>
+        <v>1.985887985045153</v>
       </c>
       <c r="F24" t="n">
         <v>114.6016496419907</v>
@@ -1357,13 +1357,13 @@
         <v>79.61111808510533</v>
       </c>
       <c r="I24" t="n">
-        <v>-2.391563208083736</v>
+        <v>-3.013473114848327</v>
       </c>
       <c r="J24" t="n">
         <v>7.181539820489898</v>
       </c>
       <c r="K24" t="n">
-        <v>3.213195998977629</v>
+        <v>3.835105905742215</v>
       </c>
       <c r="L24" t="n">
         <v>124.9697372913361</v>
@@ -1380,10 +1380,10 @@
         <v>79.02122450413128</v>
       </c>
       <c r="D25" t="n">
-        <v>-1.251310436397816</v>
+        <v>-1.938424993117306</v>
       </c>
       <c r="E25" t="n">
-        <v>1.492319050455443</v>
+        <v>2.179433607174936</v>
       </c>
       <c r="F25" t="n">
         <v>116.4223245382309</v>
@@ -1395,13 +1395,13 @@
         <v>80.32225664562347</v>
       </c>
       <c r="I25" t="n">
-        <v>-1.271912434240219</v>
+        <v>-1.970339877197411</v>
       </c>
       <c r="J25" t="n">
         <v>8.578777290053026</v>
       </c>
       <c r="K25" t="n">
-        <v>3.146829253633406</v>
+        <v>3.845256696590589</v>
       </c>
       <c r="L25" t="n">
         <v>128.5478584766388</v>
@@ -1418,10 +1418,10 @@
         <v>79.29153749712972</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.00679946950531187</v>
+        <v>-0.7638227215426732</v>
       </c>
       <c r="E26" t="n">
-        <v>1.438454059681689</v>
+        <v>2.195477311719046</v>
       </c>
       <c r="F26" t="n">
         <v>118.0742421746254</v>
@@ -1433,13 +1433,13 @@
         <v>80.95251960158225</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.006941903332736425</v>
+        <v>-0.7798231159290544</v>
       </c>
       <c r="J26" t="n">
         <v>9.922511535262368</v>
       </c>
       <c r="K26" t="n">
-        <v>2.937837427952386</v>
+        <v>3.71071864054869</v>
       </c>
       <c r="L26" t="n">
         <v>131.9393985271454</v>
@@ -1456,10 +1456,10 @@
         <v>79.50632501231924</v>
       </c>
       <c r="D27" t="n">
-        <v>1.364494902755915</v>
+        <v>0.5407462376597554</v>
       </c>
       <c r="E27" t="n">
-        <v>1.204967636198944</v>
+        <v>2.028716301295105</v>
       </c>
       <c r="F27" t="n">
         <v>119.5731292366982</v>
@@ -1471,13 +1471,13 @@
         <v>81.51958382726791</v>
       </c>
       <c r="I27" t="n">
-        <v>1.399046636728026</v>
+        <v>0.5544390115296348</v>
       </c>
       <c r="J27" t="n">
         <v>12.00788132390952</v>
       </c>
       <c r="K27" t="n">
-        <v>1.781698103370458</v>
+        <v>2.62630572856885</v>
       </c>
       <c r="L27" t="n">
         <v>135.1550590991974</v>
@@ -1494,10 +1494,10 @@
         <v>79.68342569476683</v>
       </c>
       <c r="D28" t="n">
-        <v>2.855890447971428</v>
+        <v>1.969100892571537</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7899949495013132</v>
+        <v>1.676784504901214</v>
       </c>
       <c r="F28" t="n">
         <v>120.9353822469711</v>
@@ -1509,13 +1509,13 @@
         <v>82.04094617240385</v>
       </c>
       <c r="I28" t="n">
-        <v>2.940385060926086</v>
+        <v>2.027358875788185</v>
       </c>
       <c r="J28" t="n">
         <v>10.46871370151256</v>
       </c>
       <c r="K28" t="n">
-        <v>4.039050060105634</v>
+        <v>4.952076245243514</v>
       </c>
       <c r="L28" t="n">
         <v>138.2077825069427</v>
@@ -1532,10 +1532,10 @@
         <v>79.83988401319681</v>
       </c>
       <c r="D29" t="n">
-        <v>4.459721239680142</v>
+        <v>3.513981010928326</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1944619441485713</v>
+        <v>1.140202172900374</v>
       </c>
       <c r="F29" t="n">
         <v>122.1780688166618</v>
@@ -1547,13 +1547,13 @@
         <v>82.53381451082616</v>
       </c>
       <c r="I29" t="n">
-        <v>4.610199652906718</v>
+        <v>3.632548575629016</v>
       </c>
       <c r="J29" t="n">
         <v>15.36893157473885</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.3557227354004979</v>
+        <v>0.6219283418772008</v>
       </c>
       <c r="L29" t="n">
         <v>141.1127455234528</v>
@@ -1570,10 +1570,10 @@
         <v>79.9918820205132</v>
       </c>
       <c r="D30" t="n">
-        <v>6.167504072235432</v>
+        <v>5.167215023845503</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.5779862186540967</v>
+        <v>0.422302829735834</v>
       </c>
       <c r="F30" t="n">
         <v>123.3189262151718</v>
@@ -1585,13 +1585,13 @@
         <v>83.01499901557376</v>
       </c>
       <c r="I30" t="n">
-        <v>6.400591304426055</v>
+        <v>5.362498534636183</v>
       </c>
       <c r="J30" t="n">
         <v>16.42501243902971</v>
       </c>
       <c r="K30" t="n">
-        <v>-1.116972355642734</v>
+        <v>-0.0788795858528637</v>
       </c>
       <c r="L30" t="n">
         <v>143.8873634338379</v>
@@ -1608,10 +1608,10 @@
         <v>80.15468408327416</v>
       </c>
       <c r="D31" t="n">
-        <v>7.970104978892157</v>
+        <v>6.919884265511524</v>
       </c>
       <c r="E31" t="n">
-        <v>-1.521071441128498</v>
+        <v>-0.4708507277478731</v>
       </c>
       <c r="F31" t="n">
         <v>124.3763625025749</v>
@@ -1623,13 +1623,13 @@
         <v>83.50081637634703</v>
       </c>
       <c r="I31" t="n">
-        <v>8.302824469388119</v>
+        <v>7.208761309566728</v>
       </c>
       <c r="J31" t="n">
         <v>17.51095138635368</v>
       </c>
       <c r="K31" t="n">
-        <v>-2.112804584750819</v>
+        <v>-1.018741424929431</v>
       </c>
       <c r="L31" t="n">
         <v>146.5512869358063</v>
@@ -1646,10 +1646,10 @@
         <v>80.34258184109524</v>
       </c>
       <c r="D32" t="n">
-        <v>9.857903909031506</v>
+        <v>8.762497290798427</v>
       </c>
       <c r="E32" t="n">
-        <v>-2.625972541779717</v>
+        <v>-1.530565923546632</v>
       </c>
       <c r="F32" t="n">
         <v>125.3694555163383</v>
@@ -1661,13 +1661,13 @@
         <v>84.00699883878252</v>
       </c>
       <c r="I32" t="n">
-        <v>10.30752190509329</v>
+        <v>9.162153902258808</v>
       </c>
       <c r="J32" t="n">
         <v>16.78429505996867</v>
       </c>
       <c r="K32" t="n">
-        <v>-1.491175399037754</v>
+        <v>-0.3458073962032664</v>
       </c>
       <c r="L32" t="n">
         <v>149.1264061927795</v>
@@ -1684,10 +1684,10 @@
         <v>80.56885654967969</v>
       </c>
       <c r="D33" t="n">
-        <v>11.82095848843272</v>
+        <v>10.68515237744568</v>
       </c>
       <c r="E33" t="n">
-        <v>-3.881434635364322</v>
+        <v>-2.745628524377274</v>
       </c>
       <c r="F33" t="n">
         <v>126.3179540634155</v>
@@ -1699,13 +1699,13 @@
         <v>84.54862227691086</v>
       </c>
       <c r="I33" t="n">
-        <v>12.40486457162603</v>
+        <v>11.2129543724483</v>
       </c>
       <c r="J33" t="n">
         <v>14.09183225795755</v>
       </c>
       <c r="K33" t="n">
-        <v>0.9143174614105298</v>
+        <v>2.106227660588257</v>
       </c>
       <c r="L33" t="n">
         <v>151.6368455886841</v>
@@ -1722,10 +1722,10 @@
         <v>80.84574799061514</v>
       </c>
       <c r="D34" t="n">
-        <v>13.8491525369192</v>
+        <v>12.67769699728692</v>
       </c>
       <c r="E34" t="n">
-        <v>-5.27387305087521</v>
+        <v>-4.102417511242919</v>
       </c>
       <c r="F34" t="n">
         <v>127.2422770261765</v>
@@ -1737,13 +1737,13 @@
         <v>85.14004723590099</v>
       </c>
       <c r="I34" t="n">
-        <v>14.58478065299581</v>
+        <v>13.35110068270686</v>
       </c>
       <c r="J34" t="n">
         <v>12.87527234643378</v>
       </c>
       <c r="K34" t="n">
-        <v>1.678657932346677</v>
+        <v>2.912337902635638</v>
       </c>
       <c r="L34" t="n">
         <v>154.1089663505554</v>
@@ -1760,10 +1760,10 @@
         <v>81.18443505006242</v>
       </c>
       <c r="D35" t="n">
-        <v>15.93233419637447</v>
+        <v>14.7298692473819</v>
       </c>
       <c r="E35" t="n">
-        <v>-6.787480934208141</v>
+        <v>-5.58501598521557</v>
       </c>
       <c r="F35" t="n">
         <v>128.1635135412216</v>
@@ -1775,13 +1775,13 @@
         <v>85.79487666464719</v>
       </c>
       <c r="I35" t="n">
-        <v>16.83712704923033</v>
+        <v>15.56637444833137</v>
       </c>
       <c r="J35" t="n">
         <v>10.27980921141914</v>
       </c>
       <c r="K35" t="n">
-        <v>3.676737736666551</v>
+        <v>4.94749033756551</v>
       </c>
       <c r="L35" t="n">
         <v>156.5713710784912</v>
@@ -1798,10 +1798,10 @@
         <v>81.59503189540952</v>
       </c>
       <c r="D36" t="n">
-        <v>18.06043445444522</v>
+        <v>16.83142811316937</v>
       </c>
       <c r="E36" t="n">
-        <v>-8.404335545843331</v>
+        <v>-7.175329204567483</v>
       </c>
       <c r="F36" t="n">
         <v>129.1034227609634</v>
@@ -1813,13 +1813,13 @@
         <v>86.52593143841318</v>
       </c>
       <c r="I36" t="n">
-        <v>19.15185124697768</v>
+        <v>17.84857436905551</v>
       </c>
       <c r="J36" t="n">
         <v>14.02801239268973</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.7906601081283444</v>
+        <v>0.5126167697938282</v>
       </c>
       <c r="L36" t="n">
         <v>159.0548927783966</v>
@@ -1836,10 +1836,10 @@
         <v>82.08659044442707</v>
       </c>
       <c r="D37" t="n">
-        <v>20.22356692266605</v>
+        <v>18.97226062367997</v>
       </c>
       <c r="E37" t="n">
-        <v>-10.1044923790473</v>
+        <v>-8.853186080061221</v>
       </c>
       <c r="F37" t="n">
         <v>130.0844352245331</v>
@@ -1851,13 +1851,13 @@
         <v>87.34524126200265</v>
       </c>
       <c r="I37" t="n">
-        <v>21.51913391060387</v>
+        <v>20.1876661277923</v>
       </c>
       <c r="J37" t="n">
         <v>15.6982154660028</v>
       </c>
       <c r="K37" t="n">
-        <v>-3.275352466564346</v>
+        <v>-1.94388468375276</v>
       </c>
       <c r="L37" t="n">
         <v>161.5926072597504</v>
@@ -1874,10 +1874,10 @@
         <v>82.66711946910573</v>
       </c>
       <c r="D38" t="n">
-        <v>22.4121078175164</v>
+        <v>21.14246627505702</v>
       </c>
       <c r="E38" t="n">
-        <v>-11.86607889604083</v>
+        <v>-10.59643735358145</v>
       </c>
       <c r="F38" t="n">
         <v>131.1296511292458</v>
@@ -1889,13 +1889,13 @@
         <v>88.26405360110704</v>
       </c>
       <c r="I38" t="n">
-        <v>23.92950786749431</v>
+        <v>22.57390590776101</v>
       </c>
       <c r="J38" t="n">
         <v>18.78339587273473</v>
       </c>
       <c r="K38" t="n">
-        <v>-7.240751819635936</v>
+        <v>-5.885149859902615</v>
       </c>
       <c r="L38" t="n">
         <v>164.2198252677917</v>
@@ -1912,10 +1912,10 @@
         <v>83.34361304334243</v>
       </c>
       <c r="D39" t="n">
-        <v>24.61674553921227</v>
+        <v>23.33242119172723</v>
       </c>
       <c r="E39" t="n">
-        <v>-13.66536524347681</v>
+        <v>-12.38104089599177</v>
       </c>
       <c r="F39" t="n">
         <v>132.26284044981</v>
@@ -1927,13 +1927,13 @@
         <v>89.29285677609691</v>
       </c>
       <c r="I39" t="n">
-        <v>26.37394100713384</v>
+        <v>24.99793886580123</v>
       </c>
       <c r="J39" t="n">
         <v>20.70319201533607</v>
       </c>
       <c r="K39" t="n">
-        <v>-10.07397077311593</v>
+        <v>-8.697968631783301</v>
       </c>
       <c r="L39" t="n">
         <v>166.9740915298462</v>
@@ -1950,10 +1950,10 @@
         <v>84.12208216735591</v>
       </c>
       <c r="D40" t="n">
-        <v>26.82851055131283</v>
+        <v>25.53280929394618</v>
       </c>
       <c r="E40" t="n">
-        <v>-15.47681686537363</v>
+        <v>-14.18111560800697</v>
       </c>
       <c r="F40" t="n">
         <v>133.5084449648857</v>
@@ -1965,13 +1965,13 @@
         <v>90.44140957909504</v>
       </c>
       <c r="I40" t="n">
-        <v>28.84389269325455</v>
+        <v>27.45085717760347</v>
       </c>
       <c r="J40" t="n">
         <v>19.60235190202505</v>
       </c>
       <c r="K40" t="n">
-        <v>-9.884331785613316</v>
+        <v>-8.491296269962223</v>
       </c>
       <c r="L40" t="n">
         <v>169.8951904773712</v>
@@ -1988,10 +1988,10 @@
         <v>85.00760024654458</v>
       </c>
       <c r="D41" t="n">
-        <v>29.03877544546078</v>
+        <v>27.73463143347759</v>
       </c>
       <c r="E41" t="n">
-        <v>-17.27313083830732</v>
+        <v>-15.96898682632413</v>
       </c>
       <c r="F41" t="n">
         <v>134.8915755748749</v>
@@ -2003,13 +2003,13 @@
         <v>91.71878653189268</v>
       </c>
       <c r="I41" t="n">
-        <v>31.33133082812847</v>
+        <v>29.92422715863282</v>
       </c>
       <c r="J41" t="n">
         <v>21.10090871120205</v>
       </c>
       <c r="K41" t="n">
-        <v>-12.25357980459423</v>
+        <v>-10.84647613509857</v>
       </c>
       <c r="L41" t="n">
         <v>173.0251457691193</v>
@@ -2026,10 +2026,10 @@
         <v>86.00434207432254</v>
       </c>
       <c r="D42" t="n">
-        <v>31.23922357143721</v>
+        <v>29.92918197483871</v>
       </c>
       <c r="E42" t="n">
-        <v>-19.02522867963206</v>
+        <v>-17.71518708303356</v>
       </c>
       <c r="F42" t="n">
         <v>136.4380140304565</v>
@@ -2041,13 +2041,13 @@
         <v>93.13341381582839</v>
       </c>
       <c r="I42" t="n">
-        <v>33.82870522571532</v>
+        <v>32.41007166385956</v>
       </c>
       <c r="J42" t="n">
         <v>25.84477398284949</v>
       </c>
       <c r="K42" t="n">
-        <v>-17.78646019483636</v>
+        <v>-16.36782663298061</v>
       </c>
       <c r="L42" t="n">
         <v>176.4082152843475</v>
@@ -2064,10 +2064,10 @@
         <v>87.1156297457765</v>
       </c>
       <c r="D43" t="n">
-        <v>33.42179664123002</v>
+        <v>32.10799427219749</v>
       </c>
       <c r="E43" t="n">
-        <v>-20.70223069841546</v>
+        <v>-19.38842832938291</v>
       </c>
       <c r="F43" t="n">
         <v>138.1742120981216</v>
@@ -2079,13 +2079,13 @@
         <v>94.69311221725575</v>
       </c>
       <c r="I43" t="n">
-        <v>36.32888781365586</v>
+        <v>34.90080842623542</v>
       </c>
       <c r="J43" t="n">
         <v>21.83949876143102</v>
       </c>
       <c r="K43" t="n">
-        <v>-14.44442434009626</v>
+        <v>-13.01634495267582</v>
       </c>
       <c r="L43" t="n">
         <v>180.090891122818</v>
@@ -2102,10 +2102,10 @@
         <v>88.34397025734856</v>
       </c>
       <c r="D44" t="n">
-        <v>35.57860007529752</v>
+        <v>34.26275839782028</v>
       </c>
       <c r="E44" t="n">
-        <v>-22.27137312299919</v>
+        <v>-20.95553144552195</v>
       </c>
       <c r="F44" t="n">
         <v>140.127292573452</v>
@@ -2117,13 +2117,13 @@
         <v>96.40512858497604</v>
       </c>
       <c r="I44" t="n">
-        <v>38.82505512420285</v>
+        <v>37.38914630388231</v>
       </c>
       <c r="J44" t="n">
         <v>26.89727498887758</v>
       </c>
       <c r="K44" t="n">
-        <v>-19.99249057388319</v>
+        <v>-18.55658175356264</v>
       </c>
       <c r="L44" t="n">
         <v>184.1219074726105</v>
@@ -2140,10 +2140,10 @@
         <v>89.69108782457755</v>
       </c>
       <c r="D45" t="n">
-        <v>37.70178616316623</v>
+        <v>36.38520005800807</v>
       </c>
       <c r="E45" t="n">
-        <v>-23.69789160485084</v>
+        <v>-22.38130549969269</v>
       </c>
       <c r="F45" t="n">
         <v>142.3250471949577</v>
@@ -2155,13 +2155,13 @@
         <v>98.276153679884</v>
       </c>
       <c r="I45" t="n">
-        <v>41.31053174674661</v>
+        <v>39.86792444270332</v>
       </c>
       <c r="J45" t="n">
         <v>27.71049989287422</v>
       </c>
       <c r="K45" t="n">
-        <v>-21.07261538141408</v>
+        <v>-19.63000807737079</v>
       </c>
       <c r="L45" t="n">
         <v>188.5522334575653</v>
@@ -2178,10 +2178,10 @@
         <v>91.15793866266611</v>
       </c>
       <c r="D46" t="n">
-        <v>39.78340269259307</v>
+        <v>38.46693234859023</v>
       </c>
       <c r="E46" t="n">
-        <v>-24.94483801650969</v>
+        <v>-23.62836767250685</v>
       </c>
       <c r="F46" t="n">
         <v>144.7959400415421</v>
@@ -2193,13 +2193,13 @@
         <v>100.3123143180124</v>
       </c>
       <c r="I46" t="n">
-        <v>43.77858093421194</v>
+        <v>42.32990637141121</v>
       </c>
       <c r="J46" t="n">
         <v>32.16648967399126</v>
       </c>
       <c r="K46" t="n">
-        <v>-25.51811129529925</v>
+        <v>-24.06943673249849</v>
       </c>
       <c r="L46" t="n">
         <v>193.4350755214691</v>
@@ -2216,10 +2216,10 @@
         <v>92.74471671142726</v>
       </c>
       <c r="D47" t="n">
-        <v>41.8152011156246</v>
+        <v>40.49926597294353</v>
       </c>
       <c r="E47" t="n">
-        <v>-25.97284300283886</v>
+        <v>-24.65690786015779</v>
       </c>
       <c r="F47" t="n">
         <v>147.569104373455</v>
@@ -2231,13 +2231,13 @@
         <v>102.5191470536752</v>
       </c>
       <c r="I47" t="n">
-        <v>46.2221343086331</v>
+        <v>44.76751184398767</v>
       </c>
       <c r="J47" t="n">
         <v>36.05358551818011</v>
       </c>
       <c r="K47" t="n">
-        <v>-29.05936560629097</v>
+        <v>-27.60474314164556</v>
       </c>
       <c r="L47" t="n">
         <v>198.8258740901947</v>
@@ -2254,10 +2254,10 @@
         <v>94.45083077118149</v>
       </c>
       <c r="D48" t="n">
-        <v>43.78841794483215</v>
+        <v>42.47298665511234</v>
       </c>
       <c r="E48" t="n">
-        <v>-26.73980707764143</v>
+        <v>-25.42437578792162</v>
       </c>
       <c r="F48" t="n">
         <v>150.6743430495262</v>
@@ -2269,13 +2269,13 @@
         <v>104.9015313887159</v>
       </c>
       <c r="I48" t="n">
-        <v>48.63347481432172</v>
+        <v>47.17249500502241</v>
       </c>
       <c r="J48" t="n">
         <v>38.4707042273789</v>
       </c>
       <c r="K48" t="n">
-        <v>-30.73288624511499</v>
+        <v>-29.2719064358157</v>
       </c>
       <c r="L48" t="n">
         <v>204.7823107242584</v>
@@ -2292,10 +2292,10 @@
         <v>96.27486687640318</v>
       </c>
       <c r="D49" t="n">
-        <v>45.69351068449701</v>
+        <v>44.37808796706835</v>
       </c>
       <c r="E49" t="n">
-        <v>-27.20051296060312</v>
+        <v>-25.88509024317446</v>
       </c>
       <c r="F49" t="n">
         <v>154.142130613327</v>
@@ -2307,13 +2307,13 @@
         <v>107.4635917439929</v>
       </c>
       <c r="I49" t="n">
-        <v>51.00384905078577</v>
+        <v>49.53555255282224</v>
       </c>
       <c r="J49" t="n">
         <v>41.22572997555011</v>
       </c>
       <c r="K49" t="n">
-        <v>-32.27907222605123</v>
+        <v>-30.81077572808769</v>
       </c>
       <c r="L49" t="n">
         <v>211.3643026351929</v>
@@ -2330,10 +2330,10 @@
         <v>98.21451603644549</v>
       </c>
       <c r="D50" t="n">
-        <v>47.51985513810623</v>
+        <v>46.2034656341736</v>
       </c>
       <c r="E50" t="n">
-        <v>-27.30615402976245</v>
+        <v>-25.98976452582981</v>
       </c>
       <c r="F50" t="n">
         <v>158.0036119222641</v>
@@ -2345,13 +2345,13 @@
         <v>110.2085503648415</v>
       </c>
       <c r="I50" t="n">
-        <v>53.32301740788063</v>
+        <v>51.84586937723645</v>
       </c>
       <c r="J50" t="n">
         <v>40.01047002151076</v>
       </c>
       <c r="K50" t="n">
-        <v>-29.31640718519773</v>
+        <v>-27.83925915455355</v>
       </c>
       <c r="L50" t="n">
         <v>218.6340038776398</v>
@@ -2368,10 +2368,10 @@
         <v>100.2664738217917</v>
       </c>
       <c r="D51" t="n">
-        <v>49.25539634841956</v>
+        <v>47.93656198526433</v>
       </c>
       <c r="E51" t="n">
-        <v>-27.00376620848561</v>
+        <v>-25.68493184533038</v>
       </c>
       <c r="F51" t="n">
         <v>162.2906010150909</v>
@@ -2383,13 +2383,13 @@
         <v>113.1385343319696</v>
       </c>
       <c r="I51" t="n">
-        <v>55.5787307400979</v>
+        <v>54.09058638649054</v>
       </c>
       <c r="J51" t="n">
         <v>42.19424231771825</v>
       </c>
       <c r="K51" t="n">
-        <v>-29.13413395736543</v>
+        <v>-27.64598960375806</v>
       </c>
       <c r="L51" t="n">
         <v>226.6558043956757</v>
@@ -2406,10 +2406,10 @@
         <v>102.4263047221612</v>
       </c>
       <c r="D52" t="n">
-        <v>50.88624994302766</v>
+        <v>49.56295759699294</v>
       </c>
       <c r="E52" t="n">
-        <v>-26.23555203821927</v>
+        <v>-24.91225969218455</v>
       </c>
       <c r="F52" t="n">
         <v>167.0355834364891</v>
@@ -2421,13 +2421,13 @@
         <v>116.2543280968983</v>
       </c>
       <c r="I52" t="n">
-        <v>57.75612829677298</v>
+        <v>56.2541853829743</v>
       </c>
       <c r="J52" t="n">
         <v>46.38553576714144</v>
       </c>
       <c r="K52" t="n">
-        <v>-30.2528332019558</v>
+        <v>-28.75089028815712</v>
       </c>
       <c r="L52" t="n">
         <v>235.4963324069977</v>
@@ -2444,10 +2444,10 @@
         <v>104.6882651854456</v>
       </c>
       <c r="D53" t="n">
-        <v>52.39624190719121</v>
+        <v>51.06590464695779</v>
       </c>
       <c r="E53" t="n">
-        <v>-24.93808056699839</v>
+        <v>-23.60774330676497</v>
       </c>
       <c r="F53" t="n">
         <v>172.2717146277428</v>
@@ -2459,13 +2459,13 @@
         <v>119.555063696748</v>
       </c>
       <c r="I53" t="n">
-        <v>59.83704121553594</v>
+        <v>58.31778253259164</v>
       </c>
       <c r="J53" t="n">
         <v>46.84077368544262</v>
       </c>
       <c r="K53" t="n">
-        <v>-26.83191397138485</v>
+        <v>-25.31265528844055</v>
       </c>
       <c r="L53" t="n">
         <v>245.2244517803192</v>
@@ -2482,10 +2482,10 @@
         <v>107.0450937702421</v>
       </c>
       <c r="D54" t="n">
-        <v>53.76638833935743</v>
+        <v>52.42578790223146</v>
       </c>
       <c r="E54" t="n">
-        <v>-23.04136559576231</v>
+        <v>-21.70076515863634</v>
       </c>
       <c r="F54" t="n">
         <v>178.032820045948</v>
@@ -2497,13 +2497,13 @@
         <v>123.0378579090637</v>
       </c>
       <c r="I54" t="n">
-        <v>61.79920083941686</v>
+        <v>60.25831185248238</v>
       </c>
       <c r="J54" t="n">
         <v>49.79859378482909</v>
       </c>
       <c r="K54" t="n">
-        <v>-25.00242474502474</v>
+        <v>-23.46153575809026</v>
       </c>
       <c r="L54" t="n">
         <v>255.9112646579742</v>
@@ -2520,10 +2520,10 @@
         <v>109.4877444744851</v>
       </c>
       <c r="D55" t="n">
-        <v>54.97428795010991</v>
+        <v>53.61950687490088</v>
       </c>
       <c r="E55" t="n">
-        <v>-20.46776920796201</v>
+        <v>-19.112988132753</v>
       </c>
       <c r="F55" t="n">
         <v>184.3533962965012</v>
@@ -2535,13 +2535,13 @@
         <v>126.6973659163725</v>
       </c>
       <c r="I55" t="n">
-        <v>63.61531612362553</v>
+        <v>62.04758637956878</v>
       </c>
       <c r="J55" t="n">
         <v>52.32996401969842</v>
       </c>
       <c r="K55" t="n">
-        <v>-21.71544263482865</v>
+        <v>-20.14771289077191</v>
       </c>
       <c r="L55" t="n">
         <v>267.6301095485687</v>
@@ -2558,10 +2558,10 @@
         <v>112.0050765163589</v>
       </c>
       <c r="D56" t="n">
-        <v>55.9934274127388</v>
+        <v>54.61975797799101</v>
       </c>
       <c r="E56" t="n">
-        <v>-17.13074010779429</v>
+        <v>-15.75707067304649</v>
       </c>
       <c r="F56" t="n">
         <v>191.2686094045639</v>
@@ -2573,13 +2573,13 @@
         <v>130.5252675657962</v>
       </c>
       <c r="I56" t="n">
-        <v>65.25201644682835</v>
+        <v>63.65120891118755</v>
       </c>
       <c r="J56" t="n">
         <v>54.06279900294504</v>
       </c>
       <c r="K56" t="n">
-        <v>-16.46470035859996</v>
+        <v>-14.86389282295916</v>
       </c>
       <c r="L56" t="n">
         <v>280.4565627574921</v>
@@ -2596,10 +2596,10 @@
         <v>114.5834858700164</v>
       </c>
       <c r="D57" t="n">
-        <v>56.7923684313985</v>
+        <v>55.39419727674051</v>
       </c>
       <c r="E57" t="n">
-        <v>-12.93333510945953</v>
+        <v>-11.53516395480153</v>
       </c>
       <c r="F57" t="n">
         <v>198.8142963647842</v>
@@ -2611,13 +2611,13 @@
         <v>134.509664026716</v>
       </c>
       <c r="I57" t="n">
-        <v>66.66861580432902</v>
+        <v>65.02730134407395</v>
       </c>
       <c r="J57" t="n">
         <v>56.62547839384683</v>
       </c>
       <c r="K57" t="n">
-        <v>-10.72779042789951</v>
+        <v>-9.086475967644439</v>
       </c>
       <c r="L57" t="n">
         <v>294.4684357643127</v>
@@ -2634,10 +2634,10 @@
         <v>117.2064698054924</v>
       </c>
       <c r="D58" t="n">
-        <v>57.33379372616003</v>
+        <v>55.90445685302941</v>
       </c>
       <c r="E58" t="n">
-        <v>-7.766486471661274</v>
+        <v>-6.337149598530665</v>
       </c>
       <c r="F58" t="n">
         <v>207.026964366436</v>
@@ -2649,13 +2649,13 @@
         <v>138.6343752115479</v>
       </c>
       <c r="I58" t="n">
-        <v>67.81566482570992</v>
+        <v>66.1250139196453</v>
       </c>
       <c r="J58" t="n">
         <v>58.13641802772237</v>
       </c>
       <c r="K58" t="n">
-        <v>-2.453030303712822</v>
+        <v>-0.7623793976482176</v>
       </c>
       <c r="L58" t="n">
         <v>309.7457778453827</v>
@@ -2672,10 +2672,10 @@
         <v>119.8541214043112</v>
       </c>
       <c r="D59" t="n">
-        <v>57.57337909105122</v>
+        <v>56.10497473338408</v>
       </c>
       <c r="E59" t="n">
-        <v>-1.506970236050662</v>
+        <v>-0.03856587838355097</v>
       </c>
       <c r="F59" t="n">
         <v>215.9437910914421</v>
@@ -2687,13 +2687,13 @@
         <v>142.8781279195955</v>
       </c>
       <c r="I59" t="n">
-        <v>68.63323952611856</v>
+        <v>66.88275432632541</v>
       </c>
       <c r="J59" t="n">
         <v>62.7429355864362</v>
       </c>
       <c r="K59" t="n">
-        <v>4.404833854662513</v>
+        <v>6.155319054455674</v>
       </c>
       <c r="L59" t="n">
         <v>326.3708760738373</v>
@@ -2710,10 +2710,10 @@
         <v>122.5025383545815</v>
       </c>
       <c r="D60" t="n">
-        <v>57.45843426147015</v>
+        <v>55.94158919360174</v>
       </c>
       <c r="E60" t="n">
-        <v>5.985004250210764</v>
+        <v>7.501849318079152</v>
       </c>
       <c r="F60" t="n">
         <v>225.6026241779327</v>
@@ -2725,13 +2725,13 @@
         <v>147.2136123380727</v>
       </c>
       <c r="I60" t="n">
-        <v>69.04888486830568</v>
+        <v>67.22606352274498</v>
       </c>
       <c r="J60" t="n">
         <v>64.77431477793675</v>
       </c>
       <c r="K60" t="n">
-        <v>15.73530110343063</v>
+        <v>17.5581224489913</v>
       </c>
       <c r="L60" t="n">
         <v>344.4282546043396</v>
@@ -2748,10 +2748,10 @@
         <v>125.1231257834983</v>
       </c>
       <c r="D61" t="n">
-        <v>56.92626586441737</v>
+        <v>55.34983426544289</v>
       </c>
       <c r="E61" t="n">
-        <v>14.86866580506841</v>
+        <v>16.44509740404288</v>
       </c>
       <c r="F61" t="n">
         <v>236.0419815182686</v>
@@ -2763,13 +2763,13 @@
         <v>151.6063756758792</v>
       </c>
       <c r="I61" t="n">
-        <v>68.97513784461449</v>
+        <v>67.06504265058146</v>
       </c>
       <c r="J61" t="n">
         <v>68.71950061016926</v>
       </c>
       <c r="K61" t="n">
-        <v>27.29886106514549</v>
+        <v>29.20895625917852</v>
       </c>
       <c r="L61" t="n">
         <v>364.0046718120575</v>
@@ -2786,10 +2786,10 @@
         <v>127.6817821796624</v>
       </c>
       <c r="D62" t="n">
-        <v>55.90215970604898</v>
+        <v>54.25284017856431</v>
       </c>
       <c r="E62" t="n">
-        <v>25.32614361457638</v>
+        <v>26.97546314206105</v>
       </c>
       <c r="F62" t="n">
         <v>247.3010524511337</v>
@@ -2801,13 +2801,13 @@
         <v>156.0135339024049</v>
       </c>
       <c r="I62" t="n">
-        <v>68.30648303643838</v>
+        <v>66.29119030144932</v>
       </c>
       <c r="J62" t="n">
         <v>17.3017853735327</v>
       </c>
       <c r="K62" t="n">
-        <v>96.65765199687876</v>
+        <v>98.67294473186784</v>
       </c>
       <c r="L62" t="n">
         <v>385.1891255378723</v>

</xml_diff>

<commit_message>
Stack IDA plots, some minor changes,
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -500,37 +500,37 @@
         <v>1960</v>
       </c>
       <c r="B2" t="n">
-        <v>3.198688399973083</v>
+        <v>2.957472290406829</v>
       </c>
       <c r="C2" t="n">
-        <v>8.519418801836229</v>
+        <v>8.564322552084578</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2744830222869237</v>
+        <v>-1.184753948311111</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.942829590002887</v>
+        <v>-1.707797212041673</v>
       </c>
       <c r="F2" t="n">
-        <v>8.500794589519501</v>
+        <v>8.629243682138622</v>
       </c>
       <c r="G2" t="n">
-        <v>3.078063852655954</v>
+        <v>3.009838941080147</v>
       </c>
       <c r="H2" t="n">
-        <v>8.198146171346439</v>
+        <v>8.272195929677791</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.2641320952288594</v>
+        <v>-0.2409611487482758</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.904283142004869</v>
+        <v>-1.912467472619453</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.429034735041368</v>
+        <v>-3.611257959900463</v>
       </c>
       <c r="L2" t="n">
-        <v>5.678760051727295</v>
+        <v>5.517348289489746</v>
       </c>
     </row>
     <row r="3">
@@ -538,37 +538,37 @@
         <v>1961</v>
       </c>
       <c r="B3" t="n">
-        <v>6.283104072752837</v>
+        <v>5.843796982785944</v>
       </c>
       <c r="C3" t="n">
-        <v>16.28675076265056</v>
+        <v>16.37195328550274</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.6249356946155221</v>
+        <v>-2.315647296754492</v>
       </c>
       <c r="E3" t="n">
-        <v>-5.288780363055024</v>
+        <v>-3.06883613527095</v>
       </c>
       <c r="F3" t="n">
-        <v>16.65613877773285</v>
+        <v>16.83126683626324</v>
       </c>
       <c r="G3" t="n">
-        <v>5.987611524039378</v>
+        <v>5.856665375718135</v>
       </c>
       <c r="H3" t="n">
-        <v>15.52078963302567</v>
+        <v>15.64407426294036</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.5955451514945248</v>
+        <v>-0.5510086274210471</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.600137381010331</v>
+        <v>-8.630056343137065</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.7705674118679333</v>
+        <v>-1.077342924860028</v>
       </c>
       <c r="L3" t="n">
-        <v>11.54215121269226</v>
+        <v>11.24233174324036</v>
       </c>
     </row>
     <row r="4">
@@ -576,37 +576,37 @@
         <v>1962</v>
       </c>
       <c r="B4" t="n">
-        <v>9.231758195377864</v>
+        <v>8.632361327864997</v>
       </c>
       <c r="C4" t="n">
-        <v>23.38054526910285</v>
+        <v>23.49492837964499</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.041910225050692</v>
+        <v>-3.370225307114356</v>
       </c>
       <c r="E4" t="n">
-        <v>-7.104051863125395</v>
+        <v>-4.138078618018204</v>
       </c>
       <c r="F4" t="n">
-        <v>24.46634137630463</v>
+        <v>24.61898578237742</v>
       </c>
       <c r="G4" t="n">
-        <v>8.74116821081709</v>
+        <v>8.553766230617091</v>
       </c>
       <c r="H4" t="n">
-        <v>22.13806674011207</v>
+        <v>22.29458886299748</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.9865414956707068</v>
+        <v>-0.9224908450123742</v>
       </c>
       <c r="J4" t="n">
-        <v>-11.86663873428929</v>
+        <v>-11.90034521495542</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.4766288805913597</v>
+        <v>-0.8927580320598558</v>
       </c>
       <c r="L4" t="n">
-        <v>17.54942584037781</v>
+        <v>17.13276100158691</v>
       </c>
     </row>
     <row r="5">
@@ -614,37 +614,37 @@
         <v>1963</v>
       </c>
       <c r="B5" t="n">
-        <v>12.030074056003</v>
+        <v>11.30435862025081</v>
       </c>
       <c r="C5" t="n">
-        <v>29.86034637456686</v>
+        <v>29.99029548963885</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.514198222601659</v>
+        <v>-4.331129278993711</v>
       </c>
       <c r="E5" t="n">
-        <v>-8.4438412932801</v>
+        <v>-4.958171232040508</v>
       </c>
       <c r="F5" t="n">
-        <v>31.93238091468811</v>
+        <v>32.00535359885544</v>
       </c>
       <c r="G5" t="n">
-        <v>11.34716773067868</v>
+        <v>11.11009766347402</v>
       </c>
       <c r="H5" t="n">
-        <v>28.16527622615067</v>
+        <v>28.34481344811425</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.428242347417871</v>
+        <v>-1.346632958759547</v>
       </c>
       <c r="J5" t="n">
-        <v>-11.93580062186216</v>
+        <v>-11.96388374035964</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.486324514313235</v>
+        <v>-2.995686784218959</v>
       </c>
       <c r="L5" t="n">
-        <v>23.66207647323608</v>
+        <v>23.14870762825012</v>
       </c>
     </row>
     <row r="6">
@@ -652,37 +652,37 @@
         <v>1964</v>
       </c>
       <c r="B6" t="n">
-        <v>14.66860211925968</v>
+        <v>13.84676630945767</v>
       </c>
       <c r="C6" t="n">
-        <v>35.77376767348272</v>
+        <v>35.90553506972488</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.029197988747954</v>
+        <v>-5.185338932111792</v>
       </c>
       <c r="E6" t="n">
-        <v>-9.357264494939114</v>
+        <v>-5.563602314383958</v>
       </c>
       <c r="F6" t="n">
-        <v>39.05590730905533</v>
+        <v>39.00336013268679</v>
       </c>
       <c r="G6" t="n">
-        <v>13.81129608085736</v>
+        <v>13.53166251947788</v>
       </c>
       <c r="H6" t="n">
-        <v>33.68297082770759</v>
+        <v>33.87912331637474</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.910601569353406</v>
+        <v>-1.813517812914484</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.107255176350909</v>
+        <v>-8.123394384997328</v>
       </c>
       <c r="K6" t="n">
-        <v>-7.632581246310945</v>
+        <v>-8.221373103883201</v>
       </c>
       <c r="L6" t="n">
-        <v>29.84382891654968</v>
+        <v>29.25250053405762</v>
       </c>
     </row>
     <row r="7">
@@ -690,37 +690,37 @@
         <v>1965</v>
       </c>
       <c r="B7" t="n">
-        <v>17.14178262797243</v>
+        <v>16.25093614644977</v>
       </c>
       <c r="C7" t="n">
-        <v>41.16063799466459</v>
+        <v>41.28173559479643</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.573234069733215</v>
+        <v>-5.923561835386545</v>
       </c>
       <c r="E7" t="n">
-        <v>-9.889947670838982</v>
+        <v>-5.983077903589432</v>
       </c>
       <c r="F7" t="n">
-        <v>45.83923888206482</v>
+        <v>45.62603200227022</v>
       </c>
       <c r="G7" t="n">
-        <v>16.13745747009888</v>
+        <v>15.82251006678173</v>
       </c>
       <c r="H7" t="n">
-        <v>38.74906475579328</v>
+        <v>38.95796005838631</v>
       </c>
       <c r="I7" t="n">
-        <v>-2.422470069896165</v>
+        <v>-2.312126909651921</v>
       </c>
       <c r="J7" t="n">
-        <v>-8.235904593435361</v>
+        <v>-8.250172819183792</v>
       </c>
       <c r="K7" t="n">
-        <v>-8.167496975478723</v>
+        <v>-8.809440366272508</v>
       </c>
       <c r="L7" t="n">
-        <v>36.06065058708191</v>
+        <v>35.40873003005981</v>
       </c>
     </row>
     <row r="8">
@@ -728,37 +728,37 @@
         <v>1966</v>
       </c>
       <c r="B8" t="n">
-        <v>19.44706602831662</v>
+        <v>18.51158072789739</v>
       </c>
       <c r="C8" t="n">
-        <v>46.05555277051322</v>
+        <v>46.15554486292123</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.131849799973255</v>
+        <v>-6.539719058992781</v>
       </c>
       <c r="E8" t="n">
-        <v>-10.08540204643731</v>
+        <v>-6.240973938137468</v>
       </c>
       <c r="F8" t="n">
-        <v>52.28536695241928</v>
+        <v>51.88643259368837</v>
       </c>
       <c r="G8" t="n">
-        <v>18.32847265147324</v>
+        <v>17.98546040953443</v>
       </c>
       <c r="H8" t="n">
-        <v>43.40644178271985</v>
+        <v>43.62586541582986</v>
       </c>
       <c r="I8" t="n">
-        <v>-2.95170609920023</v>
+        <v>-2.830433643507373</v>
       </c>
       <c r="J8" t="n">
-        <v>-5.130172176490072</v>
+        <v>-5.138174294387066</v>
       </c>
       <c r="K8" t="n">
-        <v>-11.37229565900633</v>
+        <v>-12.05847339780005</v>
       </c>
       <c r="L8" t="n">
-        <v>42.28074049949646</v>
+        <v>41.5842444896698</v>
       </c>
     </row>
     <row r="9">
@@ -766,37 +766,37 @@
         <v>1967</v>
       </c>
       <c r="B9" t="n">
-        <v>21.58426685842868</v>
+        <v>20.62602957244046</v>
       </c>
       <c r="C9" t="n">
-        <v>50.48951225182122</v>
+        <v>50.56042719509684</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.690078256473666</v>
+        <v>-7.03049299021945</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.985750085305469</v>
+        <v>-6.358301746412373</v>
       </c>
       <c r="F9" t="n">
-        <v>58.39795076847076</v>
+        <v>57.79766203090549</v>
       </c>
       <c r="G9" t="n">
-        <v>20.38658188093465</v>
+        <v>20.02263337352045</v>
       </c>
       <c r="H9" t="n">
-        <v>47.68791001341147</v>
+        <v>47.91670385659557</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.485320257392959</v>
+        <v>-3.355535128114878</v>
       </c>
       <c r="J9" t="n">
-        <v>-6.586913857908061</v>
+        <v>-6.596514091755518</v>
       </c>
       <c r="K9" t="n">
-        <v>-9.527720168037408</v>
+        <v>-10.23913718474513</v>
       </c>
       <c r="L9" t="n">
-        <v>48.47453761100769</v>
+        <v>47.74815082550049</v>
       </c>
     </row>
     <row r="10">
@@ -804,37 +804,37 @@
         <v>1968</v>
       </c>
       <c r="B10" t="n">
-        <v>23.55508000805843</v>
+        <v>22.59366985120897</v>
       </c>
       <c r="C10" t="n">
-        <v>54.4910019001033</v>
+        <v>54.52750038823049</v>
       </c>
       <c r="D10" t="n">
-        <v>-4.23270384904053</v>
+        <v>-7.394923434127047</v>
       </c>
       <c r="E10" t="n">
-        <v>-9.632057153435767</v>
+        <v>-6.353389564352405</v>
       </c>
       <c r="F10" t="n">
-        <v>64.18132090568542</v>
+        <v>63.37285724096</v>
       </c>
       <c r="G10" t="n">
-        <v>22.31380590281522</v>
+        <v>21.93582795370119</v>
       </c>
       <c r="H10" t="n">
-        <v>51.61950795466915</v>
+        <v>51.85716009495591</v>
       </c>
       <c r="I10" t="n">
-        <v>-4.009654482144734</v>
+        <v>-3.873818650436928</v>
       </c>
       <c r="J10" t="n">
-        <v>-14.00656624087751</v>
+        <v>-14.02635039273692</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.302373505174407</v>
+        <v>-2.021002370351409</v>
       </c>
       <c r="L10" t="n">
-        <v>54.61471962928772</v>
+        <v>53.87181663513184</v>
       </c>
     </row>
     <row r="11">
@@ -842,37 +842,37 @@
         <v>1969</v>
       </c>
       <c r="B11" t="n">
-        <v>25.36270910508928</v>
+        <v>24.41551821325659</v>
       </c>
       <c r="C11" t="n">
-        <v>58.08672636119757</v>
+        <v>58.08610443288743</v>
       </c>
       <c r="D11" t="n">
-        <v>-4.744508420970917</v>
+        <v>-7.634041474538843</v>
       </c>
       <c r="E11" t="n">
-        <v>-9.064448076695637</v>
+        <v>-6.2423892614128</v>
       </c>
       <c r="F11" t="n">
-        <v>69.6404789686203</v>
+        <v>68.62519191019237</v>
       </c>
       <c r="G11" t="n">
-        <v>24.11220133685969</v>
+        <v>23.7267956704013</v>
       </c>
       <c r="H11" t="n">
-        <v>55.22276170171533</v>
+        <v>55.46912226505163</v>
       </c>
       <c r="I11" t="n">
-        <v>-4.510580546299819</v>
+        <v>-4.371155803915822</v>
       </c>
       <c r="J11" t="n">
-        <v>-17.54095608369634</v>
+        <v>-17.56575942558975</v>
       </c>
       <c r="K11" t="n">
-        <v>3.39276897449303</v>
+        <v>2.669864395721952</v>
       </c>
       <c r="L11" t="n">
-        <v>60.6761953830719</v>
+        <v>59.92886710166931</v>
       </c>
     </row>
     <row r="12">
@@ -880,37 +880,37 @@
         <v>1970</v>
       </c>
       <c r="B12" t="n">
-        <v>27.01157611545359</v>
+        <v>26.0938875572375</v>
       </c>
       <c r="C12" t="n">
-        <v>61.3021172310517</v>
+        <v>61.26420022305548</v>
       </c>
       <c r="D12" t="n">
-        <v>-5.210510624263786</v>
+        <v>-7.750533659893609</v>
       </c>
       <c r="E12" t="n">
-        <v>-8.322086979062171</v>
+        <v>-6.039677628703732</v>
       </c>
       <c r="F12" t="n">
-        <v>74.78109574317932</v>
+        <v>73.56787649169564</v>
       </c>
       <c r="G12" t="n">
-        <v>25.78404088716725</v>
+        <v>25.39743118628412</v>
       </c>
       <c r="H12" t="n">
-        <v>58.51625578601728</v>
+        <v>58.77134256549279</v>
       </c>
       <c r="I12" t="n">
-        <v>-4.973720097072566</v>
+        <v>-4.83311566576439</v>
       </c>
       <c r="J12" t="n">
-        <v>-11.6382355191162</v>
+        <v>-11.65514480024612</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.052224075489422</v>
+        <v>-1.785326146255283</v>
       </c>
       <c r="L12" t="n">
-        <v>66.63611698150635</v>
+        <v>65.89518713951111</v>
       </c>
     </row>
     <row r="13">
@@ -918,37 +918,37 @@
         <v>1971</v>
       </c>
       <c r="B13" t="n">
-        <v>28.50708684051036</v>
+        <v>27.63212394798747</v>
       </c>
       <c r="C13" t="n">
-        <v>64.16168483293919</v>
+        <v>64.08865285623139</v>
       </c>
       <c r="D13" t="n">
-        <v>-5.616195136702888</v>
+        <v>-7.74843682086959</v>
       </c>
       <c r="E13" t="n">
-        <v>-7.443063730807939</v>
+        <v>-5.758181793866285</v>
       </c>
       <c r="F13" t="n">
-        <v>79.60951280593872</v>
+        <v>78.21415818948299</v>
       </c>
       <c r="G13" t="n">
-        <v>27.33193085612616</v>
+        <v>26.94990307184556</v>
       </c>
       <c r="H13" t="n">
-        <v>61.5167289199957</v>
+        <v>61.78059964890488</v>
       </c>
       <c r="I13" t="n">
-        <v>-5.38467708081417</v>
+        <v>-5.245197995268683</v>
       </c>
       <c r="J13" t="n">
-        <v>-13.57224390272271</v>
+        <v>-13.59289291180607</v>
       </c>
       <c r="K13" t="n">
-        <v>2.582131723238383</v>
+        <v>1.85651053434677</v>
       </c>
       <c r="L13" t="n">
-        <v>72.47387051582336</v>
+        <v>71.74892234802246</v>
       </c>
     </row>
     <row r="14">
@@ -956,37 +956,37 @@
         <v>1972</v>
       </c>
       <c r="B14" t="n">
-        <v>29.8554416643281</v>
+        <v>29.03439694790002</v>
       </c>
       <c r="C14" t="n">
-        <v>66.68926621238614</v>
+        <v>66.58543263791603</v>
       </c>
       <c r="D14" t="n">
-        <v>-5.947729212459708</v>
+        <v>-7.632859963330706</v>
       </c>
       <c r="E14" t="n">
-        <v>-6.46423631892144</v>
+        <v>-5.409648639783267</v>
       </c>
       <c r="F14" t="n">
-        <v>84.1327423453331</v>
+        <v>82.57732098270208</v>
       </c>
       <c r="G14" t="n">
-        <v>28.7588877220012</v>
+        <v>28.38673832805792</v>
       </c>
       <c r="H14" t="n">
-        <v>64.23985083952782</v>
+        <v>64.51251799001095</v>
       </c>
       <c r="I14" t="n">
-        <v>-5.72927637598373</v>
+        <v>-5.593069479059312</v>
       </c>
       <c r="J14" t="n">
-        <v>-7.089600779399854</v>
+        <v>-7.101036231906146</v>
       </c>
       <c r="K14" t="n">
-        <v>-2.008783201036794</v>
+        <v>-2.734674933427876</v>
       </c>
       <c r="L14" t="n">
-        <v>78.17107820510864</v>
+        <v>77.47047567367554</v>
       </c>
     </row>
     <row r="15">
@@ -994,37 +994,37 @@
         <v>1973</v>
       </c>
       <c r="B15" t="n">
-        <v>31.06347623583888</v>
+        <v>30.30552738309246</v>
       </c>
       <c r="C15" t="n">
-        <v>68.90819396895697</v>
+        <v>68.77975848157914</v>
       </c>
       <c r="D15" t="n">
-        <v>-6.192167984703453</v>
+        <v>-7.409731977225118</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.421035356460202</v>
+        <v>-5.004868262742708</v>
       </c>
       <c r="F15" t="n">
-        <v>88.3584668636322</v>
+        <v>86.67068562470376</v>
       </c>
       <c r="G15" t="n">
-        <v>30.06837907257269</v>
+        <v>29.7108694133733</v>
       </c>
       <c r="H15" t="n">
-        <v>66.70076722045951</v>
+        <v>66.98214963148536</v>
       </c>
       <c r="I15" t="n">
-        <v>-5.993806128829219</v>
+        <v>-5.862809674823973</v>
       </c>
       <c r="J15" t="n">
-        <v>-6.066499763697654</v>
+        <v>-6.076946494427875</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.9972391431811074</v>
+        <v>-1.710754511883047</v>
       </c>
       <c r="L15" t="n">
-        <v>83.71160125732422</v>
+        <v>83.04250836372375</v>
       </c>
     </row>
     <row r="16">
@@ -1032,37 +1032,37 @@
         <v>1974</v>
       </c>
       <c r="B16" t="n">
-        <v>32.13852726115811</v>
+        <v>31.45084805959376</v>
       </c>
       <c r="C16" t="n">
-        <v>70.84140964315219</v>
+        <v>70.69619952864835</v>
       </c>
       <c r="D16" t="n">
-        <v>-6.337640022479033</v>
+        <v>-7.085576054017685</v>
       </c>
       <c r="E16" t="n">
-        <v>-4.347258718169307</v>
+        <v>-4.55386190794615</v>
       </c>
       <c r="F16" t="n">
-        <v>92.29503816366196</v>
+        <v>90.50760962627828</v>
       </c>
       <c r="G16" t="n">
-        <v>31.26433898395915</v>
+        <v>30.92565848092752</v>
       </c>
       <c r="H16" t="n">
-        <v>68.91447847586318</v>
+        <v>69.20437860202058</v>
       </c>
       <c r="I16" t="n">
-        <v>-6.165252203717531</v>
+        <v>-6.041149443061574</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.60624493392778</v>
+        <v>-2.611050233926659</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.325782837054341</v>
+        <v>-3.027893625060829</v>
       </c>
       <c r="L16" t="n">
-        <v>89.08153748512268</v>
+        <v>88.44994378089905</v>
       </c>
     </row>
     <row r="17">
@@ -1070,37 +1070,37 @@
         <v>1975</v>
       </c>
       <c r="B17" t="n">
-        <v>33.08831705653814</v>
+        <v>32.47608684455813</v>
       </c>
       <c r="C17" t="n">
-        <v>72.51153859695562</v>
+        <v>72.35873995668099</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.373516906645429</v>
+        <v>-6.667306576011239</v>
       </c>
       <c r="E17" t="n">
-        <v>-3.274858477416259</v>
+        <v>-4.066032950014879</v>
       </c>
       <c r="F17" t="n">
-        <v>95.95148026943207</v>
+        <v>94.101487275213</v>
       </c>
       <c r="G17" t="n">
-        <v>32.35116323906335</v>
+        <v>32.03489513206893</v>
       </c>
       <c r="H17" t="n">
-        <v>70.89609960692228</v>
+        <v>71.19419187216447</v>
       </c>
       <c r="I17" t="n">
-        <v>-6.231525329665376</v>
+        <v>-6.115702198816128</v>
       </c>
       <c r="J17" t="n">
-        <v>-2.913684595265906</v>
+        <v>-2.919436298699532</v>
       </c>
       <c r="K17" t="n">
-        <v>0.167167192699921</v>
+        <v>-0.5139870637703559</v>
       </c>
       <c r="L17" t="n">
-        <v>94.26922011375427</v>
+        <v>93.67996144294739</v>
       </c>
     </row>
     <row r="18">
@@ -1108,37 +1108,37 @@
         <v>1976</v>
       </c>
       <c r="B18" t="n">
-        <v>33.92085168295264</v>
+        <v>33.38726978080729</v>
       </c>
       <c r="C18" t="n">
-        <v>73.94092447897175</v>
+        <v>73.79082642002969</v>
       </c>
       <c r="D18" t="n">
-        <v>-6.290555581382483</v>
+        <v>-6.162052037140108</v>
       </c>
       <c r="E18" t="n">
-        <v>-2.233734492266009</v>
+        <v>-3.550294561863346</v>
       </c>
       <c r="F18" t="n">
-        <v>99.33748608827591</v>
+        <v>97.46574960183352</v>
       </c>
       <c r="G18" t="n">
-        <v>33.33368904959556</v>
+        <v>33.04278326392376</v>
       </c>
       <c r="H18" t="n">
-        <v>72.66102300905231</v>
+        <v>72.9668633638472</v>
       </c>
       <c r="I18" t="n">
-        <v>-6.181667419759469</v>
+        <v>-6.075179114697664</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.7549633027352296</v>
+        <v>-0.756555698092039</v>
       </c>
       <c r="K18" t="n">
-        <v>0.207138113843764</v>
+        <v>-0.4559093087251512</v>
       </c>
       <c r="L18" t="n">
-        <v>99.26521944999695</v>
+        <v>98.7220025062561</v>
       </c>
     </row>
     <row r="19">
@@ -1146,37 +1146,37 @@
         <v>1977</v>
       </c>
       <c r="B19" t="n">
-        <v>34.64433185413752</v>
+        <v>34.19063718618862</v>
       </c>
       <c r="C19" t="n">
-        <v>75.15164310911429</v>
+        <v>75.01538640808404</v>
       </c>
       <c r="D19" t="n">
-        <v>-6.081019874168324</v>
+        <v>-5.576998418921132</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.251535830488976</v>
+        <v>-3.015160728361337</v>
       </c>
       <c r="F19" t="n">
-        <v>102.4634192585945</v>
+        <v>100.6138644469902</v>
       </c>
       <c r="G19" t="n">
-        <v>34.21716378462646</v>
+        <v>33.9539129762872</v>
       </c>
       <c r="H19" t="n">
-        <v>74.22501584891296</v>
+        <v>74.53805595060992</v>
       </c>
       <c r="I19" t="n">
-        <v>-6.006040292191001</v>
+        <v>-5.909585463996178</v>
       </c>
       <c r="J19" t="n">
-        <v>0.6365219879492631</v>
+        <v>0.6379517411818794</v>
       </c>
       <c r="K19" t="n">
-        <v>0.9896846523002222</v>
+        <v>0.3474309854923805</v>
       </c>
       <c r="L19" t="n">
-        <v>104.0623459815979</v>
+        <v>103.5677661895752</v>
       </c>
     </row>
     <row r="20">
@@ -1184,37 +1184,37 @@
         <v>1978</v>
       </c>
       <c r="B20" t="n">
-        <v>35.26707221353514</v>
+        <v>34.8925741668054</v>
       </c>
       <c r="C20" t="n">
-        <v>76.16549611589225</v>
+        <v>76.05483416045649</v>
       </c>
       <c r="D20" t="n">
-        <v>-5.738769058438906</v>
+        <v>-4.919255306834768</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.3534855979690761</v>
+        <v>-2.468816652432579</v>
       </c>
       <c r="F20" t="n">
-        <v>105.3403136730194</v>
+        <v>103.5593363679945</v>
       </c>
       <c r="G20" t="n">
-        <v>35.00720288578614</v>
+        <v>34.77322271934422</v>
       </c>
       <c r="H20" t="n">
-        <v>75.60426222175262</v>
+        <v>75.92386903804864</v>
       </c>
       <c r="I20" t="n">
-        <v>-5.696482303011815</v>
+        <v>-5.610383087900888</v>
       </c>
       <c r="J20" t="n">
-        <v>8.71675703956166</v>
+        <v>8.737521180768823</v>
       </c>
       <c r="K20" t="n">
-        <v>-4.976097096209575</v>
+        <v>-5.6130195994063</v>
       </c>
       <c r="L20" t="n">
-        <v>108.655642747879</v>
+        <v>108.2112102508545</v>
       </c>
     </row>
     <row r="21">
@@ -1222,37 +1222,37 @@
         <v>1979</v>
       </c>
       <c r="B21" t="n">
-        <v>35.79742950603747</v>
+        <v>35.49954908824827</v>
       </c>
       <c r="C21" t="n">
-        <v>77.00398172655416</v>
+        <v>76.93106420453583</v>
       </c>
       <c r="D21" t="n">
-        <v>-5.259317683109761</v>
+        <v>-4.19573959759535</v>
       </c>
       <c r="E21" t="n">
-        <v>0.437780703791141</v>
+        <v>-1.919166969956443</v>
       </c>
       <c r="F21" t="n">
-        <v>107.979874253273</v>
+        <v>106.3157067252323</v>
       </c>
       <c r="G21" t="n">
-        <v>35.70974361977261</v>
+        <v>35.50595651165987</v>
       </c>
       <c r="H21" t="n">
-        <v>76.8153602954406</v>
+        <v>77.14084260960036</v>
       </c>
       <c r="I21" t="n">
-        <v>-5.24643497229629</v>
+        <v>-5.170631051195103</v>
       </c>
       <c r="J21" t="n">
-        <v>11.85815534527128</v>
+        <v>11.88797135242909</v>
       </c>
       <c r="K21" t="n">
-        <v>-6.094431557475311</v>
+        <v>-6.715587481576241</v>
       </c>
       <c r="L21" t="n">
-        <v>113.0423927307129</v>
+        <v>112.648551940918</v>
       </c>
     </row>
     <row r="22">
@@ -1260,37 +1260,37 @@
         <v>1980</v>
       </c>
       <c r="B22" t="n">
-        <v>36.24373571812821</v>
+        <v>36.01806044817678</v>
       </c>
       <c r="C22" t="n">
-        <v>77.68825976289256</v>
+        <v>77.66542698035695</v>
       </c>
       <c r="D22" t="n">
-        <v>-4.639864327902043</v>
+        <v>-3.413079535993501</v>
       </c>
       <c r="E22" t="n">
-        <v>1.102344187724476</v>
+        <v>-1.373854269981514</v>
       </c>
       <c r="F22" t="n">
-        <v>110.3944753408432</v>
+        <v>108.8965536225587</v>
       </c>
       <c r="G22" t="n">
-        <v>36.3309916538479</v>
+        <v>36.15761574803651</v>
       </c>
       <c r="H22" t="n">
-        <v>77.87529240910662</v>
+        <v>78.20592610449425</v>
       </c>
       <c r="I22" t="n">
-        <v>-4.651034691428917</v>
+        <v>-4.585084808366894</v>
       </c>
       <c r="J22" t="n">
-        <v>6.012469489304225</v>
+        <v>6.028347001057323</v>
       </c>
       <c r="K22" t="n">
-        <v>1.654396655832775</v>
+        <v>1.071464435079722</v>
       </c>
       <c r="L22" t="n">
-        <v>117.2221155166626</v>
+        <v>116.8782684803009</v>
       </c>
     </row>
     <row r="23">
@@ -1298,37 +1298,37 @@
         <v>1981</v>
       </c>
       <c r="B23" t="n">
-        <v>36.61423951531172</v>
+        <v>36.45459175211546</v>
       </c>
       <c r="C23" t="n">
-        <v>78.23909919556851</v>
+        <v>78.27870153378181</v>
       </c>
       <c r="D23" t="n">
-        <v>-3.879287611332589</v>
+        <v>-2.577532775955327</v>
       </c>
       <c r="E23" t="n">
-        <v>1.623110789528589</v>
+        <v>-0.8402685635278289</v>
       </c>
       <c r="F23" t="n">
-        <v>112.5971618890762</v>
+        <v>111.3154919464141</v>
       </c>
       <c r="G23" t="n">
-        <v>36.87736698480389</v>
+        <v>36.73390658119995</v>
       </c>
       <c r="H23" t="n">
-        <v>78.80136285198196</v>
+        <v>79.13641873963138</v>
       </c>
       <c r="I23" t="n">
-        <v>-3.907166030934215</v>
+        <v>-3.850257821601849</v>
       </c>
       <c r="J23" t="n">
-        <v>7.249452761779999</v>
+        <v>7.269454667238326</v>
       </c>
       <c r="K23" t="n">
-        <v>2.175549537257282</v>
+        <v>1.611573939107751</v>
       </c>
       <c r="L23" t="n">
-        <v>121.1965661048889</v>
+        <v>120.9010961055756</v>
       </c>
     </row>
     <row r="24">
@@ -1336,37 +1336,37 @@
         <v>1982</v>
       </c>
       <c r="B24" t="n">
-        <v>36.91705080165021</v>
+        <v>36.81556954781459</v>
       </c>
       <c r="C24" t="n">
-        <v>78.67681847309071</v>
+        <v>78.79105255448395</v>
       </c>
       <c r="D24" t="n">
-        <v>-2.978107617795396</v>
+        <v>-1.69492133398668</v>
       </c>
       <c r="E24" t="n">
-        <v>1.985887985045153</v>
+        <v>-0.3255274183204193</v>
       </c>
       <c r="F24" t="n">
-        <v>114.6016496419907</v>
+        <v>113.5861733499914</v>
       </c>
       <c r="G24" t="n">
-        <v>37.35544659484694</v>
+        <v>37.24068737967646</v>
       </c>
       <c r="H24" t="n">
-        <v>79.61111808510533</v>
+        <v>79.94988909132729</v>
       </c>
       <c r="I24" t="n">
-        <v>-3.013473114848327</v>
+        <v>-2.964446779387793</v>
       </c>
       <c r="J24" t="n">
-        <v>7.181539820489898</v>
+        <v>7.202132006021295</v>
       </c>
       <c r="K24" t="n">
-        <v>3.835105905742215</v>
+        <v>3.291766941202474</v>
       </c>
       <c r="L24" t="n">
-        <v>124.9697372913361</v>
+        <v>124.7200286388397</v>
       </c>
     </row>
     <row r="25">
@@ -1374,37 +1374,37 @@
         <v>1983</v>
       </c>
       <c r="B25" t="n">
-        <v>37.16009142004199</v>
+        <v>37.10732825539348</v>
       </c>
       <c r="C25" t="n">
-        <v>79.02122450413128</v>
+        <v>79.22198887195808</v>
       </c>
       <c r="D25" t="n">
-        <v>-1.938424993117306</v>
+        <v>-0.7705779294815972</v>
       </c>
       <c r="E25" t="n">
-        <v>2.179433607174936</v>
+        <v>0.1635470404651187</v>
       </c>
       <c r="F25" t="n">
-        <v>116.4223245382309</v>
+        <v>115.7222862383351</v>
       </c>
       <c r="G25" t="n">
-        <v>37.77190772156911</v>
+        <v>37.68391468989272</v>
       </c>
       <c r="H25" t="n">
-        <v>80.32225664562347</v>
+        <v>80.66407967069732</v>
       </c>
       <c r="I25" t="n">
-        <v>-1.970339877197411</v>
+        <v>-1.927714390690891</v>
       </c>
       <c r="J25" t="n">
-        <v>8.578777290053026</v>
+        <v>8.604202597485406</v>
       </c>
       <c r="K25" t="n">
-        <v>3.845256696590589</v>
+        <v>3.315839211866537</v>
       </c>
       <c r="L25" t="n">
-        <v>128.5478584766388</v>
+        <v>128.3403217792511</v>
       </c>
     </row>
     <row r="26">
@@ -1412,37 +1412,37 @@
         <v>1984</v>
       </c>
       <c r="B26" t="n">
-        <v>37.35105008731929</v>
+        <v>37.3360781742457</v>
       </c>
       <c r="C26" t="n">
-        <v>79.29153749712972</v>
+        <v>79.5903083946794</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.7638227215426732</v>
+        <v>0.1906955012040819</v>
       </c>
       <c r="E26" t="n">
-        <v>2.195477311719046</v>
+        <v>0.6204737336019122</v>
       </c>
       <c r="F26" t="n">
-        <v>118.0742421746254</v>
+        <v>117.7375558037311</v>
       </c>
       <c r="G26" t="n">
-        <v>38.13347186568112</v>
+        <v>38.06958905356613</v>
       </c>
       <c r="H26" t="n">
-        <v>80.95251960158225</v>
+        <v>81.29679705576403</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.7798231159290544</v>
+        <v>-0.7418353163179738</v>
       </c>
       <c r="J26" t="n">
-        <v>9.922511535262368</v>
+        <v>9.952739366215955</v>
       </c>
       <c r="K26" t="n">
-        <v>3.71071864054869</v>
+        <v>3.1921972217533</v>
       </c>
       <c r="L26" t="n">
-        <v>131.9393985271454</v>
+        <v>131.7694873809814</v>
       </c>
     </row>
     <row r="27">
@@ -1450,37 +1450,37 @@
         <v>1985</v>
       </c>
       <c r="B27" t="n">
-        <v>37.49734168542405</v>
+        <v>37.50787686531108</v>
       </c>
       <c r="C27" t="n">
-        <v>79.50632501231924</v>
+        <v>79.91404314824423</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5407462376597554</v>
+        <v>1.184659612318105</v>
       </c>
       <c r="E27" t="n">
-        <v>2.028716301295105</v>
+        <v>1.039164357924314</v>
       </c>
       <c r="F27" t="n">
-        <v>119.5731292366982</v>
+        <v>119.6457439837977</v>
       </c>
       <c r="G27" t="n">
-        <v>38.44684920792147</v>
+        <v>38.40370478830057</v>
       </c>
       <c r="H27" t="n">
-        <v>81.51958382726791</v>
+        <v>81.86580187639369</v>
       </c>
       <c r="I27" t="n">
-        <v>0.5544390115296348</v>
+        <v>0.5897937343501688</v>
       </c>
       <c r="J27" t="n">
-        <v>12.00788132390952</v>
+        <v>12.04526892586944</v>
       </c>
       <c r="K27" t="n">
-        <v>2.62630572856885</v>
+        <v>2.112729135092854</v>
       </c>
       <c r="L27" t="n">
-        <v>135.1550590991974</v>
+        <v>135.0172984600067</v>
       </c>
     </row>
     <row r="28">
@@ -1488,37 +1488,37 @@
         <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>37.60607115473156</v>
+        <v>37.62860368579909</v>
       </c>
       <c r="C28" t="n">
-        <v>79.68342569476683</v>
+        <v>80.21040140390315</v>
       </c>
       <c r="D28" t="n">
-        <v>1.969100892571537</v>
+        <v>2.207660758845453</v>
       </c>
       <c r="E28" t="n">
-        <v>1.676784504901214</v>
+        <v>1.413983643671401</v>
       </c>
       <c r="F28" t="n">
-        <v>120.9353822469711</v>
+        <v>121.4606494922191</v>
       </c>
       <c r="G28" t="n">
-        <v>38.71868751199463</v>
+        <v>38.69219838999912</v>
       </c>
       <c r="H28" t="n">
-        <v>82.04094617240385</v>
+        <v>82.38868712503788</v>
       </c>
       <c r="I28" t="n">
-        <v>2.027358875788185</v>
+        <v>2.062276522761474</v>
       </c>
       <c r="J28" t="n">
-        <v>10.46871370151256</v>
+        <v>10.50183324351871</v>
       </c>
       <c r="K28" t="n">
-        <v>4.952076245243514</v>
+        <v>4.450793197534148</v>
       </c>
       <c r="L28" t="n">
-        <v>138.2077825069427</v>
+        <v>138.0957884788513</v>
       </c>
     </row>
     <row r="29">
@@ -1526,37 +1526,37 @@
         <v>1987</v>
       </c>
       <c r="B29" t="n">
-        <v>37.68400161963632</v>
+        <v>37.70393731341807</v>
       </c>
       <c r="C29" t="n">
-        <v>79.83988401319681</v>
+        <v>80.49570703823933</v>
       </c>
       <c r="D29" t="n">
-        <v>3.513981010928326</v>
+        <v>3.256647299911327</v>
       </c>
       <c r="E29" t="n">
-        <v>1.140202172900374</v>
+        <v>1.739816155069164</v>
       </c>
       <c r="F29" t="n">
-        <v>122.1780688166618</v>
+        <v>123.1961078066379</v>
       </c>
       <c r="G29" t="n">
-        <v>38.95552252038153</v>
+        <v>38.94090228494213</v>
       </c>
       <c r="H29" t="n">
-        <v>82.53381451082616</v>
+        <v>82.88276437652351</v>
       </c>
       <c r="I29" t="n">
-        <v>3.632548575629016</v>
+        <v>3.669367562457103</v>
       </c>
       <c r="J29" t="n">
-        <v>15.36893157473885</v>
+        <v>15.41803527155145</v>
       </c>
       <c r="K29" t="n">
-        <v>0.6219283418772008</v>
+        <v>0.1081770827423565</v>
       </c>
       <c r="L29" t="n">
-        <v>141.1127455234528</v>
+        <v>141.0192465782166</v>
       </c>
     </row>
     <row r="30">
@@ -1564,37 +1564,37 @@
         <v>1988</v>
       </c>
       <c r="B30" t="n">
-        <v>37.73752634107728</v>
+        <v>37.73933503193791</v>
       </c>
       <c r="C30" t="n">
-        <v>79.9918820205132</v>
+        <v>80.78534308575421</v>
       </c>
       <c r="D30" t="n">
-        <v>5.167215023845503</v>
+        <v>4.329179866063367</v>
       </c>
       <c r="E30" t="n">
-        <v>0.422302829735834</v>
+        <v>2.012133203526417</v>
       </c>
       <c r="F30" t="n">
-        <v>123.3189262151718</v>
+        <v>124.8659911872819</v>
       </c>
       <c r="G30" t="n">
-        <v>39.16373303045109</v>
+        <v>39.15550055166423</v>
       </c>
       <c r="H30" t="n">
-        <v>83.01499901557376</v>
+        <v>83.36495211274979</v>
       </c>
       <c r="I30" t="n">
-        <v>5.362498534636183</v>
+        <v>5.403644246849417</v>
       </c>
       <c r="J30" t="n">
-        <v>16.42501243902971</v>
+        <v>16.47767079345447</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.0788795858528637</v>
+        <v>-0.5975444056914121</v>
       </c>
       <c r="L30" t="n">
-        <v>143.8873634338379</v>
+        <v>143.8042232990265</v>
       </c>
     </row>
     <row r="31">
@@ -1602,37 +1602,37 @@
         <v>1989</v>
       </c>
       <c r="B31" t="n">
-        <v>37.7726448815371</v>
+        <v>37.74001513689075</v>
       </c>
       <c r="C31" t="n">
-        <v>80.15468408327416</v>
+        <v>81.09369381479503</v>
       </c>
       <c r="D31" t="n">
-        <v>6.919884265511524</v>
+        <v>5.423435804183097</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.4708507277478731</v>
+        <v>2.22706388291094</v>
       </c>
       <c r="F31" t="n">
-        <v>124.3763625025749</v>
+        <v>126.4842086387798</v>
       </c>
       <c r="G31" t="n">
-        <v>39.34949928846825</v>
+        <v>39.34148845561896</v>
       </c>
       <c r="H31" t="n">
-        <v>83.50081637634703</v>
+        <v>83.85167209044516</v>
       </c>
       <c r="I31" t="n">
-        <v>7.208761309566728</v>
+        <v>7.256695666441435</v>
       </c>
       <c r="J31" t="n">
-        <v>17.51095138635368</v>
+        <v>17.56690038451844</v>
       </c>
       <c r="K31" t="n">
-        <v>-1.018741424929431</v>
+        <v>-1.547230067711865</v>
       </c>
       <c r="L31" t="n">
-        <v>146.5512869358063</v>
+        <v>146.4695265293121</v>
       </c>
     </row>
     <row r="32">
@@ -1640,37 +1640,37 @@
         <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>37.79494230799132</v>
+        <v>37.7109392205759</v>
       </c>
       <c r="C32" t="n">
-        <v>80.34258184109524</v>
+        <v>81.4340923549899</v>
       </c>
       <c r="D32" t="n">
-        <v>8.762497290798427</v>
+        <v>6.538212494779707</v>
       </c>
       <c r="E32" t="n">
-        <v>-1.530565923546632</v>
+        <v>2.381461877068531</v>
       </c>
       <c r="F32" t="n">
-        <v>125.3694555163383</v>
+        <v>128.064705947414</v>
       </c>
       <c r="G32" t="n">
-        <v>39.5187657879728</v>
+        <v>39.50413506158376</v>
       </c>
       <c r="H32" t="n">
-        <v>84.00699883878252</v>
+        <v>84.3587554440672</v>
       </c>
       <c r="I32" t="n">
-        <v>9.162153902258808</v>
+        <v>9.219322653611417</v>
       </c>
       <c r="J32" t="n">
-        <v>16.78429505996867</v>
+        <v>16.83734679720862</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.3458073962032664</v>
+        <v>-0.8833355912366194</v>
       </c>
       <c r="L32" t="n">
-        <v>149.1264061927795</v>
+        <v>149.0362243652344</v>
       </c>
     </row>
     <row r="33">
@@ -1678,37 +1678,37 @@
         <v>1991</v>
       </c>
       <c r="B33" t="n">
-        <v>37.80957366066743</v>
+        <v>37.6567982083382</v>
       </c>
       <c r="C33" t="n">
-        <v>80.56885654967969</v>
+        <v>81.81877385513934</v>
       </c>
       <c r="D33" t="n">
-        <v>10.68515237744568</v>
+        <v>7.67292546961747</v>
       </c>
       <c r="E33" t="n">
-        <v>-2.745628524377274</v>
+        <v>2.472968124742678</v>
       </c>
       <c r="F33" t="n">
-        <v>126.3179540634155</v>
+        <v>129.6214656578377</v>
       </c>
       <c r="G33" t="n">
-        <v>39.6772090207791</v>
+        <v>39.64844988905512</v>
       </c>
       <c r="H33" t="n">
-        <v>84.54862227691086</v>
+        <v>84.90136814897077</v>
       </c>
       <c r="I33" t="n">
-        <v>11.2129543724483</v>
+        <v>11.28174205149252</v>
       </c>
       <c r="J33" t="n">
-        <v>14.09183225795755</v>
+        <v>14.13554071793475</v>
       </c>
       <c r="K33" t="n">
-        <v>2.106227660588257</v>
+        <v>1.560546687816604</v>
       </c>
       <c r="L33" t="n">
-        <v>151.6368455886841</v>
+        <v>151.5276474952698</v>
       </c>
     </row>
     <row r="34">
@@ -1716,37 +1716,37 @@
         <v>1992</v>
       </c>
       <c r="B34" t="n">
-        <v>37.82124954951732</v>
+        <v>37.58199846470598</v>
       </c>
       <c r="C34" t="n">
-        <v>80.84574799061514</v>
+        <v>82.25883171871135</v>
       </c>
       <c r="D34" t="n">
-        <v>12.67769699728692</v>
+        <v>8.827604153270602</v>
       </c>
       <c r="E34" t="n">
-        <v>-4.102417511242919</v>
+        <v>2.500072745699875</v>
       </c>
       <c r="F34" t="n">
-        <v>127.2422770261765</v>
+        <v>131.1685070823878</v>
       </c>
       <c r="G34" t="n">
-        <v>39.83020818287815</v>
+        <v>39.77915169321965</v>
       </c>
       <c r="H34" t="n">
-        <v>85.14004723590099</v>
+        <v>85.49394532948727</v>
       </c>
       <c r="I34" t="n">
-        <v>13.35110068270686</v>
+        <v>13.43378474406475</v>
       </c>
       <c r="J34" t="n">
-        <v>12.87527234643378</v>
+        <v>12.91410918414742</v>
       </c>
       <c r="K34" t="n">
-        <v>2.912337902635638</v>
+        <v>2.348388235711145</v>
       </c>
       <c r="L34" t="n">
-        <v>154.1089663505554</v>
+        <v>153.9693791866302</v>
       </c>
     </row>
     <row r="35">
@@ -1754,37 +1754,37 @@
         <v>1993</v>
       </c>
       <c r="B35" t="n">
-        <v>37.83422522899287</v>
+        <v>37.49064966332462</v>
       </c>
       <c r="C35" t="n">
-        <v>81.18443505006242</v>
+        <v>82.76418939185295</v>
       </c>
       <c r="D35" t="n">
-        <v>14.7298692473819</v>
+        <v>10.00288915253464</v>
       </c>
       <c r="E35" t="n">
-        <v>-5.58501598521557</v>
+        <v>2.462158091510503</v>
       </c>
       <c r="F35" t="n">
-        <v>128.1635135412216</v>
+        <v>132.7198862992227</v>
       </c>
       <c r="G35" t="n">
-        <v>39.982820416528</v>
+        <v>39.90064048309182</v>
       </c>
       <c r="H35" t="n">
-        <v>85.79487666464719</v>
+        <v>86.15014528546233</v>
       </c>
       <c r="I35" t="n">
-        <v>15.56637444833137</v>
+        <v>15.66509126650601</v>
       </c>
       <c r="J35" t="n">
-        <v>10.27980921141914</v>
+        <v>10.30965793585159</v>
       </c>
       <c r="K35" t="n">
-        <v>4.94749033756551</v>
+        <v>4.363731043187371</v>
       </c>
       <c r="L35" t="n">
-        <v>156.5713710784912</v>
+        <v>156.3892660140991</v>
       </c>
     </row>
     <row r="36">
@@ -1792,37 +1792,37 @@
         <v>1994</v>
       </c>
       <c r="B36" t="n">
-        <v>37.85229195695204</v>
+        <v>37.38655359680045</v>
       </c>
       <c r="C36" t="n">
-        <v>81.59503189540952</v>
+        <v>83.34356881255802</v>
       </c>
       <c r="D36" t="n">
-        <v>16.83142811316937</v>
+        <v>11.20002453769498</v>
       </c>
       <c r="E36" t="n">
-        <v>-7.175329204567483</v>
+        <v>2.359549215513098</v>
       </c>
       <c r="F36" t="n">
-        <v>129.1034227609634</v>
+        <v>134.2896961625665</v>
       </c>
       <c r="G36" t="n">
-        <v>40.13975780844436</v>
+        <v>40.01697232493216</v>
       </c>
       <c r="H36" t="n">
-        <v>86.52593143841318</v>
+        <v>86.88282762185351</v>
       </c>
       <c r="I36" t="n">
-        <v>17.84857436905551</v>
+        <v>17.9652891596756</v>
       </c>
       <c r="J36" t="n">
-        <v>14.02801239268973</v>
+        <v>14.06676140697225</v>
       </c>
       <c r="K36" t="n">
-        <v>0.5126167697938282</v>
+        <v>-0.1144352760067537</v>
       </c>
       <c r="L36" t="n">
-        <v>159.0548927783966</v>
+        <v>158.8174152374268</v>
       </c>
     </row>
     <row r="37">
@@ -1830,37 +1830,37 @@
         <v>1995</v>
       </c>
       <c r="B37" t="n">
-        <v>37.87877023648726</v>
+        <v>37.27319341777029</v>
       </c>
       <c r="C37" t="n">
-        <v>82.08659044442707</v>
+        <v>84.00448186645923</v>
       </c>
       <c r="D37" t="n">
-        <v>18.97226062367997</v>
+        <v>12.42085456646452</v>
       </c>
       <c r="E37" t="n">
-        <v>-8.853186080061221</v>
+        <v>2.193536431526141</v>
       </c>
       <c r="F37" t="n">
-        <v>130.0844352245331</v>
+        <v>135.8920662822202</v>
       </c>
       <c r="G37" t="n">
-        <v>40.3053690877054</v>
+        <v>40.13183303160207</v>
       </c>
       <c r="H37" t="n">
-        <v>87.34524126200265</v>
+        <v>87.70404132795244</v>
       </c>
       <c r="I37" t="n">
-        <v>20.1876661277923</v>
+        <v>20.32415261135793</v>
       </c>
       <c r="J37" t="n">
-        <v>15.6982154660028</v>
+        <v>15.73889386959164</v>
       </c>
       <c r="K37" t="n">
-        <v>-1.94388468375276</v>
+        <v>-2.612731999637994</v>
       </c>
       <c r="L37" t="n">
-        <v>161.5926072597504</v>
+        <v>161.2861888408661</v>
       </c>
     </row>
     <row r="38">
@@ -1868,37 +1868,37 @@
         <v>1996</v>
       </c>
       <c r="B38" t="n">
-        <v>37.91650273866446</v>
+        <v>37.15372379833347</v>
       </c>
       <c r="C38" t="n">
-        <v>82.66711946910573</v>
+        <v>84.75321663266378</v>
       </c>
       <c r="D38" t="n">
-        <v>21.14246627505702</v>
+        <v>13.66781636199956</v>
       </c>
       <c r="E38" t="n">
-        <v>-10.59643735358145</v>
+        <v>1.966406244534269</v>
       </c>
       <c r="F38" t="n">
-        <v>131.1296511292458</v>
+        <v>137.5411630375311</v>
       </c>
       <c r="G38" t="n">
-        <v>40.48361974609159</v>
+        <v>40.24851296235521</v>
       </c>
       <c r="H38" t="n">
-        <v>88.26405360110704</v>
+        <v>88.62503216074417</v>
       </c>
       <c r="I38" t="n">
-        <v>22.57390590776101</v>
+        <v>22.73173726158019</v>
       </c>
       <c r="J38" t="n">
-        <v>18.78339587273473</v>
+        <v>18.82828535513324</v>
       </c>
       <c r="K38" t="n">
-        <v>-5.885149859902615</v>
+        <v>-6.603358246175709</v>
       </c>
       <c r="L38" t="n">
-        <v>164.2198252677917</v>
+        <v>163.8302094936371</v>
       </c>
     </row>
     <row r="39">
@@ -1906,37 +1906,37 @@
         <v>1997</v>
       </c>
       <c r="B39" t="n">
-        <v>37.96784711073213</v>
+        <v>37.03096112726396</v>
       </c>
       <c r="C39" t="n">
-        <v>83.34361304334243</v>
+        <v>85.59484135012447</v>
       </c>
       <c r="D39" t="n">
-        <v>23.33242119172723</v>
+        <v>14.94393565484371</v>
       </c>
       <c r="E39" t="n">
-        <v>-12.38104089599177</v>
+        <v>1.681451456336966</v>
       </c>
       <c r="F39" t="n">
-        <v>132.26284044981</v>
+        <v>139.2511895885691</v>
       </c>
       <c r="G39" t="n">
-        <v>40.6780725043953</v>
+        <v>40.3698811305078</v>
       </c>
       <c r="H39" t="n">
-        <v>89.29285677609691</v>
+        <v>89.65627262807669</v>
       </c>
       <c r="I39" t="n">
-        <v>24.99793886580123</v>
+        <v>25.17848622796977</v>
       </c>
       <c r="J39" t="n">
-        <v>20.70319201533607</v>
+        <v>20.74785675431811</v>
       </c>
       <c r="K39" t="n">
-        <v>-8.697968631783301</v>
+        <v>-9.466135475689896</v>
       </c>
       <c r="L39" t="n">
-        <v>166.9740915298462</v>
+        <v>166.4863612651825</v>
       </c>
     </row>
     <row r="40">
@@ -1944,37 +1944,37 @@
         <v>1998</v>
       </c>
       <c r="B40" t="n">
-        <v>38.0346691115906</v>
+        <v>36.90737476267991</v>
       </c>
       <c r="C40" t="n">
-        <v>84.12208216735591</v>
+        <v>86.53321574292619</v>
       </c>
       <c r="D40" t="n">
-        <v>25.53280929394618</v>
+        <v>16.25282206806816</v>
       </c>
       <c r="E40" t="n">
-        <v>-14.18111560800697</v>
+        <v>1.342973266130748</v>
       </c>
       <c r="F40" t="n">
-        <v>133.5084449648857</v>
+        <v>141.036385839805</v>
       </c>
       <c r="G40" t="n">
-        <v>40.89186808860988</v>
+        <v>40.49835337523621</v>
       </c>
       <c r="H40" t="n">
-        <v>90.44140957909504</v>
+        <v>90.80749280139142</v>
       </c>
       <c r="I40" t="n">
-        <v>27.45085717760347</v>
+        <v>27.65530272773835</v>
       </c>
       <c r="J40" t="n">
-        <v>19.60235190202505</v>
+        <v>19.639469502874</v>
       </c>
       <c r="K40" t="n">
-        <v>-8.491296269962223</v>
+        <v>-9.306833073606558</v>
       </c>
       <c r="L40" t="n">
-        <v>169.8951904773712</v>
+        <v>169.2937853336334</v>
       </c>
     </row>
     <row r="41">
@@ -1982,37 +1982,37 @@
         <v>1999</v>
       </c>
       <c r="B41" t="n">
-        <v>38.11833072117684</v>
+        <v>36.78507623311542</v>
       </c>
       <c r="C41" t="n">
-        <v>85.00760024654458</v>
+        <v>87.57100275736822</v>
       </c>
       <c r="D41" t="n">
-        <v>27.73463143347759</v>
+        <v>17.59866654796113</v>
       </c>
       <c r="E41" t="n">
-        <v>-15.96898682632413</v>
+        <v>0.9562829240173585</v>
       </c>
       <c r="F41" t="n">
-        <v>134.8915755748749</v>
+        <v>142.9110284624621</v>
       </c>
       <c r="G41" t="n">
-        <v>41.12769950249029</v>
+        <v>40.63585861002883</v>
       </c>
       <c r="H41" t="n">
-        <v>91.71878653189268</v>
+        <v>92.08772849843872</v>
       </c>
       <c r="I41" t="n">
-        <v>29.92422715863282</v>
+        <v>30.1535877310979</v>
       </c>
       <c r="J41" t="n">
-        <v>21.10090871120205</v>
+        <v>21.13463250109542</v>
       </c>
       <c r="K41" t="n">
-        <v>-10.84647613509857</v>
+        <v>-11.71792544750291</v>
       </c>
       <c r="L41" t="n">
-        <v>173.0251457691193</v>
+        <v>172.293881893158</v>
       </c>
     </row>
     <row r="42">
@@ -2020,37 +2020,37 @@
         <v>2000</v>
       </c>
       <c r="B42" t="n">
-        <v>38.21967706432886</v>
+        <v>36.66580978236323</v>
       </c>
       <c r="C42" t="n">
-        <v>86.00434207432254</v>
+        <v>88.70969549280332</v>
       </c>
       <c r="D42" t="n">
-        <v>29.92918197483871</v>
+        <v>18.98623891466629</v>
       </c>
       <c r="E42" t="n">
-        <v>-17.71518708303356</v>
+        <v>0.5276867261039868</v>
       </c>
       <c r="F42" t="n">
-        <v>136.4380140304565</v>
+        <v>144.8894309159368</v>
       </c>
       <c r="G42" t="n">
-        <v>41.38778245479071</v>
+        <v>40.7837951465522</v>
       </c>
       <c r="H42" t="n">
-        <v>93.13341381582839</v>
+        <v>93.50537146557565</v>
       </c>
       <c r="I42" t="n">
-        <v>32.41007166385956</v>
+        <v>32.66523493278496</v>
       </c>
       <c r="J42" t="n">
-        <v>25.84477398284949</v>
+        <v>25.87764130903685</v>
       </c>
       <c r="K42" t="n">
-        <v>-16.36782663298061</v>
+        <v>-17.30173103105842</v>
       </c>
       <c r="L42" t="n">
-        <v>176.4082152843475</v>
+        <v>175.5303118228912</v>
       </c>
     </row>
     <row r="43">
@@ -2058,37 +2058,37 @@
         <v>2001</v>
       </c>
       <c r="B43" t="n">
-        <v>38.33901640953056</v>
+        <v>36.55094079099477</v>
       </c>
       <c r="C43" t="n">
-        <v>87.1156297457765</v>
+        <v>89.94963482152015</v>
       </c>
       <c r="D43" t="n">
-        <v>32.10799427219749</v>
+        <v>20.42088671512554</v>
       </c>
       <c r="E43" t="n">
-        <v>-19.38842832938291</v>
+        <v>0.06448107824851945</v>
       </c>
       <c r="F43" t="n">
-        <v>138.1742120981216</v>
+        <v>146.985943405889</v>
       </c>
       <c r="G43" t="n">
-        <v>41.67381667057163</v>
+        <v>40.94297977298181</v>
       </c>
       <c r="H43" t="n">
-        <v>94.69311221725575</v>
+        <v>95.06821659457839</v>
       </c>
       <c r="I43" t="n">
-        <v>34.90080842623542</v>
+        <v>35.18258501017997</v>
       </c>
       <c r="J43" t="n">
-        <v>21.83949876143102</v>
+        <v>21.85947508127694</v>
       </c>
       <c r="K43" t="n">
-        <v>-13.01634495267582</v>
+        <v>-14.00426215626746</v>
       </c>
       <c r="L43" t="n">
-        <v>180.090891122818</v>
+        <v>179.0489943027496</v>
       </c>
     </row>
     <row r="44">
@@ -2096,37 +2096,37 @@
         <v>2002</v>
       </c>
       <c r="B44" t="n">
-        <v>38.47609536380511</v>
+        <v>36.44144467127125</v>
       </c>
       <c r="C44" t="n">
-        <v>88.34397025734856</v>
+        <v>91.29004180024975</v>
       </c>
       <c r="D44" t="n">
-        <v>34.26275839782028</v>
+        <v>21.90853643144506</v>
       </c>
       <c r="E44" t="n">
-        <v>-20.95553144552195</v>
+        <v>-0.4250699861278449</v>
       </c>
       <c r="F44" t="n">
-        <v>140.127292573452</v>
+        <v>149.2149529168382</v>
       </c>
       <c r="G44" t="n">
-        <v>41.98693934843718</v>
+        <v>41.11358324143114</v>
       </c>
       <c r="H44" t="n">
-        <v>96.40512858497604</v>
+        <v>96.78350053694578</v>
       </c>
       <c r="I44" t="n">
-        <v>37.38914630388231</v>
+        <v>37.6983311260509</v>
       </c>
       <c r="J44" t="n">
-        <v>26.89727498887758</v>
+        <v>26.91148049180069</v>
       </c>
       <c r="K44" t="n">
-        <v>-18.55658175356264</v>
+        <v>-19.60878953647205</v>
       </c>
       <c r="L44" t="n">
-        <v>184.1219074726105</v>
+        <v>182.8981058597565</v>
       </c>
     </row>
     <row r="45">
@@ -2134,37 +2134,37 @@
         <v>2003</v>
       </c>
       <c r="B45" t="n">
-        <v>38.63006481206479</v>
+        <v>36.3378917065203</v>
       </c>
       <c r="C45" t="n">
-        <v>89.69108782457755</v>
+        <v>92.72903695257261</v>
       </c>
       <c r="D45" t="n">
-        <v>36.38520005800807</v>
+        <v>23.45569364799827</v>
       </c>
       <c r="E45" t="n">
-        <v>-22.38130549969269</v>
+        <v>-0.9317391051716726</v>
       </c>
       <c r="F45" t="n">
-        <v>142.3250471949577</v>
+        <v>151.5908832019195</v>
       </c>
       <c r="G45" t="n">
-        <v>42.32766351947454</v>
+        <v>41.29505238541369</v>
       </c>
       <c r="H45" t="n">
-        <v>98.276153679884</v>
+        <v>98.65793653947118</v>
       </c>
       <c r="I45" t="n">
-        <v>39.86792444270332</v>
+        <v>40.2053779697474</v>
       </c>
       <c r="J45" t="n">
-        <v>27.71049989287422</v>
+        <v>27.71364578681311</v>
       </c>
       <c r="K45" t="n">
-        <v>-19.63000807737079</v>
+        <v>-20.74392611452035</v>
       </c>
       <c r="L45" t="n">
-        <v>188.5522334575653</v>
+        <v>187.128086566925</v>
       </c>
     </row>
     <row r="46">
@@ -2172,37 +2172,37 @@
         <v>2004</v>
       </c>
       <c r="B46" t="n">
-        <v>38.79943670279255</v>
+        <v>36.24043279601353</v>
       </c>
       <c r="C46" t="n">
-        <v>91.15793866266611</v>
+        <v>94.26366266355261</v>
       </c>
       <c r="D46" t="n">
-        <v>38.46693234859023</v>
+        <v>25.06944689284385</v>
       </c>
       <c r="E46" t="n">
-        <v>-23.62836767250685</v>
+        <v>-1.4453475797716</v>
       </c>
       <c r="F46" t="n">
-        <v>144.7959400415421</v>
+        <v>154.1281947726384</v>
       </c>
       <c r="G46" t="n">
-        <v>42.69580189055277</v>
+        <v>41.48601485752346</v>
       </c>
       <c r="H46" t="n">
-        <v>100.3123143180124</v>
+        <v>100.6977156904692</v>
       </c>
       <c r="I46" t="n">
-        <v>42.32990637141121</v>
+        <v>42.69664594634199</v>
       </c>
       <c r="J46" t="n">
-        <v>32.16648967399126</v>
+        <v>32.15596216115541</v>
       </c>
       <c r="K46" t="n">
-        <v>-24.06943673249849</v>
+        <v>-25.24470910264892</v>
       </c>
       <c r="L46" t="n">
-        <v>193.4350755214691</v>
+        <v>191.7916295528412</v>
       </c>
     </row>
     <row r="47">
@@ -2210,37 +2210,37 @@
         <v>2005</v>
       </c>
       <c r="B47" t="n">
-        <v>38.98202954924204</v>
+        <v>36.14878101725054</v>
       </c>
       <c r="C47" t="n">
-        <v>92.74471671142726</v>
+        <v>95.88989445531355</v>
       </c>
       <c r="D47" t="n">
-        <v>40.49926597294353</v>
+        <v>26.75747018329687</v>
       </c>
       <c r="E47" t="n">
-        <v>-24.65690786015779</v>
+        <v>-1.95476075512714</v>
       </c>
       <c r="F47" t="n">
-        <v>147.569104373455</v>
+        <v>156.8413849007338</v>
       </c>
       <c r="G47" t="n">
-        <v>43.09037281599731</v>
+        <v>41.68416322592223</v>
       </c>
       <c r="H47" t="n">
-        <v>102.5191470536752</v>
+        <v>102.9084944909498</v>
       </c>
       <c r="I47" t="n">
-        <v>44.76751184398767</v>
+        <v>45.16482228630847</v>
       </c>
       <c r="J47" t="n">
-        <v>36.05358551818011</v>
+        <v>36.02503201034158</v>
       </c>
       <c r="K47" t="n">
-        <v>-27.60474314164556</v>
+        <v>-28.83881861409275</v>
       </c>
       <c r="L47" t="n">
-        <v>198.8258740901947</v>
+        <v>196.9436933994293</v>
       </c>
     </row>
     <row r="48">
@@ -2248,37 +2248,37 @@
         <v>2006</v>
       </c>
       <c r="B48" t="n">
-        <v>39.17490141115401</v>
+        <v>36.06219101856019</v>
       </c>
       <c r="C48" t="n">
-        <v>94.45083077118149</v>
+        <v>97.60264691990955</v>
       </c>
       <c r="D48" t="n">
-        <v>42.47298665511234</v>
+        <v>28.52802851002264</v>
       </c>
       <c r="E48" t="n">
-        <v>-25.42437578792162</v>
+        <v>-2.447878802374568</v>
       </c>
       <c r="F48" t="n">
-        <v>150.6743430495262</v>
+        <v>159.7449876461178</v>
       </c>
       <c r="G48" t="n">
-        <v>43.50948653895694</v>
+        <v>41.88611614791849</v>
       </c>
       <c r="H48" t="n">
-        <v>104.9015313887159</v>
+        <v>105.2953431826001</v>
       </c>
       <c r="I48" t="n">
-        <v>47.17249500502241</v>
+        <v>47.60205163956052</v>
       </c>
       <c r="J48" t="n">
-        <v>38.4707042273789</v>
+        <v>38.42154505654648</v>
       </c>
       <c r="K48" t="n">
-        <v>-29.2719064358157</v>
+        <v>-30.56356222932332</v>
       </c>
       <c r="L48" t="n">
-        <v>204.7823107242584</v>
+        <v>202.6414937973022</v>
       </c>
     </row>
     <row r="49">
@@ -2286,37 +2286,37 @@
         <v>2007</v>
       </c>
       <c r="B49" t="n">
-        <v>39.37426601302995</v>
+        <v>35.97943565494461</v>
       </c>
       <c r="C49" t="n">
-        <v>96.27486687640318</v>
+        <v>99.39576191009114</v>
       </c>
       <c r="D49" t="n">
-        <v>44.37808796706835</v>
+        <v>30.3899806303803</v>
       </c>
       <c r="E49" t="n">
-        <v>-25.88509024317446</v>
+        <v>-2.911604383244239</v>
       </c>
       <c r="F49" t="n">
-        <v>154.142130613327</v>
+        <v>162.8535738121718</v>
       </c>
       <c r="G49" t="n">
-        <v>43.95020409091534</v>
+        <v>42.08725253532693</v>
       </c>
       <c r="H49" t="n">
-        <v>107.4635917439929</v>
+        <v>107.8626608465575</v>
       </c>
       <c r="I49" t="n">
-        <v>49.53555255282224</v>
+        <v>49.99956430735466</v>
       </c>
       <c r="J49" t="n">
-        <v>41.22572997555011</v>
+        <v>41.15227536300872</v>
       </c>
       <c r="K49" t="n">
-        <v>-30.81077572808769</v>
+        <v>-32.15725236750969</v>
       </c>
       <c r="L49" t="n">
-        <v>211.3643026351929</v>
+        <v>208.9445006847382</v>
       </c>
     </row>
     <row r="50">
@@ -2324,37 +2324,37 @@
         <v>2008</v>
       </c>
       <c r="B50" t="n">
-        <v>39.57539477747482</v>
+        <v>35.8987781563301</v>
       </c>
       <c r="C50" t="n">
-        <v>98.21451603644549</v>
+        <v>101.2619860430899</v>
       </c>
       <c r="D50" t="n">
-        <v>46.2034656341736</v>
+        <v>32.35278547454703</v>
       </c>
       <c r="E50" t="n">
-        <v>-25.98976452582981</v>
+        <v>-3.331798696555161</v>
       </c>
       <c r="F50" t="n">
-        <v>158.0036119222641</v>
+        <v>166.1817509774119</v>
       </c>
       <c r="G50" t="n">
-        <v>44.40837326860457</v>
+        <v>42.28151589498496</v>
       </c>
       <c r="H50" t="n">
-        <v>110.2085503648415</v>
+        <v>110.614042301052</v>
       </c>
       <c r="I50" t="n">
-        <v>51.84586937723645</v>
+        <v>52.34723836034702</v>
       </c>
       <c r="J50" t="n">
-        <v>40.01047002151076</v>
+        <v>39.91843334553688</v>
       </c>
       <c r="K50" t="n">
-        <v>-27.83925915455355</v>
+        <v>-29.24677854121838</v>
       </c>
       <c r="L50" t="n">
-        <v>218.6340038776398</v>
+        <v>215.9144513607025</v>
       </c>
     </row>
     <row r="51">
@@ -2362,37 +2362,37 @@
         <v>2009</v>
       </c>
       <c r="B51" t="n">
-        <v>39.77249705336529</v>
+        <v>35.81794027541709</v>
       </c>
       <c r="C51" t="n">
-        <v>100.2664738217917</v>
+        <v>103.1929255059554</v>
       </c>
       <c r="D51" t="n">
-        <v>47.93656198526433</v>
+        <v>34.42650591571625</v>
       </c>
       <c r="E51" t="n">
-        <v>-25.68493184533038</v>
+        <v>-3.693208187630468</v>
       </c>
       <c r="F51" t="n">
-        <v>162.2906010150909</v>
+        <v>169.7441635094583</v>
       </c>
       <c r="G51" t="n">
-        <v>44.87843096325535</v>
+        <v>42.46118571723035</v>
       </c>
       <c r="H51" t="n">
-        <v>113.1385343319696</v>
+        <v>113.5521019068811</v>
       </c>
       <c r="I51" t="n">
-        <v>54.09058638649054</v>
+        <v>54.63308682361534</v>
       </c>
       <c r="J51" t="n">
-        <v>42.19424231771825</v>
+        <v>42.0748432989509</v>
       </c>
       <c r="K51" t="n">
-        <v>-27.64598960375806</v>
+        <v>-29.10588156694445</v>
       </c>
       <c r="L51" t="n">
-        <v>226.6558043956757</v>
+        <v>223.6153361797333</v>
       </c>
     </row>
     <row r="52">
@@ -2400,37 +2400,37 @@
         <v>2010</v>
       </c>
       <c r="B52" t="n">
-        <v>39.95858080951947</v>
+        <v>35.73406638845568</v>
       </c>
       <c r="C52" t="n">
-        <v>102.4263047221612</v>
+        <v>105.178983880803</v>
       </c>
       <c r="D52" t="n">
-        <v>49.56295759699294</v>
+        <v>36.62181282826435</v>
       </c>
       <c r="E52" t="n">
-        <v>-24.91225969218455</v>
+        <v>-3.979370606061686</v>
       </c>
       <c r="F52" t="n">
-        <v>167.0355834364891</v>
+        <v>173.5554924914613</v>
       </c>
       <c r="G52" t="n">
-        <v>45.35317344814079</v>
+        <v>42.61660667787145</v>
       </c>
       <c r="H52" t="n">
-        <v>116.2543280968983</v>
+        <v>116.6782419025563</v>
       </c>
       <c r="I52" t="n">
-        <v>56.2541853829743</v>
+        <v>56.84266451222359</v>
       </c>
       <c r="J52" t="n">
-        <v>46.38553576714144</v>
+        <v>46.22939701014258</v>
       </c>
       <c r="K52" t="n">
-        <v>-28.75089028815712</v>
+        <v>-30.25350272936562</v>
       </c>
       <c r="L52" t="n">
-        <v>235.4963324069977</v>
+        <v>232.1134073734283</v>
       </c>
     </row>
     <row r="53">
@@ -2438,37 +2438,37 @@
         <v>2011</v>
       </c>
       <c r="B53" t="n">
-        <v>40.12528810210435</v>
+        <v>35.6436803748902</v>
       </c>
       <c r="C53" t="n">
-        <v>104.6882651854456</v>
+        <v>107.209270429077</v>
       </c>
       <c r="D53" t="n">
-        <v>51.06590464695779</v>
+        <v>38.94998863023196</v>
       </c>
       <c r="E53" t="n">
-        <v>-23.60774330676497</v>
+        <v>-4.172483597545487</v>
       </c>
       <c r="F53" t="n">
-        <v>172.2717146277428</v>
+        <v>177.6304558366537</v>
       </c>
       <c r="G53" t="n">
-        <v>45.82348715397746</v>
+        <v>42.73587932873266</v>
       </c>
       <c r="H53" t="n">
-        <v>119.555063696748</v>
+        <v>119.9923578540402</v>
       </c>
       <c r="I53" t="n">
-        <v>58.31778253259164</v>
+        <v>58.95838404071487</v>
       </c>
       <c r="J53" t="n">
-        <v>46.84077368544262</v>
+        <v>46.65784600900004</v>
       </c>
       <c r="K53" t="n">
-        <v>-25.31265528844055</v>
+        <v>-26.86729151990228</v>
       </c>
       <c r="L53" t="n">
-        <v>245.2244517803192</v>
+        <v>241.4771757125854</v>
       </c>
     </row>
     <row r="54">
@@ -2476,37 +2476,37 @@
         <v>2012</v>
       </c>
       <c r="B54" t="n">
-        <v>40.26270353211081</v>
+        <v>35.54263844006679</v>
       </c>
       <c r="C54" t="n">
-        <v>107.0450937702421</v>
+        <v>109.2714852218703</v>
       </c>
       <c r="D54" t="n">
-        <v>52.42578790223146</v>
+        <v>41.42292849158768</v>
       </c>
       <c r="E54" t="n">
-        <v>-21.70076515863634</v>
+        <v>-4.253243990902583</v>
       </c>
       <c r="F54" t="n">
-        <v>178.032820045948</v>
+        <v>181.9838081626222</v>
       </c>
       <c r="G54" t="n">
-        <v>46.27803686968927</v>
+        <v>42.80449714600039</v>
       </c>
       <c r="H54" t="n">
-        <v>123.0378579090637</v>
+        <v>123.4924932904291</v>
       </c>
       <c r="I54" t="n">
-        <v>60.25831185248238</v>
+        <v>60.95872949849564</v>
       </c>
       <c r="J54" t="n">
-        <v>49.79859378482909</v>
+        <v>49.5773283956859</v>
       </c>
       <c r="K54" t="n">
-        <v>-23.46153575809026</v>
+        <v>-25.05563734657169</v>
       </c>
       <c r="L54" t="n">
-        <v>255.9112646579742</v>
+        <v>251.7774109840393</v>
       </c>
     </row>
     <row r="55">
@@ -2514,37 +2514,37 @@
         <v>2013</v>
       </c>
       <c r="B55" t="n">
-        <v>40.35913307986821</v>
+        <v>35.42607323491492</v>
       </c>
       <c r="C55" t="n">
-        <v>109.4877444744851</v>
+        <v>111.3517695381611</v>
       </c>
       <c r="D55" t="n">
-        <v>53.61950687490088</v>
+        <v>44.05314058284465</v>
       </c>
       <c r="E55" t="n">
-        <v>-19.112988132753</v>
+        <v>-4.200642454717183</v>
       </c>
       <c r="F55" t="n">
-        <v>184.3533962965012</v>
+        <v>186.6303409012035</v>
       </c>
       <c r="G55" t="n">
-        <v>46.70290612370096</v>
+        <v>42.80492829322611</v>
       </c>
       <c r="H55" t="n">
-        <v>126.6973659163725</v>
+        <v>127.1744101699368</v>
       </c>
       <c r="I55" t="n">
-        <v>62.04758637956878</v>
+        <v>62.81735031030982</v>
       </c>
       <c r="J55" t="n">
-        <v>52.32996401969842</v>
+        <v>52.06958600210208</v>
       </c>
       <c r="K55" t="n">
-        <v>-20.14771289077191</v>
+        <v>-21.77913302333176</v>
       </c>
       <c r="L55" t="n">
-        <v>267.6301095485687</v>
+        <v>263.087141752243</v>
       </c>
     </row>
     <row r="56">
@@ -2552,37 +2552,37 @@
         <v>2014</v>
       </c>
       <c r="B56" t="n">
-        <v>40.40084558326048</v>
+        <v>35.28833144300549</v>
       </c>
       <c r="C56" t="n">
-        <v>112.0050765163589</v>
+        <v>113.4345207760257</v>
       </c>
       <c r="D56" t="n">
-        <v>54.61975797799101</v>
+        <v>46.85374351943896</v>
       </c>
       <c r="E56" t="n">
-        <v>-15.75707067304649</v>
+        <v>-3.991713513560185</v>
       </c>
       <c r="F56" t="n">
-        <v>191.2686094045639</v>
+        <v>191.58488222491</v>
       </c>
       <c r="G56" t="n">
-        <v>47.08118010052245</v>
+        <v>42.71613498480644</v>
       </c>
       <c r="H56" t="n">
-        <v>130.5252675657962</v>
+        <v>131.0310969103514</v>
       </c>
       <c r="I56" t="n">
-        <v>63.65120891118755</v>
+        <v>64.5020104789115</v>
       </c>
       <c r="J56" t="n">
-        <v>54.06279900294504</v>
+        <v>53.76551820391873</v>
       </c>
       <c r="K56" t="n">
-        <v>-14.86389282295916</v>
+        <v>-16.53310450346419</v>
       </c>
       <c r="L56" t="n">
-        <v>280.4565627574921</v>
+        <v>275.4816560745239</v>
       </c>
     </row>
     <row r="57">
@@ -2590,37 +2590,37 @@
         <v>2015</v>
       </c>
       <c r="B57" t="n">
-        <v>40.3717771728289</v>
+        <v>35.12290158640472</v>
       </c>
       <c r="C57" t="n">
-        <v>114.5834858700164</v>
+        <v>115.5021691537448</v>
       </c>
       <c r="D57" t="n">
-        <v>55.39419727674051</v>
+        <v>49.83846238633742</v>
       </c>
       <c r="E57" t="n">
-        <v>-11.53516395480153</v>
+        <v>-3.601236040441769</v>
       </c>
       <c r="F57" t="n">
-        <v>198.8142963647842</v>
+        <v>196.8622970860451</v>
       </c>
       <c r="G57" t="n">
-        <v>47.39246796732038</v>
+        <v>42.51301164328438</v>
       </c>
       <c r="H57" t="n">
-        <v>134.509664026716</v>
+        <v>135.0521844109185</v>
       </c>
       <c r="I57" t="n">
-        <v>65.02730134407395</v>
+        <v>65.97337023793517</v>
       </c>
       <c r="J57" t="n">
-        <v>56.62547839384683</v>
+        <v>56.28522960127642</v>
       </c>
       <c r="K57" t="n">
-        <v>-9.086475967644439</v>
+        <v>-10.78529248498249</v>
       </c>
       <c r="L57" t="n">
-        <v>294.4684357643127</v>
+        <v>289.038503408432</v>
       </c>
     </row>
     <row r="58">
@@ -2628,37 +2628,37 @@
         <v>2016</v>
       </c>
       <c r="B58" t="n">
-        <v>40.25318730644486</v>
+        <v>34.92233256107177</v>
       </c>
       <c r="C58" t="n">
-        <v>117.2064698054924</v>
+        <v>117.5349025211052</v>
       </c>
       <c r="D58" t="n">
-        <v>55.90445685302941</v>
+        <v>53.02162146258124</v>
       </c>
       <c r="E58" t="n">
-        <v>-6.337149598530665</v>
+        <v>-3.001369342024432</v>
       </c>
       <c r="F58" t="n">
-        <v>207.026964366436</v>
+        <v>202.4774872027338</v>
       </c>
       <c r="G58" t="n">
-        <v>47.61235008411532</v>
+        <v>42.16573924491773</v>
       </c>
       <c r="H58" t="n">
-        <v>138.6343752115479</v>
+        <v>139.2232764876938</v>
       </c>
       <c r="I58" t="n">
-        <v>66.1250139196453</v>
+        <v>67.18355450089835</v>
       </c>
       <c r="J58" t="n">
-        <v>58.13641802772237</v>
+        <v>57.75841079223229</v>
       </c>
       <c r="K58" t="n">
-        <v>-0.7623793976482176</v>
+        <v>-2.493493089722257</v>
       </c>
       <c r="L58" t="n">
-        <v>309.7457778453827</v>
+        <v>303.8374879360199</v>
       </c>
     </row>
     <row r="59">
@@ -2666,37 +2666,37 @@
         <v>2017</v>
       </c>
       <c r="B59" t="n">
-        <v>40.02326083213039</v>
+        <v>34.67814088024927</v>
       </c>
       <c r="C59" t="n">
-        <v>119.8541214043112</v>
+        <v>119.5103402370133</v>
       </c>
       <c r="D59" t="n">
-        <v>56.10497473338408</v>
+        <v>56.41813253613271</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.03856587838355097</v>
+        <v>-2.161222607511966</v>
       </c>
       <c r="F59" t="n">
-        <v>215.9437910914421</v>
+        <v>208.4453910458833</v>
       </c>
       <c r="G59" t="n">
-        <v>47.71173918702448</v>
+        <v>41.63903249074228</v>
       </c>
       <c r="H59" t="n">
-        <v>142.8781279195955</v>
+        <v>143.5251609311375</v>
       </c>
       <c r="I59" t="n">
-        <v>66.88275432632541</v>
+        <v>68.0744626011649</v>
       </c>
       <c r="J59" t="n">
-        <v>62.7429355864362</v>
+        <v>62.30526535184973</v>
       </c>
       <c r="K59" t="n">
-        <v>6.155319054455674</v>
+        <v>4.416754818342902</v>
       </c>
       <c r="L59" t="n">
-        <v>326.3708760738373</v>
+        <v>319.9606761932373</v>
       </c>
     </row>
     <row r="60">
@@ -2704,37 +2704,37 @@
         <v>2018</v>
       </c>
       <c r="B60" t="n">
-        <v>39.6566473116703</v>
+        <v>34.3807049565674</v>
       </c>
       <c r="C60" t="n">
-        <v>122.5025383545815</v>
+        <v>121.4031450678128</v>
       </c>
       <c r="D60" t="n">
-        <v>55.94158919360174</v>
+        <v>60.04348282818503</v>
       </c>
       <c r="E60" t="n">
-        <v>7.501849318079152</v>
+        <v>-1.046348983578852</v>
       </c>
       <c r="F60" t="n">
-        <v>225.6026241779327</v>
+        <v>214.7809838689864</v>
       </c>
       <c r="G60" t="n">
-        <v>47.65614151659386</v>
+        <v>40.891259627789</v>
       </c>
       <c r="H60" t="n">
-        <v>147.2136123380727</v>
+        <v>147.9329092824738</v>
       </c>
       <c r="I60" t="n">
-        <v>67.22606352274498</v>
+        <v>68.57574564344182</v>
       </c>
       <c r="J60" t="n">
-        <v>64.77431477793675</v>
+        <v>64.29326038017102</v>
       </c>
       <c r="K60" t="n">
-        <v>17.5581224489913</v>
+        <v>15.79921760610246</v>
       </c>
       <c r="L60" t="n">
-        <v>344.4282546043396</v>
+        <v>337.492392539978</v>
       </c>
     </row>
     <row r="61">
@@ -2742,37 +2742,37 @@
         <v>2019</v>
       </c>
       <c r="B61" t="n">
-        <v>39.12392406528448</v>
+        <v>34.0191450381931</v>
       </c>
       <c r="C61" t="n">
-        <v>125.1231257834983</v>
+        <v>123.1845497628416</v>
       </c>
       <c r="D61" t="n">
-        <v>55.34983426544289</v>
+        <v>63.91371684919849</v>
       </c>
       <c r="E61" t="n">
-        <v>16.44509740404288</v>
+        <v>0.3818660178405935</v>
       </c>
       <c r="F61" t="n">
-        <v>236.0419815182686</v>
+        <v>221.4992776680738</v>
       </c>
       <c r="G61" t="n">
-        <v>47.40479661624907</v>
+        <v>39.87341524896431</v>
       </c>
       <c r="H61" t="n">
-        <v>151.6063756758792</v>
+        <v>152.4148183093906</v>
       </c>
       <c r="I61" t="n">
-        <v>67.06504265058146</v>
+        <v>68.60236465748861</v>
       </c>
       <c r="J61" t="n">
-        <v>68.71950061016926</v>
+        <v>68.17986112140895</v>
       </c>
       <c r="K61" t="n">
-        <v>29.20895625917852</v>
+        <v>27.44876316068766</v>
       </c>
       <c r="L61" t="n">
-        <v>364.0046718120575</v>
+        <v>356.5192224979401</v>
       </c>
     </row>
     <row r="62">
@@ -2780,37 +2780,37 @@
         <v>2020</v>
       </c>
       <c r="B62" t="n">
-        <v>38.39096695084599</v>
+        <v>33.58118737660537</v>
       </c>
       <c r="C62" t="n">
-        <v>127.6817821796624</v>
+        <v>124.8218058966644</v>
       </c>
       <c r="D62" t="n">
-        <v>54.25284017856431</v>
+        <v>68.04541585074797</v>
       </c>
       <c r="E62" t="n">
-        <v>26.97546314206105</v>
+        <v>2.166912119164053</v>
       </c>
       <c r="F62" t="n">
-        <v>247.3010524511337</v>
+        <v>228.6153212431818</v>
       </c>
       <c r="G62" t="n">
-        <v>46.90967122861753</v>
+        <v>38.52790217062475</v>
       </c>
       <c r="H62" t="n">
-        <v>156.0135339024049</v>
+        <v>156.9311723753005</v>
       </c>
       <c r="I62" t="n">
-        <v>66.29119030144932</v>
+        <v>68.05160096970822</v>
       </c>
       <c r="J62" t="n">
-        <v>17.3017853735327</v>
+        <v>17.1590071897419</v>
       </c>
       <c r="K62" t="n">
-        <v>98.67294473186784</v>
+        <v>96.46032503846008</v>
       </c>
       <c r="L62" t="n">
-        <v>385.1891255378723</v>
+        <v>377.1300077438354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some graphs regarding air time efficiency
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -500,37 +500,37 @@
         <v>1960</v>
       </c>
       <c r="B2" t="n">
-        <v>2.957472290406829</v>
+        <v>2.755252570979569</v>
       </c>
       <c r="C2" t="n">
-        <v>8.564322552084578</v>
+        <v>8.588104877825529</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.184753948311111</v>
+        <v>-0.9997490009044095</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.707797212041673</v>
+        <v>-2.318128058305656</v>
       </c>
       <c r="F2" t="n">
-        <v>8.629243682138622</v>
+        <v>8.025480389595032</v>
       </c>
       <c r="G2" t="n">
-        <v>3.009838941080147</v>
+        <v>2.664992669550213</v>
       </c>
       <c r="H2" t="n">
-        <v>8.272195929677791</v>
+        <v>8.306765334619181</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.2409611487482758</v>
+        <v>-0.9669980120382063</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.912467472619453</v>
+        <v>-1.945093541270408</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.611257959900463</v>
+        <v>-3.044232424142641</v>
       </c>
       <c r="L2" t="n">
-        <v>5.517348289489746</v>
+        <v>5.01543402671814</v>
       </c>
     </row>
     <row r="3">
@@ -538,37 +538,37 @@
         <v>1961</v>
       </c>
       <c r="B3" t="n">
-        <v>5.843796982785944</v>
+        <v>5.46453115983095</v>
       </c>
       <c r="C3" t="n">
-        <v>16.37195328550274</v>
+        <v>16.3845391446805</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.315647296754492</v>
+        <v>-1.962458580677453</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.06883613527095</v>
+        <v>-4.138971292906723</v>
       </c>
       <c r="F3" t="n">
-        <v>16.83126683626324</v>
+        <v>15.74764043092728</v>
       </c>
       <c r="G3" t="n">
-        <v>5.856665375718135</v>
+        <v>5.22944814093343</v>
       </c>
       <c r="H3" t="n">
-        <v>15.64407426294036</v>
+        <v>15.67967960362973</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.5510086274210471</v>
+        <v>-1.878034011741283</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.630056343137065</v>
+        <v>-8.753415186097419</v>
       </c>
       <c r="K3" t="n">
-        <v>-1.077342924860028</v>
+        <v>0.008781852903227971</v>
       </c>
       <c r="L3" t="n">
-        <v>11.24233174324036</v>
+        <v>10.28646039962769</v>
       </c>
     </row>
     <row r="4">
@@ -576,37 +576,37 @@
         <v>1962</v>
       </c>
       <c r="B4" t="n">
-        <v>8.632361327864997</v>
+        <v>8.105903906391141</v>
       </c>
       <c r="C4" t="n">
-        <v>23.49492837964499</v>
+        <v>23.48305040986538</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.370225307114356</v>
+        <v>-2.871497094671384</v>
       </c>
       <c r="E4" t="n">
-        <v>-4.138078618018204</v>
+        <v>-5.550720618801932</v>
       </c>
       <c r="F4" t="n">
-        <v>24.61898578237742</v>
+        <v>23.1667366027832</v>
       </c>
       <c r="G4" t="n">
-        <v>8.553766230617091</v>
+        <v>7.701324314756554</v>
       </c>
       <c r="H4" t="n">
-        <v>22.29458886299748</v>
+        <v>22.3109710150348</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.9224908450123742</v>
+        <v>-2.728175740833712</v>
       </c>
       <c r="J4" t="n">
-        <v>-11.90034521495542</v>
+        <v>-12.04317274164832</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.8927580320598558</v>
+        <v>0.529162567745006</v>
       </c>
       <c r="L4" t="n">
-        <v>17.13276100158691</v>
+        <v>15.77010941505432</v>
       </c>
     </row>
     <row r="5">
@@ -614,37 +614,37 @@
         <v>1963</v>
       </c>
       <c r="B5" t="n">
-        <v>11.30435862025081</v>
+        <v>10.66246506659041</v>
       </c>
       <c r="C5" t="n">
-        <v>29.99029548963885</v>
+        <v>29.95353398112397</v>
       </c>
       <c r="D5" t="n">
-        <v>-4.331129278993711</v>
+        <v>-3.713091007831708</v>
       </c>
       <c r="E5" t="n">
-        <v>-4.958171232040508</v>
+        <v>-6.619293583229076</v>
       </c>
       <c r="F5" t="n">
-        <v>32.00535359885544</v>
+        <v>30.28361445665359</v>
       </c>
       <c r="G5" t="n">
-        <v>11.11009766347402</v>
+        <v>10.08502655826333</v>
       </c>
       <c r="H5" t="n">
-        <v>28.34481344811425</v>
+        <v>28.33136463537102</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.346632958759547</v>
+        <v>-3.51200413725773</v>
       </c>
       <c r="J5" t="n">
-        <v>-11.96388374035964</v>
+        <v>-12.08501115616109</v>
       </c>
       <c r="K5" t="n">
-        <v>-2.995686784218959</v>
+        <v>-1.393737462944404</v>
       </c>
       <c r="L5" t="n">
-        <v>23.14870762825012</v>
+        <v>21.42563843727112</v>
       </c>
     </row>
     <row r="6">
@@ -652,37 +652,37 @@
         <v>1964</v>
       </c>
       <c r="B6" t="n">
-        <v>13.84676630945767</v>
+        <v>13.12120457073863</v>
       </c>
       <c r="C6" t="n">
-        <v>35.90553506972488</v>
+        <v>35.85080324176099</v>
       </c>
       <c r="D6" t="n">
-        <v>-5.185338932111792</v>
+        <v>-4.475989753468895</v>
       </c>
       <c r="E6" t="n">
-        <v>-5.563602314383958</v>
+        <v>-7.396313555017661</v>
       </c>
       <c r="F6" t="n">
-        <v>39.00336013268679</v>
+        <v>37.09970450401306</v>
       </c>
       <c r="G6" t="n">
-        <v>13.53166251947788</v>
+        <v>12.3824108185826</v>
       </c>
       <c r="H6" t="n">
-        <v>33.87912331637474</v>
+        <v>33.83221193773886</v>
       </c>
       <c r="I6" t="n">
-        <v>-1.813517812914484</v>
+        <v>-4.223967673731508</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.123394384997328</v>
+        <v>-8.193323856318347</v>
       </c>
       <c r="K6" t="n">
-        <v>-8.221373103883201</v>
+        <v>-6.582795513075803</v>
       </c>
       <c r="L6" t="n">
-        <v>29.25250053405762</v>
+        <v>27.2145357131958</v>
       </c>
     </row>
     <row r="7">
@@ -690,37 +690,37 @@
         <v>1965</v>
       </c>
       <c r="B7" t="n">
-        <v>16.25093614644977</v>
+        <v>15.47219529006907</v>
       </c>
       <c r="C7" t="n">
-        <v>41.28173559479643</v>
+        <v>41.21975235124386</v>
       </c>
       <c r="D7" t="n">
-        <v>-5.923561835386545</v>
+        <v>-5.15119808231933</v>
       </c>
       <c r="E7" t="n">
-        <v>-5.983077903589432</v>
+        <v>-7.923723229953072</v>
       </c>
       <c r="F7" t="n">
-        <v>45.62603200227022</v>
+        <v>43.61702632904053</v>
       </c>
       <c r="G7" t="n">
-        <v>15.82251006678173</v>
+        <v>14.59355353798953</v>
       </c>
       <c r="H7" t="n">
-        <v>38.95796005838631</v>
+        <v>38.8789471360054</v>
       </c>
       <c r="I7" t="n">
-        <v>-2.312126909651921</v>
+        <v>-4.858669606333579</v>
       </c>
       <c r="J7" t="n">
-        <v>-8.250172819183792</v>
+        <v>-8.311281322075134</v>
       </c>
       <c r="K7" t="n">
-        <v>-8.809440366272508</v>
+        <v>-7.202028896358314</v>
       </c>
       <c r="L7" t="n">
-        <v>35.40873003005981</v>
+        <v>33.10052084922791</v>
       </c>
     </row>
     <row r="8">
@@ -728,37 +728,37 @@
         <v>1966</v>
       </c>
       <c r="B8" t="n">
-        <v>18.51158072789739</v>
+        <v>17.70799266274854</v>
       </c>
       <c r="C8" t="n">
-        <v>46.15554486292123</v>
+        <v>46.09855780478731</v>
       </c>
       <c r="D8" t="n">
-        <v>-6.539719058992781</v>
+        <v>-5.731748817154248</v>
       </c>
       <c r="E8" t="n">
-        <v>-6.240973938137468</v>
+        <v>-8.236616041994616</v>
       </c>
       <c r="F8" t="n">
-        <v>51.88643259368837</v>
+        <v>49.83818560838699</v>
       </c>
       <c r="G8" t="n">
-        <v>17.98546040953443</v>
+        <v>16.71734054847584</v>
       </c>
       <c r="H8" t="n">
-        <v>43.62586541582986</v>
+        <v>43.51963005029914</v>
       </c>
       <c r="I8" t="n">
-        <v>-2.830433643507373</v>
+        <v>-5.411093100137896</v>
       </c>
       <c r="J8" t="n">
-        <v>-5.138174294387066</v>
+        <v>-5.171464322903</v>
       </c>
       <c r="K8" t="n">
-        <v>-12.05847339780005</v>
+        <v>-10.60487122550825</v>
       </c>
       <c r="L8" t="n">
-        <v>41.5842444896698</v>
+        <v>39.04954195022583</v>
       </c>
     </row>
     <row r="9">
@@ -766,37 +766,37 @@
         <v>1967</v>
       </c>
       <c r="B9" t="n">
-        <v>20.62602957244046</v>
+        <v>19.82318310373862</v>
       </c>
       <c r="C9" t="n">
-        <v>50.56042719509684</v>
+        <v>50.52072961031287</v>
       </c>
       <c r="D9" t="n">
-        <v>-7.03049299021945</v>
+        <v>-6.212502895641747</v>
       </c>
       <c r="E9" t="n">
-        <v>-6.358301746412373</v>
+        <v>-8.365034038304149</v>
       </c>
       <c r="F9" t="n">
-        <v>57.79766203090549</v>
+        <v>55.76637578010559</v>
       </c>
       <c r="G9" t="n">
-        <v>20.02263337352045</v>
+        <v>18.75191837698277</v>
       </c>
       <c r="H9" t="n">
-        <v>47.91670385659557</v>
+        <v>47.79053863551978</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.355535128114878</v>
+        <v>-5.876772998876862</v>
       </c>
       <c r="J9" t="n">
-        <v>-6.596514091755518</v>
+        <v>-6.634700818295123</v>
       </c>
       <c r="K9" t="n">
-        <v>-10.23913718474513</v>
+        <v>-9.001206383730835</v>
       </c>
       <c r="L9" t="n">
-        <v>47.74815082550049</v>
+        <v>45.02977681159973</v>
       </c>
     </row>
     <row r="10">
@@ -804,37 +804,37 @@
         <v>1968</v>
       </c>
       <c r="B10" t="n">
-        <v>22.59366985120897</v>
+        <v>21.81403671758004</v>
       </c>
       <c r="C10" t="n">
-        <v>54.52750038823049</v>
+        <v>54.5164815714009</v>
       </c>
       <c r="D10" t="n">
-        <v>-7.394923434127047</v>
+        <v>-6.589966680374216</v>
       </c>
       <c r="E10" t="n">
-        <v>-6.353389564352405</v>
+        <v>-8.335174637838755</v>
       </c>
       <c r="F10" t="n">
-        <v>63.37285724096</v>
+        <v>61.40537697076797</v>
       </c>
       <c r="G10" t="n">
-        <v>21.93582795370119</v>
+        <v>20.69503881460975</v>
       </c>
       <c r="H10" t="n">
-        <v>51.85716009495591</v>
+        <v>51.71994146534372</v>
       </c>
       <c r="I10" t="n">
-        <v>-3.873818650436928</v>
+        <v>-6.251920174289443</v>
       </c>
       <c r="J10" t="n">
-        <v>-14.02635039273692</v>
+        <v>-14.10077749305779</v>
       </c>
       <c r="K10" t="n">
-        <v>-2.021002370351409</v>
+        <v>-1.050647309108927</v>
       </c>
       <c r="L10" t="n">
-        <v>53.87181663513184</v>
+        <v>51.01163530349731</v>
       </c>
     </row>
     <row r="11">
@@ -842,37 +842,37 @@
         <v>1969</v>
       </c>
       <c r="B11" t="n">
-        <v>24.41551821325659</v>
+        <v>23.67823699386431</v>
       </c>
       <c r="C11" t="n">
-        <v>58.08610443288743</v>
+        <v>58.11366103734048</v>
       </c>
       <c r="D11" t="n">
-        <v>-7.634041474538843</v>
+        <v>-6.862121878992839</v>
       </c>
       <c r="E11" t="n">
-        <v>-6.2423892614128</v>
+        <v>-8.170218785840795</v>
       </c>
       <c r="F11" t="n">
-        <v>68.62519191019237</v>
+        <v>66.75955736637115</v>
       </c>
       <c r="G11" t="n">
-        <v>23.7267956704013</v>
+        <v>22.54432173840143</v>
       </c>
       <c r="H11" t="n">
-        <v>55.46912226505163</v>
+        <v>55.33068497294368</v>
       </c>
       <c r="I11" t="n">
-        <v>-4.371155803915822</v>
+        <v>-6.533505154468463</v>
       </c>
       <c r="J11" t="n">
-        <v>-17.56575942558975</v>
+        <v>-17.65367011789323</v>
       </c>
       <c r="K11" t="n">
-        <v>2.669864395721952</v>
+        <v>3.279922686611684</v>
       </c>
       <c r="L11" t="n">
-        <v>59.92886710166931</v>
+        <v>56.96775412559509</v>
       </c>
     </row>
     <row r="12">
@@ -880,37 +880,37 @@
         <v>1970</v>
       </c>
       <c r="B12" t="n">
-        <v>26.0938875572375</v>
+        <v>25.41466571329314</v>
       </c>
       <c r="C12" t="n">
-        <v>61.26420022305548</v>
+        <v>61.33839707871358</v>
       </c>
       <c r="D12" t="n">
-        <v>-7.750533659893609</v>
+        <v>-7.028263776347697</v>
       </c>
       <c r="E12" t="n">
-        <v>-6.039677628703732</v>
+        <v>-7.890927055019073</v>
       </c>
       <c r="F12" t="n">
-        <v>73.56787649169564</v>
+        <v>71.83387196063995</v>
       </c>
       <c r="G12" t="n">
-        <v>25.39743118628412</v>
+        <v>24.29745494400631</v>
       </c>
       <c r="H12" t="n">
-        <v>58.77134256549279</v>
+        <v>58.6420044304606</v>
       </c>
       <c r="I12" t="n">
-        <v>-4.83311566576439</v>
+        <v>-6.719306260679208</v>
       </c>
       <c r="J12" t="n">
-        <v>-11.65514480024612</v>
+        <v>-11.71180985000244</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.785326146255283</v>
+        <v>-1.635340019385231</v>
       </c>
       <c r="L12" t="n">
-        <v>65.89518713951111</v>
+        <v>62.87300324440002</v>
       </c>
     </row>
     <row r="13">
@@ -918,37 +918,37 @@
         <v>1971</v>
       </c>
       <c r="B13" t="n">
-        <v>27.63212394798747</v>
+        <v>27.02323036184836</v>
       </c>
       <c r="C13" t="n">
-        <v>64.08865285623139</v>
+        <v>64.21555839472347</v>
       </c>
       <c r="D13" t="n">
-        <v>-7.74843682086959</v>
+        <v>-7.08884862380919</v>
       </c>
       <c r="E13" t="n">
-        <v>-5.758181793866285</v>
+        <v>-7.516077816154219</v>
       </c>
       <c r="F13" t="n">
-        <v>78.21415818948299</v>
+        <v>76.63386231660843</v>
       </c>
       <c r="G13" t="n">
-        <v>26.94990307184556</v>
+        <v>25.95234446962981</v>
       </c>
       <c r="H13" t="n">
-        <v>61.78059964890488</v>
+        <v>61.67080210078565</v>
       </c>
       <c r="I13" t="n">
-        <v>-5.245197995268683</v>
+        <v>-6.807929285829981</v>
       </c>
       <c r="J13" t="n">
-        <v>-13.59289291180607</v>
+        <v>-13.65893444570869</v>
       </c>
       <c r="K13" t="n">
-        <v>1.85651053434677</v>
+        <v>1.548197332326826</v>
       </c>
       <c r="L13" t="n">
-        <v>71.74892234802246</v>
+        <v>68.70448017120361</v>
       </c>
     </row>
     <row r="14">
@@ -956,37 +956,37 @@
         <v>1972</v>
       </c>
       <c r="B14" t="n">
-        <v>29.03439694790002</v>
+        <v>28.50472331395008</v>
       </c>
       <c r="C14" t="n">
-        <v>66.58543263791603</v>
+        <v>66.7690783450869</v>
       </c>
       <c r="D14" t="n">
-        <v>-7.632859963330706</v>
+        <v>-7.045346159560669</v>
       </c>
       <c r="E14" t="n">
-        <v>-5.409648639783267</v>
+        <v>-7.062797442740322</v>
       </c>
       <c r="F14" t="n">
-        <v>82.57732098270208</v>
+        <v>81.16565805673599</v>
       </c>
       <c r="G14" t="n">
-        <v>28.38673832805792</v>
+        <v>27.50722739444926</v>
       </c>
       <c r="H14" t="n">
-        <v>64.51251799001095</v>
+        <v>64.43255739504981</v>
       </c>
       <c r="I14" t="n">
-        <v>-5.593069479059312</v>
+        <v>-6.798800912717553</v>
       </c>
       <c r="J14" t="n">
-        <v>-7.101036231906146</v>
+        <v>-7.136389072964776</v>
       </c>
       <c r="K14" t="n">
-        <v>-2.734674933427876</v>
+        <v>-3.563079834944676</v>
       </c>
       <c r="L14" t="n">
-        <v>77.47047567367554</v>
+        <v>74.44151496887207</v>
       </c>
     </row>
     <row r="15">
@@ -994,37 +994,37 @@
         <v>1973</v>
       </c>
       <c r="B15" t="n">
-        <v>30.30552738309246</v>
+        <v>29.8607052777427</v>
       </c>
       <c r="C15" t="n">
-        <v>68.77975848157914</v>
+        <v>69.02218743856436</v>
       </c>
       <c r="D15" t="n">
-        <v>-7.409731977225118</v>
+        <v>-6.900100197779203</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.004868262742708</v>
+        <v>-6.546816549690107</v>
       </c>
       <c r="F15" t="n">
-        <v>86.67068562470376</v>
+        <v>85.43597596883774</v>
       </c>
       <c r="G15" t="n">
-        <v>29.7108694133733</v>
+        <v>28.96075377193128</v>
       </c>
       <c r="H15" t="n">
-        <v>66.98214963148536</v>
+        <v>66.94197463240423</v>
       </c>
       <c r="I15" t="n">
-        <v>-5.862809674823973</v>
+        <v>-6.692142766583846</v>
       </c>
       <c r="J15" t="n">
-        <v>-6.076946494427875</v>
+        <v>-6.108594804165955</v>
       </c>
       <c r="K15" t="n">
-        <v>-1.710754511883047</v>
+        <v>-3.036326780622455</v>
       </c>
       <c r="L15" t="n">
-        <v>83.04250836372375</v>
+        <v>80.06566405296326</v>
       </c>
     </row>
     <row r="16">
@@ -1032,37 +1032,37 @@
         <v>1974</v>
       </c>
       <c r="B16" t="n">
-        <v>31.45084805959376</v>
+        <v>31.09340785783231</v>
       </c>
       <c r="C16" t="n">
-        <v>70.69619952864835</v>
+        <v>70.99756997985759</v>
       </c>
       <c r="D16" t="n">
-        <v>-7.085576054017685</v>
+        <v>-6.656195515776425</v>
       </c>
       <c r="E16" t="n">
-        <v>-4.55386190794615</v>
+        <v>-5.982662971480121</v>
       </c>
       <c r="F16" t="n">
-        <v>90.50760962627828</v>
+        <v>89.45211935043335</v>
       </c>
       <c r="G16" t="n">
-        <v>30.92565848092752</v>
+        <v>30.3120461043778</v>
       </c>
       <c r="H16" t="n">
-        <v>69.20437860202058</v>
+        <v>69.21343663480525</v>
       </c>
       <c r="I16" t="n">
-        <v>-6.041149443061574</v>
+        <v>-6.488928658977612</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.611050233926659</v>
+        <v>-2.625501860007036</v>
       </c>
       <c r="K16" t="n">
-        <v>-3.027893625060829</v>
+        <v>-4.850337260100135</v>
       </c>
       <c r="L16" t="n">
-        <v>88.44994378089905</v>
+        <v>85.56071496009827</v>
       </c>
     </row>
     <row r="17">
@@ -1070,37 +1070,37 @@
         <v>1975</v>
       </c>
       <c r="B17" t="n">
-        <v>32.47608684455813</v>
+        <v>32.20565097363226</v>
       </c>
       <c r="C17" t="n">
-        <v>72.35873995668099</v>
+        <v>72.71747930781416</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.667306576011239</v>
+        <v>-6.317331177193699</v>
       </c>
       <c r="E17" t="n">
-        <v>-4.066032950014879</v>
+        <v>-5.383819784203439</v>
       </c>
       <c r="F17" t="n">
-        <v>94.101487275213</v>
+        <v>93.22197932004929</v>
       </c>
       <c r="G17" t="n">
-        <v>32.03489513206893</v>
+        <v>31.5607398441365</v>
       </c>
       <c r="H17" t="n">
-        <v>71.19419187216447</v>
+        <v>71.26132766061156</v>
       </c>
       <c r="I17" t="n">
-        <v>-6.115702198816128</v>
+        <v>-6.190827999592402</v>
       </c>
       <c r="J17" t="n">
-        <v>-2.919436298699532</v>
+        <v>-2.936803997128449</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.5139870637703559</v>
+        <v>-2.781746060624252</v>
       </c>
       <c r="L17" t="n">
-        <v>93.67996144294739</v>
+        <v>90.91268944740295</v>
       </c>
     </row>
     <row r="18">
@@ -1108,37 +1108,37 @@
         <v>1976</v>
       </c>
       <c r="B18" t="n">
-        <v>33.38726978080729</v>
+        <v>33.20077226741804</v>
       </c>
       <c r="C18" t="n">
-        <v>73.79082642002969</v>
+        <v>74.20380672758927</v>
       </c>
       <c r="D18" t="n">
-        <v>-6.162052037140108</v>
+        <v>-5.887702313787974</v>
       </c>
       <c r="E18" t="n">
-        <v>-3.550294561863346</v>
+        <v>-4.762842460047004</v>
       </c>
       <c r="F18" t="n">
-        <v>97.46574960183352</v>
+        <v>96.75403422117233</v>
       </c>
       <c r="G18" t="n">
-        <v>33.04278326392376</v>
+        <v>32.70700815622536</v>
       </c>
       <c r="H18" t="n">
-        <v>72.9668633638472</v>
+        <v>73.10024273875044</v>
       </c>
       <c r="I18" t="n">
-        <v>-6.075179114697664</v>
+        <v>-5.800140010221092</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.756555698092039</v>
+        <v>-0.7614292659290338</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.4559093087251512</v>
+        <v>-3.135847663060898</v>
       </c>
       <c r="L18" t="n">
-        <v>98.7220025062561</v>
+        <v>96.10983395576477</v>
       </c>
     </row>
     <row r="19">
@@ -1146,37 +1146,37 @@
         <v>1977</v>
       </c>
       <c r="B19" t="n">
-        <v>34.19063718618862</v>
+        <v>34.08256552897463</v>
       </c>
       <c r="C19" t="n">
-        <v>75.01538640808404</v>
+        <v>75.4781175208816</v>
       </c>
       <c r="D19" t="n">
-        <v>-5.576998418921132</v>
+        <v>-5.371888711386704</v>
       </c>
       <c r="E19" t="n">
-        <v>-3.015160728361337</v>
+        <v>-4.131444895033852</v>
       </c>
       <c r="F19" t="n">
-        <v>100.6138644469902</v>
+        <v>100.0573494434357</v>
       </c>
       <c r="G19" t="n">
-        <v>33.9539129762872</v>
+        <v>33.75157581675575</v>
       </c>
       <c r="H19" t="n">
-        <v>74.53805595060992</v>
+        <v>74.74511869848305</v>
       </c>
       <c r="I19" t="n">
-        <v>-5.909585463996178</v>
+        <v>-5.319720106381245</v>
       </c>
       <c r="J19" t="n">
-        <v>0.6379517411818794</v>
+        <v>0.6424210080266849</v>
       </c>
       <c r="K19" t="n">
-        <v>0.3474309854923805</v>
+        <v>-2.676769608168425</v>
       </c>
       <c r="L19" t="n">
-        <v>103.5677661895752</v>
+        <v>101.1426258087158</v>
       </c>
     </row>
     <row r="20">
@@ -1184,37 +1184,37 @@
         <v>1978</v>
       </c>
       <c r="B20" t="n">
-        <v>34.8925741668054</v>
+        <v>34.85522711483112</v>
       </c>
       <c r="C20" t="n">
-        <v>76.05483416045649</v>
+        <v>76.5616685062319</v>
       </c>
       <c r="D20" t="n">
-        <v>-4.919255306834768</v>
+        <v>-4.774751108100355</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.468816652432579</v>
+        <v>-3.500566792320569</v>
       </c>
       <c r="F20" t="n">
-        <v>103.5593363679945</v>
+        <v>103.1415777206421</v>
       </c>
       <c r="G20" t="n">
-        <v>34.77322271934422</v>
+        <v>34.69572345247781</v>
       </c>
       <c r="H20" t="n">
-        <v>75.92386903804864</v>
+        <v>76.21130881750022</v>
       </c>
       <c r="I20" t="n">
-        <v>-5.610383087900888</v>
+        <v>-4.75290100550144</v>
       </c>
       <c r="J20" t="n">
-        <v>8.737521180768823</v>
+        <v>8.804224115684887</v>
       </c>
       <c r="K20" t="n">
-        <v>-5.6130195994063</v>
+        <v>-8.954580260379982</v>
       </c>
       <c r="L20" t="n">
-        <v>108.2112102508545</v>
+        <v>106.0037751197815</v>
       </c>
     </row>
     <row r="21">
@@ -1222,37 +1222,37 @@
         <v>1979</v>
       </c>
       <c r="B21" t="n">
-        <v>35.49954908824827</v>
+        <v>35.5233083131959</v>
       </c>
       <c r="C21" t="n">
-        <v>76.93106420453583</v>
+        <v>77.47540131647709</v>
       </c>
       <c r="D21" t="n">
-        <v>-4.19573959759535</v>
+        <v>-4.101335960962701</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.919166969956443</v>
+        <v>-2.880414895574155</v>
       </c>
       <c r="F21" t="n">
-        <v>106.3157067252323</v>
+        <v>106.0169587731361</v>
       </c>
       <c r="G21" t="n">
-        <v>35.50595651165987</v>
+        <v>35.54128298783034</v>
       </c>
       <c r="H21" t="n">
-        <v>77.14084260960036</v>
+        <v>77.51460360919593</v>
       </c>
       <c r="I21" t="n">
-        <v>-5.170631051195103</v>
+        <v>-4.103411223176875</v>
       </c>
       <c r="J21" t="n">
-        <v>11.88797135242909</v>
+        <v>11.98689558311575</v>
       </c>
       <c r="K21" t="n">
-        <v>-6.715587481576241</v>
+        <v>-10.25115260178631</v>
       </c>
       <c r="L21" t="n">
-        <v>112.648551940918</v>
+        <v>110.6882183551788</v>
       </c>
     </row>
     <row r="22">
@@ -1260,37 +1260,37 @@
         <v>1980</v>
       </c>
       <c r="B22" t="n">
-        <v>36.01806044817678</v>
+        <v>36.09167291442412</v>
       </c>
       <c r="C22" t="n">
-        <v>77.66542698035695</v>
+        <v>78.23991896721151</v>
       </c>
       <c r="D22" t="n">
-        <v>-3.413079535993501</v>
+        <v>-3.35678731937662</v>
       </c>
       <c r="E22" t="n">
-        <v>-1.373854269981514</v>
+        <v>-2.280485135245613</v>
       </c>
       <c r="F22" t="n">
-        <v>108.8965536225587</v>
+        <v>108.6943194270134</v>
       </c>
       <c r="G22" t="n">
-        <v>36.15761574803651</v>
+        <v>36.2906284256927</v>
       </c>
       <c r="H22" t="n">
-        <v>78.20592610449425</v>
+        <v>78.67121687674987</v>
       </c>
       <c r="I22" t="n">
-        <v>-4.585084808366894</v>
+        <v>-3.375291624758362</v>
       </c>
       <c r="J22" t="n">
-        <v>6.028347001057323</v>
+        <v>6.082978953432057</v>
       </c>
       <c r="K22" t="n">
-        <v>1.071464435079722</v>
+        <v>-2.476404760556565</v>
       </c>
       <c r="L22" t="n">
-        <v>116.8782684803009</v>
+        <v>115.1931278705597</v>
       </c>
     </row>
     <row r="23">
@@ -1298,37 +1298,37 @@
         <v>1981</v>
       </c>
       <c r="B23" t="n">
-        <v>36.45459175211546</v>
+        <v>36.56545889134948</v>
       </c>
       <c r="C23" t="n">
-        <v>78.27870153378181</v>
+        <v>78.87544951269686</v>
       </c>
       <c r="D23" t="n">
-        <v>-2.577532775955327</v>
+        <v>-2.546266874782809</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.8402685635278289</v>
+        <v>-1.709567497910527</v>
       </c>
       <c r="F23" t="n">
-        <v>111.3154919464141</v>
+        <v>111.185074031353</v>
       </c>
       <c r="G23" t="n">
-        <v>36.73390658119995</v>
+        <v>36.94665876890706</v>
       </c>
       <c r="H23" t="n">
-        <v>79.13641873963138</v>
+        <v>79.69773679168007</v>
       </c>
       <c r="I23" t="n">
-        <v>-3.850257821601849</v>
+        <v>-2.572812052946176</v>
       </c>
       <c r="J23" t="n">
-        <v>7.269454667238326</v>
+        <v>7.341080459717278</v>
       </c>
       <c r="K23" t="n">
-        <v>1.611573939107751</v>
+        <v>-1.894768268810874</v>
       </c>
       <c r="L23" t="n">
-        <v>120.9010961055756</v>
+        <v>119.5178956985474</v>
       </c>
     </row>
     <row r="24">
@@ -1336,37 +1336,37 @@
         <v>1982</v>
       </c>
       <c r="B24" t="n">
-        <v>36.81556954781459</v>
+        <v>36.95004395153364</v>
       </c>
       <c r="C24" t="n">
-        <v>78.79105255448395</v>
+        <v>79.40180009844106</v>
       </c>
       <c r="D24" t="n">
-        <v>-1.69492133398668</v>
+        <v>-1.674882023311786</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.3255274183204193</v>
+        <v>-1.175737508840648</v>
       </c>
       <c r="F24" t="n">
-        <v>113.5861733499914</v>
+        <v>113.5012245178223</v>
       </c>
       <c r="G24" t="n">
-        <v>37.24068737967646</v>
+        <v>37.51278097172949</v>
       </c>
       <c r="H24" t="n">
-        <v>79.94988909132729</v>
+        <v>80.61106340660362</v>
       </c>
       <c r="I24" t="n">
-        <v>-2.964446779387793</v>
+        <v>-1.700389925825092</v>
       </c>
       <c r="J24" t="n">
-        <v>7.202132006021295</v>
+        <v>7.279113576748939</v>
       </c>
       <c r="K24" t="n">
-        <v>3.291766941202474</v>
+        <v>-0.03841230759252845</v>
       </c>
       <c r="L24" t="n">
-        <v>124.7200286388397</v>
+        <v>123.6641557216644</v>
       </c>
     </row>
     <row r="25">
@@ -1374,37 +1374,37 @@
         <v>1983</v>
       </c>
       <c r="B25" t="n">
-        <v>37.10732825539348</v>
+        <v>37.25101350402231</v>
       </c>
       <c r="C25" t="n">
-        <v>79.22198887195808</v>
+        <v>79.83830216533475</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.7705779294815972</v>
+        <v>-0.7476201626578376</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1635470404651187</v>
+        <v>-0.6863367749525509</v>
       </c>
       <c r="F25" t="n">
-        <v>115.7222862383351</v>
+        <v>115.6553587317467</v>
       </c>
       <c r="G25" t="n">
-        <v>37.68391468989272</v>
+        <v>37.99288479471285</v>
       </c>
       <c r="H25" t="n">
-        <v>80.66407967069732</v>
+        <v>81.42831915286028</v>
       </c>
       <c r="I25" t="n">
-        <v>-1.927714390690891</v>
+        <v>-0.7625093665437226</v>
       </c>
       <c r="J25" t="n">
-        <v>8.604202597485406</v>
+        <v>8.703718248815735</v>
       </c>
       <c r="K25" t="n">
-        <v>3.315839211866537</v>
+        <v>0.2733501000712391</v>
       </c>
       <c r="L25" t="n">
-        <v>128.3403217792511</v>
+        <v>127.6357629299164</v>
       </c>
     </row>
     <row r="26">
@@ -1412,37 +1412,37 @@
         <v>1984</v>
       </c>
       <c r="B26" t="n">
-        <v>37.3360781742457</v>
+        <v>37.47413213812481</v>
       </c>
       <c r="C26" t="n">
-        <v>79.5903083946794</v>
+        <v>80.20374879690084</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1906955012040819</v>
+        <v>0.2307093098416394</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6204737336019122</v>
+        <v>-0.2479367729205748</v>
       </c>
       <c r="F26" t="n">
-        <v>117.7375558037311</v>
+        <v>117.6606534719467</v>
       </c>
       <c r="G26" t="n">
-        <v>38.06958905356613</v>
+        <v>38.39131892043434</v>
       </c>
       <c r="H26" t="n">
-        <v>81.29679705576403</v>
+        <v>82.16675138271263</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.7418353163179738</v>
+        <v>0.2363559657471734</v>
       </c>
       <c r="J26" t="n">
-        <v>9.952739366215955</v>
+        <v>10.07696011453443</v>
       </c>
       <c r="K26" t="n">
-        <v>3.1921972217533</v>
+        <v>0.5674213424777861</v>
       </c>
       <c r="L26" t="n">
-        <v>131.7694873809814</v>
+        <v>131.4388077259064</v>
       </c>
     </row>
     <row r="27">
@@ -1450,37 +1450,37 @@
         <v>1985</v>
       </c>
       <c r="B27" t="n">
-        <v>37.50787686531108</v>
+        <v>37.6253166397716</v>
       </c>
       <c r="C27" t="n">
-        <v>79.91404314824423</v>
+        <v>80.51632838374668</v>
       </c>
       <c r="D27" t="n">
-        <v>1.184659612318105</v>
+        <v>1.255526336255743</v>
       </c>
       <c r="E27" t="n">
-        <v>1.039164357924314</v>
+        <v>0.1336999719177214</v>
       </c>
       <c r="F27" t="n">
-        <v>119.6457439837977</v>
+        <v>119.5308713316917</v>
       </c>
       <c r="G27" t="n">
-        <v>38.40370478830057</v>
+        <v>38.71286252940088</v>
       </c>
       <c r="H27" t="n">
-        <v>81.86580187639369</v>
+        <v>82.84362313637675</v>
       </c>
       <c r="I27" t="n">
-        <v>0.5897937343501688</v>
+        <v>1.291816861579134</v>
       </c>
       <c r="J27" t="n">
-        <v>12.04526892586944</v>
+        <v>12.20704447342378</v>
       </c>
       <c r="K27" t="n">
-        <v>2.112729135092854</v>
+        <v>0.02625986414867043</v>
       </c>
       <c r="L27" t="n">
-        <v>135.0172984600067</v>
+        <v>135.0816068649292</v>
       </c>
     </row>
     <row r="28">
@@ -1488,37 +1488,37 @@
         <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>37.62860368579909</v>
+        <v>37.71061179496347</v>
       </c>
       <c r="C28" t="n">
-        <v>80.21040140390315</v>
+        <v>80.79355754137686</v>
       </c>
       <c r="D28" t="n">
-        <v>2.207660758845453</v>
+        <v>2.322525694821369</v>
       </c>
       <c r="E28" t="n">
-        <v>1.413983643671401</v>
+        <v>0.4536679921194064</v>
       </c>
       <c r="F28" t="n">
-        <v>121.4606494922191</v>
+        <v>121.2803630232811</v>
       </c>
       <c r="G28" t="n">
-        <v>38.69219838999912</v>
+        <v>38.96269685331959</v>
       </c>
       <c r="H28" t="n">
-        <v>82.38868712503788</v>
+        <v>83.47610235817838</v>
       </c>
       <c r="I28" t="n">
-        <v>2.062276522761474</v>
+        <v>2.399639259988254</v>
       </c>
       <c r="J28" t="n">
-        <v>10.50183324351871</v>
+        <v>10.65317729503711</v>
       </c>
       <c r="K28" t="n">
-        <v>4.450793197534148</v>
+        <v>3.083091979982411</v>
       </c>
       <c r="L28" t="n">
-        <v>138.0957884788513</v>
+        <v>138.5747077465057</v>
       </c>
     </row>
     <row r="29">
@@ -1526,37 +1526,37 @@
         <v>1987</v>
       </c>
       <c r="B29" t="n">
-        <v>37.70393731341807</v>
+        <v>37.7361678445486</v>
       </c>
       <c r="C29" t="n">
-        <v>80.49570703823933</v>
+        <v>81.05221390576605</v>
       </c>
       <c r="D29" t="n">
-        <v>3.256647299911327</v>
+        <v>3.427716470148489</v>
       </c>
       <c r="E29" t="n">
-        <v>1.739816155069164</v>
+        <v>0.7079673098370094</v>
       </c>
       <c r="F29" t="n">
-        <v>123.1961078066379</v>
+        <v>122.9240655303001</v>
       </c>
       <c r="G29" t="n">
-        <v>38.94090228494213</v>
+        <v>39.14637564117176</v>
       </c>
       <c r="H29" t="n">
-        <v>82.88276437652351</v>
+        <v>84.08115061323279</v>
       </c>
       <c r="I29" t="n">
-        <v>3.669367562457103</v>
+        <v>3.555810889028792</v>
       </c>
       <c r="J29" t="n">
-        <v>15.41803527155145</v>
+        <v>15.65577074704103</v>
       </c>
       <c r="K29" t="n">
-        <v>0.1081770827423565</v>
+        <v>-0.5082175687428219</v>
       </c>
       <c r="L29" t="n">
-        <v>141.0192465782166</v>
+        <v>141.9308903217316</v>
       </c>
     </row>
     <row r="30">
@@ -1564,37 +1564,37 @@
         <v>1988</v>
       </c>
       <c r="B30" t="n">
-        <v>37.73933503193791</v>
+        <v>37.70821977079174</v>
       </c>
       <c r="C30" t="n">
-        <v>80.78534308575421</v>
+        <v>81.30826869889769</v>
       </c>
       <c r="D30" t="n">
-        <v>4.329179866063367</v>
+        <v>4.567456964033441</v>
       </c>
       <c r="E30" t="n">
-        <v>2.012133203526417</v>
+        <v>0.8935583428274256</v>
       </c>
       <c r="F30" t="n">
-        <v>124.8659911872819</v>
+        <v>124.4775037765503</v>
       </c>
       <c r="G30" t="n">
-        <v>39.15550055166423</v>
+        <v>39.26979423973023</v>
       </c>
       <c r="H30" t="n">
-        <v>83.36495211274979</v>
+        <v>84.67541032705108</v>
       </c>
       <c r="I30" t="n">
-        <v>5.403644246849417</v>
+        <v>4.756604694325779</v>
       </c>
       <c r="J30" t="n">
-        <v>16.47767079345447</v>
+        <v>16.74875078235079</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.5975444056914121</v>
+        <v>-0.2853962880410066</v>
       </c>
       <c r="L30" t="n">
-        <v>143.8042232990265</v>
+        <v>145.1651637554169</v>
       </c>
     </row>
     <row r="31">
@@ -1602,37 +1602,37 @@
         <v>1989</v>
       </c>
       <c r="B31" t="n">
-        <v>37.74001513689075</v>
+        <v>37.63306922278267</v>
       </c>
       <c r="C31" t="n">
-        <v>81.09369381479503</v>
+        <v>81.57682547474236</v>
       </c>
       <c r="D31" t="n">
-        <v>5.423435804183097</v>
+        <v>5.738483518576856</v>
       </c>
       <c r="E31" t="n">
-        <v>2.22706388291094</v>
+        <v>1.008412171528576</v>
       </c>
       <c r="F31" t="n">
-        <v>126.4842086387798</v>
+        <v>125.9567903876305</v>
       </c>
       <c r="G31" t="n">
-        <v>39.34148845561896</v>
+        <v>39.33915982804758</v>
       </c>
       <c r="H31" t="n">
-        <v>83.85167209044516</v>
+        <v>85.27510091238689</v>
       </c>
       <c r="I31" t="n">
-        <v>7.256695666441435</v>
+        <v>5.998636969297387</v>
       </c>
       <c r="J31" t="n">
-        <v>17.56690038451844</v>
+        <v>17.87438333782273</v>
       </c>
       <c r="K31" t="n">
-        <v>-1.547230067711865</v>
+        <v>-0.1925172440725333</v>
       </c>
       <c r="L31" t="n">
-        <v>146.4695265293121</v>
+        <v>148.2947638034821</v>
       </c>
     </row>
     <row r="32">
@@ -1640,37 +1640,37 @@
         <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>37.7109392205759</v>
+        <v>37.51706709036858</v>
       </c>
       <c r="C32" t="n">
-        <v>81.4340923549899</v>
+        <v>81.87206625962428</v>
       </c>
       <c r="D32" t="n">
-        <v>6.538212494779707</v>
+        <v>6.937936218857907</v>
       </c>
       <c r="E32" t="n">
-        <v>2.381461877068531</v>
+        <v>1.051553976319056</v>
       </c>
       <c r="F32" t="n">
-        <v>128.064705947414</v>
+        <v>127.3786235451698</v>
       </c>
       <c r="G32" t="n">
-        <v>39.50413506158376</v>
+        <v>39.36096207950109</v>
       </c>
       <c r="H32" t="n">
-        <v>84.3587554440672</v>
+        <v>85.89592804931095</v>
       </c>
       <c r="I32" t="n">
-        <v>9.219322653611417</v>
+        <v>7.278923050212781</v>
       </c>
       <c r="J32" t="n">
-        <v>16.83734679720862</v>
+        <v>17.15004722638063</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.8833355912366194</v>
+        <v>1.653299560109701</v>
       </c>
       <c r="L32" t="n">
-        <v>149.0362243652344</v>
+        <v>151.3391599655151</v>
       </c>
     </row>
     <row r="33">
@@ -1678,37 +1678,37 @@
         <v>1991</v>
       </c>
       <c r="B33" t="n">
-        <v>37.6567982083382</v>
+        <v>37.36659926070372</v>
       </c>
       <c r="C33" t="n">
-        <v>81.81877385513934</v>
+        <v>82.2072009042118</v>
       </c>
       <c r="D33" t="n">
-        <v>7.67292546961747</v>
+        <v>8.163380236682379</v>
       </c>
       <c r="E33" t="n">
-        <v>2.472968124742678</v>
+        <v>1.023109803880779</v>
       </c>
       <c r="F33" t="n">
-        <v>129.6214656578377</v>
+        <v>128.7602902054787</v>
       </c>
       <c r="G33" t="n">
-        <v>39.64844988905512</v>
+        <v>39.34194435857267</v>
       </c>
       <c r="H33" t="n">
-        <v>84.90136814897077</v>
+        <v>86.55299620077325</v>
       </c>
       <c r="I33" t="n">
-        <v>11.28174205149252</v>
+        <v>8.594928556615498</v>
       </c>
       <c r="J33" t="n">
-        <v>14.13554071793475</v>
+        <v>14.41333063084411</v>
       </c>
       <c r="K33" t="n">
-        <v>1.560546687816604</v>
+        <v>5.416849539083154</v>
       </c>
       <c r="L33" t="n">
-        <v>151.5276474952698</v>
+        <v>154.3200492858887</v>
       </c>
     </row>
     <row r="34">
@@ -1716,37 +1716,37 @@
         <v>1992</v>
       </c>
       <c r="B34" t="n">
-        <v>37.58199846470598</v>
+        <v>37.18807371396998</v>
       </c>
       <c r="C34" t="n">
-        <v>82.25883171871135</v>
+        <v>82.59442842984855</v>
       </c>
       <c r="D34" t="n">
-        <v>8.827604153270602</v>
+        <v>9.412823540830098</v>
       </c>
       <c r="E34" t="n">
-        <v>2.500072745699875</v>
+        <v>0.9243387459696564</v>
       </c>
       <c r="F34" t="n">
-        <v>131.1685070823878</v>
+        <v>130.1196644306183</v>
       </c>
       <c r="G34" t="n">
-        <v>39.77915169321965</v>
+        <v>39.28907739495488</v>
       </c>
       <c r="H34" t="n">
-        <v>85.49394532948727</v>
+        <v>87.26074160042742</v>
       </c>
       <c r="I34" t="n">
-        <v>13.43378474406475</v>
+        <v>9.944617068503899</v>
       </c>
       <c r="J34" t="n">
-        <v>12.91410918414742</v>
+        <v>13.18193450379734</v>
       </c>
       <c r="K34" t="n">
-        <v>2.348388235711145</v>
+        <v>7.584990792866384</v>
       </c>
       <c r="L34" t="n">
-        <v>153.9693791866302</v>
+        <v>157.2613613605499</v>
       </c>
     </row>
     <row r="35">
@@ -1754,37 +1754,37 @@
         <v>1993</v>
       </c>
       <c r="B35" t="n">
-        <v>37.49064966332462</v>
+        <v>36.98790954798916</v>
       </c>
       <c r="C35" t="n">
-        <v>82.76418939185295</v>
+        <v>83.04491049241632</v>
       </c>
       <c r="D35" t="n">
-        <v>10.00288915253464</v>
+        <v>10.6847322135076</v>
       </c>
       <c r="E35" t="n">
-        <v>2.462158091510503</v>
+        <v>0.7576535847671835</v>
       </c>
       <c r="F35" t="n">
-        <v>132.7198862992227</v>
+        <v>131.4752058386803</v>
       </c>
       <c r="G35" t="n">
-        <v>39.90064048309182</v>
+        <v>39.20953391717236</v>
       </c>
       <c r="H35" t="n">
-        <v>86.15014528546233</v>
+        <v>88.03288086276724</v>
       </c>
       <c r="I35" t="n">
-        <v>15.66509126650601</v>
+        <v>11.32649493418603</v>
       </c>
       <c r="J35" t="n">
-        <v>10.30965793585159</v>
+        <v>10.53469710115306</v>
       </c>
       <c r="K35" t="n">
-        <v>4.363731043187371</v>
+        <v>11.08564651495203</v>
       </c>
       <c r="L35" t="n">
-        <v>156.3892660140991</v>
+        <v>160.1892533302307</v>
       </c>
     </row>
     <row r="36">
@@ -1792,37 +1792,37 @@
         <v>1994</v>
       </c>
       <c r="B36" t="n">
-        <v>37.38655359680045</v>
+        <v>36.77252929020101</v>
       </c>
       <c r="C36" t="n">
-        <v>83.34356881255802</v>
+        <v>83.56875065539455</v>
       </c>
       <c r="D36" t="n">
-        <v>11.20002453769498</v>
+        <v>11.97804226748578</v>
       </c>
       <c r="E36" t="n">
-        <v>2.359549215513098</v>
+        <v>0.5266417418441804</v>
       </c>
       <c r="F36" t="n">
-        <v>134.2896961625665</v>
+        <v>132.8459639549255</v>
       </c>
       <c r="G36" t="n">
-        <v>40.01697232493216</v>
+        <v>39.11066735850467</v>
       </c>
       <c r="H36" t="n">
-        <v>86.88282762185351</v>
+        <v>88.88237147505414</v>
       </c>
       <c r="I36" t="n">
-        <v>17.9652891596756</v>
+        <v>12.73965201122516</v>
       </c>
       <c r="J36" t="n">
-        <v>14.06676140697225</v>
+        <v>14.38907876825045</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.1144352760067537</v>
+        <v>8.010344797365965</v>
       </c>
       <c r="L36" t="n">
-        <v>158.8174152374268</v>
+        <v>163.1321144104004</v>
       </c>
     </row>
     <row r="37">
@@ -1830,37 +1830,37 @@
         <v>1995</v>
       </c>
       <c r="B37" t="n">
-        <v>37.27319341777029</v>
+        <v>36.54835200856295</v>
       </c>
       <c r="C37" t="n">
-        <v>84.00448186645923</v>
+        <v>84.17498847128414</v>
       </c>
       <c r="D37" t="n">
-        <v>12.42085456646452</v>
+        <v>13.29216992967017</v>
       </c>
       <c r="E37" t="n">
-        <v>2.193536431526141</v>
+        <v>0.2360624974537231</v>
       </c>
       <c r="F37" t="n">
-        <v>135.8920662822202</v>
+        <v>134.251572906971</v>
       </c>
       <c r="G37" t="n">
-        <v>40.13183303160207</v>
+        <v>38.99999225307309</v>
       </c>
       <c r="H37" t="n">
-        <v>87.70404132795244</v>
+        <v>89.82139324677243</v>
       </c>
       <c r="I37" t="n">
-        <v>20.32415261135793</v>
+        <v>14.183800248017</v>
       </c>
       <c r="J37" t="n">
-        <v>15.73889386959164</v>
+        <v>16.11645711097677</v>
       </c>
       <c r="K37" t="n">
-        <v>-2.612731999637994</v>
+        <v>6.998918502473568</v>
       </c>
       <c r="L37" t="n">
-        <v>161.2861888408661</v>
+        <v>166.1205613613129</v>
       </c>
     </row>
     <row r="38">
@@ -1868,37 +1868,37 @@
         <v>1996</v>
       </c>
       <c r="B38" t="n">
-        <v>37.15372379833347</v>
+        <v>36.32179043256151</v>
       </c>
       <c r="C38" t="n">
-        <v>84.75321663266378</v>
+        <v>84.87160657781986</v>
       </c>
       <c r="D38" t="n">
-        <v>13.66781636199956</v>
+        <v>14.62701961362257</v>
       </c>
       <c r="E38" t="n">
-        <v>1.966406244534269</v>
+        <v>-0.1081612057033112</v>
       </c>
       <c r="F38" t="n">
-        <v>137.5411630375311</v>
+        <v>135.7122554183006</v>
       </c>
       <c r="G38" t="n">
-        <v>40.24851296235521</v>
+        <v>38.88516981348979</v>
       </c>
       <c r="H38" t="n">
-        <v>88.62503216074417</v>
+        <v>90.86134782506865</v>
       </c>
       <c r="I38" t="n">
-        <v>22.73173726158019</v>
+        <v>15.65930904747109</v>
       </c>
       <c r="J38" t="n">
-        <v>18.82828535513324</v>
+        <v>19.29991270224928</v>
       </c>
       <c r="K38" t="n">
-        <v>-6.603358246175709</v>
+        <v>4.481702914425053</v>
       </c>
       <c r="L38" t="n">
-        <v>163.8302094936371</v>
+        <v>169.1874423027039</v>
       </c>
     </row>
     <row r="39">
@@ -1906,37 +1906,37 @@
         <v>1997</v>
       </c>
       <c r="B39" t="n">
-        <v>37.03096112726396</v>
+        <v>36.09924980912688</v>
       </c>
       <c r="C39" t="n">
-        <v>85.59484135012447</v>
+        <v>85.6655400753896</v>
       </c>
       <c r="D39" t="n">
-        <v>14.94393565484371</v>
+        <v>15.98299062570808</v>
       </c>
       <c r="E39" t="n">
-        <v>1.681451456336966</v>
+        <v>-0.4989588344471301</v>
       </c>
       <c r="F39" t="n">
-        <v>139.2511895885691</v>
+        <v>137.2488216757774</v>
       </c>
       <c r="G39" t="n">
-        <v>40.3698811305078</v>
+        <v>38.77399697719627</v>
       </c>
       <c r="H39" t="n">
-        <v>89.65627262807669</v>
+        <v>92.01286479624437</v>
       </c>
       <c r="I39" t="n">
-        <v>25.17848622796977</v>
+        <v>17.16723847405489</v>
       </c>
       <c r="J39" t="n">
-        <v>20.74785675431811</v>
+        <v>21.28907576483529</v>
       </c>
       <c r="K39" t="n">
-        <v>-9.466135475689896</v>
+        <v>3.124660224622911</v>
       </c>
       <c r="L39" t="n">
-        <v>166.4863612651825</v>
+        <v>172.3678362369537</v>
       </c>
     </row>
     <row r="40">
@@ -1944,37 +1944,37 @@
         <v>1998</v>
       </c>
       <c r="B40" t="n">
-        <v>36.90737476267991</v>
+        <v>35.88712985688779</v>
       </c>
       <c r="C40" t="n">
-        <v>86.53321574292619</v>
+        <v>86.56270617655886</v>
       </c>
       <c r="D40" t="n">
-        <v>16.25282206806816</v>
+        <v>17.36098196906059</v>
       </c>
       <c r="E40" t="n">
-        <v>1.342973266130748</v>
+        <v>-0.9281500437708203</v>
       </c>
       <c r="F40" t="n">
-        <v>141.036385839805</v>
+        <v>138.8826679587364</v>
       </c>
       <c r="G40" t="n">
-        <v>40.49835337523621</v>
+        <v>38.67440060583528</v>
       </c>
       <c r="H40" t="n">
-        <v>90.80749280139142</v>
+        <v>93.28583226208926</v>
       </c>
       <c r="I40" t="n">
-        <v>27.65530272773835</v>
+        <v>18.7093694664263</v>
       </c>
       <c r="J40" t="n">
-        <v>19.639469502874</v>
+        <v>20.17153856923074</v>
       </c>
       <c r="K40" t="n">
-        <v>-9.306833073606558</v>
+        <v>4.857910953413057</v>
       </c>
       <c r="L40" t="n">
-        <v>169.2937853336334</v>
+        <v>175.6990518569946</v>
       </c>
     </row>
     <row r="41">
@@ -1982,37 +1982,37 @@
         <v>1999</v>
       </c>
       <c r="B41" t="n">
-        <v>36.78507623311542</v>
+        <v>35.6918297195195</v>
       </c>
       <c r="C41" t="n">
-        <v>87.57100275736822</v>
+        <v>87.5680304102724</v>
       </c>
       <c r="D41" t="n">
-        <v>17.59866654796113</v>
+        <v>18.76239679410936</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9562829240173585</v>
+        <v>-1.386478556381874</v>
       </c>
       <c r="F41" t="n">
-        <v>142.9110284624621</v>
+        <v>140.6357783675194</v>
       </c>
       <c r="G41" t="n">
-        <v>40.63585861002883</v>
+        <v>38.59443687368142</v>
       </c>
       <c r="H41" t="n">
-        <v>92.08772849843872</v>
+        <v>94.68942467731159</v>
       </c>
       <c r="I41" t="n">
-        <v>30.1535877310979</v>
+        <v>20.2882324711193</v>
       </c>
       <c r="J41" t="n">
-        <v>21.13463250109542</v>
+        <v>21.7276702831632</v>
       </c>
       <c r="K41" t="n">
-        <v>-11.71792544750291</v>
+        <v>3.920862048942016</v>
       </c>
       <c r="L41" t="n">
-        <v>172.293881893158</v>
+        <v>179.2206263542175</v>
       </c>
     </row>
     <row r="42">
@@ -2020,37 +2020,37 @@
         <v>2000</v>
       </c>
       <c r="B42" t="n">
-        <v>36.66580978236323</v>
+        <v>35.51975583605706</v>
       </c>
       <c r="C42" t="n">
-        <v>88.70969549280332</v>
+        <v>88.68548387644834</v>
       </c>
       <c r="D42" t="n">
-        <v>18.98623891466629</v>
+        <v>20.18914540424724</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5276867261039868</v>
+        <v>-1.863660233673116</v>
       </c>
       <c r="F42" t="n">
-        <v>144.8894309159368</v>
+        <v>142.5307248830795</v>
       </c>
       <c r="G42" t="n">
-        <v>40.7837951465522</v>
+        <v>38.54229680382326</v>
       </c>
       <c r="H42" t="n">
-        <v>93.50537146557565</v>
+        <v>96.23214352973977</v>
       </c>
       <c r="I42" t="n">
-        <v>32.66523493278496</v>
+        <v>21.90713353936219</v>
       </c>
       <c r="J42" t="n">
-        <v>25.87764130903685</v>
+        <v>26.62762764498752</v>
       </c>
       <c r="K42" t="n">
-        <v>-17.30173103105842</v>
+        <v>-0.3348749073475474</v>
       </c>
       <c r="L42" t="n">
-        <v>175.5303118228912</v>
+        <v>182.9743266105652</v>
       </c>
     </row>
     <row r="43">
@@ -2058,37 +2058,37 @@
         <v>2001</v>
       </c>
       <c r="B43" t="n">
-        <v>36.55094079099477</v>
+        <v>35.37733296577623</v>
       </c>
       <c r="C43" t="n">
-        <v>89.94963482152015</v>
+        <v>89.91812070085572</v>
       </c>
       <c r="D43" t="n">
-        <v>20.42088671512554</v>
+        <v>21.64364857815559</v>
       </c>
       <c r="E43" t="n">
-        <v>0.06448107824851945</v>
+        <v>-2.348436606340741</v>
       </c>
       <c r="F43" t="n">
-        <v>146.985943405889</v>
+        <v>144.5906656384468</v>
       </c>
       <c r="G43" t="n">
-        <v>40.94297977298181</v>
+        <v>38.52631843076895</v>
       </c>
       <c r="H43" t="n">
-        <v>95.06821659457839</v>
+        <v>97.92185731379864</v>
       </c>
       <c r="I43" t="n">
-        <v>35.18258501017997</v>
+        <v>23.57017975132106</v>
       </c>
       <c r="J43" t="n">
-        <v>21.85947508127694</v>
+        <v>22.51197264230167</v>
       </c>
       <c r="K43" t="n">
-        <v>-14.00426215626746</v>
+        <v>4.473823206108992</v>
       </c>
       <c r="L43" t="n">
-        <v>179.0489943027496</v>
+        <v>187.0041513442993</v>
       </c>
     </row>
     <row r="44">
@@ -2096,37 +2096,37 @@
         <v>2002</v>
       </c>
       <c r="B44" t="n">
-        <v>36.44144467127125</v>
+        <v>35.2710187148443</v>
       </c>
       <c r="C44" t="n">
-        <v>91.29004180024975</v>
+        <v>91.26811576546687</v>
       </c>
       <c r="D44" t="n">
-        <v>21.90853643144506</v>
+        <v>23.12883915031966</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.4250699861278449</v>
+        <v>-2.828627281391491</v>
       </c>
       <c r="F44" t="n">
-        <v>149.2149529168382</v>
+        <v>146.8393463492393</v>
       </c>
       <c r="G44" t="n">
-        <v>41.11358324143114</v>
+        <v>38.55500553267243</v>
       </c>
       <c r="H44" t="n">
-        <v>96.78350053694578</v>
+        <v>99.76583712375761</v>
       </c>
       <c r="I44" t="n">
-        <v>37.6983311260509</v>
+        <v>25.2823012744332</v>
       </c>
       <c r="J44" t="n">
-        <v>26.91148049180069</v>
+        <v>27.73643980695459</v>
       </c>
       <c r="K44" t="n">
-        <v>-19.60878953647205</v>
+        <v>0.01674689534563356</v>
       </c>
       <c r="L44" t="n">
-        <v>182.8981058597565</v>
+        <v>191.3563306331635</v>
       </c>
     </row>
     <row r="45">
@@ -2134,37 +2134,37 @@
         <v>2003</v>
       </c>
       <c r="B45" t="n">
-        <v>36.3378917065203</v>
+        <v>35.20732046136307</v>
       </c>
       <c r="C45" t="n">
-        <v>92.72903695257261</v>
+        <v>92.73679486039016</v>
       </c>
       <c r="D45" t="n">
-        <v>23.45569364799827</v>
+        <v>24.64816486405611</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.9317391051716726</v>
+        <v>-3.291180468192309</v>
       </c>
       <c r="F45" t="n">
-        <v>151.5908832019195</v>
+        <v>149.301099717617</v>
       </c>
       <c r="G45" t="n">
-        <v>41.29505238541369</v>
+        <v>38.63705233192732</v>
       </c>
       <c r="H45" t="n">
-        <v>98.65793653947118</v>
+        <v>101.770778041692</v>
       </c>
       <c r="I45" t="n">
-        <v>40.2053779697474</v>
+        <v>27.04927336869073</v>
       </c>
       <c r="J45" t="n">
-        <v>27.71364578681311</v>
+        <v>28.58353428039268</v>
       </c>
       <c r="K45" t="n">
-        <v>-20.74392611452035</v>
+        <v>0.03868216963427429</v>
       </c>
       <c r="L45" t="n">
-        <v>187.128086566925</v>
+        <v>196.079320192337</v>
       </c>
     </row>
     <row r="46">
@@ -2172,37 +2172,37 @@
         <v>2004</v>
       </c>
       <c r="B46" t="n">
-        <v>36.24043279601353</v>
+        <v>35.1928167723481</v>
       </c>
       <c r="C46" t="n">
-        <v>94.26366266355261</v>
+        <v>94.32466335839256</v>
       </c>
       <c r="D46" t="n">
-        <v>25.06944689284385</v>
+        <v>26.20559042371366</v>
       </c>
       <c r="E46" t="n">
-        <v>-1.4453475797716</v>
+        <v>-3.722223870475283</v>
       </c>
       <c r="F46" t="n">
-        <v>154.1281947726384</v>
+        <v>152.000846683979</v>
       </c>
       <c r="G46" t="n">
-        <v>41.48601485752346</v>
+        <v>38.78137783272454</v>
       </c>
       <c r="H46" t="n">
-        <v>100.6977156904692</v>
+        <v>103.942814021087</v>
       </c>
       <c r="I46" t="n">
-        <v>42.69664594634199</v>
+        <v>28.87773690084937</v>
       </c>
       <c r="J46" t="n">
-        <v>32.15596216115541</v>
+        <v>33.18634592045535</v>
       </c>
       <c r="K46" t="n">
-        <v>-25.24470910264892</v>
+        <v>-3.564465671286293</v>
       </c>
       <c r="L46" t="n">
-        <v>191.7916295528412</v>
+        <v>201.22380900383</v>
       </c>
     </row>
     <row r="47">
@@ -2210,37 +2210,37 @@
         <v>2005</v>
       </c>
       <c r="B47" t="n">
-        <v>36.14878101725054</v>
+        <v>35.23418059817782</v>
       </c>
       <c r="C47" t="n">
-        <v>95.88989445531355</v>
+        <v>96.03141448261972</v>
       </c>
       <c r="D47" t="n">
-        <v>26.75747018329687</v>
+        <v>27.80559985299436</v>
       </c>
       <c r="E47" t="n">
-        <v>-1.95476075512714</v>
+        <v>-4.107100891013893</v>
       </c>
       <c r="F47" t="n">
-        <v>156.8413849007338</v>
+        <v>154.964094042778</v>
       </c>
       <c r="G47" t="n">
-        <v>41.68416322592223</v>
+        <v>38.99716536776136</v>
       </c>
       <c r="H47" t="n">
-        <v>102.9084944909498</v>
+        <v>106.2874994536535</v>
       </c>
       <c r="I47" t="n">
-        <v>45.16482228630847</v>
+        <v>30.77521762129754</v>
       </c>
       <c r="J47" t="n">
-        <v>36.02503201034158</v>
+        <v>37.1998620319838</v>
       </c>
       <c r="K47" t="n">
-        <v>-28.83881861409275</v>
+        <v>-6.417030641841002</v>
       </c>
       <c r="L47" t="n">
-        <v>196.9436933994293</v>
+        <v>206.8427138328552</v>
       </c>
     </row>
     <row r="48">
@@ -2248,37 +2248,37 @@
         <v>2006</v>
       </c>
       <c r="B48" t="n">
-        <v>36.06219101856019</v>
+        <v>35.33820622605195</v>
       </c>
       <c r="C48" t="n">
-        <v>97.60264691990955</v>
+        <v>97.85593171878809</v>
       </c>
       <c r="D48" t="n">
-        <v>28.52802851002264</v>
+        <v>29.45319967817029</v>
       </c>
       <c r="E48" t="n">
-        <v>-2.447878802374568</v>
+        <v>-4.430401451955476</v>
       </c>
       <c r="F48" t="n">
-        <v>159.7449876461178</v>
+        <v>158.2169361710548</v>
       </c>
       <c r="G48" t="n">
-        <v>41.88611614791849</v>
+        <v>39.2939107908675</v>
       </c>
       <c r="H48" t="n">
-        <v>105.2953431826001</v>
+        <v>108.80977451766</v>
       </c>
       <c r="I48" t="n">
-        <v>47.60205163956052</v>
+        <v>32.75014564283192</v>
       </c>
       <c r="J48" t="n">
-        <v>38.42154505654648</v>
+        <v>39.69275712450992</v>
       </c>
       <c r="K48" t="n">
-        <v>-30.56356222932332</v>
+        <v>-7.555404318087341</v>
       </c>
       <c r="L48" t="n">
-        <v>202.6414937973022</v>
+        <v>212.991183757782</v>
       </c>
     </row>
     <row r="49">
@@ -2286,37 +2286,37 @@
         <v>2007</v>
       </c>
       <c r="B49" t="n">
-        <v>35.97943565494461</v>
+        <v>35.51183888957578</v>
       </c>
       <c r="C49" t="n">
-        <v>99.39576191009114</v>
+        <v>99.79626703674111</v>
       </c>
       <c r="D49" t="n">
-        <v>30.3899806303803</v>
+        <v>31.15392217729106</v>
       </c>
       <c r="E49" t="n">
-        <v>-2.911604383244239</v>
+        <v>-4.675972300309013</v>
       </c>
       <c r="F49" t="n">
-        <v>162.8535738121718</v>
+        <v>161.786055803299</v>
       </c>
       <c r="G49" t="n">
-        <v>42.08725253532693</v>
+        <v>39.68147723019083</v>
       </c>
       <c r="H49" t="n">
-        <v>107.8626608465575</v>
+        <v>111.5138900688956</v>
       </c>
       <c r="I49" t="n">
-        <v>49.99956430735466</v>
+        <v>34.81187379097394</v>
       </c>
       <c r="J49" t="n">
-        <v>41.15227536300872</v>
+        <v>42.52924426710228</v>
       </c>
       <c r="K49" t="n">
-        <v>-32.15725236750969</v>
+        <v>-8.809888048050126</v>
       </c>
       <c r="L49" t="n">
-        <v>208.9445006847382</v>
+        <v>219.7265973091125</v>
       </c>
     </row>
     <row r="50">
@@ -2324,37 +2324,37 @@
         <v>2008</v>
       </c>
       <c r="B50" t="n">
-        <v>35.8987781563301</v>
+        <v>35.76220646011388</v>
       </c>
       <c r="C50" t="n">
-        <v>101.2619860430899</v>
+        <v>101.8495973124623</v>
       </c>
       <c r="D50" t="n">
-        <v>32.35278547454703</v>
+        <v>32.91382934246298</v>
       </c>
       <c r="E50" t="n">
-        <v>-3.331798696555161</v>
+        <v>-4.826911885009089</v>
       </c>
       <c r="F50" t="n">
-        <v>166.1817509774119</v>
+        <v>165.6987212300301</v>
       </c>
       <c r="G50" t="n">
-        <v>42.28151589498496</v>
+        <v>40.1701566951564</v>
       </c>
       <c r="H50" t="n">
-        <v>110.614042301052</v>
+        <v>114.4032957793948</v>
       </c>
       <c r="I50" t="n">
-        <v>52.34723836034702</v>
+        <v>36.9706965256462</v>
       </c>
       <c r="J50" t="n">
-        <v>39.91843334553688</v>
+        <v>41.26485909291869</v>
       </c>
       <c r="K50" t="n">
-        <v>-29.24677854121838</v>
+        <v>-5.700446577307943</v>
       </c>
       <c r="L50" t="n">
-        <v>215.9144513607025</v>
+        <v>227.1085615158081</v>
       </c>
     </row>
     <row r="51">
@@ -2362,37 +2362,37 @@
         <v>2009</v>
       </c>
       <c r="B51" t="n">
-        <v>35.81794027541709</v>
+        <v>36.09665393760542</v>
       </c>
       <c r="C51" t="n">
-        <v>103.1929255059554</v>
+        <v>104.0121596041666</v>
       </c>
       <c r="D51" t="n">
-        <v>34.42650591571625</v>
+        <v>34.73951859192005</v>
       </c>
       <c r="E51" t="n">
-        <v>-3.693208187630468</v>
+        <v>-4.865542855661687</v>
       </c>
       <c r="F51" t="n">
-        <v>169.7441635094583</v>
+        <v>169.9827892780304</v>
       </c>
       <c r="G51" t="n">
-        <v>42.46118571723035</v>
+        <v>40.77073842495055</v>
       </c>
       <c r="H51" t="n">
-        <v>113.5521019068811</v>
+        <v>117.4804888997698</v>
       </c>
       <c r="I51" t="n">
-        <v>54.63308682361534</v>
+        <v>39.23787030144425</v>
       </c>
       <c r="J51" t="n">
-        <v>42.0748432989509</v>
+        <v>43.50071802861427</v>
       </c>
       <c r="K51" t="n">
-        <v>-29.10588156694445</v>
+        <v>-5.790901603722958</v>
       </c>
       <c r="L51" t="n">
-        <v>223.6153361797333</v>
+        <v>235.1989140510559</v>
       </c>
     </row>
     <row r="52">
@@ -2400,37 +2400,37 @@
         <v>2010</v>
       </c>
       <c r="B52" t="n">
-        <v>35.73406638845568</v>
+        <v>36.52277887251248</v>
       </c>
       <c r="C52" t="n">
-        <v>105.178983880803</v>
+        <v>106.2791537116574</v>
       </c>
       <c r="D52" t="n">
-        <v>36.62181282826435</v>
+        <v>36.63812826787804</v>
       </c>
       <c r="E52" t="n">
-        <v>-3.979370606061686</v>
+        <v>-4.773358104702936</v>
       </c>
       <c r="F52" t="n">
-        <v>173.5554924914613</v>
+        <v>174.666702747345</v>
       </c>
       <c r="G52" t="n">
-        <v>42.61660667787145</v>
+        <v>41.49458234716073</v>
       </c>
       <c r="H52" t="n">
-        <v>116.6782419025563</v>
+        <v>120.7468114862955</v>
       </c>
       <c r="I52" t="n">
-        <v>56.84266451222359</v>
+        <v>41.62563412176416</v>
       </c>
       <c r="J52" t="n">
-        <v>46.22939701014258</v>
+        <v>47.79824615604387</v>
       </c>
       <c r="K52" t="n">
-        <v>-30.25350272936562</v>
+        <v>-7.603550163739243</v>
       </c>
       <c r="L52" t="n">
-        <v>232.1134073734283</v>
+        <v>244.061723947525</v>
       </c>
     </row>
     <row r="53">
@@ -2438,37 +2438,37 @@
         <v>2011</v>
       </c>
       <c r="B53" t="n">
-        <v>35.6436803748902</v>
+        <v>37.04846928523311</v>
       </c>
       <c r="C53" t="n">
-        <v>107.209270429077</v>
+        <v>108.6446134231781</v>
       </c>
       <c r="D53" t="n">
-        <v>38.94998863023196</v>
+        <v>38.61734572915741</v>
       </c>
       <c r="E53" t="n">
-        <v>-4.172483597545487</v>
+        <v>-4.530935642101255</v>
       </c>
       <c r="F53" t="n">
-        <v>177.6304558366537</v>
+        <v>179.7794927954674</v>
       </c>
       <c r="G53" t="n">
-        <v>42.73587932873266</v>
+        <v>42.35369782390887</v>
       </c>
       <c r="H53" t="n">
-        <v>119.9923578540402</v>
+        <v>124.2021928542878</v>
       </c>
       <c r="I53" t="n">
-        <v>58.95838404071487</v>
+        <v>44.14723262064886</v>
       </c>
       <c r="J53" t="n">
-        <v>46.65784600900004</v>
+        <v>48.23811911783717</v>
       </c>
       <c r="K53" t="n">
-        <v>-26.86729151990228</v>
+        <v>-5.177955826106512</v>
       </c>
       <c r="L53" t="n">
-        <v>241.4771757125854</v>
+        <v>253.7632865905762</v>
       </c>
     </row>
     <row r="54">
@@ -2476,37 +2476,37 @@
         <v>2012</v>
       </c>
       <c r="B54" t="n">
-        <v>35.54263844006679</v>
+        <v>37.68194098452431</v>
       </c>
       <c r="C54" t="n">
-        <v>109.2714852218703</v>
+        <v>111.101244405763</v>
       </c>
       <c r="D54" t="n">
-        <v>41.42292849158768</v>
+        <v>40.68541605311608</v>
       </c>
       <c r="E54" t="n">
-        <v>-4.253243990902583</v>
+        <v>-4.11782411538902</v>
       </c>
       <c r="F54" t="n">
-        <v>181.9838081626222</v>
+        <v>185.3507773280144</v>
       </c>
       <c r="G54" t="n">
-        <v>42.80449714600039</v>
+        <v>43.36082611602388</v>
       </c>
       <c r="H54" t="n">
-        <v>123.4924932904291</v>
+        <v>127.8448406341554</v>
       </c>
       <c r="I54" t="n">
-        <v>60.95872949849564</v>
+        <v>46.8169421437653</v>
       </c>
       <c r="J54" t="n">
-        <v>49.5773283956859</v>
+        <v>51.2475175541022</v>
       </c>
       <c r="K54" t="n">
-        <v>-25.05563734657169</v>
+        <v>-4.897993431460492</v>
       </c>
       <c r="L54" t="n">
-        <v>251.7774109840393</v>
+        <v>264.3721330165863</v>
       </c>
     </row>
     <row r="55">
@@ -2514,37 +2514,37 @@
         <v>2013</v>
       </c>
       <c r="B55" t="n">
-        <v>35.42607323491492</v>
+        <v>38.43177634961764</v>
       </c>
       <c r="C55" t="n">
-        <v>111.3517695381611</v>
+        <v>113.6402216585881</v>
       </c>
       <c r="D55" t="n">
-        <v>44.05314058284465</v>
+        <v>42.85115224128357</v>
       </c>
       <c r="E55" t="n">
-        <v>-4.200642454717183</v>
+        <v>-3.512389131554158</v>
       </c>
       <c r="F55" t="n">
-        <v>186.6303409012035</v>
+        <v>191.4107611179352</v>
       </c>
       <c r="G55" t="n">
-        <v>42.80492829322611</v>
+        <v>44.52952543831268</v>
       </c>
       <c r="H55" t="n">
-        <v>127.1744101699368</v>
+        <v>131.670862546845</v>
       </c>
       <c r="I55" t="n">
-        <v>62.81735031030982</v>
+        <v>49.65009830486878</v>
       </c>
       <c r="J55" t="n">
-        <v>52.06958600210208</v>
+        <v>53.8084524036118</v>
       </c>
       <c r="K55" t="n">
-        <v>-21.77913302333176</v>
+        <v>-3.699918079014267</v>
       </c>
       <c r="L55" t="n">
-        <v>263.087141752243</v>
+        <v>275.959020614624</v>
       </c>
     </row>
     <row r="56">
@@ -2552,37 +2552,37 @@
         <v>2014</v>
       </c>
       <c r="B56" t="n">
-        <v>35.28833144300549</v>
+        <v>39.30696215735033</v>
       </c>
       <c r="C56" t="n">
-        <v>113.4345207760257</v>
+        <v>116.2509439752739</v>
       </c>
       <c r="D56" t="n">
-        <v>46.85374351943896</v>
+        <v>45.12394799421905</v>
       </c>
       <c r="E56" t="n">
-        <v>-3.991713513560185</v>
+        <v>-2.691617665680774</v>
       </c>
       <c r="F56" t="n">
-        <v>191.58488222491</v>
+        <v>197.9902364611626</v>
       </c>
       <c r="G56" t="n">
-        <v>42.71613498480644</v>
+        <v>45.87425774419418</v>
       </c>
       <c r="H56" t="n">
-        <v>131.0310969103514</v>
+        <v>135.6738214868723</v>
       </c>
       <c r="I56" t="n">
-        <v>64.5020104789115</v>
+        <v>52.66312905168957</v>
       </c>
       <c r="J56" t="n">
-        <v>53.76551820391873</v>
+        <v>55.53933021340457</v>
       </c>
       <c r="K56" t="n">
-        <v>-16.53310450346419</v>
+        <v>-1.15360274710666</v>
       </c>
       <c r="L56" t="n">
-        <v>275.4816560745239</v>
+        <v>288.596935749054</v>
       </c>
     </row>
     <row r="57">
@@ -2590,37 +2590,37 @@
         <v>2015</v>
       </c>
       <c r="B57" t="n">
-        <v>35.12290158640472</v>
+        <v>40.31692718529091</v>
       </c>
       <c r="C57" t="n">
-        <v>115.5021691537448</v>
+        <v>118.9207411146118</v>
       </c>
       <c r="D57" t="n">
-        <v>49.83846238633742</v>
+        <v>47.51379115243535</v>
       </c>
       <c r="E57" t="n">
-        <v>-3.601236040441769</v>
+        <v>-1.630875977702011</v>
       </c>
       <c r="F57" t="n">
-        <v>196.8622970860451</v>
+        <v>205.1205834746361</v>
       </c>
       <c r="G57" t="n">
-        <v>42.51301164328438</v>
+        <v>47.41047671287962</v>
       </c>
       <c r="H57" t="n">
-        <v>135.0521844109185</v>
+        <v>139.844214847546</v>
       </c>
       <c r="I57" t="n">
-        <v>65.97337023793517</v>
+        <v>55.87359072828872</v>
       </c>
       <c r="J57" t="n">
-        <v>56.28522960127642</v>
+        <v>58.11351133572528</v>
       </c>
       <c r="K57" t="n">
-        <v>-10.78529248498249</v>
+        <v>1.119302996120076</v>
       </c>
       <c r="L57" t="n">
-        <v>289.038503408432</v>
+        <v>302.3610966205597</v>
       </c>
     </row>
     <row r="58">
@@ -2628,37 +2628,37 @@
         <v>2016</v>
       </c>
       <c r="B58" t="n">
-        <v>34.92233256107177</v>
+        <v>41.47157749352299</v>
       </c>
       <c r="C58" t="n">
-        <v>117.5349025211052</v>
+        <v>121.6345254686473</v>
       </c>
       <c r="D58" t="n">
-        <v>53.02162146258124</v>
+        <v>50.03127972260462</v>
       </c>
       <c r="E58" t="n">
-        <v>-3.001369342024432</v>
+        <v>-0.3036146150308028</v>
       </c>
       <c r="F58" t="n">
-        <v>202.4774872027338</v>
+        <v>212.8337680697441</v>
       </c>
       <c r="G58" t="n">
-        <v>42.16573924491773</v>
+        <v>49.15471372923957</v>
       </c>
       <c r="H58" t="n">
-        <v>139.2232764876938</v>
+        <v>144.1688655305442</v>
       </c>
       <c r="I58" t="n">
-        <v>67.18355450089835</v>
+        <v>59.30020946650092</v>
       </c>
       <c r="J58" t="n">
-        <v>57.75841079223229</v>
+        <v>59.59933730424572</v>
       </c>
       <c r="K58" t="n">
-        <v>-2.493493089722257</v>
+        <v>5.105825089846185</v>
       </c>
       <c r="L58" t="n">
-        <v>303.8374879360199</v>
+        <v>317.3289511203766</v>
       </c>
     </row>
     <row r="59">
@@ -2666,37 +2666,37 @@
         <v>2017</v>
       </c>
       <c r="B59" t="n">
-        <v>34.67814088024927</v>
+        <v>42.78133110546195</v>
       </c>
       <c r="C59" t="n">
-        <v>119.5103402370133</v>
+        <v>124.3743836727143</v>
       </c>
       <c r="D59" t="n">
-        <v>56.41813253613271</v>
+        <v>52.68763974886764</v>
       </c>
       <c r="E59" t="n">
-        <v>-2.161222607511966</v>
+        <v>1.318990941954034</v>
       </c>
       <c r="F59" t="n">
-        <v>208.4453910458833</v>
+        <v>221.162345468998</v>
       </c>
       <c r="G59" t="n">
-        <v>41.63903249074228</v>
+        <v>51.12466315781803</v>
       </c>
       <c r="H59" t="n">
-        <v>143.5251609311375</v>
+        <v>148.6302157138101</v>
       </c>
       <c r="I59" t="n">
-        <v>68.0744626011649</v>
+        <v>62.96292717262885</v>
       </c>
       <c r="J59" t="n">
-        <v>62.30526535184973</v>
+        <v>64.24728210828241</v>
       </c>
       <c r="K59" t="n">
-        <v>4.416754818342902</v>
+        <v>6.615089869845292</v>
       </c>
       <c r="L59" t="n">
-        <v>319.9606761932373</v>
+        <v>333.5801780223846</v>
       </c>
     </row>
     <row r="60">
@@ -2704,37 +2704,37 @@
         <v>2018</v>
       </c>
       <c r="B60" t="n">
-        <v>34.3807049565674</v>
+        <v>44.25714870948202</v>
       </c>
       <c r="C60" t="n">
-        <v>121.4031450678128</v>
+        <v>127.1190980533219</v>
       </c>
       <c r="D60" t="n">
-        <v>60.04348282818503</v>
+        <v>55.494745145435</v>
       </c>
       <c r="E60" t="n">
-        <v>-1.046348983578852</v>
+        <v>3.268463529421254</v>
       </c>
       <c r="F60" t="n">
-        <v>214.7809838689864</v>
+        <v>230.1394554376602</v>
       </c>
       <c r="G60" t="n">
-        <v>40.891259627789</v>
+        <v>53.33926304455639</v>
       </c>
       <c r="H60" t="n">
-        <v>147.9329092824738</v>
+        <v>153.2055093192255</v>
       </c>
       <c r="I60" t="n">
-        <v>68.57574564344182</v>
+        <v>66.8829532678139</v>
       </c>
       <c r="J60" t="n">
-        <v>64.29326038017102</v>
+        <v>66.24644729424173</v>
       </c>
       <c r="K60" t="n">
-        <v>15.79921760610246</v>
+        <v>11.52251000415518</v>
       </c>
       <c r="L60" t="n">
-        <v>337.492392539978</v>
+        <v>351.1966829299927</v>
       </c>
     </row>
     <row r="61">
@@ -2742,37 +2742,37 @@
         <v>2019</v>
       </c>
       <c r="B61" t="n">
-        <v>34.0191450381931</v>
+        <v>45.9105630603154</v>
       </c>
       <c r="C61" t="n">
-        <v>123.1845497628416</v>
+        <v>129.843586020921</v>
       </c>
       <c r="D61" t="n">
-        <v>63.91371684919849</v>
+        <v>58.46513907216551</v>
       </c>
       <c r="E61" t="n">
-        <v>0.3818660178405935</v>
+        <v>5.579539196737706</v>
       </c>
       <c r="F61" t="n">
-        <v>221.4992776680738</v>
+        <v>239.7988273501396</v>
       </c>
       <c r="G61" t="n">
-        <v>39.87341524896431</v>
+        <v>55.8187734274934</v>
       </c>
       <c r="H61" t="n">
-        <v>152.4148183093906</v>
+        <v>157.8658423246366</v>
       </c>
       <c r="I61" t="n">
-        <v>68.60236465748861</v>
+        <v>71.08282133217817</v>
       </c>
       <c r="J61" t="n">
-        <v>68.17986112140895</v>
+        <v>70.19190504927502</v>
       </c>
       <c r="K61" t="n">
-        <v>27.44876316068766</v>
+        <v>15.30326424878677</v>
       </c>
       <c r="L61" t="n">
-        <v>356.5192224979401</v>
+        <v>370.26260638237</v>
       </c>
     </row>
     <row r="62">
@@ -2780,37 +2780,37 @@
         <v>2020</v>
       </c>
       <c r="B62" t="n">
-        <v>33.58118737660537</v>
+        <v>47.75370372563103</v>
       </c>
       <c r="C62" t="n">
-        <v>124.8218058966644</v>
+        <v>132.5182336147943</v>
       </c>
       <c r="D62" t="n">
-        <v>68.04541585074797</v>
+        <v>61.61205748172289</v>
       </c>
       <c r="E62" t="n">
-        <v>2.166912119164053</v>
+        <v>8.290781374331601</v>
       </c>
       <c r="F62" t="n">
-        <v>228.6153212431818</v>
+        <v>250.1747761964798</v>
       </c>
       <c r="G62" t="n">
-        <v>38.52790217062475</v>
+        <v>58.58484741858675</v>
       </c>
       <c r="H62" t="n">
-        <v>156.9311723753005</v>
+        <v>162.5750442543452</v>
       </c>
       <c r="I62" t="n">
-        <v>68.05160096970822</v>
+        <v>75.58645099970693</v>
       </c>
       <c r="J62" t="n">
-        <v>17.1590071897419</v>
+        <v>17.64928148140623</v>
       </c>
       <c r="K62" t="n">
-        <v>96.46032503846008</v>
+        <v>76.46869111733241</v>
       </c>
       <c r="L62" t="n">
-        <v>377.1300077438354</v>
+        <v>390.8643152713776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring some files for a better overview
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>YEAR</t>
+          <t>YOI</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -464,625 +464,2353 @@
           <t>deltaC_Tot</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Structural_Ops</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Engine_Ops</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Aerodyn_Ops</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_SLF_Ops</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Res_Ops</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Tot_Ops</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1992</v>
+        <v>1960</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2579348831061763</v>
+        <v>2.755252570979569</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6622618281829495</v>
+        <v>8.588104877825529</v>
       </c>
       <c r="D2" t="n">
-        <v>0.642198110205514</v>
+        <v>-0.9997490009044095</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.017153098105614</v>
+        <v>-2.318128058305656</v>
       </c>
       <c r="F2" t="n">
-        <v>1.545241723389026</v>
+        <v>8.025480389595032</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.664992669550213</v>
+      </c>
+      <c r="H2" t="n">
+        <v>8.306765334619181</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-0.9669980120382063</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1.945093541270408</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-3.044232424142641</v>
+      </c>
+      <c r="L2" t="n">
+        <v>5.01543402671814</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1993</v>
+        <v>1961</v>
       </c>
       <c r="B3" t="n">
-        <v>1.325871802501397</v>
+        <v>5.46453115983095</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9393757563251039</v>
+        <v>16.3845391446805</v>
       </c>
       <c r="D3" t="n">
-        <v>1.359164545545607</v>
+        <v>-1.962458580677453</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.590118265298865</v>
+        <v>-4.138971292906723</v>
       </c>
       <c r="F3" t="n">
-        <v>3.034293839073243</v>
+        <v>15.74764043092728</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5.22944814093343</v>
+      </c>
+      <c r="H3" t="n">
+        <v>15.67967960362973</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1.878034011741283</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-8.753415186097419</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.008781852903227971</v>
+      </c>
+      <c r="L3" t="n">
+        <v>10.28646039962769</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1994</v>
+        <v>1962</v>
       </c>
       <c r="B4" t="n">
-        <v>2.375928217139952</v>
+        <v>8.105903906391141</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8530057112932889</v>
+        <v>23.48305040986538</v>
       </c>
       <c r="D4" t="n">
-        <v>1.391905845046296</v>
+        <v>-2.871497094671384</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.8170541696149118</v>
+        <v>-5.550720618801932</v>
       </c>
       <c r="F4" t="n">
-        <v>3.803785603864625</v>
+        <v>23.1667366027832</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.701324314756554</v>
+      </c>
+      <c r="H4" t="n">
+        <v>22.3109710150348</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-2.728175740833712</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-12.04317274164832</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.529162567745006</v>
+      </c>
+      <c r="L4" t="n">
+        <v>15.77010941505432</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1995</v>
+        <v>1963</v>
       </c>
       <c r="B5" t="n">
-        <v>2.927858784337561</v>
+        <v>10.66246506659041</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0086380418832</v>
+        <v>29.95353398112397</v>
       </c>
       <c r="D5" t="n">
-        <v>1.638646633794471</v>
+        <v>-3.713091007831708</v>
       </c>
       <c r="E5" t="n">
-        <v>-1.051676426943166</v>
+        <v>-6.619293583229076</v>
       </c>
       <c r="F5" t="n">
-        <v>4.523467033072066</v>
+        <v>30.28361445665359</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10.08502655826333</v>
+      </c>
+      <c r="H5" t="n">
+        <v>28.33136463537102</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-3.51200413725773</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-12.08501115616109</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-1.393737462944404</v>
+      </c>
+      <c r="L5" t="n">
+        <v>21.42563843727112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1996</v>
+        <v>1964</v>
       </c>
       <c r="B6" t="n">
-        <v>2.90849236646695</v>
+        <v>13.12120457073863</v>
       </c>
       <c r="C6" t="n">
-        <v>1.237634337645746</v>
+        <v>35.85080324176099</v>
       </c>
       <c r="D6" t="n">
-        <v>2.086733605704967</v>
+        <v>-4.475989753468895</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.137743502095656</v>
+        <v>-7.396313555017661</v>
       </c>
       <c r="F6" t="n">
-        <v>5.095116807722007</v>
+        <v>37.09970450401306</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12.3824108185826</v>
+      </c>
+      <c r="H6" t="n">
+        <v>33.83221193773886</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-4.223967673731508</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-8.193323856318347</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-6.582795513075803</v>
+      </c>
+      <c r="L6" t="n">
+        <v>27.2145357131958</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1997</v>
+        <v>1965</v>
       </c>
       <c r="B7" t="n">
-        <v>4.057863805482786</v>
+        <v>15.47219529006907</v>
       </c>
       <c r="C7" t="n">
-        <v>1.411155077245218</v>
+        <v>41.21975235124386</v>
       </c>
       <c r="D7" t="n">
-        <v>2.415548385957253</v>
+        <v>-5.15119808231933</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.447178731530483</v>
+        <v>-7.923723229953072</v>
       </c>
       <c r="F7" t="n">
-        <v>5.437388537154774</v>
+        <v>43.61702632904053</v>
+      </c>
+      <c r="G7" t="n">
+        <v>14.59355353798953</v>
+      </c>
+      <c r="H7" t="n">
+        <v>38.8789471360054</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-4.858669606333579</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-8.311281322075134</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-7.202028896358314</v>
+      </c>
+      <c r="L7" t="n">
+        <v>33.10052084922791</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1998</v>
+        <v>1966</v>
       </c>
       <c r="B8" t="n">
-        <v>4.524356549959569</v>
+        <v>17.70799266274854</v>
       </c>
       <c r="C8" t="n">
-        <v>1.924516368987691</v>
+        <v>46.09855780478731</v>
       </c>
       <c r="D8" t="n">
-        <v>3.146254707872744</v>
+        <v>-5.731748817154248</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.931751679269328</v>
+        <v>-8.236616041994616</v>
       </c>
       <c r="F8" t="n">
-        <v>6.663375947550676</v>
+        <v>49.83818560838699</v>
+      </c>
+      <c r="G8" t="n">
+        <v>16.71734054847584</v>
+      </c>
+      <c r="H8" t="n">
+        <v>43.51963005029914</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-5.411093100137896</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-5.171464322903</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-10.60487122550825</v>
+      </c>
+      <c r="L8" t="n">
+        <v>39.04954195022583</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1999</v>
+        <v>1967</v>
       </c>
       <c r="B9" t="n">
-        <v>4.305335242314772</v>
+        <v>19.82318310373862</v>
       </c>
       <c r="C9" t="n">
-        <v>2.540966127302716</v>
+        <v>50.52072961031287</v>
       </c>
       <c r="D9" t="n">
-        <v>4.101731825163949</v>
+        <v>-6.212502895641747</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.072113770118313</v>
+        <v>-8.365034038304149</v>
       </c>
       <c r="F9" t="n">
-        <v>7.875919424663124</v>
+        <v>55.76637578010559</v>
+      </c>
+      <c r="G9" t="n">
+        <v>18.75191837698277</v>
+      </c>
+      <c r="H9" t="n">
+        <v>47.79053863551978</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-5.876772998876862</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-6.634700818295123</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-9.001206383730835</v>
+      </c>
+      <c r="L9" t="n">
+        <v>45.02977681159973</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2000</v>
+        <v>1968</v>
       </c>
       <c r="B10" t="n">
-        <v>4.069052712510547</v>
+        <v>21.81403671758004</v>
       </c>
       <c r="C10" t="n">
-        <v>3.34634948185565</v>
+        <v>54.5164815714009</v>
       </c>
       <c r="D10" t="n">
-        <v>5.400798558120081</v>
+        <v>-6.589966680374216</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.876202316501685</v>
+        <v>-8.335174637838755</v>
       </c>
       <c r="F10" t="n">
-        <v>9.939998435984592</v>
+        <v>61.40537697076797</v>
+      </c>
+      <c r="G10" t="n">
+        <v>20.69503881460975</v>
+      </c>
+      <c r="H10" t="n">
+        <v>51.71994146534372</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-6.251920174289443</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-14.10077749305779</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1.050647309108927</v>
+      </c>
+      <c r="L10" t="n">
+        <v>51.01163530349731</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2001</v>
+        <v>1969</v>
       </c>
       <c r="B11" t="n">
-        <v>4.326853348457012</v>
+        <v>23.67823699386431</v>
       </c>
       <c r="C11" t="n">
-        <v>4.189560203751294</v>
+        <v>58.11366103734048</v>
       </c>
       <c r="D11" t="n">
-        <v>6.706362861437633</v>
+        <v>-6.862121878992839</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.362427778571765</v>
+        <v>-8.170218785840795</v>
       </c>
       <c r="F11" t="n">
-        <v>12.86034863507417</v>
+        <v>66.75955736637115</v>
+      </c>
+      <c r="G11" t="n">
+        <v>22.54432173840143</v>
+      </c>
+      <c r="H11" t="n">
+        <v>55.33068497294368</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-6.533505154468463</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-17.65367011789323</v>
+      </c>
+      <c r="K11" t="n">
+        <v>3.279922686611684</v>
+      </c>
+      <c r="L11" t="n">
+        <v>56.96775412559509</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2002</v>
+        <v>1970</v>
       </c>
       <c r="B12" t="n">
-        <v>4.797652379201252</v>
+        <v>25.41466571329314</v>
       </c>
       <c r="C12" t="n">
-        <v>5.168869811867041</v>
+        <v>61.33839707871358</v>
       </c>
       <c r="D12" t="n">
-        <v>7.739416977617052</v>
+        <v>-7.028263776347697</v>
       </c>
       <c r="E12" t="n">
-        <v>-1.747742485710104</v>
+        <v>-7.890927055019073</v>
       </c>
       <c r="F12" t="n">
-        <v>15.95819668297524</v>
+        <v>71.83387196063995</v>
+      </c>
+      <c r="G12" t="n">
+        <v>24.29745494400631</v>
+      </c>
+      <c r="H12" t="n">
+        <v>58.6420044304606</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-6.719306260679208</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-11.71180985000244</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-1.635340019385231</v>
+      </c>
+      <c r="L12" t="n">
+        <v>62.87300324440002</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2003</v>
+        <v>1971</v>
       </c>
       <c r="B13" t="n">
-        <v>5.563161039935872</v>
+        <v>27.02323036184836</v>
       </c>
       <c r="C13" t="n">
-        <v>5.255116806724629</v>
+        <v>64.21555839472347</v>
       </c>
       <c r="D13" t="n">
-        <v>7.793222553393603</v>
+        <v>-7.08884862380919</v>
       </c>
       <c r="E13" t="n">
-        <v>-1.521306914527606</v>
+        <v>-7.516077816154219</v>
       </c>
       <c r="F13" t="n">
-        <v>17.0901934855265</v>
+        <v>76.63386231660843</v>
+      </c>
+      <c r="G13" t="n">
+        <v>25.95234446962981</v>
+      </c>
+      <c r="H13" t="n">
+        <v>61.67080210078565</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-6.807929285829981</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-13.65893444570869</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.548197332326826</v>
+      </c>
+      <c r="L13" t="n">
+        <v>68.70448017120361</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2004</v>
+        <v>1972</v>
       </c>
       <c r="B14" t="n">
-        <v>5.323155963463688</v>
+        <v>28.50472331395008</v>
       </c>
       <c r="C14" t="n">
-        <v>5.374479092076554</v>
+        <v>66.7690783450869</v>
       </c>
       <c r="D14" t="n">
-        <v>8.578211271316528</v>
+        <v>-7.045346159560669</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.265029251032038</v>
+        <v>-7.062797442740322</v>
       </c>
       <c r="F14" t="n">
-        <v>18.01081707582473</v>
+        <v>81.16565805673599</v>
+      </c>
+      <c r="G14" t="n">
+        <v>27.50722739444926</v>
+      </c>
+      <c r="H14" t="n">
+        <v>64.43255739504981</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-6.798800912717553</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-7.136389072964776</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-3.563079834944676</v>
+      </c>
+      <c r="L14" t="n">
+        <v>74.44151496887207</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2005</v>
+        <v>1973</v>
       </c>
       <c r="B15" t="n">
-        <v>5.412500118783438</v>
+        <v>29.8607052777427</v>
       </c>
       <c r="C15" t="n">
-        <v>5.831499880714054</v>
+        <v>69.02218743856436</v>
       </c>
       <c r="D15" t="n">
-        <v>8.980668737239036</v>
+        <v>-6.900100197779203</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.068286262378203</v>
+        <v>-6.546816549690107</v>
       </c>
       <c r="F15" t="n">
-        <v>19.15638247435832</v>
+        <v>85.43597596883774</v>
+      </c>
+      <c r="G15" t="n">
+        <v>28.96075377193128</v>
+      </c>
+      <c r="H15" t="n">
+        <v>66.94197463240423</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-6.692142766583846</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-6.108594804165955</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-3.036326780622455</v>
+      </c>
+      <c r="L15" t="n">
+        <v>80.06566405296326</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2006</v>
+        <v>1974</v>
       </c>
       <c r="B16" t="n">
-        <v>6.900181259148984</v>
+        <v>31.09340785783231</v>
       </c>
       <c r="C16" t="n">
-        <v>5.696699974213906</v>
+        <v>70.99756997985759</v>
       </c>
       <c r="D16" t="n">
-        <v>8.511626123965849</v>
+        <v>-6.656195515776425</v>
       </c>
       <c r="E16" t="n">
-        <v>-1.253006444032854</v>
+        <v>-5.982662971480121</v>
       </c>
       <c r="F16" t="n">
-        <v>19.85550091329588</v>
+        <v>89.45211935043335</v>
+      </c>
+      <c r="G16" t="n">
+        <v>30.3120461043778</v>
+      </c>
+      <c r="H16" t="n">
+        <v>69.21343663480525</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-6.488928658977612</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-2.625501860007036</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-4.850337260100135</v>
+      </c>
+      <c r="L16" t="n">
+        <v>85.56071496009827</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2007</v>
+        <v>1975</v>
       </c>
       <c r="B17" t="n">
-        <v>7.07996245115241</v>
+        <v>32.20565097363226</v>
       </c>
       <c r="C17" t="n">
-        <v>5.901359758003004</v>
+        <v>72.71747930781416</v>
       </c>
       <c r="D17" t="n">
-        <v>8.662937535908885</v>
+        <v>-6.317331177193699</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.8648790333109222</v>
+        <v>-5.383819784203439</v>
       </c>
       <c r="F17" t="n">
-        <v>20.77938071175338</v>
+        <v>93.22197932004929</v>
+      </c>
+      <c r="G17" t="n">
+        <v>31.5607398441365</v>
+      </c>
+      <c r="H17" t="n">
+        <v>71.26132766061156</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-6.190827999592402</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-2.936803997128449</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-2.781746060624252</v>
+      </c>
+      <c r="L17" t="n">
+        <v>90.91268944740295</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2008</v>
+        <v>1976</v>
       </c>
       <c r="B18" t="n">
-        <v>7.193027568634641</v>
+        <v>33.20077226741804</v>
       </c>
       <c r="C18" t="n">
-        <v>6.153202877873352</v>
+        <v>74.20380672758927</v>
       </c>
       <c r="D18" t="n">
-        <v>8.927758359737245</v>
+        <v>-5.887702313787974</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.5603517671926674</v>
+        <v>-4.762842460047004</v>
       </c>
       <c r="F18" t="n">
-        <v>21.71363703905257</v>
+        <v>96.75403422117233</v>
+      </c>
+      <c r="G18" t="n">
+        <v>32.70700815622536</v>
+      </c>
+      <c r="H18" t="n">
+        <v>73.10024273875044</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-5.800140010221092</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-0.7614292659290338</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-3.135847663060898</v>
+      </c>
+      <c r="L18" t="n">
+        <v>96.10983395576477</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2009</v>
+        <v>1977</v>
       </c>
       <c r="B19" t="n">
-        <v>7.751731354409989</v>
+        <v>34.08256552897463</v>
       </c>
       <c r="C19" t="n">
-        <v>6.552186742922697</v>
+        <v>75.4781175208816</v>
       </c>
       <c r="D19" t="n">
-        <v>9.060280934474338</v>
+        <v>-5.371888711386704</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.354949141598019</v>
+        <v>-4.131444895033852</v>
       </c>
       <c r="F19" t="n">
-        <v>23.00924989020901</v>
+        <v>100.0573494434357</v>
+      </c>
+      <c r="G19" t="n">
+        <v>33.75157581675575</v>
+      </c>
+      <c r="H19" t="n">
+        <v>74.74511869848305</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-5.319720106381245</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.6424210080266849</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-2.676769608168425</v>
+      </c>
+      <c r="L19" t="n">
+        <v>101.1426258087158</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2010</v>
+        <v>1978</v>
       </c>
       <c r="B20" t="n">
-        <v>7.735840008642302</v>
+        <v>34.85522711483112</v>
       </c>
       <c r="C20" t="n">
-        <v>6.820134739501226</v>
+        <v>76.5616685062319</v>
       </c>
       <c r="D20" t="n">
-        <v>9.750520834318523</v>
+        <v>-4.774751108100355</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.04899252252981867</v>
+        <v>-3.500566792320569</v>
       </c>
       <c r="F20" t="n">
-        <v>24.25750305993223</v>
+        <v>103.1415777206421</v>
+      </c>
+      <c r="G20" t="n">
+        <v>34.69572345247781</v>
+      </c>
+      <c r="H20" t="n">
+        <v>76.21130881750022</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-4.75290100550144</v>
+      </c>
+      <c r="J20" t="n">
+        <v>8.804224115684887</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-8.954580260379982</v>
+      </c>
+      <c r="L20" t="n">
+        <v>106.0037751197815</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2011</v>
+        <v>1979</v>
       </c>
       <c r="B21" t="n">
-        <v>7.599223480906269</v>
+        <v>35.5233083131959</v>
       </c>
       <c r="C21" t="n">
-        <v>7.033282279902609</v>
+        <v>77.47540131647709</v>
       </c>
       <c r="D21" t="n">
-        <v>9.940769985566382</v>
+        <v>-4.101335960962701</v>
       </c>
       <c r="E21" t="n">
-        <v>0.357065553951343</v>
+        <v>-2.880414895574155</v>
       </c>
       <c r="F21" t="n">
-        <v>24.9303413003266</v>
+        <v>106.0169587731361</v>
+      </c>
+      <c r="G21" t="n">
+        <v>35.54128298783034</v>
+      </c>
+      <c r="H21" t="n">
+        <v>77.51460360919593</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-4.103411223176875</v>
+      </c>
+      <c r="J21" t="n">
+        <v>11.98689558311575</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-10.25115260178631</v>
+      </c>
+      <c r="L21" t="n">
+        <v>110.6882183551788</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2012</v>
+        <v>1980</v>
       </c>
       <c r="B22" t="n">
-        <v>7.14316856320882</v>
+        <v>36.09167291442412</v>
       </c>
       <c r="C22" t="n">
-        <v>7.347022511260692</v>
+        <v>78.23991896721151</v>
       </c>
       <c r="D22" t="n">
-        <v>10.46249529633845</v>
+        <v>-3.35678731937662</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8098071879972411</v>
+        <v>-2.280485135245613</v>
       </c>
       <c r="F22" t="n">
-        <v>25.7624935588052</v>
+        <v>108.6943194270134</v>
+      </c>
+      <c r="G22" t="n">
+        <v>36.2906284256927</v>
+      </c>
+      <c r="H22" t="n">
+        <v>78.67121687674987</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-3.375291624758362</v>
+      </c>
+      <c r="J22" t="n">
+        <v>6.082978953432057</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-2.476404760556565</v>
+      </c>
+      <c r="L22" t="n">
+        <v>115.1931278705597</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2013</v>
+        <v>1981</v>
       </c>
       <c r="B23" t="n">
-        <v>7.373462998092215</v>
+        <v>36.56545889134948</v>
       </c>
       <c r="C23" t="n">
-        <v>7.427653309973181</v>
+        <v>78.87544951269686</v>
       </c>
       <c r="D23" t="n">
-        <v>10.72817078894757</v>
+        <v>-2.546266874782809</v>
       </c>
       <c r="E23" t="n">
-        <v>1.308597928956196</v>
+        <v>-1.709567497910527</v>
       </c>
       <c r="F23" t="n">
-        <v>26.83788502596916</v>
+        <v>111.185074031353</v>
+      </c>
+      <c r="G23" t="n">
+        <v>36.94665876890706</v>
+      </c>
+      <c r="H23" t="n">
+        <v>79.69773679168007</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-2.572812052946176</v>
+      </c>
+      <c r="J23" t="n">
+        <v>7.341080459717278</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-1.894768268810874</v>
+      </c>
+      <c r="L23" t="n">
+        <v>119.5178956985474</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2014</v>
+        <v>1982</v>
       </c>
       <c r="B24" t="n">
-        <v>8.044192119528969</v>
+        <v>36.95004395153364</v>
       </c>
       <c r="C24" t="n">
-        <v>7.669894848537093</v>
+        <v>79.40180009844106</v>
       </c>
       <c r="D24" t="n">
-        <v>11.18866211953442</v>
+        <v>-1.674882023311786</v>
       </c>
       <c r="E24" t="n">
-        <v>1.420231633699963</v>
+        <v>-1.175737508840648</v>
       </c>
       <c r="F24" t="n">
-        <v>28.32298072130044</v>
+        <v>113.5012245178223</v>
+      </c>
+      <c r="G24" t="n">
+        <v>37.51278097172949</v>
+      </c>
+      <c r="H24" t="n">
+        <v>80.61106340660362</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-1.700389925825092</v>
+      </c>
+      <c r="J24" t="n">
+        <v>7.279113576748939</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-0.03841230759252845</v>
+      </c>
+      <c r="L24" t="n">
+        <v>123.6641557216644</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2015</v>
+        <v>1983</v>
       </c>
       <c r="B25" t="n">
-        <v>8.303368061852378</v>
+        <v>37.25101350402231</v>
       </c>
       <c r="C25" t="n">
-        <v>8.040990247248489</v>
+        <v>79.83830216533475</v>
       </c>
       <c r="D25" t="n">
-        <v>11.80631458806267</v>
+        <v>-0.7476201626578376</v>
       </c>
       <c r="E25" t="n">
-        <v>1.44543867457064</v>
+        <v>-0.6863367749525509</v>
       </c>
       <c r="F25" t="n">
-        <v>29.59611157173418</v>
+        <v>115.6553587317467</v>
+      </c>
+      <c r="G25" t="n">
+        <v>37.99288479471285</v>
+      </c>
+      <c r="H25" t="n">
+        <v>81.42831915286028</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-0.7625093665437226</v>
+      </c>
+      <c r="J25" t="n">
+        <v>8.703718248815735</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.2733501000712391</v>
+      </c>
+      <c r="L25" t="n">
+        <v>127.6357629299164</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2016</v>
+        <v>1984</v>
       </c>
       <c r="B26" t="n">
-        <v>8.756504070176302</v>
+        <v>37.47413213812481</v>
       </c>
       <c r="C26" t="n">
-        <v>8.306097409201941</v>
+        <v>80.20374879690084</v>
       </c>
       <c r="D26" t="n">
-        <v>12.36811995721189</v>
+        <v>0.2307093098416394</v>
       </c>
       <c r="E26" t="n">
-        <v>1.735306652177753</v>
+        <v>-0.2479367729205748</v>
       </c>
       <c r="F26" t="n">
-        <v>31.16602808876789</v>
+        <v>117.6606534719467</v>
+      </c>
+      <c r="G26" t="n">
+        <v>38.39131892043434</v>
+      </c>
+      <c r="H26" t="n">
+        <v>82.16675138271263</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.2363559657471734</v>
+      </c>
+      <c r="J26" t="n">
+        <v>10.07696011453443</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.5674213424777861</v>
+      </c>
+      <c r="L26" t="n">
+        <v>131.4388077259064</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2017</v>
+        <v>1985</v>
       </c>
       <c r="B27" t="n">
-        <v>8.779956555221373</v>
+        <v>37.6253166397716</v>
       </c>
       <c r="C27" t="n">
-        <v>8.684311652648006</v>
+        <v>80.51632838374668</v>
       </c>
       <c r="D27" t="n">
-        <v>13.17757904132317</v>
+        <v>1.255526336255743</v>
       </c>
       <c r="E27" t="n">
-        <v>1.708467851990635</v>
+        <v>0.1336999719177214</v>
       </c>
       <c r="F27" t="n">
-        <v>32.35031510118318</v>
+        <v>119.5308713316917</v>
+      </c>
+      <c r="G27" t="n">
+        <v>38.71286252940088</v>
+      </c>
+      <c r="H27" t="n">
+        <v>82.84362313637675</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1.291816861579134</v>
+      </c>
+      <c r="J27" t="n">
+        <v>12.20704447342378</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.02625986414867043</v>
+      </c>
+      <c r="L27" t="n">
+        <v>135.0816068649292</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2018</v>
+        <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>8.885188202699942</v>
+        <v>37.71061179496347</v>
       </c>
       <c r="C28" t="n">
-        <v>9.199651554215457</v>
+        <v>80.79355754137686</v>
       </c>
       <c r="D28" t="n">
-        <v>14.10949466693122</v>
+        <v>2.322525694821369</v>
       </c>
       <c r="E28" t="n">
-        <v>1.271698067854624</v>
+        <v>0.4536679921194064</v>
       </c>
       <c r="F28" t="n">
-        <v>33.46603249170124</v>
+        <v>121.2803630232811</v>
+      </c>
+      <c r="G28" t="n">
+        <v>38.96269685331959</v>
+      </c>
+      <c r="H28" t="n">
+        <v>83.47610235817838</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2.399639259988254</v>
+      </c>
+      <c r="J28" t="n">
+        <v>10.65317729503711</v>
+      </c>
+      <c r="K28" t="n">
+        <v>3.083091979982411</v>
+      </c>
+      <c r="L28" t="n">
+        <v>138.5747077465057</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2019</v>
+        <v>1987</v>
       </c>
       <c r="B29" t="n">
-        <v>9.116753227883414</v>
+        <v>37.7361678445486</v>
       </c>
       <c r="C29" t="n">
-        <v>9.580613991652431</v>
+        <v>81.05221390576605</v>
       </c>
       <c r="D29" t="n">
-        <v>14.44658938758577</v>
+        <v>3.427716470148489</v>
       </c>
       <c r="E29" t="n">
-        <v>1.940871568303589</v>
+        <v>0.7079673098370094</v>
       </c>
       <c r="F29" t="n">
-        <v>35.0848281754252</v>
+        <v>122.9240655303001</v>
+      </c>
+      <c r="G29" t="n">
+        <v>39.14637564117176</v>
+      </c>
+      <c r="H29" t="n">
+        <v>84.08115061323279</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3.555810889028792</v>
+      </c>
+      <c r="J29" t="n">
+        <v>15.65577074704103</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-0.5082175687428219</v>
+      </c>
+      <c r="L29" t="n">
+        <v>141.9308903217316</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2020</v>
+        <v>1988</v>
       </c>
       <c r="B30" t="n">
-        <v>12.33872973304803</v>
+        <v>37.70821977079174</v>
       </c>
       <c r="C30" t="n">
-        <v>9.449171668234293</v>
+        <v>81.30826869889769</v>
       </c>
       <c r="D30" t="n">
-        <v>12.93334684681425</v>
+        <v>4.567456964033441</v>
       </c>
       <c r="E30" t="n">
-        <v>4.452458262130937</v>
+        <v>0.8935583428274256</v>
       </c>
       <c r="F30" t="n">
-        <v>39.1737065102275</v>
+        <v>124.4775037765503</v>
+      </c>
+      <c r="G30" t="n">
+        <v>39.26979423973023</v>
+      </c>
+      <c r="H30" t="n">
+        <v>84.67541032705108</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4.756604694325779</v>
+      </c>
+      <c r="J30" t="n">
+        <v>16.74875078235079</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-0.2853962880410066</v>
+      </c>
+      <c r="L30" t="n">
+        <v>145.1651637554169</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2021</v>
+        <v>1989</v>
       </c>
       <c r="B31" t="n">
-        <v>13.50179316350726</v>
+        <v>37.63306922278267</v>
       </c>
       <c r="C31" t="n">
-        <v>9.986127450817863</v>
+        <v>81.57682547474236</v>
       </c>
       <c r="D31" t="n">
-        <v>13.85799485155957</v>
+        <v>5.738483518576856</v>
       </c>
       <c r="E31" t="n">
-        <v>4.317345976686402</v>
+        <v>1.008412171528576</v>
       </c>
       <c r="F31" t="n">
-        <v>41.6632614425711</v>
+        <v>125.9567903876305</v>
+      </c>
+      <c r="G31" t="n">
+        <v>39.33915982804758</v>
+      </c>
+      <c r="H31" t="n">
+        <v>85.27510091238689</v>
+      </c>
+      <c r="I31" t="n">
+        <v>5.998636969297387</v>
+      </c>
+      <c r="J31" t="n">
+        <v>17.87438333782273</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-0.1925172440725333</v>
+      </c>
+      <c r="L31" t="n">
+        <v>148.2947638034821</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2022</v>
+        <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>13.30293239543494</v>
+        <v>37.51706709036858</v>
       </c>
       <c r="C32" t="n">
-        <v>10.20360568097759</v>
+        <v>81.87206625962428</v>
       </c>
       <c r="D32" t="n">
-        <v>14.22861184065802</v>
+        <v>6.937936218857907</v>
       </c>
       <c r="E32" t="n">
-        <v>3.975135474266034</v>
+        <v>1.051553976319056</v>
       </c>
       <c r="F32" t="n">
-        <v>41.71028539133658</v>
+        <v>127.3786235451698</v>
+      </c>
+      <c r="G32" t="n">
+        <v>39.36096207950109</v>
+      </c>
+      <c r="H32" t="n">
+        <v>85.89592804931095</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7.278923050212781</v>
+      </c>
+      <c r="J32" t="n">
+        <v>17.15004722638063</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1.653299560109701</v>
+      </c>
+      <c r="L32" t="n">
+        <v>151.3391599655151</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1991</v>
+      </c>
+      <c r="B33" t="n">
+        <v>37.36659926070372</v>
+      </c>
+      <c r="C33" t="n">
+        <v>82.2072009042118</v>
+      </c>
+      <c r="D33" t="n">
+        <v>8.163380236682379</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1.023109803880779</v>
+      </c>
+      <c r="F33" t="n">
+        <v>128.7602902054787</v>
+      </c>
+      <c r="G33" t="n">
+        <v>39.34194435857267</v>
+      </c>
+      <c r="H33" t="n">
+        <v>86.55299620077325</v>
+      </c>
+      <c r="I33" t="n">
+        <v>8.594928556615498</v>
+      </c>
+      <c r="J33" t="n">
+        <v>14.41333063084411</v>
+      </c>
+      <c r="K33" t="n">
+        <v>5.416849539083154</v>
+      </c>
+      <c r="L33" t="n">
+        <v>154.3200492858887</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1992</v>
+      </c>
+      <c r="B34" t="n">
+        <v>37.18807371396998</v>
+      </c>
+      <c r="C34" t="n">
+        <v>82.59442842984855</v>
+      </c>
+      <c r="D34" t="n">
+        <v>9.412823540830098</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.9243387459696564</v>
+      </c>
+      <c r="F34" t="n">
+        <v>130.1196644306183</v>
+      </c>
+      <c r="G34" t="n">
+        <v>39.28907739495488</v>
+      </c>
+      <c r="H34" t="n">
+        <v>87.26074160042742</v>
+      </c>
+      <c r="I34" t="n">
+        <v>9.944617068503899</v>
+      </c>
+      <c r="J34" t="n">
+        <v>13.18193450379734</v>
+      </c>
+      <c r="K34" t="n">
+        <v>7.584990792866384</v>
+      </c>
+      <c r="L34" t="n">
+        <v>157.2613613605499</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1993</v>
+      </c>
+      <c r="B35" t="n">
+        <v>36.98790954798916</v>
+      </c>
+      <c r="C35" t="n">
+        <v>83.04491049241632</v>
+      </c>
+      <c r="D35" t="n">
+        <v>10.6847322135076</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.7576535847671835</v>
+      </c>
+      <c r="F35" t="n">
+        <v>131.4752058386803</v>
+      </c>
+      <c r="G35" t="n">
+        <v>39.20953391717236</v>
+      </c>
+      <c r="H35" t="n">
+        <v>88.03288086276724</v>
+      </c>
+      <c r="I35" t="n">
+        <v>11.32649493418603</v>
+      </c>
+      <c r="J35" t="n">
+        <v>10.53469710115306</v>
+      </c>
+      <c r="K35" t="n">
+        <v>11.08564651495203</v>
+      </c>
+      <c r="L35" t="n">
+        <v>160.1892533302307</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1994</v>
+      </c>
+      <c r="B36" t="n">
+        <v>36.77252929020101</v>
+      </c>
+      <c r="C36" t="n">
+        <v>83.56875065539455</v>
+      </c>
+      <c r="D36" t="n">
+        <v>11.97804226748578</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.5266417418441804</v>
+      </c>
+      <c r="F36" t="n">
+        <v>132.8459639549255</v>
+      </c>
+      <c r="G36" t="n">
+        <v>39.11066735850467</v>
+      </c>
+      <c r="H36" t="n">
+        <v>88.88237147505414</v>
+      </c>
+      <c r="I36" t="n">
+        <v>12.73965201122516</v>
+      </c>
+      <c r="J36" t="n">
+        <v>14.38907876825045</v>
+      </c>
+      <c r="K36" t="n">
+        <v>8.010344797365965</v>
+      </c>
+      <c r="L36" t="n">
+        <v>163.1321144104004</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36.54835200856295</v>
+      </c>
+      <c r="C37" t="n">
+        <v>84.17498847128414</v>
+      </c>
+      <c r="D37" t="n">
+        <v>13.29216992967017</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.2360624974537231</v>
+      </c>
+      <c r="F37" t="n">
+        <v>134.251572906971</v>
+      </c>
+      <c r="G37" t="n">
+        <v>38.99999225307309</v>
+      </c>
+      <c r="H37" t="n">
+        <v>89.82139324677243</v>
+      </c>
+      <c r="I37" t="n">
+        <v>14.183800248017</v>
+      </c>
+      <c r="J37" t="n">
+        <v>16.11645711097677</v>
+      </c>
+      <c r="K37" t="n">
+        <v>6.998918502473568</v>
+      </c>
+      <c r="L37" t="n">
+        <v>166.1205613613129</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B38" t="n">
+        <v>36.32179043256151</v>
+      </c>
+      <c r="C38" t="n">
+        <v>84.87160657781986</v>
+      </c>
+      <c r="D38" t="n">
+        <v>14.62701961362257</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.1081612057033112</v>
+      </c>
+      <c r="F38" t="n">
+        <v>135.7122554183006</v>
+      </c>
+      <c r="G38" t="n">
+        <v>38.88516981348979</v>
+      </c>
+      <c r="H38" t="n">
+        <v>90.86134782506865</v>
+      </c>
+      <c r="I38" t="n">
+        <v>15.65930904747109</v>
+      </c>
+      <c r="J38" t="n">
+        <v>19.29991270224928</v>
+      </c>
+      <c r="K38" t="n">
+        <v>4.481702914425053</v>
+      </c>
+      <c r="L38" t="n">
+        <v>169.1874423027039</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B39" t="n">
+        <v>36.09924980912688</v>
+      </c>
+      <c r="C39" t="n">
+        <v>85.6655400753896</v>
+      </c>
+      <c r="D39" t="n">
+        <v>15.98299062570808</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.4989588344471301</v>
+      </c>
+      <c r="F39" t="n">
+        <v>137.2488216757774</v>
+      </c>
+      <c r="G39" t="n">
+        <v>38.77399697719627</v>
+      </c>
+      <c r="H39" t="n">
+        <v>92.01286479624437</v>
+      </c>
+      <c r="I39" t="n">
+        <v>17.16723847405489</v>
+      </c>
+      <c r="J39" t="n">
+        <v>21.28907576483529</v>
+      </c>
+      <c r="K39" t="n">
+        <v>3.124660224622911</v>
+      </c>
+      <c r="L39" t="n">
+        <v>172.3678362369537</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B40" t="n">
+        <v>35.88712985688779</v>
+      </c>
+      <c r="C40" t="n">
+        <v>86.56270617655886</v>
+      </c>
+      <c r="D40" t="n">
+        <v>17.36098196906059</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-0.9281500437708203</v>
+      </c>
+      <c r="F40" t="n">
+        <v>138.8826679587364</v>
+      </c>
+      <c r="G40" t="n">
+        <v>38.67440060583528</v>
+      </c>
+      <c r="H40" t="n">
+        <v>93.28583226208926</v>
+      </c>
+      <c r="I40" t="n">
+        <v>18.7093694664263</v>
+      </c>
+      <c r="J40" t="n">
+        <v>20.17153856923074</v>
+      </c>
+      <c r="K40" t="n">
+        <v>4.857910953413057</v>
+      </c>
+      <c r="L40" t="n">
+        <v>175.6990518569946</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B41" t="n">
+        <v>35.6918297195195</v>
+      </c>
+      <c r="C41" t="n">
+        <v>87.5680304102724</v>
+      </c>
+      <c r="D41" t="n">
+        <v>18.76239679410936</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-1.386478556381874</v>
+      </c>
+      <c r="F41" t="n">
+        <v>140.6357783675194</v>
+      </c>
+      <c r="G41" t="n">
+        <v>38.59443687368142</v>
+      </c>
+      <c r="H41" t="n">
+        <v>94.68942467731159</v>
+      </c>
+      <c r="I41" t="n">
+        <v>20.2882324711193</v>
+      </c>
+      <c r="J41" t="n">
+        <v>21.7276702831632</v>
+      </c>
+      <c r="K41" t="n">
+        <v>3.920862048942016</v>
+      </c>
+      <c r="L41" t="n">
+        <v>179.2206263542175</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B42" t="n">
+        <v>35.51975583605706</v>
+      </c>
+      <c r="C42" t="n">
+        <v>88.68548387644834</v>
+      </c>
+      <c r="D42" t="n">
+        <v>20.18914540424724</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-1.863660233673116</v>
+      </c>
+      <c r="F42" t="n">
+        <v>142.5307248830795</v>
+      </c>
+      <c r="G42" t="n">
+        <v>38.54229680382326</v>
+      </c>
+      <c r="H42" t="n">
+        <v>96.23214352973977</v>
+      </c>
+      <c r="I42" t="n">
+        <v>21.90713353936219</v>
+      </c>
+      <c r="J42" t="n">
+        <v>26.62762764498752</v>
+      </c>
+      <c r="K42" t="n">
+        <v>-0.3348749073475474</v>
+      </c>
+      <c r="L42" t="n">
+        <v>182.9743266105652</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B43" t="n">
+        <v>35.37733296577623</v>
+      </c>
+      <c r="C43" t="n">
+        <v>89.91812070085572</v>
+      </c>
+      <c r="D43" t="n">
+        <v>21.64364857815559</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-2.348436606340741</v>
+      </c>
+      <c r="F43" t="n">
+        <v>144.5906656384468</v>
+      </c>
+      <c r="G43" t="n">
+        <v>38.52631843076895</v>
+      </c>
+      <c r="H43" t="n">
+        <v>97.92185731379864</v>
+      </c>
+      <c r="I43" t="n">
+        <v>23.57017975132106</v>
+      </c>
+      <c r="J43" t="n">
+        <v>22.51197264230167</v>
+      </c>
+      <c r="K43" t="n">
+        <v>4.473823206108992</v>
+      </c>
+      <c r="L43" t="n">
+        <v>187.0041513442993</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B44" t="n">
+        <v>35.2710187148443</v>
+      </c>
+      <c r="C44" t="n">
+        <v>91.26811576546687</v>
+      </c>
+      <c r="D44" t="n">
+        <v>23.12883915031966</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-2.828627281391491</v>
+      </c>
+      <c r="F44" t="n">
+        <v>146.8393463492393</v>
+      </c>
+      <c r="G44" t="n">
+        <v>38.55500553267243</v>
+      </c>
+      <c r="H44" t="n">
+        <v>99.76583712375761</v>
+      </c>
+      <c r="I44" t="n">
+        <v>25.2823012744332</v>
+      </c>
+      <c r="J44" t="n">
+        <v>27.73643980695459</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.01674689534563356</v>
+      </c>
+      <c r="L44" t="n">
+        <v>191.3563306331635</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B45" t="n">
+        <v>35.20732046136307</v>
+      </c>
+      <c r="C45" t="n">
+        <v>92.73679486039016</v>
+      </c>
+      <c r="D45" t="n">
+        <v>24.64816486405611</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-3.291180468192309</v>
+      </c>
+      <c r="F45" t="n">
+        <v>149.301099717617</v>
+      </c>
+      <c r="G45" t="n">
+        <v>38.63705233192732</v>
+      </c>
+      <c r="H45" t="n">
+        <v>101.770778041692</v>
+      </c>
+      <c r="I45" t="n">
+        <v>27.04927336869073</v>
+      </c>
+      <c r="J45" t="n">
+        <v>28.58353428039268</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.03868216963427429</v>
+      </c>
+      <c r="L45" t="n">
+        <v>196.079320192337</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B46" t="n">
+        <v>35.1928167723481</v>
+      </c>
+      <c r="C46" t="n">
+        <v>94.32466335839256</v>
+      </c>
+      <c r="D46" t="n">
+        <v>26.20559042371366</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-3.722223870475283</v>
+      </c>
+      <c r="F46" t="n">
+        <v>152.000846683979</v>
+      </c>
+      <c r="G46" t="n">
+        <v>38.78137783272454</v>
+      </c>
+      <c r="H46" t="n">
+        <v>103.942814021087</v>
+      </c>
+      <c r="I46" t="n">
+        <v>28.87773690084937</v>
+      </c>
+      <c r="J46" t="n">
+        <v>33.18634592045535</v>
+      </c>
+      <c r="K46" t="n">
+        <v>-3.564465671286293</v>
+      </c>
+      <c r="L46" t="n">
+        <v>201.22380900383</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B47" t="n">
+        <v>35.23418059817782</v>
+      </c>
+      <c r="C47" t="n">
+        <v>96.03141448261972</v>
+      </c>
+      <c r="D47" t="n">
+        <v>27.80559985299436</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-4.107100891013893</v>
+      </c>
+      <c r="F47" t="n">
+        <v>154.964094042778</v>
+      </c>
+      <c r="G47" t="n">
+        <v>38.99716536776136</v>
+      </c>
+      <c r="H47" t="n">
+        <v>106.2874994536535</v>
+      </c>
+      <c r="I47" t="n">
+        <v>30.77521762129754</v>
+      </c>
+      <c r="J47" t="n">
+        <v>37.1998620319838</v>
+      </c>
+      <c r="K47" t="n">
+        <v>-6.417030641841002</v>
+      </c>
+      <c r="L47" t="n">
+        <v>206.8427138328552</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B48" t="n">
+        <v>35.33820622605195</v>
+      </c>
+      <c r="C48" t="n">
+        <v>97.85593171878809</v>
+      </c>
+      <c r="D48" t="n">
+        <v>29.45319967817029</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-4.430401451955476</v>
+      </c>
+      <c r="F48" t="n">
+        <v>158.2169361710548</v>
+      </c>
+      <c r="G48" t="n">
+        <v>39.2939107908675</v>
+      </c>
+      <c r="H48" t="n">
+        <v>108.80977451766</v>
+      </c>
+      <c r="I48" t="n">
+        <v>32.75014564283192</v>
+      </c>
+      <c r="J48" t="n">
+        <v>39.69275712450992</v>
+      </c>
+      <c r="K48" t="n">
+        <v>-7.555404318087341</v>
+      </c>
+      <c r="L48" t="n">
+        <v>212.991183757782</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B49" t="n">
+        <v>35.51183888957578</v>
+      </c>
+      <c r="C49" t="n">
+        <v>99.79626703674111</v>
+      </c>
+      <c r="D49" t="n">
+        <v>31.15392217729106</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-4.675972300309013</v>
+      </c>
+      <c r="F49" t="n">
+        <v>161.786055803299</v>
+      </c>
+      <c r="G49" t="n">
+        <v>39.68147723019083</v>
+      </c>
+      <c r="H49" t="n">
+        <v>111.5138900688956</v>
+      </c>
+      <c r="I49" t="n">
+        <v>34.81187379097394</v>
+      </c>
+      <c r="J49" t="n">
+        <v>42.52924426710228</v>
+      </c>
+      <c r="K49" t="n">
+        <v>-8.809888048050126</v>
+      </c>
+      <c r="L49" t="n">
+        <v>219.7265973091125</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B50" t="n">
+        <v>35.76220646011388</v>
+      </c>
+      <c r="C50" t="n">
+        <v>101.8495973124623</v>
+      </c>
+      <c r="D50" t="n">
+        <v>32.91382934246298</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-4.826911885009089</v>
+      </c>
+      <c r="F50" t="n">
+        <v>165.6987212300301</v>
+      </c>
+      <c r="G50" t="n">
+        <v>40.1701566951564</v>
+      </c>
+      <c r="H50" t="n">
+        <v>114.4032957793948</v>
+      </c>
+      <c r="I50" t="n">
+        <v>36.9706965256462</v>
+      </c>
+      <c r="J50" t="n">
+        <v>41.26485909291869</v>
+      </c>
+      <c r="K50" t="n">
+        <v>-5.700446577307943</v>
+      </c>
+      <c r="L50" t="n">
+        <v>227.1085615158081</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B51" t="n">
+        <v>36.09665393760542</v>
+      </c>
+      <c r="C51" t="n">
+        <v>104.0121596041666</v>
+      </c>
+      <c r="D51" t="n">
+        <v>34.73951859192005</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-4.865542855661687</v>
+      </c>
+      <c r="F51" t="n">
+        <v>169.9827892780304</v>
+      </c>
+      <c r="G51" t="n">
+        <v>40.77073842495055</v>
+      </c>
+      <c r="H51" t="n">
+        <v>117.4804888997698</v>
+      </c>
+      <c r="I51" t="n">
+        <v>39.23787030144425</v>
+      </c>
+      <c r="J51" t="n">
+        <v>43.50071802861427</v>
+      </c>
+      <c r="K51" t="n">
+        <v>-5.790901603722958</v>
+      </c>
+      <c r="L51" t="n">
+        <v>235.1989140510559</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B52" t="n">
+        <v>36.52277887251248</v>
+      </c>
+      <c r="C52" t="n">
+        <v>106.2791537116574</v>
+      </c>
+      <c r="D52" t="n">
+        <v>36.63812826787804</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-4.773358104702936</v>
+      </c>
+      <c r="F52" t="n">
+        <v>174.666702747345</v>
+      </c>
+      <c r="G52" t="n">
+        <v>41.49458234716073</v>
+      </c>
+      <c r="H52" t="n">
+        <v>120.7468114862955</v>
+      </c>
+      <c r="I52" t="n">
+        <v>41.62563412176416</v>
+      </c>
+      <c r="J52" t="n">
+        <v>47.79824615604387</v>
+      </c>
+      <c r="K52" t="n">
+        <v>-7.603550163739243</v>
+      </c>
+      <c r="L52" t="n">
+        <v>244.061723947525</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B53" t="n">
+        <v>37.04846928523311</v>
+      </c>
+      <c r="C53" t="n">
+        <v>108.6446134231781</v>
+      </c>
+      <c r="D53" t="n">
+        <v>38.61734572915741</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-4.530935642101255</v>
+      </c>
+      <c r="F53" t="n">
+        <v>179.7794927954674</v>
+      </c>
+      <c r="G53" t="n">
+        <v>42.35369782390887</v>
+      </c>
+      <c r="H53" t="n">
+        <v>124.2021928542878</v>
+      </c>
+      <c r="I53" t="n">
+        <v>44.14723262064886</v>
+      </c>
+      <c r="J53" t="n">
+        <v>48.23811911783717</v>
+      </c>
+      <c r="K53" t="n">
+        <v>-5.177955826106512</v>
+      </c>
+      <c r="L53" t="n">
+        <v>253.7632865905762</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B54" t="n">
+        <v>37.68194098452431</v>
+      </c>
+      <c r="C54" t="n">
+        <v>111.101244405763</v>
+      </c>
+      <c r="D54" t="n">
+        <v>40.68541605311608</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-4.11782411538902</v>
+      </c>
+      <c r="F54" t="n">
+        <v>185.3507773280144</v>
+      </c>
+      <c r="G54" t="n">
+        <v>43.36082611602388</v>
+      </c>
+      <c r="H54" t="n">
+        <v>127.8448406341554</v>
+      </c>
+      <c r="I54" t="n">
+        <v>46.8169421437653</v>
+      </c>
+      <c r="J54" t="n">
+        <v>51.2475175541022</v>
+      </c>
+      <c r="K54" t="n">
+        <v>-4.897993431460492</v>
+      </c>
+      <c r="L54" t="n">
+        <v>264.3721330165863</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B55" t="n">
+        <v>38.43177634961764</v>
+      </c>
+      <c r="C55" t="n">
+        <v>113.6402216585881</v>
+      </c>
+      <c r="D55" t="n">
+        <v>42.85115224128357</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-3.512389131554158</v>
+      </c>
+      <c r="F55" t="n">
+        <v>191.4107611179352</v>
+      </c>
+      <c r="G55" t="n">
+        <v>44.52952543831268</v>
+      </c>
+      <c r="H55" t="n">
+        <v>131.670862546845</v>
+      </c>
+      <c r="I55" t="n">
+        <v>49.65009830486878</v>
+      </c>
+      <c r="J55" t="n">
+        <v>53.8084524036118</v>
+      </c>
+      <c r="K55" t="n">
+        <v>-3.699918079014267</v>
+      </c>
+      <c r="L55" t="n">
+        <v>275.959020614624</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B56" t="n">
+        <v>39.30696215735033</v>
+      </c>
+      <c r="C56" t="n">
+        <v>116.2509439752739</v>
+      </c>
+      <c r="D56" t="n">
+        <v>45.12394799421905</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-2.691617665680774</v>
+      </c>
+      <c r="F56" t="n">
+        <v>197.9902364611626</v>
+      </c>
+      <c r="G56" t="n">
+        <v>45.87425774419418</v>
+      </c>
+      <c r="H56" t="n">
+        <v>135.6738214868723</v>
+      </c>
+      <c r="I56" t="n">
+        <v>52.66312905168957</v>
+      </c>
+      <c r="J56" t="n">
+        <v>55.53933021340457</v>
+      </c>
+      <c r="K56" t="n">
+        <v>-1.15360274710666</v>
+      </c>
+      <c r="L56" t="n">
+        <v>288.596935749054</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B57" t="n">
+        <v>40.31692718529091</v>
+      </c>
+      <c r="C57" t="n">
+        <v>118.9207411146118</v>
+      </c>
+      <c r="D57" t="n">
+        <v>47.51379115243535</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.630875977702011</v>
+      </c>
+      <c r="F57" t="n">
+        <v>205.1205834746361</v>
+      </c>
+      <c r="G57" t="n">
+        <v>47.41047671287962</v>
+      </c>
+      <c r="H57" t="n">
+        <v>139.844214847546</v>
+      </c>
+      <c r="I57" t="n">
+        <v>55.87359072828872</v>
+      </c>
+      <c r="J57" t="n">
+        <v>58.11351133572528</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1.119302996120076</v>
+      </c>
+      <c r="L57" t="n">
+        <v>302.3610966205597</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B58" t="n">
+        <v>41.47157749352299</v>
+      </c>
+      <c r="C58" t="n">
+        <v>121.6345254686473</v>
+      </c>
+      <c r="D58" t="n">
+        <v>50.03127972260462</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.3036146150308028</v>
+      </c>
+      <c r="F58" t="n">
+        <v>212.8337680697441</v>
+      </c>
+      <c r="G58" t="n">
+        <v>49.15471372923957</v>
+      </c>
+      <c r="H58" t="n">
+        <v>144.1688655305442</v>
+      </c>
+      <c r="I58" t="n">
+        <v>59.30020946650092</v>
+      </c>
+      <c r="J58" t="n">
+        <v>59.59933730424572</v>
+      </c>
+      <c r="K58" t="n">
+        <v>5.105825089846185</v>
+      </c>
+      <c r="L58" t="n">
+        <v>317.3289511203766</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B59" t="n">
+        <v>42.78133110546195</v>
+      </c>
+      <c r="C59" t="n">
+        <v>124.3743836727143</v>
+      </c>
+      <c r="D59" t="n">
+        <v>52.68763974886764</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.318990941954034</v>
+      </c>
+      <c r="F59" t="n">
+        <v>221.162345468998</v>
+      </c>
+      <c r="G59" t="n">
+        <v>51.12466315781803</v>
+      </c>
+      <c r="H59" t="n">
+        <v>148.6302157138101</v>
+      </c>
+      <c r="I59" t="n">
+        <v>62.96292717262885</v>
+      </c>
+      <c r="J59" t="n">
+        <v>64.24728210828241</v>
+      </c>
+      <c r="K59" t="n">
+        <v>6.615089869845292</v>
+      </c>
+      <c r="L59" t="n">
+        <v>333.5801780223846</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B60" t="n">
+        <v>44.25714870948202</v>
+      </c>
+      <c r="C60" t="n">
+        <v>127.1190980533219</v>
+      </c>
+      <c r="D60" t="n">
+        <v>55.494745145435</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.268463529421254</v>
+      </c>
+      <c r="F60" t="n">
+        <v>230.1394554376602</v>
+      </c>
+      <c r="G60" t="n">
+        <v>53.33926304455639</v>
+      </c>
+      <c r="H60" t="n">
+        <v>153.2055093192255</v>
+      </c>
+      <c r="I60" t="n">
+        <v>66.8829532678139</v>
+      </c>
+      <c r="J60" t="n">
+        <v>66.24644729424173</v>
+      </c>
+      <c r="K60" t="n">
+        <v>11.52251000415518</v>
+      </c>
+      <c r="L60" t="n">
+        <v>351.1966829299927</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B61" t="n">
+        <v>45.9105630603154</v>
+      </c>
+      <c r="C61" t="n">
+        <v>129.843586020921</v>
+      </c>
+      <c r="D61" t="n">
+        <v>58.46513907216551</v>
+      </c>
+      <c r="E61" t="n">
+        <v>5.579539196737706</v>
+      </c>
+      <c r="F61" t="n">
+        <v>239.7988273501396</v>
+      </c>
+      <c r="G61" t="n">
+        <v>55.8187734274934</v>
+      </c>
+      <c r="H61" t="n">
+        <v>157.8658423246366</v>
+      </c>
+      <c r="I61" t="n">
+        <v>71.08282133217817</v>
+      </c>
+      <c r="J61" t="n">
+        <v>70.19190504927502</v>
+      </c>
+      <c r="K61" t="n">
+        <v>15.30326424878677</v>
+      </c>
+      <c r="L61" t="n">
+        <v>370.26260638237</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B62" t="n">
+        <v>47.75370372563103</v>
+      </c>
+      <c r="C62" t="n">
+        <v>132.5182336147943</v>
+      </c>
+      <c r="D62" t="n">
+        <v>61.61205748172289</v>
+      </c>
+      <c r="E62" t="n">
+        <v>8.290781374331601</v>
+      </c>
+      <c r="F62" t="n">
+        <v>250.1747761964798</v>
+      </c>
+      <c r="G62" t="n">
+        <v>58.58484741858675</v>
+      </c>
+      <c r="H62" t="n">
+        <v>162.5750442543452</v>
+      </c>
+      <c r="I62" t="n">
+        <v>75.58645099970693</v>
+      </c>
+      <c r="J62" t="n">
+        <v>17.64928148140623</v>
+      </c>
+      <c r="K62" t="n">
+        <v>76.46869111733241</v>
+      </c>
+      <c r="L62" t="n">
+        <v>390.8643152713776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit just to save before trying something
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -515,7 +515,7 @@
         <v>8.025480389595032</v>
       </c>
       <c r="G2" t="n">
-        <v>2.664992669550213</v>
+        <v>0.07867893939452165</v>
       </c>
       <c r="H2" t="n">
         <v>8.306765334619181</v>
@@ -527,7 +527,7 @@
         <v>-1.945093541270408</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.044232424142641</v>
+        <v>-0.4579186939869491</v>
       </c>
       <c r="L2" t="n">
         <v>5.01543402671814</v>
@@ -553,7 +553,7 @@
         <v>15.74764043092728</v>
       </c>
       <c r="G3" t="n">
-        <v>5.22944814093343</v>
+        <v>0.2834097224933642</v>
       </c>
       <c r="H3" t="n">
         <v>15.67967960362973</v>
@@ -565,7 +565,7 @@
         <v>-8.753415186097419</v>
       </c>
       <c r="K3" t="n">
-        <v>0.008781852903227971</v>
+        <v>4.954820271343294</v>
       </c>
       <c r="L3" t="n">
         <v>10.28646039962769</v>
@@ -591,7 +591,7 @@
         <v>23.1667366027832</v>
       </c>
       <c r="G4" t="n">
-        <v>7.701324314756554</v>
+        <v>0.6100384473891095</v>
       </c>
       <c r="H4" t="n">
         <v>22.3109710150348</v>
@@ -603,7 +603,7 @@
         <v>-12.04317274164832</v>
       </c>
       <c r="K4" t="n">
-        <v>0.529162567745006</v>
+        <v>7.620448435112452</v>
       </c>
       <c r="L4" t="n">
         <v>15.77010941505432</v>
@@ -629,7 +629,7 @@
         <v>30.28361445665359</v>
       </c>
       <c r="G5" t="n">
-        <v>10.08502655826333</v>
+        <v>1.053359069074734</v>
       </c>
       <c r="H5" t="n">
         <v>28.33136463537102</v>
@@ -641,7 +641,7 @@
         <v>-12.08501115616109</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.393737462944404</v>
+        <v>7.637930026244192</v>
       </c>
       <c r="L5" t="n">
         <v>21.42563843727112</v>
@@ -667,7 +667,7 @@
         <v>37.09970450401306</v>
       </c>
       <c r="G6" t="n">
-        <v>12.3824108185826</v>
+        <v>1.607051367755741</v>
       </c>
       <c r="H6" t="n">
         <v>33.83221193773886</v>
@@ -679,7 +679,7 @@
         <v>-8.193323856318347</v>
       </c>
       <c r="K6" t="n">
-        <v>-6.582795513075803</v>
+        <v>4.192563937751054</v>
       </c>
       <c r="L6" t="n">
         <v>27.2145357131958</v>
@@ -705,7 +705,7 @@
         <v>43.61702632904053</v>
       </c>
       <c r="G7" t="n">
-        <v>14.59355353798953</v>
+        <v>2.263696227475027</v>
       </c>
       <c r="H7" t="n">
         <v>38.8789471360054</v>
@@ -717,7 +717,7 @@
         <v>-8.311281322075134</v>
       </c>
       <c r="K7" t="n">
-        <v>-7.202028896358314</v>
+        <v>5.127828414156189</v>
       </c>
       <c r="L7" t="n">
         <v>33.10052084922791</v>
@@ -743,7 +743,7 @@
         <v>49.83818560838699</v>
       </c>
       <c r="G8" t="n">
-        <v>16.71734054847584</v>
+        <v>3.01485362797923</v>
       </c>
       <c r="H8" t="n">
         <v>43.51963005029914</v>
@@ -755,7 +755,7 @@
         <v>-5.171464322903</v>
       </c>
       <c r="K8" t="n">
-        <v>-10.60487122550825</v>
+        <v>3.097615694988355</v>
       </c>
       <c r="L8" t="n">
         <v>39.04954195022583</v>
@@ -781,7 +781,7 @@
         <v>55.76637578010559</v>
       </c>
       <c r="G9" t="n">
-        <v>18.75191837698277</v>
+        <v>3.851180243942212</v>
       </c>
       <c r="H9" t="n">
         <v>47.79053863551978</v>
@@ -793,7 +793,7 @@
         <v>-6.634700818295123</v>
       </c>
       <c r="K9" t="n">
-        <v>-9.001206383730835</v>
+        <v>5.899531749309721</v>
       </c>
       <c r="L9" t="n">
         <v>45.02977681159973</v>
@@ -819,7 +819,7 @@
         <v>61.40537697076797</v>
       </c>
       <c r="G10" t="n">
-        <v>20.69503881460975</v>
+        <v>4.762574860949703</v>
       </c>
       <c r="H10" t="n">
         <v>51.71994146534372</v>
@@ -831,7 +831,7 @@
         <v>-14.10077749305779</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.050647309108927</v>
+        <v>14.88181664455112</v>
       </c>
       <c r="L10" t="n">
         <v>51.01163530349731</v>
@@ -857,7 +857,7 @@
         <v>66.75955736637115</v>
       </c>
       <c r="G11" t="n">
-        <v>22.54432173840143</v>
+        <v>5.738338041100786</v>
       </c>
       <c r="H11" t="n">
         <v>55.33068497294368</v>
@@ -869,7 +869,7 @@
         <v>-17.65367011789323</v>
       </c>
       <c r="K11" t="n">
-        <v>3.279922686611684</v>
+        <v>20.08590638391232</v>
       </c>
       <c r="L11" t="n">
         <v>56.96775412559509</v>
@@ -895,7 +895,7 @@
         <v>71.83387196063995</v>
       </c>
       <c r="G12" t="n">
-        <v>24.29745494400631</v>
+        <v>6.767340374005929</v>
       </c>
       <c r="H12" t="n">
         <v>58.6420044304606</v>
@@ -907,7 +907,7 @@
         <v>-11.71180985000244</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.635340019385231</v>
+        <v>15.89477455061515</v>
       </c>
       <c r="L12" t="n">
         <v>62.87300324440002</v>
@@ -933,7 +933,7 @@
         <v>76.63386231660843</v>
       </c>
       <c r="G13" t="n">
-        <v>25.95234446962981</v>
+        <v>7.838185056218411</v>
       </c>
       <c r="H13" t="n">
         <v>61.67080210078565</v>
@@ -945,7 +945,7 @@
         <v>-13.65893444570869</v>
       </c>
       <c r="K13" t="n">
-        <v>1.548197332326826</v>
+        <v>19.66235674573823</v>
       </c>
       <c r="L13" t="n">
         <v>68.70448017120361</v>
@@ -971,7 +971,7 @@
         <v>81.16565805673599</v>
       </c>
       <c r="G14" t="n">
-        <v>27.50722739444926</v>
+        <v>8.939369493888595</v>
       </c>
       <c r="H14" t="n">
         <v>64.43255739504981</v>
@@ -983,7 +983,7 @@
         <v>-7.136389072964776</v>
       </c>
       <c r="K14" t="n">
-        <v>-3.563079834944676</v>
+        <v>15.00477806561599</v>
       </c>
       <c r="L14" t="n">
         <v>74.44151496887207</v>
@@ -1009,7 +1009,7 @@
         <v>85.43597596883774</v>
       </c>
       <c r="G15" t="n">
-        <v>28.96075377193128</v>
+        <v>10.0594354568538</v>
       </c>
       <c r="H15" t="n">
         <v>66.94197463240423</v>
@@ -1021,7 +1021,7 @@
         <v>-6.108594804165955</v>
       </c>
       <c r="K15" t="n">
-        <v>-3.036326780622455</v>
+        <v>15.86499153445503</v>
       </c>
       <c r="L15" t="n">
         <v>80.06566405296326</v>
@@ -1047,7 +1047,7 @@
         <v>89.45211935043335</v>
       </c>
       <c r="G16" t="n">
-        <v>30.3120461043778</v>
+        <v>11.18710685144444</v>
       </c>
       <c r="H16" t="n">
         <v>69.21343663480525</v>
@@ -1059,7 +1059,7 @@
         <v>-2.625501860007036</v>
       </c>
       <c r="K16" t="n">
-        <v>-4.850337260100135</v>
+        <v>14.27460199283323</v>
       </c>
       <c r="L16" t="n">
         <v>85.56071496009827</v>
@@ -1085,7 +1085,7 @@
         <v>93.22197932004929</v>
       </c>
       <c r="G17" t="n">
-        <v>31.5607398441365</v>
+        <v>12.3114161914133</v>
       </c>
       <c r="H17" t="n">
         <v>71.26132766061156</v>
@@ -1097,7 +1097,7 @@
         <v>-2.936803997128449</v>
       </c>
       <c r="K17" t="n">
-        <v>-2.781746060624252</v>
+        <v>16.46757759209895</v>
       </c>
       <c r="L17" t="n">
         <v>90.91268944740295</v>
@@ -1123,7 +1123,7 @@
         <v>96.75403422117233</v>
       </c>
       <c r="G18" t="n">
-        <v>32.70700815622536</v>
+        <v>13.42181709598683</v>
       </c>
       <c r="H18" t="n">
         <v>73.10024273875044</v>
@@ -1135,7 +1135,7 @@
         <v>-0.7614292659290338</v>
       </c>
       <c r="K18" t="n">
-        <v>-3.135847663060898</v>
+        <v>16.14934339717764</v>
       </c>
       <c r="L18" t="n">
         <v>96.10983395576477</v>
@@ -1161,7 +1161,7 @@
         <v>100.0573494434357</v>
       </c>
       <c r="G19" t="n">
-        <v>33.75157581675575</v>
+        <v>14.50828356327137</v>
       </c>
       <c r="H19" t="n">
         <v>74.74511869848305</v>
@@ -1173,7 +1173,7 @@
         <v>0.6424210080266849</v>
       </c>
       <c r="K19" t="n">
-        <v>-2.676769608168425</v>
+        <v>16.56652264531595</v>
       </c>
       <c r="L19" t="n">
         <v>101.1426258087158</v>
@@ -1199,7 +1199,7 @@
         <v>103.1415777206421</v>
       </c>
       <c r="G20" t="n">
-        <v>34.69572345247781</v>
+        <v>15.56139371975123</v>
       </c>
       <c r="H20" t="n">
         <v>76.21130881750022</v>
@@ -1211,7 +1211,7 @@
         <v>8.804224115684887</v>
       </c>
       <c r="K20" t="n">
-        <v>-8.954580260379982</v>
+        <v>10.17974947234659</v>
       </c>
       <c r="L20" t="n">
         <v>106.0037751197815</v>
@@ -1237,7 +1237,7 @@
         <v>106.0169587731361</v>
       </c>
       <c r="G21" t="n">
-        <v>35.54128298783034</v>
+        <v>16.57240536301691</v>
       </c>
       <c r="H21" t="n">
         <v>77.51460360919593</v>
@@ -1249,7 +1249,7 @@
         <v>11.98689558311575</v>
       </c>
       <c r="K21" t="n">
-        <v>-10.25115260178631</v>
+        <v>8.717725023027125</v>
       </c>
       <c r="L21" t="n">
         <v>110.6882183551788</v>
@@ -1275,7 +1275,7 @@
         <v>108.6943194270134</v>
       </c>
       <c r="G22" t="n">
-        <v>36.2906284256927</v>
+        <v>17.53331467743018</v>
       </c>
       <c r="H22" t="n">
         <v>78.67121687674987</v>
@@ -1287,7 +1287,7 @@
         <v>6.082978953432057</v>
       </c>
       <c r="K22" t="n">
-        <v>-2.476404760556565</v>
+        <v>16.28090898770595</v>
       </c>
       <c r="L22" t="n">
         <v>115.1931278705597</v>
@@ -1313,7 +1313,7 @@
         <v>111.185074031353</v>
       </c>
       <c r="G23" t="n">
-        <v>36.94665876890706</v>
+        <v>18.43690513843573</v>
       </c>
       <c r="H23" t="n">
         <v>79.69773679168007</v>
@@ -1325,7 +1325,7 @@
         <v>7.341080459717278</v>
       </c>
       <c r="K23" t="n">
-        <v>-1.894768268810874</v>
+        <v>16.61498536166046</v>
       </c>
       <c r="L23" t="n">
         <v>119.5178956985474</v>
@@ -1351,7 +1351,7 @@
         <v>113.5012245178223</v>
       </c>
       <c r="G24" t="n">
-        <v>37.51278097172949</v>
+        <v>19.27678848726305</v>
       </c>
       <c r="H24" t="n">
         <v>80.61106340660362</v>
@@ -1363,7 +1363,7 @@
         <v>7.279113576748939</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.03841230759252845</v>
+        <v>18.19758017687391</v>
       </c>
       <c r="L24" t="n">
         <v>123.6641557216644</v>
@@ -1389,7 +1389,7 @@
         <v>115.6553587317467</v>
       </c>
       <c r="G25" t="n">
-        <v>37.99288479471285</v>
+        <v>20.04743223365554</v>
       </c>
       <c r="H25" t="n">
         <v>81.42831915286028</v>
@@ -1401,7 +1401,7 @@
         <v>8.703718248815735</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2733501000712391</v>
+        <v>18.21880266112855</v>
       </c>
       <c r="L25" t="n">
         <v>127.6357629299164</v>
@@ -1427,7 +1427,7 @@
         <v>117.6606534719467</v>
       </c>
       <c r="G26" t="n">
-        <v>38.39131892043434</v>
+        <v>20.74418055680502</v>
       </c>
       <c r="H26" t="n">
         <v>82.16675138271263</v>
@@ -1439,7 +1439,7 @@
         <v>10.07696011453443</v>
       </c>
       <c r="K26" t="n">
-        <v>0.5674213424777861</v>
+        <v>18.21455970610711</v>
       </c>
       <c r="L26" t="n">
         <v>131.4388077259064</v>
@@ -1465,7 +1465,7 @@
         <v>119.5308713316917</v>
       </c>
       <c r="G27" t="n">
-        <v>38.71286252940088</v>
+        <v>21.36326783575629</v>
       </c>
       <c r="H27" t="n">
         <v>82.84362313637675</v>
@@ -1477,7 +1477,7 @@
         <v>12.20704447342378</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02625986414867043</v>
+        <v>17.37585455779326</v>
       </c>
       <c r="L27" t="n">
         <v>135.0816068649292</v>
@@ -1503,7 +1503,7 @@
         <v>121.2803630232811</v>
       </c>
       <c r="G28" t="n">
-        <v>38.96269685331959</v>
+        <v>21.90182322228899</v>
       </c>
       <c r="H28" t="n">
         <v>83.47610235817838</v>
@@ -1515,7 +1515,7 @@
         <v>10.65317729503711</v>
       </c>
       <c r="K28" t="n">
-        <v>3.083091979982411</v>
+        <v>20.14396561101301</v>
       </c>
       <c r="L28" t="n">
         <v>138.5747077465057</v>
@@ -1541,7 +1541,7 @@
         <v>122.9240655303001</v>
       </c>
       <c r="G29" t="n">
-        <v>39.14637564117176</v>
+        <v>22.35787096932565</v>
       </c>
       <c r="H29" t="n">
         <v>84.08115061323279</v>
@@ -1553,7 +1553,7 @@
         <v>15.65577074704103</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.5082175687428219</v>
+        <v>16.28028710310328</v>
       </c>
       <c r="L29" t="n">
         <v>141.9308903217316</v>
@@ -1579,7 +1579,7 @@
         <v>124.4775037765503</v>
       </c>
       <c r="G30" t="n">
-        <v>39.26979423973023</v>
+        <v>22.73032595258459</v>
       </c>
       <c r="H30" t="n">
         <v>84.67541032705108</v>
@@ -1591,7 +1591,7 @@
         <v>16.74875078235079</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.2853962880410066</v>
+        <v>16.25407199910463</v>
       </c>
       <c r="L30" t="n">
         <v>145.1651637554169</v>
@@ -1617,7 +1617,7 @@
         <v>125.9567903876305</v>
       </c>
       <c r="G31" t="n">
-        <v>39.33915982804758</v>
+        <v>23.01898193551957</v>
       </c>
       <c r="H31" t="n">
         <v>85.27510091238689</v>
@@ -1629,7 +1629,7 @@
         <v>17.87438333782273</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.1925172440725333</v>
+        <v>16.12766064845548</v>
       </c>
       <c r="L31" t="n">
         <v>148.2947638034821</v>
@@ -1655,7 +1655,7 @@
         <v>127.3786235451698</v>
       </c>
       <c r="G32" t="n">
-        <v>39.36096207950109</v>
+        <v>23.22450110330703</v>
       </c>
       <c r="H32" t="n">
         <v>85.89592804931095</v>
@@ -1667,7 +1667,7 @@
         <v>17.15004722638063</v>
       </c>
       <c r="K32" t="n">
-        <v>1.653299560109701</v>
+        <v>17.78976053630376</v>
       </c>
       <c r="L32" t="n">
         <v>151.3391599655151</v>
@@ -1693,7 +1693,7 @@
         <v>128.7602902054787</v>
       </c>
       <c r="G33" t="n">
-        <v>39.34194435857267</v>
+        <v>23.34839834846756</v>
       </c>
       <c r="H33" t="n">
         <v>86.55299620077325</v>
@@ -1705,7 +1705,7 @@
         <v>14.41333063084411</v>
       </c>
       <c r="K33" t="n">
-        <v>5.416849539083154</v>
+        <v>21.41039554918826</v>
       </c>
       <c r="L33" t="n">
         <v>154.3200492858887</v>
@@ -1731,7 +1731,7 @@
         <v>130.1196644306183</v>
       </c>
       <c r="G34" t="n">
-        <v>39.28907739495488</v>
+        <v>23.3930243426538</v>
       </c>
       <c r="H34" t="n">
         <v>87.26074160042742</v>
@@ -1743,7 +1743,7 @@
         <v>13.18193450379734</v>
       </c>
       <c r="K34" t="n">
-        <v>7.584990792866384</v>
+        <v>23.48104384516746</v>
       </c>
       <c r="L34" t="n">
         <v>157.2613613605499</v>
@@ -1769,7 +1769,7 @@
         <v>131.4752058386803</v>
       </c>
       <c r="G35" t="n">
-        <v>39.20953391717236</v>
+        <v>23.36155418262033</v>
       </c>
       <c r="H35" t="n">
         <v>88.03288086276724</v>
@@ -1781,7 +1781,7 @@
         <v>10.53469710115306</v>
       </c>
       <c r="K35" t="n">
-        <v>11.08564651495203</v>
+        <v>26.93362624950406</v>
       </c>
       <c r="L35" t="n">
         <v>160.1892533302307</v>
@@ -1807,7 +1807,7 @@
         <v>132.8459639549255</v>
       </c>
       <c r="G36" t="n">
-        <v>39.11066735850467</v>
+        <v>23.25797045704835</v>
       </c>
       <c r="H36" t="n">
         <v>88.88237147505414</v>
@@ -1819,7 +1819,7 @@
         <v>14.38907876825045</v>
       </c>
       <c r="K36" t="n">
-        <v>8.010344797365965</v>
+        <v>23.86304169882229</v>
       </c>
       <c r="L36" t="n">
         <v>163.1321144104004</v>
@@ -1845,7 +1845,7 @@
         <v>134.251572906971</v>
       </c>
       <c r="G37" t="n">
-        <v>38.99999225307309</v>
+        <v>23.08705582812599</v>
       </c>
       <c r="H37" t="n">
         <v>89.82139324677243</v>
@@ -1857,7 +1857,7 @@
         <v>16.11645711097677</v>
       </c>
       <c r="K37" t="n">
-        <v>6.998918502473568</v>
+        <v>22.91185492742067</v>
       </c>
       <c r="L37" t="n">
         <v>166.1205613613129</v>
@@ -1883,7 +1883,7 @@
         <v>135.7122554183006</v>
       </c>
       <c r="G38" t="n">
-        <v>38.88516981348979</v>
+        <v>22.85438830034078</v>
       </c>
       <c r="H38" t="n">
         <v>90.86134782506865</v>
@@ -1895,7 +1895,7 @@
         <v>19.29991270224928</v>
       </c>
       <c r="K38" t="n">
-        <v>4.481702914425053</v>
+        <v>20.51248442757407</v>
       </c>
       <c r="L38" t="n">
         <v>169.1874423027039</v>
@@ -1921,7 +1921,7 @@
         <v>137.2488216757774</v>
       </c>
       <c r="G39" t="n">
-        <v>38.77399697719627</v>
+        <v>22.56634638413218</v>
       </c>
       <c r="H39" t="n">
         <v>92.01286479624437</v>
@@ -1933,7 +1933,7 @@
         <v>21.28907576483529</v>
       </c>
       <c r="K39" t="n">
-        <v>3.124660224622911</v>
+        <v>19.332310817687</v>
       </c>
       <c r="L39" t="n">
         <v>172.3678362369537</v>
@@ -1959,7 +1959,7 @@
         <v>138.8826679587364</v>
       </c>
       <c r="G40" t="n">
-        <v>38.67440060583528</v>
+        <v>22.23012006344638</v>
       </c>
       <c r="H40" t="n">
         <v>93.28583226208926</v>
@@ -1971,7 +1971,7 @@
         <v>20.17153856923074</v>
       </c>
       <c r="K40" t="n">
-        <v>4.857910953413057</v>
+        <v>21.30219149580196</v>
       </c>
       <c r="L40" t="n">
         <v>175.6990518569946</v>
@@ -1997,7 +1997,7 @@
         <v>140.6357783675194</v>
       </c>
       <c r="G41" t="n">
-        <v>38.59443687368142</v>
+        <v>21.85373722402712</v>
       </c>
       <c r="H41" t="n">
         <v>94.68942467731159</v>
@@ -2009,7 +2009,7 @@
         <v>21.7276702831632</v>
       </c>
       <c r="K41" t="n">
-        <v>3.920862048942016</v>
+        <v>20.66156169859631</v>
       </c>
       <c r="L41" t="n">
         <v>179.2206263542175</v>
@@ -2035,7 +2035,7 @@
         <v>142.5307248830795</v>
       </c>
       <c r="G42" t="n">
-        <v>38.54229680382326</v>
+        <v>21.44610387769768</v>
       </c>
       <c r="H42" t="n">
         <v>96.23214352973977</v>
@@ -2047,7 +2047,7 @@
         <v>26.62762764498752</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.3348749073475474</v>
+        <v>16.76131801877803</v>
       </c>
       <c r="L42" t="n">
         <v>182.9743266105652</v>
@@ -2073,7 +2073,7 @@
         <v>144.5906656384468</v>
       </c>
       <c r="G43" t="n">
-        <v>38.52631843076895</v>
+        <v>21.01706271973296</v>
       </c>
       <c r="H43" t="n">
         <v>97.92185731379864</v>
@@ -2085,7 +2085,7 @@
         <v>22.51197264230167</v>
       </c>
       <c r="K43" t="n">
-        <v>4.473823206108992</v>
+        <v>21.98307891714498</v>
       </c>
       <c r="L43" t="n">
         <v>187.0041513442993</v>
@@ -2111,7 +2111,7 @@
         <v>146.8393463492393</v>
       </c>
       <c r="G44" t="n">
-        <v>38.55500553267243</v>
+        <v>20.57746698417667</v>
       </c>
       <c r="H44" t="n">
         <v>99.76583712375761</v>
@@ -2123,7 +2123,7 @@
         <v>27.73643980695459</v>
       </c>
       <c r="K44" t="n">
-        <v>0.01674689534563356</v>
+        <v>17.99428544384139</v>
       </c>
       <c r="L44" t="n">
         <v>191.3563306331635</v>
@@ -2149,7 +2149,7 @@
         <v>149.301099717617</v>
       </c>
       <c r="G45" t="n">
-        <v>38.63705233192732</v>
+        <v>20.13928514792284</v>
       </c>
       <c r="H45" t="n">
         <v>101.770778041692</v>
@@ -2161,7 +2161,7 @@
         <v>28.58353428039268</v>
       </c>
       <c r="K45" t="n">
-        <v>0.03868216963427429</v>
+        <v>18.53644935363875</v>
       </c>
       <c r="L45" t="n">
         <v>196.079320192337</v>
@@ -2187,7 +2187,7 @@
         <v>152.000846683979</v>
       </c>
       <c r="G46" t="n">
-        <v>38.78137783272454</v>
+        <v>19.71572056659708</v>
       </c>
       <c r="H46" t="n">
         <v>103.942814021087</v>
@@ -2199,7 +2199,7 @@
         <v>33.18634592045535</v>
       </c>
       <c r="K46" t="n">
-        <v>-3.564465671286293</v>
+        <v>15.50119159484117</v>
       </c>
       <c r="L46" t="n">
         <v>201.22380900383</v>
@@ -2225,7 +2225,7 @@
         <v>154.964094042778</v>
       </c>
       <c r="G47" t="n">
-        <v>38.99716536776136</v>
+        <v>19.32136718589418</v>
       </c>
       <c r="H47" t="n">
         <v>106.2874994536535</v>
@@ -2237,7 +2237,7 @@
         <v>37.1998620319838</v>
       </c>
       <c r="K47" t="n">
-        <v>-6.417030641841002</v>
+        <v>13.25876754002618</v>
       </c>
       <c r="L47" t="n">
         <v>206.8427138328552</v>
@@ -2263,7 +2263,7 @@
         <v>158.2169361710548</v>
       </c>
       <c r="G48" t="n">
-        <v>39.2939107908675</v>
+        <v>18.9723857526461</v>
       </c>
       <c r="H48" t="n">
         <v>108.80977451766</v>
@@ -2275,7 +2275,7 @@
         <v>39.69275712450992</v>
       </c>
       <c r="K48" t="n">
-        <v>-7.555404318087341</v>
+        <v>12.76612072013405</v>
       </c>
       <c r="L48" t="n">
         <v>212.991183757782</v>
@@ -2301,7 +2301,7 @@
         <v>161.786055803299</v>
       </c>
       <c r="G49" t="n">
-        <v>39.68147723019083</v>
+        <v>18.6867157605099</v>
       </c>
       <c r="H49" t="n">
         <v>111.5138900688956</v>
@@ -2313,7 +2313,7 @@
         <v>42.52924426710228</v>
       </c>
       <c r="K49" t="n">
-        <v>-8.809888048050126</v>
+        <v>12.1848734216308</v>
       </c>
       <c r="L49" t="n">
         <v>219.7265973091125</v>
@@ -2339,7 +2339,7 @@
         <v>165.6987212300301</v>
       </c>
       <c r="G50" t="n">
-        <v>40.1701566951564</v>
+        <v>18.48430975228594</v>
       </c>
       <c r="H50" t="n">
         <v>114.4032957793948</v>
@@ -2351,7 +2351,7 @@
         <v>41.26485909291869</v>
       </c>
       <c r="K50" t="n">
-        <v>-5.700446577307943</v>
+        <v>15.98540036556252</v>
       </c>
       <c r="L50" t="n">
         <v>227.1085615158081</v>
@@ -2377,7 +2377,7 @@
         <v>169.9827892780304</v>
       </c>
       <c r="G51" t="n">
-        <v>40.77073842495055</v>
+        <v>18.38739757509961</v>
       </c>
       <c r="H51" t="n">
         <v>117.4804888997698</v>
@@ -2389,7 +2389,7 @@
         <v>43.50071802861427</v>
       </c>
       <c r="K51" t="n">
-        <v>-5.790901603722958</v>
+        <v>16.59243924612798</v>
       </c>
       <c r="L51" t="n">
         <v>235.1989140510559</v>
@@ -2415,7 +2415,7 @@
         <v>174.666702747345</v>
       </c>
       <c r="G52" t="n">
-        <v>41.49458234716073</v>
+        <v>18.42077588820602</v>
       </c>
       <c r="H52" t="n">
         <v>120.7468114862955</v>
@@ -2427,7 +2427,7 @@
         <v>47.79824615604387</v>
       </c>
       <c r="K52" t="n">
-        <v>-7.603550163739243</v>
+        <v>15.47025629521547</v>
       </c>
       <c r="L52" t="n">
         <v>244.061723947525</v>
@@ -2453,7 +2453,7 @@
         <v>179.7794927954674</v>
       </c>
       <c r="G53" t="n">
-        <v>42.35369782390887</v>
+        <v>18.61211176586196</v>
       </c>
       <c r="H53" t="n">
         <v>124.2021928542878</v>
@@ -2465,7 +2465,7 @@
         <v>48.23811911783717</v>
       </c>
       <c r="K53" t="n">
-        <v>-5.177955826106512</v>
+        <v>18.56363023194041</v>
       </c>
       <c r="L53" t="n">
         <v>253.7632865905762</v>
@@ -2491,7 +2491,7 @@
         <v>185.3507773280144</v>
       </c>
       <c r="G54" t="n">
-        <v>43.36082611602388</v>
+        <v>18.99226673737393</v>
       </c>
       <c r="H54" t="n">
         <v>127.8448406341554</v>
@@ -2503,7 +2503,7 @@
         <v>51.2475175541022</v>
       </c>
       <c r="K54" t="n">
-        <v>-4.897993431460492</v>
+        <v>19.47056594718946</v>
       </c>
       <c r="L54" t="n">
         <v>264.3721330165863</v>
@@ -2529,7 +2529,7 @@
         <v>191.4107611179352</v>
       </c>
       <c r="G55" t="n">
-        <v>44.52952543831268</v>
+        <v>19.59561757915424</v>
       </c>
       <c r="H55" t="n">
         <v>131.670862546845</v>
@@ -2541,7 +2541,7 @@
         <v>53.8084524036118</v>
       </c>
       <c r="K55" t="n">
-        <v>-3.699918079014267</v>
+        <v>21.23398978014418</v>
       </c>
       <c r="L55" t="n">
         <v>275.959020614624</v>
@@ -2567,7 +2567,7 @@
         <v>197.9902364611626</v>
       </c>
       <c r="G56" t="n">
-        <v>45.87425774419418</v>
+        <v>20.46038267041456</v>
       </c>
       <c r="H56" t="n">
         <v>135.6738214868723</v>
@@ -2579,7 +2579,7 @@
         <v>55.53933021340457</v>
       </c>
       <c r="K56" t="n">
-        <v>-1.15360274710666</v>
+        <v>24.26027232667296</v>
       </c>
       <c r="L56" t="n">
         <v>288.596935749054</v>
@@ -2605,7 +2605,7 @@
         <v>205.1205834746361</v>
       </c>
       <c r="G57" t="n">
-        <v>47.41047671287962</v>
+        <v>21.62892370321029</v>
       </c>
       <c r="H57" t="n">
         <v>139.844214847546</v>
@@ -2617,7 +2617,7 @@
         <v>58.11351133572528</v>
       </c>
       <c r="K57" t="n">
-        <v>1.119302996120076</v>
+        <v>26.90085600578941</v>
       </c>
       <c r="L57" t="n">
         <v>302.3610966205597</v>
@@ -2643,7 +2643,7 @@
         <v>212.8337680697441</v>
       </c>
       <c r="G58" t="n">
-        <v>49.15471372923957</v>
+        <v>23.14802977229899</v>
       </c>
       <c r="H58" t="n">
         <v>144.1688655305442</v>
@@ -2655,7 +2655,7 @@
         <v>59.59933730424572</v>
       </c>
       <c r="K58" t="n">
-        <v>5.105825089846185</v>
+        <v>31.11250904678676</v>
       </c>
       <c r="L58" t="n">
         <v>317.3289511203766</v>
@@ -2681,7 +2681,7 @@
         <v>221.162345468998</v>
       </c>
       <c r="G59" t="n">
-        <v>51.12466315781803</v>
+        <v>25.06915655309442</v>
       </c>
       <c r="H59" t="n">
         <v>148.6302157138101</v>
@@ -2693,7 +2693,7 @@
         <v>64.24728210828241</v>
       </c>
       <c r="K59" t="n">
-        <v>6.615089869845292</v>
+        <v>32.6705964745689</v>
       </c>
       <c r="L59" t="n">
         <v>333.5801780223846</v>
@@ -2719,7 +2719,7 @@
         <v>230.1394554376602</v>
       </c>
       <c r="G60" t="n">
-        <v>53.33926304455639</v>
+        <v>27.44862204242059</v>
       </c>
       <c r="H60" t="n">
         <v>153.2055093192255</v>
@@ -2731,7 +2731,7 @@
         <v>66.24644729424173</v>
       </c>
       <c r="K60" t="n">
-        <v>11.52251000415518</v>
+        <v>37.41315100629097</v>
       </c>
       <c r="L60" t="n">
         <v>351.1966829299927</v>
@@ -2757,7 +2757,7 @@
         <v>239.7988273501396</v>
       </c>
       <c r="G61" t="n">
-        <v>55.8187734274934</v>
+        <v>30.34773555612693</v>
       </c>
       <c r="H61" t="n">
         <v>157.8658423246366</v>
@@ -2769,7 +2769,7 @@
         <v>70.19190504927502</v>
       </c>
       <c r="K61" t="n">
-        <v>15.30326424878677</v>
+        <v>40.77430212015324</v>
       </c>
       <c r="L61" t="n">
         <v>370.26260638237</v>
@@ -2795,7 +2795,7 @@
         <v>250.1747761964798</v>
       </c>
       <c r="G62" t="n">
-        <v>58.58484741858675</v>
+        <v>33.83286349733605</v>
       </c>
       <c r="H62" t="n">
         <v>162.5750442543452</v>
@@ -2807,7 +2807,7 @@
         <v>17.64928148140623</v>
       </c>
       <c r="K62" t="n">
-        <v>76.46869111733241</v>
+        <v>101.2206750385831</v>
       </c>
       <c r="L62" t="n">
         <v>390.8643152713776</v>

</xml_diff>

<commit_message>
create tech limit and tech freeze future scenario
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -515,7 +515,7 @@
         <v>8.025480389595032</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07867893939452165</v>
+        <v>2.664992669550213</v>
       </c>
       <c r="H2" t="n">
         <v>8.306765334619181</v>
@@ -527,7 +527,7 @@
         <v>-1.945093541270408</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.4579186939869491</v>
+        <v>-3.044232424142641</v>
       </c>
       <c r="L2" t="n">
         <v>5.01543402671814</v>
@@ -553,7 +553,7 @@
         <v>15.74764043092728</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2834097224933642</v>
+        <v>5.22944814093343</v>
       </c>
       <c r="H3" t="n">
         <v>15.67967960362973</v>
@@ -565,7 +565,7 @@
         <v>-8.753415186097419</v>
       </c>
       <c r="K3" t="n">
-        <v>4.954820271343294</v>
+        <v>0.008781852903227971</v>
       </c>
       <c r="L3" t="n">
         <v>10.28646039962769</v>
@@ -591,7 +591,7 @@
         <v>23.1667366027832</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6100384473891095</v>
+        <v>7.701324314756554</v>
       </c>
       <c r="H4" t="n">
         <v>22.3109710150348</v>
@@ -603,7 +603,7 @@
         <v>-12.04317274164832</v>
       </c>
       <c r="K4" t="n">
-        <v>7.620448435112452</v>
+        <v>0.529162567745006</v>
       </c>
       <c r="L4" t="n">
         <v>15.77010941505432</v>
@@ -629,7 +629,7 @@
         <v>30.28361445665359</v>
       </c>
       <c r="G5" t="n">
-        <v>1.053359069074734</v>
+        <v>10.08502655826333</v>
       </c>
       <c r="H5" t="n">
         <v>28.33136463537102</v>
@@ -641,7 +641,7 @@
         <v>-12.08501115616109</v>
       </c>
       <c r="K5" t="n">
-        <v>7.637930026244192</v>
+        <v>-1.393737462944404</v>
       </c>
       <c r="L5" t="n">
         <v>21.42563843727112</v>
@@ -667,7 +667,7 @@
         <v>37.09970450401306</v>
       </c>
       <c r="G6" t="n">
-        <v>1.607051367755741</v>
+        <v>12.3824108185826</v>
       </c>
       <c r="H6" t="n">
         <v>33.83221193773886</v>
@@ -679,7 +679,7 @@
         <v>-8.193323856318347</v>
       </c>
       <c r="K6" t="n">
-        <v>4.192563937751054</v>
+        <v>-6.582795513075803</v>
       </c>
       <c r="L6" t="n">
         <v>27.2145357131958</v>
@@ -705,7 +705,7 @@
         <v>43.61702632904053</v>
       </c>
       <c r="G7" t="n">
-        <v>2.263696227475027</v>
+        <v>14.59355353798953</v>
       </c>
       <c r="H7" t="n">
         <v>38.8789471360054</v>
@@ -717,7 +717,7 @@
         <v>-8.311281322075134</v>
       </c>
       <c r="K7" t="n">
-        <v>5.127828414156189</v>
+        <v>-7.202028896358314</v>
       </c>
       <c r="L7" t="n">
         <v>33.10052084922791</v>
@@ -743,7 +743,7 @@
         <v>49.83818560838699</v>
       </c>
       <c r="G8" t="n">
-        <v>3.01485362797923</v>
+        <v>16.71734054847584</v>
       </c>
       <c r="H8" t="n">
         <v>43.51963005029914</v>
@@ -755,7 +755,7 @@
         <v>-5.171464322903</v>
       </c>
       <c r="K8" t="n">
-        <v>3.097615694988355</v>
+        <v>-10.60487122550825</v>
       </c>
       <c r="L8" t="n">
         <v>39.04954195022583</v>
@@ -781,7 +781,7 @@
         <v>55.76637578010559</v>
       </c>
       <c r="G9" t="n">
-        <v>3.851180243942212</v>
+        <v>18.75191837698277</v>
       </c>
       <c r="H9" t="n">
         <v>47.79053863551978</v>
@@ -793,7 +793,7 @@
         <v>-6.634700818295123</v>
       </c>
       <c r="K9" t="n">
-        <v>5.899531749309721</v>
+        <v>-9.001206383730835</v>
       </c>
       <c r="L9" t="n">
         <v>45.02977681159973</v>
@@ -819,7 +819,7 @@
         <v>61.40537697076797</v>
       </c>
       <c r="G10" t="n">
-        <v>4.762574860949703</v>
+        <v>20.69503881460975</v>
       </c>
       <c r="H10" t="n">
         <v>51.71994146534372</v>
@@ -831,7 +831,7 @@
         <v>-14.10077749305779</v>
       </c>
       <c r="K10" t="n">
-        <v>14.88181664455112</v>
+        <v>-1.050647309108927</v>
       </c>
       <c r="L10" t="n">
         <v>51.01163530349731</v>
@@ -857,7 +857,7 @@
         <v>66.75955736637115</v>
       </c>
       <c r="G11" t="n">
-        <v>5.738338041100786</v>
+        <v>22.54432173840143</v>
       </c>
       <c r="H11" t="n">
         <v>55.33068497294368</v>
@@ -869,7 +869,7 @@
         <v>-17.65367011789323</v>
       </c>
       <c r="K11" t="n">
-        <v>20.08590638391232</v>
+        <v>3.279922686611684</v>
       </c>
       <c r="L11" t="n">
         <v>56.96775412559509</v>
@@ -895,7 +895,7 @@
         <v>71.83387196063995</v>
       </c>
       <c r="G12" t="n">
-        <v>6.767340374005929</v>
+        <v>24.29745494400631</v>
       </c>
       <c r="H12" t="n">
         <v>58.6420044304606</v>
@@ -907,7 +907,7 @@
         <v>-11.71180985000244</v>
       </c>
       <c r="K12" t="n">
-        <v>15.89477455061515</v>
+        <v>-1.635340019385231</v>
       </c>
       <c r="L12" t="n">
         <v>62.87300324440002</v>
@@ -933,7 +933,7 @@
         <v>76.63386231660843</v>
       </c>
       <c r="G13" t="n">
-        <v>7.838185056218411</v>
+        <v>25.95234446962981</v>
       </c>
       <c r="H13" t="n">
         <v>61.67080210078565</v>
@@ -945,7 +945,7 @@
         <v>-13.65893444570869</v>
       </c>
       <c r="K13" t="n">
-        <v>19.66235674573823</v>
+        <v>1.548197332326826</v>
       </c>
       <c r="L13" t="n">
         <v>68.70448017120361</v>
@@ -971,7 +971,7 @@
         <v>81.16565805673599</v>
       </c>
       <c r="G14" t="n">
-        <v>8.939369493888595</v>
+        <v>27.50722739444926</v>
       </c>
       <c r="H14" t="n">
         <v>64.43255739504981</v>
@@ -983,7 +983,7 @@
         <v>-7.136389072964776</v>
       </c>
       <c r="K14" t="n">
-        <v>15.00477806561599</v>
+        <v>-3.563079834944676</v>
       </c>
       <c r="L14" t="n">
         <v>74.44151496887207</v>
@@ -1009,7 +1009,7 @@
         <v>85.43597596883774</v>
       </c>
       <c r="G15" t="n">
-        <v>10.0594354568538</v>
+        <v>28.96075377193128</v>
       </c>
       <c r="H15" t="n">
         <v>66.94197463240423</v>
@@ -1021,7 +1021,7 @@
         <v>-6.108594804165955</v>
       </c>
       <c r="K15" t="n">
-        <v>15.86499153445503</v>
+        <v>-3.036326780622455</v>
       </c>
       <c r="L15" t="n">
         <v>80.06566405296326</v>
@@ -1047,7 +1047,7 @@
         <v>89.45211935043335</v>
       </c>
       <c r="G16" t="n">
-        <v>11.18710685144444</v>
+        <v>30.3120461043778</v>
       </c>
       <c r="H16" t="n">
         <v>69.21343663480525</v>
@@ -1059,7 +1059,7 @@
         <v>-2.625501860007036</v>
       </c>
       <c r="K16" t="n">
-        <v>14.27460199283323</v>
+        <v>-4.850337260100135</v>
       </c>
       <c r="L16" t="n">
         <v>85.56071496009827</v>
@@ -1085,7 +1085,7 @@
         <v>93.22197932004929</v>
       </c>
       <c r="G17" t="n">
-        <v>12.3114161914133</v>
+        <v>31.5607398441365</v>
       </c>
       <c r="H17" t="n">
         <v>71.26132766061156</v>
@@ -1097,7 +1097,7 @@
         <v>-2.936803997128449</v>
       </c>
       <c r="K17" t="n">
-        <v>16.46757759209895</v>
+        <v>-2.781746060624252</v>
       </c>
       <c r="L17" t="n">
         <v>90.91268944740295</v>
@@ -1123,7 +1123,7 @@
         <v>96.75403422117233</v>
       </c>
       <c r="G18" t="n">
-        <v>13.42181709598683</v>
+        <v>32.70700815622536</v>
       </c>
       <c r="H18" t="n">
         <v>73.10024273875044</v>
@@ -1135,7 +1135,7 @@
         <v>-0.7614292659290338</v>
       </c>
       <c r="K18" t="n">
-        <v>16.14934339717764</v>
+        <v>-3.135847663060898</v>
       </c>
       <c r="L18" t="n">
         <v>96.10983395576477</v>
@@ -1161,7 +1161,7 @@
         <v>100.0573494434357</v>
       </c>
       <c r="G19" t="n">
-        <v>14.50828356327137</v>
+        <v>33.75157581675575</v>
       </c>
       <c r="H19" t="n">
         <v>74.74511869848305</v>
@@ -1173,7 +1173,7 @@
         <v>0.6424210080266849</v>
       </c>
       <c r="K19" t="n">
-        <v>16.56652264531595</v>
+        <v>-2.676769608168425</v>
       </c>
       <c r="L19" t="n">
         <v>101.1426258087158</v>
@@ -1199,7 +1199,7 @@
         <v>103.1415777206421</v>
       </c>
       <c r="G20" t="n">
-        <v>15.56139371975123</v>
+        <v>34.69572345247781</v>
       </c>
       <c r="H20" t="n">
         <v>76.21130881750022</v>
@@ -1211,7 +1211,7 @@
         <v>8.804224115684887</v>
       </c>
       <c r="K20" t="n">
-        <v>10.17974947234659</v>
+        <v>-8.954580260379982</v>
       </c>
       <c r="L20" t="n">
         <v>106.0037751197815</v>
@@ -1237,7 +1237,7 @@
         <v>106.0169587731361</v>
       </c>
       <c r="G21" t="n">
-        <v>16.57240536301691</v>
+        <v>35.54128298783034</v>
       </c>
       <c r="H21" t="n">
         <v>77.51460360919593</v>
@@ -1249,7 +1249,7 @@
         <v>11.98689558311575</v>
       </c>
       <c r="K21" t="n">
-        <v>8.717725023027125</v>
+        <v>-10.25115260178631</v>
       </c>
       <c r="L21" t="n">
         <v>110.6882183551788</v>
@@ -1275,7 +1275,7 @@
         <v>108.6943194270134</v>
       </c>
       <c r="G22" t="n">
-        <v>17.53331467743018</v>
+        <v>36.2906284256927</v>
       </c>
       <c r="H22" t="n">
         <v>78.67121687674987</v>
@@ -1287,7 +1287,7 @@
         <v>6.082978953432057</v>
       </c>
       <c r="K22" t="n">
-        <v>16.28090898770595</v>
+        <v>-2.476404760556565</v>
       </c>
       <c r="L22" t="n">
         <v>115.1931278705597</v>
@@ -1313,7 +1313,7 @@
         <v>111.185074031353</v>
       </c>
       <c r="G23" t="n">
-        <v>18.43690513843573</v>
+        <v>36.94665876890706</v>
       </c>
       <c r="H23" t="n">
         <v>79.69773679168007</v>
@@ -1325,7 +1325,7 @@
         <v>7.341080459717278</v>
       </c>
       <c r="K23" t="n">
-        <v>16.61498536166046</v>
+        <v>-1.894768268810874</v>
       </c>
       <c r="L23" t="n">
         <v>119.5178956985474</v>
@@ -1351,7 +1351,7 @@
         <v>113.5012245178223</v>
       </c>
       <c r="G24" t="n">
-        <v>19.27678848726305</v>
+        <v>37.51278097172949</v>
       </c>
       <c r="H24" t="n">
         <v>80.61106340660362</v>
@@ -1363,7 +1363,7 @@
         <v>7.279113576748939</v>
       </c>
       <c r="K24" t="n">
-        <v>18.19758017687391</v>
+        <v>-0.03841230759252845</v>
       </c>
       <c r="L24" t="n">
         <v>123.6641557216644</v>
@@ -1389,7 +1389,7 @@
         <v>115.6553587317467</v>
       </c>
       <c r="G25" t="n">
-        <v>20.04743223365554</v>
+        <v>37.99288479471285</v>
       </c>
       <c r="H25" t="n">
         <v>81.42831915286028</v>
@@ -1401,7 +1401,7 @@
         <v>8.703718248815735</v>
       </c>
       <c r="K25" t="n">
-        <v>18.21880266112855</v>
+        <v>0.2733501000712391</v>
       </c>
       <c r="L25" t="n">
         <v>127.6357629299164</v>
@@ -1427,7 +1427,7 @@
         <v>117.6606534719467</v>
       </c>
       <c r="G26" t="n">
-        <v>20.74418055680502</v>
+        <v>38.39131892043434</v>
       </c>
       <c r="H26" t="n">
         <v>82.16675138271263</v>
@@ -1439,7 +1439,7 @@
         <v>10.07696011453443</v>
       </c>
       <c r="K26" t="n">
-        <v>18.21455970610711</v>
+        <v>0.5674213424777861</v>
       </c>
       <c r="L26" t="n">
         <v>131.4388077259064</v>
@@ -1465,7 +1465,7 @@
         <v>119.5308713316917</v>
       </c>
       <c r="G27" t="n">
-        <v>21.36326783575629</v>
+        <v>38.71286252940088</v>
       </c>
       <c r="H27" t="n">
         <v>82.84362313637675</v>
@@ -1477,7 +1477,7 @@
         <v>12.20704447342378</v>
       </c>
       <c r="K27" t="n">
-        <v>17.37585455779326</v>
+        <v>0.02625986414867043</v>
       </c>
       <c r="L27" t="n">
         <v>135.0816068649292</v>
@@ -1503,7 +1503,7 @@
         <v>121.2803630232811</v>
       </c>
       <c r="G28" t="n">
-        <v>21.90182322228899</v>
+        <v>38.96269685331959</v>
       </c>
       <c r="H28" t="n">
         <v>83.47610235817838</v>
@@ -1515,7 +1515,7 @@
         <v>10.65317729503711</v>
       </c>
       <c r="K28" t="n">
-        <v>20.14396561101301</v>
+        <v>3.083091979982411</v>
       </c>
       <c r="L28" t="n">
         <v>138.5747077465057</v>
@@ -1541,7 +1541,7 @@
         <v>122.9240655303001</v>
       </c>
       <c r="G29" t="n">
-        <v>22.35787096932565</v>
+        <v>39.14637564117176</v>
       </c>
       <c r="H29" t="n">
         <v>84.08115061323279</v>
@@ -1553,7 +1553,7 @@
         <v>15.65577074704103</v>
       </c>
       <c r="K29" t="n">
-        <v>16.28028710310328</v>
+        <v>-0.5082175687428219</v>
       </c>
       <c r="L29" t="n">
         <v>141.9308903217316</v>
@@ -1579,7 +1579,7 @@
         <v>124.4775037765503</v>
       </c>
       <c r="G30" t="n">
-        <v>22.73032595258459</v>
+        <v>39.26979423973023</v>
       </c>
       <c r="H30" t="n">
         <v>84.67541032705108</v>
@@ -1591,7 +1591,7 @@
         <v>16.74875078235079</v>
       </c>
       <c r="K30" t="n">
-        <v>16.25407199910463</v>
+        <v>-0.2853962880410066</v>
       </c>
       <c r="L30" t="n">
         <v>145.1651637554169</v>
@@ -1617,7 +1617,7 @@
         <v>125.9567903876305</v>
       </c>
       <c r="G31" t="n">
-        <v>23.01898193551957</v>
+        <v>39.33915982804758</v>
       </c>
       <c r="H31" t="n">
         <v>85.27510091238689</v>
@@ -1629,7 +1629,7 @@
         <v>17.87438333782273</v>
       </c>
       <c r="K31" t="n">
-        <v>16.12766064845548</v>
+        <v>-0.1925172440725333</v>
       </c>
       <c r="L31" t="n">
         <v>148.2947638034821</v>
@@ -1655,7 +1655,7 @@
         <v>127.3786235451698</v>
       </c>
       <c r="G32" t="n">
-        <v>23.22450110330703</v>
+        <v>39.36096207950109</v>
       </c>
       <c r="H32" t="n">
         <v>85.89592804931095</v>
@@ -1667,7 +1667,7 @@
         <v>17.15004722638063</v>
       </c>
       <c r="K32" t="n">
-        <v>17.78976053630376</v>
+        <v>1.653299560109701</v>
       </c>
       <c r="L32" t="n">
         <v>151.3391599655151</v>
@@ -1693,7 +1693,7 @@
         <v>128.7602902054787</v>
       </c>
       <c r="G33" t="n">
-        <v>23.34839834846756</v>
+        <v>39.34194435857267</v>
       </c>
       <c r="H33" t="n">
         <v>86.55299620077325</v>
@@ -1705,7 +1705,7 @@
         <v>14.41333063084411</v>
       </c>
       <c r="K33" t="n">
-        <v>21.41039554918826</v>
+        <v>5.416849539083154</v>
       </c>
       <c r="L33" t="n">
         <v>154.3200492858887</v>
@@ -1731,7 +1731,7 @@
         <v>130.1196644306183</v>
       </c>
       <c r="G34" t="n">
-        <v>23.3930243426538</v>
+        <v>39.28907739495488</v>
       </c>
       <c r="H34" t="n">
         <v>87.26074160042742</v>
@@ -1743,7 +1743,7 @@
         <v>13.18193450379734</v>
       </c>
       <c r="K34" t="n">
-        <v>23.48104384516746</v>
+        <v>7.584990792866384</v>
       </c>
       <c r="L34" t="n">
         <v>157.2613613605499</v>
@@ -1769,7 +1769,7 @@
         <v>131.4752058386803</v>
       </c>
       <c r="G35" t="n">
-        <v>23.36155418262033</v>
+        <v>39.20953391717236</v>
       </c>
       <c r="H35" t="n">
         <v>88.03288086276724</v>
@@ -1781,7 +1781,7 @@
         <v>10.53469710115306</v>
       </c>
       <c r="K35" t="n">
-        <v>26.93362624950406</v>
+        <v>11.08564651495203</v>
       </c>
       <c r="L35" t="n">
         <v>160.1892533302307</v>
@@ -1807,7 +1807,7 @@
         <v>132.8459639549255</v>
       </c>
       <c r="G36" t="n">
-        <v>23.25797045704835</v>
+        <v>39.11066735850467</v>
       </c>
       <c r="H36" t="n">
         <v>88.88237147505414</v>
@@ -1819,7 +1819,7 @@
         <v>14.38907876825045</v>
       </c>
       <c r="K36" t="n">
-        <v>23.86304169882229</v>
+        <v>8.010344797365965</v>
       </c>
       <c r="L36" t="n">
         <v>163.1321144104004</v>
@@ -1845,7 +1845,7 @@
         <v>134.251572906971</v>
       </c>
       <c r="G37" t="n">
-        <v>23.08705582812599</v>
+        <v>38.99999225307309</v>
       </c>
       <c r="H37" t="n">
         <v>89.82139324677243</v>
@@ -1857,7 +1857,7 @@
         <v>16.11645711097677</v>
       </c>
       <c r="K37" t="n">
-        <v>22.91185492742067</v>
+        <v>6.998918502473568</v>
       </c>
       <c r="L37" t="n">
         <v>166.1205613613129</v>
@@ -1883,7 +1883,7 @@
         <v>135.7122554183006</v>
       </c>
       <c r="G38" t="n">
-        <v>22.85438830034078</v>
+        <v>38.88516981348979</v>
       </c>
       <c r="H38" t="n">
         <v>90.86134782506865</v>
@@ -1895,7 +1895,7 @@
         <v>19.29991270224928</v>
       </c>
       <c r="K38" t="n">
-        <v>20.51248442757407</v>
+        <v>4.481702914425053</v>
       </c>
       <c r="L38" t="n">
         <v>169.1874423027039</v>
@@ -1921,7 +1921,7 @@
         <v>137.2488216757774</v>
       </c>
       <c r="G39" t="n">
-        <v>22.56634638413218</v>
+        <v>38.77399697719627</v>
       </c>
       <c r="H39" t="n">
         <v>92.01286479624437</v>
@@ -1933,7 +1933,7 @@
         <v>21.28907576483529</v>
       </c>
       <c r="K39" t="n">
-        <v>19.332310817687</v>
+        <v>3.124660224622911</v>
       </c>
       <c r="L39" t="n">
         <v>172.3678362369537</v>
@@ -1959,7 +1959,7 @@
         <v>138.8826679587364</v>
       </c>
       <c r="G40" t="n">
-        <v>22.23012006344638</v>
+        <v>38.67440060583528</v>
       </c>
       <c r="H40" t="n">
         <v>93.28583226208926</v>
@@ -1971,7 +1971,7 @@
         <v>20.17153856923074</v>
       </c>
       <c r="K40" t="n">
-        <v>21.30219149580196</v>
+        <v>4.857910953413057</v>
       </c>
       <c r="L40" t="n">
         <v>175.6990518569946</v>
@@ -1997,7 +1997,7 @@
         <v>140.6357783675194</v>
       </c>
       <c r="G41" t="n">
-        <v>21.85373722402712</v>
+        <v>38.59443687368142</v>
       </c>
       <c r="H41" t="n">
         <v>94.68942467731159</v>
@@ -2009,7 +2009,7 @@
         <v>21.7276702831632</v>
       </c>
       <c r="K41" t="n">
-        <v>20.66156169859631</v>
+        <v>3.920862048942016</v>
       </c>
       <c r="L41" t="n">
         <v>179.2206263542175</v>
@@ -2035,7 +2035,7 @@
         <v>142.5307248830795</v>
       </c>
       <c r="G42" t="n">
-        <v>21.44610387769768</v>
+        <v>38.54229680382326</v>
       </c>
       <c r="H42" t="n">
         <v>96.23214352973977</v>
@@ -2047,7 +2047,7 @@
         <v>26.62762764498752</v>
       </c>
       <c r="K42" t="n">
-        <v>16.76131801877803</v>
+        <v>-0.3348749073475474</v>
       </c>
       <c r="L42" t="n">
         <v>182.9743266105652</v>
@@ -2073,7 +2073,7 @@
         <v>144.5906656384468</v>
       </c>
       <c r="G43" t="n">
-        <v>21.01706271973296</v>
+        <v>38.52631843076895</v>
       </c>
       <c r="H43" t="n">
         <v>97.92185731379864</v>
@@ -2085,7 +2085,7 @@
         <v>22.51197264230167</v>
       </c>
       <c r="K43" t="n">
-        <v>21.98307891714498</v>
+        <v>4.473823206108992</v>
       </c>
       <c r="L43" t="n">
         <v>187.0041513442993</v>
@@ -2111,7 +2111,7 @@
         <v>146.8393463492393</v>
       </c>
       <c r="G44" t="n">
-        <v>20.57746698417667</v>
+        <v>38.55500553267243</v>
       </c>
       <c r="H44" t="n">
         <v>99.76583712375761</v>
@@ -2123,7 +2123,7 @@
         <v>27.73643980695459</v>
       </c>
       <c r="K44" t="n">
-        <v>17.99428544384139</v>
+        <v>0.01674689534563356</v>
       </c>
       <c r="L44" t="n">
         <v>191.3563306331635</v>
@@ -2149,7 +2149,7 @@
         <v>149.301099717617</v>
       </c>
       <c r="G45" t="n">
-        <v>20.13928514792284</v>
+        <v>38.63705233192732</v>
       </c>
       <c r="H45" t="n">
         <v>101.770778041692</v>
@@ -2161,7 +2161,7 @@
         <v>28.58353428039268</v>
       </c>
       <c r="K45" t="n">
-        <v>18.53644935363875</v>
+        <v>0.03868216963427429</v>
       </c>
       <c r="L45" t="n">
         <v>196.079320192337</v>
@@ -2187,7 +2187,7 @@
         <v>152.000846683979</v>
       </c>
       <c r="G46" t="n">
-        <v>19.71572056659708</v>
+        <v>38.78137783272454</v>
       </c>
       <c r="H46" t="n">
         <v>103.942814021087</v>
@@ -2199,7 +2199,7 @@
         <v>33.18634592045535</v>
       </c>
       <c r="K46" t="n">
-        <v>15.50119159484117</v>
+        <v>-3.564465671286293</v>
       </c>
       <c r="L46" t="n">
         <v>201.22380900383</v>
@@ -2225,7 +2225,7 @@
         <v>154.964094042778</v>
       </c>
       <c r="G47" t="n">
-        <v>19.32136718589418</v>
+        <v>38.99716536776136</v>
       </c>
       <c r="H47" t="n">
         <v>106.2874994536535</v>
@@ -2237,7 +2237,7 @@
         <v>37.1998620319838</v>
       </c>
       <c r="K47" t="n">
-        <v>13.25876754002618</v>
+        <v>-6.417030641841002</v>
       </c>
       <c r="L47" t="n">
         <v>206.8427138328552</v>
@@ -2263,7 +2263,7 @@
         <v>158.2169361710548</v>
       </c>
       <c r="G48" t="n">
-        <v>18.9723857526461</v>
+        <v>39.2939107908675</v>
       </c>
       <c r="H48" t="n">
         <v>108.80977451766</v>
@@ -2275,7 +2275,7 @@
         <v>39.69275712450992</v>
       </c>
       <c r="K48" t="n">
-        <v>12.76612072013405</v>
+        <v>-7.555404318087341</v>
       </c>
       <c r="L48" t="n">
         <v>212.991183757782</v>
@@ -2301,7 +2301,7 @@
         <v>161.786055803299</v>
       </c>
       <c r="G49" t="n">
-        <v>18.6867157605099</v>
+        <v>39.68147723019083</v>
       </c>
       <c r="H49" t="n">
         <v>111.5138900688956</v>
@@ -2313,7 +2313,7 @@
         <v>42.52924426710228</v>
       </c>
       <c r="K49" t="n">
-        <v>12.1848734216308</v>
+        <v>-8.809888048050126</v>
       </c>
       <c r="L49" t="n">
         <v>219.7265973091125</v>
@@ -2339,7 +2339,7 @@
         <v>165.6987212300301</v>
       </c>
       <c r="G50" t="n">
-        <v>18.48430975228594</v>
+        <v>40.1701566951564</v>
       </c>
       <c r="H50" t="n">
         <v>114.4032957793948</v>
@@ -2351,7 +2351,7 @@
         <v>41.26485909291869</v>
       </c>
       <c r="K50" t="n">
-        <v>15.98540036556252</v>
+        <v>-5.700446577307943</v>
       </c>
       <c r="L50" t="n">
         <v>227.1085615158081</v>
@@ -2377,7 +2377,7 @@
         <v>169.9827892780304</v>
       </c>
       <c r="G51" t="n">
-        <v>18.38739757509961</v>
+        <v>40.77073842495055</v>
       </c>
       <c r="H51" t="n">
         <v>117.4804888997698</v>
@@ -2389,7 +2389,7 @@
         <v>43.50071802861427</v>
       </c>
       <c r="K51" t="n">
-        <v>16.59243924612798</v>
+        <v>-5.790901603722958</v>
       </c>
       <c r="L51" t="n">
         <v>235.1989140510559</v>
@@ -2415,7 +2415,7 @@
         <v>174.666702747345</v>
       </c>
       <c r="G52" t="n">
-        <v>18.42077588820602</v>
+        <v>41.49458234716073</v>
       </c>
       <c r="H52" t="n">
         <v>120.7468114862955</v>
@@ -2427,7 +2427,7 @@
         <v>47.79824615604387</v>
       </c>
       <c r="K52" t="n">
-        <v>15.47025629521547</v>
+        <v>-7.603550163739243</v>
       </c>
       <c r="L52" t="n">
         <v>244.061723947525</v>
@@ -2453,7 +2453,7 @@
         <v>179.7794927954674</v>
       </c>
       <c r="G53" t="n">
-        <v>18.61211176586196</v>
+        <v>42.35369782390887</v>
       </c>
       <c r="H53" t="n">
         <v>124.2021928542878</v>
@@ -2465,7 +2465,7 @@
         <v>48.23811911783717</v>
       </c>
       <c r="K53" t="n">
-        <v>18.56363023194041</v>
+        <v>-5.177955826106512</v>
       </c>
       <c r="L53" t="n">
         <v>253.7632865905762</v>
@@ -2491,7 +2491,7 @@
         <v>185.3507773280144</v>
       </c>
       <c r="G54" t="n">
-        <v>18.99226673737393</v>
+        <v>43.36082611602388</v>
       </c>
       <c r="H54" t="n">
         <v>127.8448406341554</v>
@@ -2503,7 +2503,7 @@
         <v>51.2475175541022</v>
       </c>
       <c r="K54" t="n">
-        <v>19.47056594718946</v>
+        <v>-4.897993431460492</v>
       </c>
       <c r="L54" t="n">
         <v>264.3721330165863</v>
@@ -2529,7 +2529,7 @@
         <v>191.4107611179352</v>
       </c>
       <c r="G55" t="n">
-        <v>19.59561757915424</v>
+        <v>44.52952543831268</v>
       </c>
       <c r="H55" t="n">
         <v>131.670862546845</v>
@@ -2541,7 +2541,7 @@
         <v>53.8084524036118</v>
       </c>
       <c r="K55" t="n">
-        <v>21.23398978014418</v>
+        <v>-3.699918079014267</v>
       </c>
       <c r="L55" t="n">
         <v>275.959020614624</v>
@@ -2567,7 +2567,7 @@
         <v>197.9902364611626</v>
       </c>
       <c r="G56" t="n">
-        <v>20.46038267041456</v>
+        <v>45.87425774419418</v>
       </c>
       <c r="H56" t="n">
         <v>135.6738214868723</v>
@@ -2579,7 +2579,7 @@
         <v>55.53933021340457</v>
       </c>
       <c r="K56" t="n">
-        <v>24.26027232667296</v>
+        <v>-1.15360274710666</v>
       </c>
       <c r="L56" t="n">
         <v>288.596935749054</v>
@@ -2605,7 +2605,7 @@
         <v>205.1205834746361</v>
       </c>
       <c r="G57" t="n">
-        <v>21.62892370321029</v>
+        <v>47.41047671287962</v>
       </c>
       <c r="H57" t="n">
         <v>139.844214847546</v>
@@ -2617,7 +2617,7 @@
         <v>58.11351133572528</v>
       </c>
       <c r="K57" t="n">
-        <v>26.90085600578941</v>
+        <v>1.119302996120076</v>
       </c>
       <c r="L57" t="n">
         <v>302.3610966205597</v>
@@ -2643,7 +2643,7 @@
         <v>212.8337680697441</v>
       </c>
       <c r="G58" t="n">
-        <v>23.14802977229899</v>
+        <v>49.15471372923957</v>
       </c>
       <c r="H58" t="n">
         <v>144.1688655305442</v>
@@ -2655,7 +2655,7 @@
         <v>59.59933730424572</v>
       </c>
       <c r="K58" t="n">
-        <v>31.11250904678676</v>
+        <v>5.105825089846185</v>
       </c>
       <c r="L58" t="n">
         <v>317.3289511203766</v>
@@ -2681,7 +2681,7 @@
         <v>221.162345468998</v>
       </c>
       <c r="G59" t="n">
-        <v>25.06915655309442</v>
+        <v>51.12466315781803</v>
       </c>
       <c r="H59" t="n">
         <v>148.6302157138101</v>
@@ -2693,7 +2693,7 @@
         <v>64.24728210828241</v>
       </c>
       <c r="K59" t="n">
-        <v>32.6705964745689</v>
+        <v>6.615089869845292</v>
       </c>
       <c r="L59" t="n">
         <v>333.5801780223846</v>
@@ -2719,7 +2719,7 @@
         <v>230.1394554376602</v>
       </c>
       <c r="G60" t="n">
-        <v>27.44862204242059</v>
+        <v>53.33926304455639</v>
       </c>
       <c r="H60" t="n">
         <v>153.2055093192255</v>
@@ -2731,7 +2731,7 @@
         <v>66.24644729424173</v>
       </c>
       <c r="K60" t="n">
-        <v>37.41315100629097</v>
+        <v>11.52251000415518</v>
       </c>
       <c r="L60" t="n">
         <v>351.1966829299927</v>
@@ -2757,7 +2757,7 @@
         <v>239.7988273501396</v>
       </c>
       <c r="G61" t="n">
-        <v>30.34773555612693</v>
+        <v>55.8187734274934</v>
       </c>
       <c r="H61" t="n">
         <v>157.8658423246366</v>
@@ -2769,7 +2769,7 @@
         <v>70.19190504927502</v>
       </c>
       <c r="K61" t="n">
-        <v>40.77430212015324</v>
+        <v>15.30326424878677</v>
       </c>
       <c r="L61" t="n">
         <v>370.26260638237</v>
@@ -2795,7 +2795,7 @@
         <v>250.1747761964798</v>
       </c>
       <c r="G62" t="n">
-        <v>33.83286349733605</v>
+        <v>58.58484741858675</v>
       </c>
       <c r="H62" t="n">
         <v>162.5750442543452</v>
@@ -2807,7 +2807,7 @@
         <v>17.64928148140623</v>
       </c>
       <c r="K62" t="n">
-        <v>101.2206750385831</v>
+        <v>76.46869111733241</v>
       </c>
       <c r="L62" t="n">
         <v>390.8643152713776</v>

</xml_diff>

<commit_message>
removing the not maintained folder, updating some files
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -506,10 +506,10 @@
         <v>8.588104877825529</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.9997490009044095</v>
+        <v>-0.8661664253000624</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.318128058305656</v>
+        <v>-2.451710633910005</v>
       </c>
       <c r="F2" t="n">
         <v>8.025480389595032</v>
@@ -521,13 +521,13 @@
         <v>8.306765334619181</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.9669980120382063</v>
+        <v>-0.8377914962672564</v>
       </c>
       <c r="J2" t="n">
         <v>-1.945093541270408</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.044232424142641</v>
+        <v>-3.173438939913591</v>
       </c>
       <c r="L2" t="n">
         <v>5.01543402671814</v>
@@ -544,10 +544,10 @@
         <v>16.3845391446805</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.962458580677453</v>
+        <v>-1.694930593802125</v>
       </c>
       <c r="E3" t="n">
-        <v>-4.138971292906723</v>
+        <v>-4.406499279782053</v>
       </c>
       <c r="F3" t="n">
         <v>15.74764043092728</v>
@@ -559,13 +559,13 @@
         <v>15.67967960362973</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.878034011741283</v>
+        <v>-1.622015024440618</v>
       </c>
       <c r="J3" t="n">
         <v>-8.753415186097419</v>
       </c>
       <c r="K3" t="n">
-        <v>0.008781852903227971</v>
+        <v>-0.2472371343974373</v>
       </c>
       <c r="L3" t="n">
         <v>10.28646039962769</v>
@@ -582,10 +582,10 @@
         <v>23.48305040986538</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.871497094671384</v>
+        <v>-2.472200796769541</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.550720618801932</v>
+        <v>-5.950016916703774</v>
       </c>
       <c r="F4" t="n">
         <v>23.1667366027832</v>
@@ -597,13 +597,13 @@
         <v>22.3109710150348</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.728175740833712</v>
+        <v>-2.348809007236099</v>
       </c>
       <c r="J4" t="n">
         <v>-12.04317274164832</v>
       </c>
       <c r="K4" t="n">
-        <v>0.529162567745006</v>
+        <v>0.1497958341473922</v>
       </c>
       <c r="L4" t="n">
         <v>15.77010941505432</v>
@@ -620,10 +620,10 @@
         <v>29.95353398112397</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.713091007831708</v>
+        <v>-3.186475915690775</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.619293583229076</v>
+        <v>-7.145908675370006</v>
       </c>
       <c r="F5" t="n">
         <v>30.28361445665359</v>
@@ -635,13 +635,13 @@
         <v>28.33136463537102</v>
       </c>
       <c r="I5" t="n">
-        <v>-3.51200413725773</v>
+        <v>-3.013908513304431</v>
       </c>
       <c r="J5" t="n">
         <v>-12.08501115616109</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.393737462944404</v>
+        <v>-1.891833086897702</v>
       </c>
       <c r="L5" t="n">
         <v>21.42563843727112</v>
@@ -658,10 +658,10 @@
         <v>35.85080324176099</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.475989753468895</v>
+        <v>-3.828514272141826</v>
       </c>
       <c r="E6" t="n">
-        <v>-7.396313555017661</v>
+        <v>-8.043789036344732</v>
       </c>
       <c r="F6" t="n">
         <v>37.09970450401306</v>
@@ -673,13 +673,13 @@
         <v>33.83221193773886</v>
       </c>
       <c r="I6" t="n">
-        <v>-4.223967673731508</v>
+        <v>-3.612948512988407</v>
       </c>
       <c r="J6" t="n">
         <v>-8.193323856318347</v>
       </c>
       <c r="K6" t="n">
-        <v>-6.582795513075803</v>
+        <v>-7.193814673818904</v>
       </c>
       <c r="L6" t="n">
         <v>27.2145357131958</v>
@@ -696,10 +696,10 @@
         <v>41.21975235124386</v>
       </c>
       <c r="D7" t="n">
-        <v>-5.15119808231933</v>
+        <v>-4.391066881186413</v>
       </c>
       <c r="E7" t="n">
-        <v>-7.923723229953072</v>
+        <v>-8.683854431085994</v>
       </c>
       <c r="F7" t="n">
         <v>43.61702632904053</v>
@@ -711,13 +711,13 @@
         <v>38.8789471360054</v>
       </c>
       <c r="I7" t="n">
-        <v>-4.858669606333579</v>
+        <v>-4.141705066288662</v>
       </c>
       <c r="J7" t="n">
         <v>-8.311281322075134</v>
       </c>
       <c r="K7" t="n">
-        <v>-7.202028896358314</v>
+        <v>-7.918993436403225</v>
       </c>
       <c r="L7" t="n">
         <v>33.10052084922791</v>
@@ -734,10 +734,10 @@
         <v>46.09855780478731</v>
       </c>
       <c r="D8" t="n">
-        <v>-5.731748817154248</v>
+        <v>-4.868651418406087</v>
       </c>
       <c r="E8" t="n">
-        <v>-8.236616041994616</v>
+        <v>-9.099713440742775</v>
       </c>
       <c r="F8" t="n">
         <v>49.83818560838699</v>
@@ -749,13 +749,13 @@
         <v>43.51963005029914</v>
       </c>
       <c r="I8" t="n">
-        <v>-5.411093100137896</v>
+        <v>-4.596280635722908</v>
       </c>
       <c r="J8" t="n">
         <v>-5.171464322903</v>
       </c>
       <c r="K8" t="n">
-        <v>-10.60487122550825</v>
+        <v>-11.41968368992325</v>
       </c>
       <c r="L8" t="n">
         <v>39.04954195022583</v>
@@ -772,10 +772,10 @@
         <v>50.52072961031287</v>
       </c>
       <c r="D9" t="n">
-        <v>-6.212502895641747</v>
+        <v>-5.257353895268258</v>
       </c>
       <c r="E9" t="n">
-        <v>-8.365034038304149</v>
+        <v>-9.320183038677637</v>
       </c>
       <c r="F9" t="n">
         <v>55.76637578010559</v>
@@ -787,13 +787,13 @@
         <v>47.79053863551978</v>
       </c>
       <c r="I9" t="n">
-        <v>-5.876772998876862</v>
+        <v>-4.973241209903859</v>
       </c>
       <c r="J9" t="n">
         <v>-6.634700818295123</v>
       </c>
       <c r="K9" t="n">
-        <v>-9.001206383730835</v>
+        <v>-9.904738172703833</v>
       </c>
       <c r="L9" t="n">
         <v>45.02977681159973</v>
@@ -810,10 +810,10 @@
         <v>54.5164815714009</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.589966680374216</v>
+        <v>-5.554650181203242</v>
       </c>
       <c r="E10" t="n">
-        <v>-8.335174637838755</v>
+        <v>-9.370491137009729</v>
       </c>
       <c r="F10" t="n">
         <v>61.40537697076797</v>
@@ -825,13 +825,13 @@
         <v>51.71994146534372</v>
       </c>
       <c r="I10" t="n">
-        <v>-6.251920174289443</v>
+        <v>-5.269712460369079</v>
       </c>
       <c r="J10" t="n">
         <v>-14.10077749305779</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.050647309108927</v>
+        <v>-2.032855023029294</v>
       </c>
       <c r="L10" t="n">
         <v>51.01163530349731</v>
@@ -848,10 +848,10 @@
         <v>58.11366103734048</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.862121878992839</v>
+        <v>-5.759241621532886</v>
       </c>
       <c r="E11" t="n">
-        <v>-8.170218785840795</v>
+        <v>-9.273099043300753</v>
       </c>
       <c r="F11" t="n">
         <v>66.75955736637115</v>
@@ -863,13 +863,13 @@
         <v>55.33068497294368</v>
       </c>
       <c r="I11" t="n">
-        <v>-6.533505154468463</v>
+        <v>-5.483440178366101</v>
       </c>
       <c r="J11" t="n">
         <v>-17.65367011789323</v>
       </c>
       <c r="K11" t="n">
-        <v>3.279922686611684</v>
+        <v>2.229857710509322</v>
       </c>
       <c r="L11" t="n">
         <v>56.96775412559509</v>
@@ -886,10 +886,10 @@
         <v>61.33839707871358</v>
       </c>
       <c r="D12" t="n">
-        <v>-7.028263776347697</v>
+        <v>-5.870902843962126</v>
       </c>
       <c r="E12" t="n">
-        <v>-7.890927055019073</v>
+        <v>-9.048287987404645</v>
       </c>
       <c r="F12" t="n">
         <v>71.83387196063995</v>
@@ -901,13 +901,13 @@
         <v>58.6420044304606</v>
       </c>
       <c r="I12" t="n">
-        <v>-6.719306260679208</v>
+        <v>-5.612822098116215</v>
       </c>
       <c r="J12" t="n">
         <v>-11.71180985000244</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.635340019385231</v>
+        <v>-2.741824181948223</v>
       </c>
       <c r="L12" t="n">
         <v>62.87300324440002</v>
@@ -924,10 +924,10 @@
         <v>64.21555839472347</v>
       </c>
       <c r="D13" t="n">
-        <v>-7.08884862380919</v>
+        <v>-5.890339029386893</v>
       </c>
       <c r="E13" t="n">
-        <v>-7.516077816154219</v>
+        <v>-8.71458741057651</v>
       </c>
       <c r="F13" t="n">
         <v>76.63386231660843</v>
@@ -939,13 +939,13 @@
         <v>61.67080210078565</v>
       </c>
       <c r="I13" t="n">
-        <v>-6.807929285829981</v>
+        <v>-5.656914642942694</v>
       </c>
       <c r="J13" t="n">
         <v>-13.65893444570869</v>
       </c>
       <c r="K13" t="n">
-        <v>1.548197332326826</v>
+        <v>0.3971826894395356</v>
       </c>
       <c r="L13" t="n">
         <v>68.70448017120361</v>
@@ -962,10 +962,10 @@
         <v>66.7690783450869</v>
       </c>
       <c r="D14" t="n">
-        <v>-7.045346159560669</v>
+        <v>-5.819052165834346</v>
       </c>
       <c r="E14" t="n">
-        <v>-7.062797442740322</v>
+        <v>-8.289091436466638</v>
       </c>
       <c r="F14" t="n">
         <v>81.16565805673599</v>
@@ -977,13 +977,13 @@
         <v>64.43255739504981</v>
       </c>
       <c r="I14" t="n">
-        <v>-6.798800912717553</v>
+        <v>-5.615419921211172</v>
       </c>
       <c r="J14" t="n">
         <v>-7.136389072964776</v>
       </c>
       <c r="K14" t="n">
-        <v>-3.563079834944676</v>
+        <v>-4.746460826451059</v>
       </c>
       <c r="L14" t="n">
         <v>74.44151496887207</v>
@@ -1000,10 +1000,10 @@
         <v>69.02218743856436</v>
       </c>
       <c r="D15" t="n">
-        <v>-6.900100197779203</v>
+        <v>-5.659216255400888</v>
       </c>
       <c r="E15" t="n">
-        <v>-6.546816549690107</v>
+        <v>-7.787700492068424</v>
       </c>
       <c r="F15" t="n">
         <v>85.43597596883774</v>
@@ -1015,13 +1015,13 @@
         <v>66.94197463240423</v>
       </c>
       <c r="I15" t="n">
-        <v>-6.692142766583846</v>
+        <v>-5.488656982155703</v>
       </c>
       <c r="J15" t="n">
         <v>-6.108594804165955</v>
       </c>
       <c r="K15" t="n">
-        <v>-3.036326780622455</v>
+        <v>-4.239812565050594</v>
       </c>
       <c r="L15" t="n">
         <v>80.06566405296326</v>
@@ -1038,10 +1038,10 @@
         <v>70.99756997985759</v>
       </c>
       <c r="D16" t="n">
-        <v>-6.656195515776425</v>
+        <v>-5.413559518893639</v>
       </c>
       <c r="E16" t="n">
-        <v>-5.982662971480121</v>
+        <v>-7.225298968362917</v>
       </c>
       <c r="F16" t="n">
         <v>89.45211935043335</v>
@@ -1053,13 +1053,13 @@
         <v>69.21343663480525</v>
       </c>
       <c r="I16" t="n">
-        <v>-6.488928658977612</v>
+        <v>-5.277519481807528</v>
       </c>
       <c r="J16" t="n">
         <v>-2.625501860007036</v>
       </c>
       <c r="K16" t="n">
-        <v>-4.850337260100135</v>
+        <v>-6.061746437270218</v>
       </c>
       <c r="L16" t="n">
         <v>85.56071496009827</v>
@@ -1076,10 +1076,10 @@
         <v>72.71747930781416</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.317331177193699</v>
+        <v>-5.085255092202721</v>
       </c>
       <c r="E17" t="n">
-        <v>-5.383819784203439</v>
+        <v>-6.615895869194418</v>
       </c>
       <c r="F17" t="n">
         <v>93.22197932004929</v>
@@ -1091,13 +1091,13 @@
         <v>71.26132766061156</v>
       </c>
       <c r="I17" t="n">
-        <v>-6.190827999592402</v>
+        <v>-4.983423969212176</v>
       </c>
       <c r="J17" t="n">
         <v>-2.936803997128449</v>
       </c>
       <c r="K17" t="n">
-        <v>-2.781746060624252</v>
+        <v>-3.989150091004484</v>
       </c>
       <c r="L17" t="n">
         <v>90.91268944740295</v>
@@ -1114,10 +1114,10 @@
         <v>74.20380672758927</v>
       </c>
       <c r="D18" t="n">
-        <v>-5.887702313787974</v>
+        <v>-4.67782019799734</v>
       </c>
       <c r="E18" t="n">
-        <v>-4.762842460047004</v>
+        <v>-5.972724575837638</v>
       </c>
       <c r="F18" t="n">
         <v>96.75403422117233</v>
@@ -1129,13 +1129,13 @@
         <v>73.10024273875044</v>
       </c>
       <c r="I18" t="n">
-        <v>-5.800140010221092</v>
+        <v>-4.608251342376171</v>
       </c>
       <c r="J18" t="n">
         <v>-0.7614292659290338</v>
       </c>
       <c r="K18" t="n">
-        <v>-3.135847663060898</v>
+        <v>-4.327736330905819</v>
       </c>
       <c r="L18" t="n">
         <v>96.10983395576477</v>
@@ -1152,10 +1152,10 @@
         <v>75.4781175208816</v>
       </c>
       <c r="D19" t="n">
-        <v>-5.371888711386704</v>
+        <v>-4.195021780230052</v>
       </c>
       <c r="E19" t="n">
-        <v>-4.131444895033852</v>
+        <v>-5.308311826190504</v>
       </c>
       <c r="F19" t="n">
         <v>100.0573494434357</v>
@@ -1167,13 +1167,13 @@
         <v>74.74511869848305</v>
       </c>
       <c r="I19" t="n">
-        <v>-5.319720106381245</v>
+        <v>-4.154282210592611</v>
       </c>
       <c r="J19" t="n">
         <v>0.6424210080266849</v>
       </c>
       <c r="K19" t="n">
-        <v>-2.676769608168425</v>
+        <v>-3.842207503957053</v>
       </c>
       <c r="L19" t="n">
         <v>101.1426258087158</v>
@@ -1190,10 +1190,10 @@
         <v>76.5616685062319</v>
       </c>
       <c r="D20" t="n">
-        <v>-4.774751108100355</v>
+        <v>-3.640790406996849</v>
       </c>
       <c r="E20" t="n">
-        <v>-3.500566792320569</v>
+        <v>-4.634527493424088</v>
       </c>
       <c r="F20" t="n">
         <v>103.1415777206421</v>
@@ -1205,13 +1205,13 @@
         <v>76.21130881750022</v>
       </c>
       <c r="I20" t="n">
-        <v>-4.75290100550144</v>
+        <v>-3.624129508421619</v>
       </c>
       <c r="J20" t="n">
         <v>8.804224115684887</v>
       </c>
       <c r="K20" t="n">
-        <v>-8.954580260379982</v>
+        <v>-10.08335175745981</v>
       </c>
       <c r="L20" t="n">
         <v>106.0037751197815</v>
@@ -1228,10 +1228,10 @@
         <v>77.47540131647709</v>
       </c>
       <c r="D21" t="n">
-        <v>-4.101335960962701</v>
+        <v>-3.019141688486402</v>
       </c>
       <c r="E21" t="n">
-        <v>-2.880414895574155</v>
+        <v>-3.962609168050456</v>
       </c>
       <c r="F21" t="n">
         <v>106.0169587731361</v>
@@ -1243,13 +1243,13 @@
         <v>77.51460360919593</v>
       </c>
       <c r="I21" t="n">
-        <v>-4.103411223176875</v>
+        <v>-3.020669364035293</v>
       </c>
       <c r="J21" t="n">
         <v>11.98689558311575</v>
       </c>
       <c r="K21" t="n">
-        <v>-10.25115260178631</v>
+        <v>-11.33389446092788</v>
       </c>
       <c r="L21" t="n">
         <v>110.6882183551788</v>
@@ -1266,10 +1266,10 @@
         <v>78.23991896721151</v>
       </c>
       <c r="D22" t="n">
-        <v>-3.35678731937662</v>
+        <v>-2.334104189993511</v>
       </c>
       <c r="E22" t="n">
-        <v>-2.280485135245613</v>
+        <v>-3.303168264628724</v>
       </c>
       <c r="F22" t="n">
         <v>108.6943194270134</v>
@@ -1281,13 +1281,13 @@
         <v>78.67121687674987</v>
       </c>
       <c r="I22" t="n">
-        <v>-3.375291624758362</v>
+        <v>-2.346970949968183</v>
       </c>
       <c r="J22" t="n">
         <v>6.082978953432057</v>
       </c>
       <c r="K22" t="n">
-        <v>-2.476404760556565</v>
+        <v>-3.504725435346745</v>
       </c>
       <c r="L22" t="n">
         <v>115.1931278705597</v>
@@ -1304,10 +1304,10 @@
         <v>78.87544951269686</v>
       </c>
       <c r="D23" t="n">
-        <v>-2.546266874782809</v>
+        <v>-1.589655569333166</v>
       </c>
       <c r="E23" t="n">
-        <v>-1.709567497910527</v>
+        <v>-2.666178803360182</v>
       </c>
       <c r="F23" t="n">
         <v>111.185074031353</v>
@@ -1319,13 +1319,13 @@
         <v>79.69773679168007</v>
       </c>
       <c r="I23" t="n">
-        <v>-2.572812052946176</v>
+        <v>-1.606227944650241</v>
       </c>
       <c r="J23" t="n">
         <v>7.341080459717278</v>
       </c>
       <c r="K23" t="n">
-        <v>-1.894768268810874</v>
+        <v>-2.861352377106807</v>
       </c>
       <c r="L23" t="n">
         <v>119.5178956985474</v>
@@ -1342,10 +1342,10 @@
         <v>79.40180009844106</v>
       </c>
       <c r="D24" t="n">
-        <v>-1.674882023311786</v>
+        <v>-0.7896628264023733</v>
       </c>
       <c r="E24" t="n">
-        <v>-1.175737508840648</v>
+        <v>-2.060956705750051</v>
       </c>
       <c r="F24" t="n">
         <v>113.5012245178223</v>
@@ -1357,13 +1357,13 @@
         <v>80.61106340660362</v>
       </c>
       <c r="I24" t="n">
-        <v>-1.700389925825092</v>
+        <v>-0.8016891316070972</v>
       </c>
       <c r="J24" t="n">
         <v>7.279113576748939</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.03841230759252845</v>
+        <v>-0.9371131018105299</v>
       </c>
       <c r="L24" t="n">
         <v>123.6641557216644</v>
@@ -1380,10 +1380,10 @@
         <v>79.83830216533475</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.7476201626578376</v>
+        <v>0.06216905449482216</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.6863367749525509</v>
+        <v>-1.496125992105206</v>
       </c>
       <c r="F25" t="n">
         <v>115.6553587317467</v>
@@ -1395,13 +1395,13 @@
         <v>81.42831915286028</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.7625093665437226</v>
+        <v>0.06340718018217034</v>
       </c>
       <c r="J25" t="n">
         <v>8.703718248815735</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2733501000712391</v>
+        <v>-0.5525664466546534</v>
       </c>
       <c r="L25" t="n">
         <v>127.6357629299164</v>
@@ -1418,10 +1418,10 @@
         <v>80.20374879690084</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2307093098416394</v>
+        <v>0.9623437497390522</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.2479367729205748</v>
+        <v>-0.9795712128179801</v>
       </c>
       <c r="F26" t="n">
         <v>117.6606534719467</v>
@@ -1433,13 +1433,13 @@
         <v>82.16675138271263</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2363559657471734</v>
+        <v>0.9858973030020209</v>
       </c>
       <c r="J26" t="n">
         <v>10.07696011453443</v>
       </c>
       <c r="K26" t="n">
-        <v>0.5674213424777861</v>
+        <v>-0.1821199947770538</v>
       </c>
       <c r="L26" t="n">
         <v>131.4388077259064</v>
@@ -1456,10 +1456,10 @@
         <v>80.51632838374668</v>
       </c>
       <c r="D27" t="n">
-        <v>1.255526336255743</v>
+        <v>1.90761514358131</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1336999719177214</v>
+        <v>-0.5183888354078476</v>
       </c>
       <c r="F27" t="n">
         <v>119.5308713316917</v>
@@ -1471,13 +1471,13 @@
         <v>82.84362313637675</v>
       </c>
       <c r="I27" t="n">
-        <v>1.291816861579134</v>
+        <v>1.962754055188594</v>
       </c>
       <c r="J27" t="n">
         <v>12.20704447342378</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02625986414867043</v>
+        <v>-0.6446773294607908</v>
       </c>
       <c r="L27" t="n">
         <v>135.0816068649292</v>
@@ -1494,10 +1494,10 @@
         <v>80.79355754137686</v>
       </c>
       <c r="D28" t="n">
-        <v>2.322525694821369</v>
+        <v>2.895024033035791</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4536679921194064</v>
+        <v>-0.1188303460950237</v>
       </c>
       <c r="F28" t="n">
         <v>121.2803630232811</v>
@@ -1509,13 +1509,13 @@
         <v>83.47610235817838</v>
       </c>
       <c r="I28" t="n">
-        <v>2.399639259988254</v>
+        <v>2.991145951053311</v>
       </c>
       <c r="J28" t="n">
         <v>10.65317729503711</v>
       </c>
       <c r="K28" t="n">
-        <v>3.083091979982411</v>
+        <v>2.491585288917348</v>
       </c>
       <c r="L28" t="n">
         <v>138.5747077465057</v>
@@ -1532,10 +1532,10 @@
         <v>81.05221390576605</v>
       </c>
       <c r="D29" t="n">
-        <v>3.427716470148489</v>
+        <v>3.921929946438994</v>
       </c>
       <c r="E29" t="n">
-        <v>0.7079673098370094</v>
+        <v>0.2137538335464981</v>
       </c>
       <c r="F29" t="n">
         <v>122.9240655303001</v>
@@ -1547,13 +1547,13 @@
         <v>84.08115061323279</v>
       </c>
       <c r="I29" t="n">
-        <v>3.555810889028792</v>
+        <v>4.068493217279361</v>
       </c>
       <c r="J29" t="n">
         <v>15.65577074704103</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.5082175687428219</v>
+        <v>-1.02089989699337</v>
       </c>
       <c r="L29" t="n">
         <v>141.9308903217316</v>
@@ -1570,10 +1570,10 @@
         <v>81.30826869889769</v>
       </c>
       <c r="D30" t="n">
-        <v>4.567456964033441</v>
+        <v>4.986040124720872</v>
       </c>
       <c r="E30" t="n">
-        <v>0.8935583428274256</v>
+        <v>0.4749751821399926</v>
       </c>
       <c r="F30" t="n">
         <v>124.4775037765503</v>
@@ -1585,13 +1585,13 @@
         <v>84.67541032705108</v>
       </c>
       <c r="I30" t="n">
-        <v>4.756604694325779</v>
+        <v>5.192522239421445</v>
       </c>
       <c r="J30" t="n">
         <v>16.74875078235079</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.2853962880410066</v>
+        <v>-0.7213138331366693</v>
       </c>
       <c r="L30" t="n">
         <v>145.1651637554169</v>
@@ -1608,10 +1608,10 @@
         <v>81.57682547474236</v>
       </c>
       <c r="D31" t="n">
-        <v>5.738483518576856</v>
+        <v>6.085434319992491</v>
       </c>
       <c r="E31" t="n">
-        <v>1.008412171528576</v>
+        <v>0.6614613701129457</v>
       </c>
       <c r="F31" t="n">
         <v>125.9567903876305</v>
@@ -1623,13 +1623,13 @@
         <v>85.27510091238689</v>
       </c>
       <c r="I31" t="n">
-        <v>5.998636969297387</v>
+        <v>6.361316742997482</v>
       </c>
       <c r="J31" t="n">
         <v>17.87438333782273</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.1925172440725333</v>
+        <v>-0.5551970177726133</v>
       </c>
       <c r="L31" t="n">
         <v>148.2947638034821</v>
@@ -1646,10 +1646,10 @@
         <v>81.87206625962428</v>
       </c>
       <c r="D32" t="n">
-        <v>6.937936218857907</v>
+        <v>7.218587216502891</v>
       </c>
       <c r="E32" t="n">
-        <v>1.051553976319056</v>
+        <v>0.7709029786740729</v>
       </c>
       <c r="F32" t="n">
         <v>127.3786235451698</v>
@@ -1661,13 +1661,13 @@
         <v>85.89592804931095</v>
       </c>
       <c r="I32" t="n">
-        <v>7.278923050212781</v>
+        <v>7.573367529288659</v>
       </c>
       <c r="J32" t="n">
         <v>17.15004722638063</v>
       </c>
       <c r="K32" t="n">
-        <v>1.653299560109701</v>
+        <v>1.358855081033823</v>
       </c>
       <c r="L32" t="n">
         <v>151.3391599655151</v>
@@ -1684,10 +1684,10 @@
         <v>82.2072009042118</v>
       </c>
       <c r="D33" t="n">
-        <v>8.163380236682379</v>
+        <v>8.38438764590081</v>
       </c>
       <c r="E33" t="n">
-        <v>1.023109803880779</v>
+        <v>0.8021023946623345</v>
       </c>
       <c r="F33" t="n">
         <v>128.7602902054787</v>
@@ -1699,13 +1699,13 @@
         <v>86.55299620077325</v>
       </c>
       <c r="I33" t="n">
-        <v>8.594928556615498</v>
+        <v>8.827619284921825</v>
       </c>
       <c r="J33" t="n">
         <v>14.41333063084411</v>
       </c>
       <c r="K33" t="n">
-        <v>5.416849539083154</v>
+        <v>5.184158810776802</v>
       </c>
       <c r="L33" t="n">
         <v>154.3200492858887</v>
@@ -1722,10 +1722,10 @@
         <v>82.59442842984855</v>
       </c>
       <c r="D34" t="n">
-        <v>9.412823540830098</v>
+        <v>9.582156841162433</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9243387459696564</v>
+        <v>0.7550054456373303</v>
       </c>
       <c r="F34" t="n">
         <v>130.1196644306183</v>
@@ -1737,13 +1737,13 @@
         <v>87.26074160042742</v>
       </c>
       <c r="I34" t="n">
-        <v>9.944617068503899</v>
+        <v>10.12351714258332</v>
       </c>
       <c r="J34" t="n">
         <v>13.18193450379734</v>
       </c>
       <c r="K34" t="n">
-        <v>7.584990792866384</v>
+        <v>7.406090718786961</v>
       </c>
       <c r="L34" t="n">
         <v>157.2613613605499</v>
@@ -1760,10 +1760,10 @@
         <v>83.04491049241632</v>
       </c>
       <c r="D35" t="n">
-        <v>10.6847322135076</v>
+        <v>10.8116637764354</v>
       </c>
       <c r="E35" t="n">
-        <v>0.7576535847671835</v>
+        <v>0.6307220218393894</v>
       </c>
       <c r="F35" t="n">
         <v>131.4752058386803</v>
@@ -1775,13 +1775,13 @@
         <v>88.03288086276724</v>
       </c>
       <c r="I35" t="n">
-        <v>11.32649493418603</v>
+        <v>11.46105045469524</v>
       </c>
       <c r="J35" t="n">
         <v>10.53469710115306</v>
       </c>
       <c r="K35" t="n">
-        <v>11.08564651495203</v>
+        <v>10.95109099444283</v>
       </c>
       <c r="L35" t="n">
         <v>160.1892533302307</v>
@@ -1798,10 +1798,10 @@
         <v>83.56875065539455</v>
       </c>
       <c r="D36" t="n">
-        <v>11.97804226748578</v>
+        <v>12.07314060156116</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5266417418441804</v>
+        <v>0.4315434077688067</v>
       </c>
       <c r="F36" t="n">
         <v>132.8459639549255</v>
@@ -1813,13 +1813,13 @@
         <v>88.88237147505414</v>
       </c>
       <c r="I36" t="n">
-        <v>12.73965201122516</v>
+        <v>12.84079706113505</v>
       </c>
       <c r="J36" t="n">
         <v>14.38907876825045</v>
       </c>
       <c r="K36" t="n">
-        <v>8.010344797365965</v>
+        <v>7.909199747456077</v>
       </c>
       <c r="L36" t="n">
         <v>163.1321144104004</v>
@@ -1836,10 +1836,10 @@
         <v>84.17498847128414</v>
       </c>
       <c r="D37" t="n">
-        <v>13.29216992967017</v>
+        <v>13.36729509409701</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2360624974537231</v>
+        <v>0.1609373330268866</v>
       </c>
       <c r="F37" t="n">
         <v>134.251572906971</v>
@@ -1851,13 +1851,13 @@
         <v>89.82139324677243</v>
       </c>
       <c r="I37" t="n">
-        <v>14.183800248017</v>
+        <v>14.26396476076907</v>
       </c>
       <c r="J37" t="n">
         <v>16.11645711097677</v>
       </c>
       <c r="K37" t="n">
-        <v>6.998918502473568</v>
+        <v>6.91875398972152</v>
       </c>
       <c r="L37" t="n">
         <v>166.1205613613129</v>
@@ -1874,10 +1874,10 @@
         <v>84.87160657781986</v>
       </c>
       <c r="D38" t="n">
-        <v>14.62701961362257</v>
+        <v>14.69532515082411</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.1081612057033112</v>
+        <v>-0.1764667429048501</v>
       </c>
       <c r="F38" t="n">
         <v>135.7122554183006</v>
@@ -1889,13 +1889,13 @@
         <v>90.86134782506865</v>
       </c>
       <c r="I38" t="n">
-        <v>15.65930904747109</v>
+        <v>15.73243518970284</v>
       </c>
       <c r="J38" t="n">
         <v>19.29991270224928</v>
       </c>
       <c r="K38" t="n">
-        <v>4.481702914425053</v>
+        <v>4.408576772193296</v>
       </c>
       <c r="L38" t="n">
         <v>169.1874423027039</v>
@@ -1912,10 +1912,10 @@
         <v>85.6655400753896</v>
       </c>
       <c r="D39" t="n">
-        <v>15.98299062570808</v>
+        <v>16.05893035312515</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.4989588344471301</v>
+        <v>-0.5748985618641953</v>
       </c>
       <c r="F39" t="n">
         <v>137.2488216757774</v>
@@ -1927,13 +1927,13 @@
         <v>92.01286479624437</v>
       </c>
       <c r="I39" t="n">
-        <v>17.16723847405489</v>
+        <v>17.24880489930991</v>
       </c>
       <c r="J39" t="n">
         <v>21.28907576483529</v>
       </c>
       <c r="K39" t="n">
-        <v>3.124660224622911</v>
+        <v>3.043093799367906</v>
       </c>
       <c r="L39" t="n">
         <v>172.3678362369537</v>
@@ -1950,10 +1950,10 @@
         <v>86.56270617655886</v>
       </c>
       <c r="D40" t="n">
-        <v>17.36098196906059</v>
+        <v>17.46032460410036</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.9281500437708203</v>
+        <v>-1.027492678810596</v>
       </c>
       <c r="F40" t="n">
         <v>138.8826679587364</v>
@@ -1965,13 +1965,13 @@
         <v>93.28583226208926</v>
       </c>
       <c r="I40" t="n">
-        <v>18.7093694664263</v>
+        <v>18.81642781520172</v>
       </c>
       <c r="J40" t="n">
         <v>20.17153856923074</v>
       </c>
       <c r="K40" t="n">
-        <v>4.857910953413057</v>
+        <v>4.750852604637618</v>
       </c>
       <c r="L40" t="n">
         <v>175.6990518569946</v>
@@ -1988,10 +1988,10 @@
         <v>87.5680304102724</v>
       </c>
       <c r="D41" t="n">
-        <v>18.76239679410936</v>
+        <v>18.90224923951075</v>
       </c>
       <c r="E41" t="n">
-        <v>-1.386478556381874</v>
+        <v>-1.526331001783277</v>
       </c>
       <c r="F41" t="n">
         <v>140.6357783675194</v>
@@ -2003,13 +2003,13 @@
         <v>94.68942467731159</v>
       </c>
       <c r="I41" t="n">
-        <v>20.2882324711193</v>
+        <v>20.4394582955752</v>
       </c>
       <c r="J41" t="n">
         <v>21.7276702831632</v>
       </c>
       <c r="K41" t="n">
-        <v>3.920862048942016</v>
+        <v>3.76963622448611</v>
       </c>
       <c r="L41" t="n">
         <v>179.2206263542175</v>
@@ -2026,10 +2026,10 @@
         <v>88.68548387644834</v>
       </c>
       <c r="D42" t="n">
-        <v>20.18914540424724</v>
+        <v>20.38798519919897</v>
       </c>
       <c r="E42" t="n">
-        <v>-1.863660233673116</v>
+        <v>-2.062500028624839</v>
       </c>
       <c r="F42" t="n">
         <v>142.5307248830795</v>
@@ -2041,13 +2041,13 @@
         <v>96.23214352973977</v>
       </c>
       <c r="I42" t="n">
-        <v>21.90713353936219</v>
+        <v>22.122893535822</v>
       </c>
       <c r="J42" t="n">
         <v>26.62762764498752</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.3348749073475474</v>
+        <v>-0.5506349038073566</v>
       </c>
       <c r="L42" t="n">
         <v>182.9743266105652</v>
@@ -2064,10 +2064,10 @@
         <v>89.91812070085572</v>
       </c>
       <c r="D43" t="n">
-        <v>21.64364857815559</v>
+        <v>21.92136649076343</v>
       </c>
       <c r="E43" t="n">
-        <v>-2.348436606340741</v>
+        <v>-2.626154518948582</v>
       </c>
       <c r="F43" t="n">
         <v>144.5906656384468</v>
@@ -2079,13 +2079,13 @@
         <v>97.92185731379864</v>
       </c>
       <c r="I43" t="n">
-        <v>23.57017975132106</v>
+        <v>23.87261772044125</v>
       </c>
       <c r="J43" t="n">
         <v>22.51197264230167</v>
       </c>
       <c r="K43" t="n">
-        <v>4.473823206108992</v>
+        <v>4.171385236988815</v>
       </c>
       <c r="L43" t="n">
         <v>187.0041513442993</v>
@@ -2102,10 +2102,10 @@
         <v>91.26811576546687</v>
       </c>
       <c r="D44" t="n">
-        <v>23.12883915031966</v>
+        <v>23.50679434422921</v>
       </c>
       <c r="E44" t="n">
-        <v>-2.828627281391491</v>
+        <v>-3.206582475301033</v>
       </c>
       <c r="F44" t="n">
         <v>146.8393463492393</v>
@@ -2117,13 +2117,13 @@
         <v>99.76583712375761</v>
       </c>
       <c r="I44" t="n">
-        <v>25.2823012744332</v>
+        <v>25.69544682914755</v>
       </c>
       <c r="J44" t="n">
         <v>27.73643980695459</v>
       </c>
       <c r="K44" t="n">
-        <v>0.01674689534563356</v>
+        <v>-0.3963986593687281</v>
       </c>
       <c r="L44" t="n">
         <v>191.3563306331635</v>
@@ -2140,10 +2140,10 @@
         <v>92.73679486039016</v>
       </c>
       <c r="D45" t="n">
-        <v>24.64816486405611</v>
+        <v>25.1492507253371</v>
       </c>
       <c r="E45" t="n">
-        <v>-3.291180468192309</v>
+        <v>-3.792266329473307</v>
       </c>
       <c r="F45" t="n">
         <v>149.301099717617</v>
@@ -2155,13 +2155,13 @@
         <v>101.770778041692</v>
       </c>
       <c r="I45" t="n">
-        <v>27.04927336869073</v>
+        <v>27.59917266211605</v>
       </c>
       <c r="J45" t="n">
         <v>28.58353428039268</v>
       </c>
       <c r="K45" t="n">
-        <v>0.03868216963427429</v>
+        <v>-0.5112171237910381</v>
       </c>
       <c r="L45" t="n">
         <v>196.079320192337</v>
@@ -2178,10 +2178,10 @@
         <v>94.32466335839256</v>
       </c>
       <c r="D46" t="n">
-        <v>26.20559042371366</v>
+        <v>26.85431442569104</v>
       </c>
       <c r="E46" t="n">
-        <v>-3.722223870475283</v>
+        <v>-4.370947872452668</v>
       </c>
       <c r="F46" t="n">
         <v>152.000846683979</v>
@@ -2193,13 +2193,13 @@
         <v>103.942814021087</v>
       </c>
       <c r="I46" t="n">
-        <v>28.87773690084937</v>
+        <v>29.59261035904922</v>
       </c>
       <c r="J46" t="n">
         <v>33.18634592045535</v>
       </c>
       <c r="K46" t="n">
-        <v>-3.564465671286293</v>
+        <v>-4.279339129486154</v>
       </c>
       <c r="L46" t="n">
         <v>201.22380900383</v>
@@ -2216,10 +2216,10 @@
         <v>96.03141448261972</v>
       </c>
       <c r="D47" t="n">
-        <v>27.80559985299436</v>
+        <v>28.62817624732453</v>
       </c>
       <c r="E47" t="n">
-        <v>-4.107100891013893</v>
+        <v>-4.929677285344049</v>
       </c>
       <c r="F47" t="n">
         <v>154.964094042778</v>
@@ -2231,13 +2231,13 @@
         <v>106.2874994536535</v>
       </c>
       <c r="I47" t="n">
-        <v>30.77521762129754</v>
+        <v>31.68564457412327</v>
       </c>
       <c r="J47" t="n">
         <v>37.1998620319838</v>
       </c>
       <c r="K47" t="n">
-        <v>-6.417030641841002</v>
+        <v>-7.327457594666733</v>
       </c>
       <c r="L47" t="n">
         <v>206.8427138328552</v>
@@ -2254,10 +2254,10 @@
         <v>97.85593171878809</v>
       </c>
       <c r="D48" t="n">
-        <v>29.45319967817029</v>
+        <v>30.47765552076696</v>
       </c>
       <c r="E48" t="n">
-        <v>-4.430401451955476</v>
+        <v>-5.454857294552156</v>
       </c>
       <c r="F48" t="n">
         <v>158.2169361710548</v>
@@ -2269,13 +2269,13 @@
         <v>108.80977451766</v>
       </c>
       <c r="I48" t="n">
-        <v>32.75014564283192</v>
+        <v>33.88927750002561</v>
       </c>
       <c r="J48" t="n">
         <v>39.69275712450992</v>
       </c>
       <c r="K48" t="n">
-        <v>-7.555404318087341</v>
+        <v>-8.694536175281058</v>
       </c>
       <c r="L48" t="n">
         <v>212.991183757782</v>
@@ -2292,10 +2292,10 @@
         <v>99.79626703674111</v>
       </c>
       <c r="D49" t="n">
-        <v>31.15392217729106</v>
+        <v>32.41021770580462</v>
       </c>
       <c r="E49" t="n">
-        <v>-4.675972300309013</v>
+        <v>-5.932267828822575</v>
       </c>
       <c r="F49" t="n">
         <v>161.786055803299</v>
@@ -2307,13 +2307,13 @@
         <v>111.5138900688956</v>
       </c>
       <c r="I49" t="n">
-        <v>34.81187379097394</v>
+        <v>36.21567781712181</v>
       </c>
       <c r="J49" t="n">
         <v>42.52924426710228</v>
       </c>
       <c r="K49" t="n">
-        <v>-8.809888048050126</v>
+        <v>-10.21369207419799</v>
       </c>
       <c r="L49" t="n">
         <v>219.7265973091125</v>
@@ -2330,10 +2330,10 @@
         <v>101.8495973124623</v>
       </c>
       <c r="D50" t="n">
-        <v>32.91382934246298</v>
+        <v>34.43399221694381</v>
       </c>
       <c r="E50" t="n">
-        <v>-4.826911885009089</v>
+        <v>-6.347074759489921</v>
       </c>
       <c r="F50" t="n">
         <v>165.6987212300301</v>
@@ -2345,13 +2345,13 @@
         <v>114.4032957793948</v>
       </c>
       <c r="I50" t="n">
-        <v>36.9706965256462</v>
+        <v>38.67823045362577</v>
       </c>
       <c r="J50" t="n">
         <v>41.26485909291869</v>
       </c>
       <c r="K50" t="n">
-        <v>-5.700446577307943</v>
+        <v>-7.407980505287512</v>
       </c>
       <c r="L50" t="n">
         <v>227.1085615158081</v>
@@ -2368,10 +2368,10 @@
         <v>104.0121596041666</v>
       </c>
       <c r="D51" t="n">
-        <v>34.73951859192005</v>
+        <v>36.55779117055905</v>
       </c>
       <c r="E51" t="n">
-        <v>-4.865542855661687</v>
+        <v>-6.683815434300698</v>
       </c>
       <c r="F51" t="n">
         <v>169.9827892780304</v>
@@ -2383,13 +2383,13 @@
         <v>117.4804888997698</v>
       </c>
       <c r="I51" t="n">
-        <v>39.23787030144425</v>
+        <v>41.29158740821798</v>
       </c>
       <c r="J51" t="n">
         <v>43.50071802861427</v>
       </c>
       <c r="K51" t="n">
-        <v>-5.790901603722958</v>
+        <v>-7.844618710496704</v>
       </c>
       <c r="L51" t="n">
         <v>235.1989140510559</v>
@@ -2406,10 +2406,10 @@
         <v>106.2791537116574</v>
       </c>
       <c r="D52" t="n">
-        <v>36.63812826787804</v>
+        <v>38.79112815264403</v>
       </c>
       <c r="E52" t="n">
-        <v>-4.773358104702936</v>
+        <v>-6.926357989468926</v>
       </c>
       <c r="F52" t="n">
         <v>174.666702747345</v>
@@ -2421,13 +2421,13 @@
         <v>120.7468114862955</v>
       </c>
       <c r="I52" t="n">
-        <v>41.62563412176416</v>
+        <v>44.07171938060208</v>
       </c>
       <c r="J52" t="n">
         <v>47.79824615604387</v>
       </c>
       <c r="K52" t="n">
-        <v>-7.603550163739243</v>
+        <v>-10.04963542257715</v>
       </c>
       <c r="L52" t="n">
         <v>244.061723947525</v>
@@ -2444,10 +2444,10 @@
         <v>108.6446134231781</v>
       </c>
       <c r="D53" t="n">
-        <v>38.61734572915741</v>
+        <v>41.1442387652895</v>
       </c>
       <c r="E53" t="n">
-        <v>-4.530935642101255</v>
+        <v>-7.057828678233349</v>
       </c>
       <c r="F53" t="n">
         <v>179.7794927954674</v>
@@ -2459,13 +2459,13 @@
         <v>124.2021928542878</v>
       </c>
       <c r="I53" t="n">
-        <v>44.14723262064886</v>
+        <v>47.03596908265261</v>
       </c>
       <c r="J53" t="n">
         <v>48.23811911783717</v>
       </c>
       <c r="K53" t="n">
-        <v>-5.177955826106512</v>
+        <v>-8.066692288110232</v>
       </c>
       <c r="L53" t="n">
         <v>253.7632865905762</v>
@@ -2482,10 +2482,10 @@
         <v>111.101244405763</v>
       </c>
       <c r="D54" t="n">
-        <v>40.68541605311608</v>
+        <v>43.62810007811899</v>
       </c>
       <c r="E54" t="n">
-        <v>-4.11782411538902</v>
+        <v>-7.060508140391924</v>
       </c>
       <c r="F54" t="n">
         <v>185.3507773280144</v>
@@ -2497,13 +2497,13 @@
         <v>127.8448406341554</v>
       </c>
       <c r="I54" t="n">
-        <v>46.8169421437653</v>
+        <v>50.20310556817477</v>
       </c>
       <c r="J54" t="n">
         <v>51.2475175541022</v>
       </c>
       <c r="K54" t="n">
-        <v>-4.897993431460492</v>
+        <v>-8.284156855869981</v>
       </c>
       <c r="L54" t="n">
         <v>264.3721330165863</v>
@@ -2520,10 +2520,10 @@
         <v>113.6402216585881</v>
       </c>
       <c r="D55" t="n">
-        <v>42.85115224128357</v>
+        <v>46.25445188540107</v>
       </c>
       <c r="E55" t="n">
-        <v>-3.512389131554158</v>
+        <v>-6.915688775671669</v>
       </c>
       <c r="F55" t="n">
         <v>191.4107611179352</v>
@@ -2535,13 +2535,13 @@
         <v>131.670862546845</v>
       </c>
       <c r="I55" t="n">
-        <v>49.65009830486878</v>
+        <v>53.5933799449962</v>
       </c>
       <c r="J55" t="n">
         <v>53.8084524036118</v>
       </c>
       <c r="K55" t="n">
-        <v>-3.699918079014267</v>
+        <v>-7.643199719141691</v>
       </c>
       <c r="L55" t="n">
         <v>275.959020614624</v>
@@ -2558,10 +2558,10 @@
         <v>116.2509439752739</v>
       </c>
       <c r="D56" t="n">
-        <v>45.12394799421905</v>
+        <v>49.03581660781452</v>
       </c>
       <c r="E56" t="n">
-        <v>-2.691617665680774</v>
+        <v>-6.603486279276233</v>
       </c>
       <c r="F56" t="n">
         <v>197.9902364611626</v>
@@ -2573,13 +2573,13 @@
         <v>135.6738214868723</v>
       </c>
       <c r="I56" t="n">
-        <v>52.66312905168957</v>
+        <v>57.22858156168326</v>
       </c>
       <c r="J56" t="n">
         <v>55.53933021340457</v>
       </c>
       <c r="K56" t="n">
-        <v>-1.15360274710666</v>
+        <v>-5.719055257100351</v>
       </c>
       <c r="L56" t="n">
         <v>288.596935749054</v>
@@ -2596,10 +2596,10 @@
         <v>118.9207411146118</v>
       </c>
       <c r="D57" t="n">
-        <v>47.51379115243535</v>
+        <v>51.98552097167747</v>
       </c>
       <c r="E57" t="n">
-        <v>-1.630875977702011</v>
+        <v>-6.102605796944154</v>
       </c>
       <c r="F57" t="n">
         <v>205.1205834746361</v>
@@ -2611,13 +2611,13 @@
         <v>139.844214847546</v>
       </c>
       <c r="I57" t="n">
-        <v>55.87359072828872</v>
+        <v>61.1320976945343</v>
       </c>
       <c r="J57" t="n">
         <v>58.11351133572528</v>
       </c>
       <c r="K57" t="n">
-        <v>1.119302996120076</v>
+        <v>-4.139203970125514</v>
       </c>
       <c r="L57" t="n">
         <v>302.3610966205597</v>
@@ -2634,10 +2634,10 @@
         <v>121.6345254686473</v>
       </c>
       <c r="D58" t="n">
-        <v>50.03127972260462</v>
+        <v>55.11771615559132</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.3036146150308028</v>
+        <v>-5.390051048017519</v>
       </c>
       <c r="F58" t="n">
         <v>212.8337680697441</v>
@@ -2649,13 +2649,13 @@
         <v>144.1688655305442</v>
       </c>
       <c r="I58" t="n">
-        <v>59.30020946650092</v>
+        <v>65.32897282387464</v>
       </c>
       <c r="J58" t="n">
         <v>59.59933730424572</v>
       </c>
       <c r="K58" t="n">
-        <v>5.105825089846185</v>
+        <v>-0.9229382675275346</v>
       </c>
       <c r="L58" t="n">
         <v>317.3289511203766</v>
@@ -2672,10 +2672,10 @@
         <v>124.3743836727143</v>
       </c>
       <c r="D59" t="n">
-        <v>52.68763974886764</v>
+        <v>58.44739909389794</v>
       </c>
       <c r="E59" t="n">
-        <v>1.318990941954034</v>
+        <v>-4.440768403076255</v>
       </c>
       <c r="F59" t="n">
         <v>221.162345468998</v>
@@ -2687,13 +2687,13 @@
         <v>148.6302157138101</v>
       </c>
       <c r="I59" t="n">
-        <v>62.96292717262885</v>
+        <v>69.84597051830852</v>
       </c>
       <c r="J59" t="n">
         <v>64.24728210828241</v>
       </c>
       <c r="K59" t="n">
-        <v>6.615089869845292</v>
+        <v>-0.2679534758343678</v>
       </c>
       <c r="L59" t="n">
         <v>333.5801780223846</v>
@@ -2710,10 +2710,10 @@
         <v>127.1190980533219</v>
       </c>
       <c r="D60" t="n">
-        <v>55.494745145435</v>
+        <v>61.99043204845722</v>
       </c>
       <c r="E60" t="n">
-        <v>3.268463529421254</v>
+        <v>-3.227223373600978</v>
       </c>
       <c r="F60" t="n">
         <v>230.1394554376602</v>
@@ -2725,13 +2725,13 @@
         <v>153.2055093192255</v>
       </c>
       <c r="I60" t="n">
-        <v>66.8829532678139</v>
+        <v>74.71163546895963</v>
       </c>
       <c r="J60" t="n">
         <v>66.24644729424173</v>
       </c>
       <c r="K60" t="n">
-        <v>11.52251000415518</v>
+        <v>3.693827803009441</v>
       </c>
       <c r="L60" t="n">
         <v>351.1966829299927</v>
@@ -2748,10 +2748,10 @@
         <v>129.843586020921</v>
       </c>
       <c r="D61" t="n">
-        <v>58.46513907216551</v>
+        <v>65.76356302988859</v>
       </c>
       <c r="E61" t="n">
-        <v>5.579539196737706</v>
+        <v>-1.718884760985354</v>
       </c>
       <c r="F61" t="n">
         <v>239.7988273501396</v>
@@ -2763,13 +2763,13 @@
         <v>157.8658423246366</v>
       </c>
       <c r="I61" t="n">
-        <v>71.08282133217817</v>
+        <v>79.95635818553201</v>
       </c>
       <c r="J61" t="n">
         <v>70.19190504927502</v>
       </c>
       <c r="K61" t="n">
-        <v>15.30326424878677</v>
+        <v>6.429727395432963</v>
       </c>
       <c r="L61" t="n">
         <v>370.26260638237</v>
@@ -2786,10 +2786,10 @@
         <v>132.5182336147943</v>
       </c>
       <c r="D62" t="n">
-        <v>61.61205748172289</v>
+        <v>69.78444452063586</v>
       </c>
       <c r="E62" t="n">
-        <v>8.290781374331601</v>
+        <v>0.1183943354186283</v>
       </c>
       <c r="F62" t="n">
         <v>250.1747761964798</v>
@@ -2801,13 +2801,13 @@
         <v>162.5750442543452</v>
       </c>
       <c r="I62" t="n">
-        <v>75.58645099970693</v>
+        <v>85.61243873190821</v>
       </c>
       <c r="J62" t="n">
         <v>17.64928148140623</v>
       </c>
       <c r="K62" t="n">
-        <v>76.46869111733241</v>
+        <v>66.4427033851311</v>
       </c>
       <c r="L62" t="n">
         <v>390.8643152713776</v>

</xml_diff>

<commit_message>
Add the Comet 4, improve code readability and add notations
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,2320 +497,2700 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1960</v>
+        <v>1950</v>
       </c>
       <c r="B2" t="n">
-        <v>2.755252570979569</v>
+        <v>0.9132065475827132</v>
       </c>
       <c r="C2" t="n">
-        <v>8.588104877825529</v>
+        <v>3.659758381057158</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.8661664253000624</v>
+        <v>-0.8713571247171499</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.451710633910005</v>
+        <v>-3.318826059919425</v>
       </c>
       <c r="F2" t="n">
-        <v>8.025480389595032</v>
+        <v>0.3827817440032959</v>
       </c>
       <c r="G2" t="n">
-        <v>2.664992669550213</v>
+        <v>0.9446767031497476</v>
       </c>
       <c r="H2" t="n">
-        <v>8.306765334619181</v>
+        <v>3.785877894648572</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.8377914962672564</v>
+        <v>-0.9013851006902512</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.945093541270408</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>-3.173438939913591</v>
+        <v>-7.226075872993079</v>
       </c>
       <c r="L2" t="n">
-        <v>5.01543402671814</v>
+        <v>-3.39690637588501</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1961</v>
+        <v>1951</v>
       </c>
       <c r="B3" t="n">
-        <v>5.46453115983095</v>
+        <v>1.926302743666822</v>
       </c>
       <c r="C3" t="n">
-        <v>16.3845391446805</v>
+        <v>7.255034025449946</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.694930593802125</v>
+        <v>-1.707475598112461</v>
       </c>
       <c r="E3" t="n">
-        <v>-4.406499279782053</v>
+        <v>-6.003424359557163</v>
       </c>
       <c r="F3" t="n">
-        <v>15.74764043092728</v>
+        <v>1.470436811447144</v>
       </c>
       <c r="G3" t="n">
-        <v>5.22944814093343</v>
+        <v>1.957779554059642</v>
       </c>
       <c r="H3" t="n">
-        <v>15.67967960362973</v>
+        <v>7.373585136464739</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.622015024440618</v>
+        <v>-1.735376656670808</v>
       </c>
       <c r="J3" t="n">
-        <v>-8.753415186097419</v>
+        <v>4.2390532078429</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.2472371343974373</v>
+        <v>-17.47535272126495</v>
       </c>
       <c r="L3" t="n">
-        <v>10.28646039962769</v>
+        <v>-5.640311479568481</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1962</v>
+        <v>1952</v>
       </c>
       <c r="B4" t="n">
-        <v>8.105903906391141</v>
+        <v>3.036678858962268</v>
       </c>
       <c r="C4" t="n">
-        <v>23.48305040986538</v>
+        <v>10.81432212542889</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.472200796769541</v>
+        <v>-2.515621244020234</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.950016916703774</v>
+        <v>-8.132291933669265</v>
       </c>
       <c r="F4" t="n">
-        <v>23.1667366027832</v>
+        <v>3.20308780670166</v>
       </c>
       <c r="G4" t="n">
-        <v>7.701324314756554</v>
+        <v>3.039026839022135</v>
       </c>
       <c r="H4" t="n">
-        <v>22.3109710150348</v>
+        <v>10.82268383040028</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.348809007236099</v>
+        <v>-2.517566338906282</v>
       </c>
       <c r="J4" t="n">
-        <v>-12.04317274164832</v>
+        <v>2.504873567786579</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1497958341473922</v>
+        <v>-20.66482333348338</v>
       </c>
       <c r="L4" t="n">
-        <v>15.77010941505432</v>
+        <v>-6.815805435180664</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1963</v>
+        <v>1953</v>
       </c>
       <c r="B5" t="n">
-        <v>10.66246506659041</v>
+        <v>4.242105846552328</v>
       </c>
       <c r="C5" t="n">
-        <v>29.95353398112397</v>
+        <v>14.36025604106698</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.186475915690775</v>
+        <v>-3.301010623425174</v>
       </c>
       <c r="E5" t="n">
-        <v>-7.145908675370006</v>
+        <v>-9.778489783481245</v>
       </c>
       <c r="F5" t="n">
-        <v>30.28361445665359</v>
+        <v>5.522861480712891</v>
       </c>
       <c r="G5" t="n">
-        <v>10.08502655826333</v>
+        <v>4.190458154857925</v>
       </c>
       <c r="H5" t="n">
-        <v>28.33136463537102</v>
+        <v>14.18541974431015</v>
       </c>
       <c r="I5" t="n">
-        <v>-3.013908513304431</v>
+        <v>-3.260820777832996</v>
       </c>
       <c r="J5" t="n">
-        <v>-12.08501115616109</v>
+        <v>2.754397577499184</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.891833086897702</v>
+        <v>-24.87568064239963</v>
       </c>
       <c r="L5" t="n">
-        <v>21.42563843727112</v>
+        <v>-7.006225943565369</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1964</v>
+        <v>1954</v>
       </c>
       <c r="B6" t="n">
-        <v>13.12120457073863</v>
+        <v>5.54017307698284</v>
       </c>
       <c r="C6" t="n">
-        <v>35.85080324176099</v>
+        <v>17.90972156307743</v>
       </c>
       <c r="D6" t="n">
-        <v>-3.828514272141826</v>
+        <v>-4.066986731430564</v>
       </c>
       <c r="E6" t="n">
-        <v>-8.043789036344732</v>
+        <v>-11.00901464767389</v>
       </c>
       <c r="F6" t="n">
-        <v>37.09970450401306</v>
+        <v>8.373893260955811</v>
       </c>
       <c r="G6" t="n">
-        <v>12.3824108185826</v>
+        <v>5.415212565089421</v>
       </c>
       <c r="H6" t="n">
-        <v>33.83221193773886</v>
+        <v>17.50576162476995</v>
       </c>
       <c r="I6" t="n">
-        <v>-3.612948512988407</v>
+        <v>-3.975254444954764</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.193323856318347</v>
+        <v>-0.6335383784258507</v>
       </c>
       <c r="K6" t="n">
-        <v>-7.193814673818904</v>
+        <v>-24.60383321145709</v>
       </c>
       <c r="L6" t="n">
-        <v>27.2145357131958</v>
+        <v>-6.291651844978333</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1965</v>
+        <v>1955</v>
       </c>
       <c r="B7" t="n">
-        <v>15.47219529006907</v>
+        <v>6.927884744528988</v>
       </c>
       <c r="C7" t="n">
-        <v>41.21975235124386</v>
+        <v>21.47422453556341</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.391066881186413</v>
+        <v>-4.815227479649375</v>
       </c>
       <c r="E7" t="n">
-        <v>-8.683854431085994</v>
+        <v>-11.88455836370596</v>
       </c>
       <c r="F7" t="n">
-        <v>43.61702632904053</v>
+        <v>11.70232343673706</v>
       </c>
       <c r="G7" t="n">
-        <v>14.59355353798953</v>
+        <v>6.716501754055951</v>
       </c>
       <c r="H7" t="n">
-        <v>38.8789471360054</v>
+        <v>20.81900494577425</v>
       </c>
       <c r="I7" t="n">
-        <v>-4.141705066288662</v>
+        <v>-4.668305695874026</v>
       </c>
       <c r="J7" t="n">
-        <v>-8.311281322075134</v>
+        <v>1.168090994400017</v>
       </c>
       <c r="K7" t="n">
-        <v>-7.918993436403225</v>
+        <v>-28.78469619032701</v>
       </c>
       <c r="L7" t="n">
-        <v>33.10052084922791</v>
+        <v>-4.749404191970825</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1966</v>
+        <v>1956</v>
       </c>
       <c r="B8" t="n">
-        <v>17.70799266274854</v>
+        <v>8.40139856721728</v>
       </c>
       <c r="C8" t="n">
-        <v>46.09855780478731</v>
+        <v>25.06041422771064</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.868651418406087</v>
+        <v>-5.545971051685223</v>
       </c>
       <c r="E8" t="n">
-        <v>-9.099713440742775</v>
+        <v>-12.45954363037343</v>
       </c>
       <c r="F8" t="n">
-        <v>49.83818560838699</v>
+        <v>15.45629811286926</v>
       </c>
       <c r="G8" t="n">
-        <v>16.71734054847584</v>
+        <v>8.096816413395338</v>
       </c>
       <c r="H8" t="n">
-        <v>43.51963005029914</v>
+        <v>24.15188038300883</v>
       </c>
       <c r="I8" t="n">
-        <v>-4.596280635722908</v>
+        <v>-5.344908836336008</v>
       </c>
       <c r="J8" t="n">
-        <v>-5.171464322903</v>
+        <v>2.2225897486764</v>
       </c>
       <c r="K8" t="n">
-        <v>-11.41968368992325</v>
+        <v>-31.58041740162329</v>
       </c>
       <c r="L8" t="n">
-        <v>39.04954195022583</v>
+        <v>-2.454039692878723</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1967</v>
+        <v>1957</v>
       </c>
       <c r="B9" t="n">
-        <v>19.82318310373862</v>
+        <v>9.955882984948611</v>
       </c>
       <c r="C9" t="n">
-        <v>50.52072961031287</v>
+        <v>28.67069356924484</v>
       </c>
       <c r="D9" t="n">
-        <v>-5.257353895268258</v>
+        <v>-6.258244443995435</v>
       </c>
       <c r="E9" t="n">
-        <v>-9.320183038677637</v>
+        <v>-12.78236147001551</v>
       </c>
       <c r="F9" t="n">
-        <v>55.76637578010559</v>
+        <v>19.5859706401825</v>
       </c>
       <c r="G9" t="n">
-        <v>18.75191837698277</v>
+        <v>9.557372116552234</v>
       </c>
       <c r="H9" t="n">
-        <v>47.79053863551978</v>
+        <v>27.52307230761696</v>
       </c>
       <c r="I9" t="n">
-        <v>-4.973241209903859</v>
+        <v>-6.00774145678839</v>
       </c>
       <c r="J9" t="n">
-        <v>-6.634700818295123</v>
+        <v>1.261131954599775</v>
       </c>
       <c r="K9" t="n">
-        <v>-9.904738172703833</v>
+        <v>-31.81118503775665</v>
       </c>
       <c r="L9" t="n">
-        <v>45.02977681159973</v>
+        <v>0.522649884223938</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1968</v>
+        <v>1958</v>
       </c>
       <c r="B10" t="n">
-        <v>21.81403671758004</v>
+        <v>11.58547278164227</v>
       </c>
       <c r="C10" t="n">
-        <v>54.5164815714009</v>
+        <v>32.30385724495742</v>
       </c>
       <c r="D10" t="n">
-        <v>-5.554650181203242</v>
+        <v>-6.950084751527919</v>
       </c>
       <c r="E10" t="n">
-        <v>-9.370491137009729</v>
+        <v>-12.89574413638464</v>
       </c>
       <c r="F10" t="n">
-        <v>61.40537697076797</v>
+        <v>24.04350113868713</v>
       </c>
       <c r="G10" t="n">
-        <v>20.69503881460975</v>
+        <v>11.09778071124175</v>
       </c>
       <c r="H10" t="n">
-        <v>51.71994146534372</v>
+        <v>30.94402193062482</v>
       </c>
       <c r="I10" t="n">
-        <v>-5.269712460369079</v>
+        <v>-6.657519977882894</v>
       </c>
       <c r="J10" t="n">
-        <v>-14.10077749305779</v>
+        <v>-4.463098459022535</v>
       </c>
       <c r="K10" t="n">
-        <v>-2.032855023029294</v>
+        <v>-26.80954303636678</v>
       </c>
       <c r="L10" t="n">
-        <v>51.01163530349731</v>
+        <v>4.11164116859436</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1969</v>
+        <v>1959</v>
       </c>
       <c r="B11" t="n">
-        <v>23.67823699386431</v>
+        <v>13.283295499332</v>
       </c>
       <c r="C11" t="n">
-        <v>58.11366103734048</v>
+        <v>35.95571210172286</v>
       </c>
       <c r="D11" t="n">
-        <v>-5.759241621532886</v>
+        <v>-7.618745887949796</v>
       </c>
       <c r="E11" t="n">
-        <v>-9.273099043300753</v>
+        <v>-12.83720712287984</v>
       </c>
       <c r="F11" t="n">
-        <v>66.75955736637115</v>
+        <v>28.78305459022522</v>
       </c>
       <c r="G11" t="n">
-        <v>22.54432173840143</v>
+        <v>12.71590745495737</v>
       </c>
       <c r="H11" t="n">
-        <v>55.33068497294368</v>
+        <v>34.41988530523852</v>
       </c>
       <c r="I11" t="n">
-        <v>-5.483440178366101</v>
+        <v>-7.293315701580117</v>
       </c>
       <c r="J11" t="n">
-        <v>-17.65367011789323</v>
+        <v>-0.633307727389012</v>
       </c>
       <c r="K11" t="n">
-        <v>2.229857710509322</v>
+        <v>-30.9624864489178</v>
       </c>
       <c r="L11" t="n">
-        <v>56.96775412559509</v>
+        <v>8.24668288230896</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1970</v>
+        <v>1960</v>
       </c>
       <c r="B12" t="n">
-        <v>25.41466571329314</v>
+        <v>15.04154844148763</v>
       </c>
       <c r="C12" t="n">
-        <v>61.33839707871358</v>
+        <v>39.61965934872611</v>
       </c>
       <c r="D12" t="n">
-        <v>-5.870902843962126</v>
+        <v>-8.260887452244436</v>
       </c>
       <c r="E12" t="n">
-        <v>-9.048287987404645</v>
+        <v>-12.63951830740596</v>
       </c>
       <c r="F12" t="n">
-        <v>71.83387196063995</v>
+        <v>33.76080203056335</v>
       </c>
       <c r="G12" t="n">
-        <v>24.29745494400631</v>
+        <v>14.40787127605117</v>
       </c>
       <c r="H12" t="n">
-        <v>58.6420044304606</v>
+        <v>37.95054439494837</v>
       </c>
       <c r="I12" t="n">
-        <v>-5.612822098116215</v>
+        <v>-7.912869044093752</v>
       </c>
       <c r="J12" t="n">
-        <v>-11.71180985000244</v>
+        <v>-2.837581849060681</v>
       </c>
       <c r="K12" t="n">
-        <v>-2.741824181948223</v>
+        <v>-28.74366571893092</v>
       </c>
       <c r="L12" t="n">
-        <v>62.87300324440002</v>
+        <v>12.86429905891418</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1971</v>
+        <v>1961</v>
       </c>
       <c r="B13" t="n">
-        <v>27.02323036184836</v>
+        <v>16.85161134246109</v>
       </c>
       <c r="C13" t="n">
-        <v>64.21555839472347</v>
+        <v>43.28722115030608</v>
       </c>
       <c r="D13" t="n">
-        <v>-5.890339029386893</v>
+        <v>-8.872743211879946</v>
       </c>
       <c r="E13" t="n">
-        <v>-8.71458741057651</v>
+        <v>-12.33116706256447</v>
       </c>
       <c r="F13" t="n">
-        <v>76.63386231660843</v>
+        <v>38.93492221832275</v>
       </c>
       <c r="G13" t="n">
-        <v>25.95234446962981</v>
+        <v>16.16814827838056</v>
       </c>
       <c r="H13" t="n">
-        <v>61.67080210078565</v>
+        <v>41.53158982213902</v>
       </c>
       <c r="I13" t="n">
-        <v>-5.656914642942694</v>
+        <v>-8.512884908768523</v>
       </c>
       <c r="J13" t="n">
-        <v>-13.65893444570869</v>
+        <v>-10.47486073079117</v>
       </c>
       <c r="K13" t="n">
-        <v>0.3971826894395356</v>
+        <v>-20.80820234464976</v>
       </c>
       <c r="L13" t="n">
-        <v>68.70448017120361</v>
+        <v>17.90379011631012</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1972</v>
+        <v>1962</v>
       </c>
       <c r="B14" t="n">
-        <v>28.50472331395008</v>
+        <v>18.70417874389799</v>
       </c>
       <c r="C14" t="n">
-        <v>66.7690783450869</v>
+        <v>46.94850765564462</v>
       </c>
       <c r="D14" t="n">
-        <v>-5.819052165834346</v>
+        <v>-9.450269589119602</v>
       </c>
       <c r="E14" t="n">
-        <v>-8.289091436466638</v>
+        <v>-11.93681732121097</v>
       </c>
       <c r="F14" t="n">
-        <v>81.16565805673599</v>
+        <v>44.26559948921204</v>
       </c>
       <c r="G14" t="n">
-        <v>27.50722739444926</v>
+        <v>17.98974078822075</v>
       </c>
       <c r="H14" t="n">
-        <v>64.43255739504981</v>
+        <v>45.15522946413149</v>
       </c>
       <c r="I14" t="n">
-        <v>-5.615419921211172</v>
+        <v>-9.089300450709716</v>
       </c>
       <c r="J14" t="n">
-        <v>-7.136389072964776</v>
+        <v>-14.12907762420487</v>
       </c>
       <c r="K14" t="n">
-        <v>-4.746460826451059</v>
+        <v>-16.61935347943198</v>
       </c>
       <c r="L14" t="n">
-        <v>74.44151496887207</v>
+        <v>23.30723869800568</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1973</v>
+        <v>1963</v>
       </c>
       <c r="B15" t="n">
-        <v>29.8607052777427</v>
+        <v>20.58940038901413</v>
       </c>
       <c r="C15" t="n">
-        <v>69.02218743856436</v>
+        <v>50.59262524499342</v>
       </c>
       <c r="D15" t="n">
-        <v>-5.659216255400888</v>
+        <v>-9.98927463016631</v>
       </c>
       <c r="E15" t="n">
-        <v>-7.787700492068424</v>
+        <v>-11.47772724781402</v>
       </c>
       <c r="F15" t="n">
-        <v>85.43597596883774</v>
+        <v>49.71502375602722</v>
       </c>
       <c r="G15" t="n">
-        <v>28.96075377193128</v>
+        <v>19.86438115526018</v>
       </c>
       <c r="H15" t="n">
-        <v>66.94197463240423</v>
+        <v>48.81109563773504</v>
       </c>
       <c r="I15" t="n">
-        <v>-5.488656982155703</v>
+        <v>-9.637520033078319</v>
       </c>
       <c r="J15" t="n">
-        <v>-6.108594804165955</v>
+        <v>-14.15300565806115</v>
       </c>
       <c r="K15" t="n">
-        <v>-4.239812565050594</v>
+        <v>-15.86544142873715</v>
       </c>
       <c r="L15" t="n">
-        <v>80.06566405296326</v>
+        <v>29.01950967311859</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1974</v>
+        <v>1964</v>
       </c>
       <c r="B16" t="n">
-        <v>31.09340785783231</v>
+        <v>22.49702815821988</v>
       </c>
       <c r="C16" t="n">
-        <v>70.99756997985759</v>
+        <v>54.2080289306336</v>
       </c>
       <c r="D16" t="n">
-        <v>-5.413559518893639</v>
+        <v>-10.48552928578224</v>
       </c>
       <c r="E16" t="n">
-        <v>-7.225298968362917</v>
+        <v>-10.97213610232662</v>
       </c>
       <c r="F16" t="n">
-        <v>89.45211935043335</v>
+        <v>55.24739170074463</v>
       </c>
       <c r="G16" t="n">
-        <v>30.3120461043778</v>
+        <v>21.78275606097747</v>
       </c>
       <c r="H16" t="n">
-        <v>69.21343663480525</v>
+        <v>52.48694460610187</v>
       </c>
       <c r="I16" t="n">
-        <v>-5.277519481807528</v>
+        <v>-10.15261771448583</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.625501860007036</v>
+        <v>-9.815174003880767</v>
       </c>
       <c r="K16" t="n">
-        <v>-6.061746437270218</v>
+        <v>-19.31365356712857</v>
       </c>
       <c r="L16" t="n">
-        <v>85.56071496009827</v>
+        <v>34.98825538158417</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1975</v>
+        <v>1965</v>
       </c>
       <c r="B17" t="n">
-        <v>32.20565097363226</v>
+        <v>24.4165571001426</v>
       </c>
       <c r="C17" t="n">
-        <v>72.71747930781416</v>
+        <v>57.78282169562615</v>
       </c>
       <c r="D17" t="n">
-        <v>-5.085255092202721</v>
+        <v>-10.93486213972361</v>
       </c>
       <c r="E17" t="n">
-        <v>-6.615895869194418</v>
+        <v>-10.43560940468711</v>
       </c>
       <c r="F17" t="n">
-        <v>93.22197932004929</v>
+        <v>60.82890725135803</v>
       </c>
       <c r="G17" t="n">
-        <v>31.5607398441365</v>
+        <v>23.73472976500977</v>
       </c>
       <c r="H17" t="n">
-        <v>71.26132766061156</v>
+        <v>56.16924828428904</v>
       </c>
       <c r="I17" t="n">
-        <v>-4.983423969212176</v>
+        <v>-10.62950836350554</v>
       </c>
       <c r="J17" t="n">
-        <v>-2.936803997128449</v>
+        <v>-9.947676938802596</v>
       </c>
       <c r="K17" t="n">
-        <v>-3.989150091004484</v>
+        <v>-18.16287460944032</v>
       </c>
       <c r="L17" t="n">
-        <v>90.91268944740295</v>
+        <v>41.16391813755035</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1976</v>
+        <v>1966</v>
       </c>
       <c r="B18" t="n">
-        <v>33.20077226741804</v>
+        <v>26.3373609947235</v>
       </c>
       <c r="C18" t="n">
-        <v>74.20380672758927</v>
+        <v>61.30501233306438</v>
       </c>
       <c r="D18" t="n">
-        <v>-4.67782019799734</v>
+        <v>-11.33323947708277</v>
       </c>
       <c r="E18" t="n">
-        <v>-5.972724575837638</v>
+        <v>-9.881355129849389</v>
       </c>
       <c r="F18" t="n">
-        <v>96.75403422117233</v>
+        <v>66.42777872085571</v>
       </c>
       <c r="G18" t="n">
-        <v>32.70700815622536</v>
+        <v>25.7095613207795</v>
       </c>
       <c r="H18" t="n">
-        <v>73.10024273875044</v>
+        <v>59.84369406501386</v>
       </c>
       <c r="I18" t="n">
-        <v>-4.608251342376171</v>
+        <v>-11.06309076894655</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.7614292659290338</v>
+        <v>-6.474974139409201</v>
       </c>
       <c r="K18" t="n">
-        <v>-4.327736330905819</v>
+        <v>-20.51545786387407</v>
       </c>
       <c r="L18" t="n">
-        <v>96.10983395576477</v>
+        <v>47.49973261356354</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1977</v>
+        <v>1967</v>
       </c>
       <c r="B19" t="n">
-        <v>34.08256552897463</v>
+        <v>28.24882167714172</v>
       </c>
       <c r="C19" t="n">
-        <v>75.4781175208816</v>
+        <v>64.76273235275475</v>
       </c>
       <c r="D19" t="n">
-        <v>-4.195021780230052</v>
+        <v>-11.67683227374706</v>
       </c>
       <c r="E19" t="n">
-        <v>-5.308311826190504</v>
+        <v>-9.320499611068836</v>
       </c>
       <c r="F19" t="n">
-        <v>100.0573494434357</v>
+        <v>72.01422214508057</v>
       </c>
       <c r="G19" t="n">
-        <v>33.75157581675575</v>
+        <v>27.69611096696993</v>
       </c>
       <c r="H19" t="n">
-        <v>74.74511869848305</v>
+        <v>63.49559787895399</v>
       </c>
       <c r="I19" t="n">
-        <v>-4.154282210592611</v>
+        <v>-11.44836574398019</v>
       </c>
       <c r="J19" t="n">
-        <v>0.6424210080266849</v>
+        <v>-8.107181697624965</v>
       </c>
       <c r="K19" t="n">
-        <v>-3.842207503957053</v>
+        <v>-17.68443294114585</v>
       </c>
       <c r="L19" t="n">
-        <v>101.1426258087158</v>
+        <v>53.95172846317291</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1978</v>
+        <v>1968</v>
       </c>
       <c r="B20" t="n">
-        <v>34.85522711483112</v>
+        <v>30.14044713605225</v>
       </c>
       <c r="C20" t="n">
-        <v>76.5616685062319</v>
+        <v>68.14441819647351</v>
       </c>
       <c r="D20" t="n">
-        <v>-3.640790406996849</v>
+        <v>-11.96207126203547</v>
       </c>
       <c r="E20" t="n">
-        <v>-4.634527493424088</v>
+        <v>-8.762335887201722</v>
       </c>
       <c r="F20" t="n">
-        <v>103.1415777206421</v>
+        <v>77.56045818328857</v>
       </c>
       <c r="G20" t="n">
-        <v>34.69572345247781</v>
+        <v>29.68303042512066</v>
       </c>
       <c r="H20" t="n">
-        <v>76.21130881750022</v>
+        <v>67.11024655664758</v>
       </c>
       <c r="I20" t="n">
-        <v>-3.624129508421619</v>
+        <v>-11.78053277098685</v>
       </c>
       <c r="J20" t="n">
-        <v>8.804224115684887</v>
+        <v>-16.38043429366912</v>
       </c>
       <c r="K20" t="n">
-        <v>-10.08335175745981</v>
+        <v>-8.153574470182335</v>
       </c>
       <c r="L20" t="n">
-        <v>106.0037751197815</v>
+        <v>60.47873544692993</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1979</v>
+        <v>1969</v>
       </c>
       <c r="B21" t="n">
-        <v>35.5233083131959</v>
+        <v>32.00197962039925</v>
       </c>
       <c r="C21" t="n">
-        <v>77.47540131647709</v>
+        <v>71.43896901844505</v>
       </c>
       <c r="D21" t="n">
-        <v>-3.019141688486402</v>
+        <v>-12.18569172383114</v>
       </c>
       <c r="E21" t="n">
-        <v>-3.962609168050456</v>
+        <v>-8.214541220585673</v>
       </c>
       <c r="F21" t="n">
-        <v>106.0169587731361</v>
+        <v>83.04071569442749</v>
       </c>
       <c r="G21" t="n">
-        <v>35.54128298783034</v>
+        <v>31.65893568603431</v>
       </c>
       <c r="H21" t="n">
-        <v>77.51460360919593</v>
+        <v>70.67318186122054</v>
       </c>
       <c r="I21" t="n">
-        <v>-3.020669364035293</v>
+        <v>-12.05506769114672</v>
       </c>
       <c r="J21" t="n">
-        <v>11.98689558311575</v>
+        <v>-20.32256507200328</v>
       </c>
       <c r="K21" t="n">
-        <v>-11.33389446092788</v>
+        <v>-2.912101828553709</v>
       </c>
       <c r="L21" t="n">
-        <v>110.6882183551788</v>
+        <v>67.04238295555115</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="B22" t="n">
-        <v>36.09167291442412</v>
+        <v>33.82349471824228</v>
       </c>
       <c r="C22" t="n">
-        <v>78.23991896721151</v>
+        <v>74.63587563724801</v>
       </c>
       <c r="D22" t="n">
-        <v>-2.334104189993511</v>
+        <v>-12.34476848431023</v>
       </c>
       <c r="E22" t="n">
-        <v>-3.303168264628724</v>
+        <v>-7.683372995066158</v>
       </c>
       <c r="F22" t="n">
-        <v>108.6943194270134</v>
+        <v>88.43122887611389</v>
       </c>
       <c r="G22" t="n">
-        <v>36.2906284256927</v>
+        <v>33.61256566596752</v>
       </c>
       <c r="H22" t="n">
-        <v>78.67121687674987</v>
+        <v>74.17043365246779</v>
       </c>
       <c r="I22" t="n">
-        <v>-2.346970949968183</v>
+        <v>-12.26778441336672</v>
       </c>
       <c r="J22" t="n">
-        <v>6.082978953432057</v>
+        <v>-13.7668364805827</v>
       </c>
       <c r="K22" t="n">
-        <v>-3.504725435346745</v>
+        <v>-8.14127090438244</v>
       </c>
       <c r="L22" t="n">
-        <v>115.1931278705597</v>
+        <v>73.60710752010345</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1981</v>
+        <v>1971</v>
       </c>
       <c r="B23" t="n">
-        <v>36.56545889134948</v>
+        <v>35.5954897028445</v>
       </c>
       <c r="C23" t="n">
-        <v>78.87544951269686</v>
+        <v>77.72533143444505</v>
       </c>
       <c r="D23" t="n">
-        <v>-1.589655569333166</v>
+        <v>-12.43674276247808</v>
       </c>
       <c r="E23" t="n">
-        <v>-2.666178803360182</v>
+        <v>-7.173840871759708</v>
       </c>
       <c r="F23" t="n">
-        <v>111.185074031353</v>
+        <v>93.71023750305176</v>
       </c>
       <c r="G23" t="n">
-        <v>36.94665876890706</v>
+        <v>35.53292272943708</v>
       </c>
       <c r="H23" t="n">
-        <v>79.69773679168007</v>
+        <v>77.58871191367038</v>
       </c>
       <c r="I23" t="n">
-        <v>-1.606227944650241</v>
+        <v>-12.41488242679537</v>
       </c>
       <c r="J23" t="n">
-        <v>7.341080459717278</v>
+        <v>-15.93806109752243</v>
       </c>
       <c r="K23" t="n">
-        <v>-2.861352377106807</v>
+        <v>-4.628540094924908</v>
       </c>
       <c r="L23" t="n">
-        <v>119.5178956985474</v>
+        <v>80.14015102386475</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1982</v>
+        <v>1972</v>
       </c>
       <c r="B24" t="n">
-        <v>36.95004395153364</v>
+        <v>37.30896248773059</v>
       </c>
       <c r="C24" t="n">
-        <v>79.40180009844106</v>
+        <v>80.69832548398503</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.7896628264023733</v>
+        <v>-12.45944104503199</v>
       </c>
       <c r="E24" t="n">
-        <v>-2.060956705750051</v>
+        <v>-6.689858569139695</v>
       </c>
       <c r="F24" t="n">
-        <v>113.5012245178223</v>
+        <v>98.85798835754395</v>
       </c>
       <c r="G24" t="n">
-        <v>37.51278097172949</v>
+        <v>37.40939877704282</v>
       </c>
       <c r="H24" t="n">
-        <v>80.61106340660362</v>
+        <v>80.91556659241809</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.8016891316070972</v>
+        <v>-12.49298204810542</v>
       </c>
       <c r="J24" t="n">
-        <v>7.279113576748939</v>
+        <v>-8.742404792191639</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.9371131018105299</v>
+        <v>-10.47801079349186</v>
       </c>
       <c r="L24" t="n">
-        <v>123.6641557216644</v>
+        <v>86.611567735672</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1983</v>
+        <v>1973</v>
       </c>
       <c r="B25" t="n">
-        <v>37.25101350402231</v>
+        <v>38.95548189732101</v>
       </c>
       <c r="C25" t="n">
-        <v>79.83830216533475</v>
+        <v>83.54672036647345</v>
       </c>
       <c r="D25" t="n">
-        <v>0.06216905449482216</v>
+        <v>-12.41108725429237</v>
       </c>
       <c r="E25" t="n">
-        <v>-1.496125992105206</v>
+        <v>-6.234380256847068</v>
       </c>
       <c r="F25" t="n">
-        <v>115.6553587317467</v>
+        <v>103.856734752655</v>
       </c>
       <c r="G25" t="n">
-        <v>37.99288479471285</v>
+        <v>39.23188669989649</v>
       </c>
       <c r="H25" t="n">
-        <v>81.42831915286028</v>
+        <v>84.13951792984568</v>
       </c>
       <c r="I25" t="n">
-        <v>0.06340718018217034</v>
+        <v>-12.49914890711216</v>
       </c>
       <c r="J25" t="n">
-        <v>8.703718248815735</v>
+        <v>-7.62358808821358</v>
       </c>
       <c r="K25" t="n">
-        <v>-0.5525664466546534</v>
+        <v>-10.25444368212303</v>
       </c>
       <c r="L25" t="n">
-        <v>127.6357629299164</v>
+        <v>92.9942239522934</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1984</v>
+        <v>1974</v>
       </c>
       <c r="B26" t="n">
-        <v>37.47413213812481</v>
+        <v>40.52724824140295</v>
       </c>
       <c r="C26" t="n">
-        <v>80.20374879690084</v>
+        <v>86.26331700729254</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9623437497390522</v>
+        <v>-12.29030828541107</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.9795712128179801</v>
+        <v>-5.809521384747434</v>
       </c>
       <c r="F26" t="n">
-        <v>117.6606534719467</v>
+        <v>108.690735578537</v>
       </c>
       <c r="G26" t="n">
-        <v>38.39131892043434</v>
+        <v>40.99087792164252</v>
       </c>
       <c r="H26" t="n">
-        <v>82.16675138271263</v>
+        <v>87.25016501242401</v>
       </c>
       <c r="I26" t="n">
-        <v>0.9858973030020209</v>
+        <v>-12.43090879365356</v>
       </c>
       <c r="J26" t="n">
-        <v>10.07696011453443</v>
+        <v>-3.786208066921161</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.1821199947770538</v>
+        <v>-12.76012271064543</v>
       </c>
       <c r="L26" t="n">
-        <v>131.4388077259064</v>
+        <v>99.26380336284637</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1985</v>
+        <v>1975</v>
       </c>
       <c r="B27" t="n">
-        <v>37.6253166397716</v>
+        <v>42.01714762070976</v>
       </c>
       <c r="C27" t="n">
-        <v>80.51632838374668</v>
+        <v>88.84191003242972</v>
       </c>
       <c r="D27" t="n">
-        <v>1.90761514358131</v>
+        <v>-12.0961339575979</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.5183888354078476</v>
+        <v>-5.416667916275223</v>
       </c>
       <c r="F27" t="n">
-        <v>119.5308713316917</v>
+        <v>113.3462557792664</v>
       </c>
       <c r="G27" t="n">
-        <v>38.71286252940088</v>
+        <v>42.67754884177296</v>
       </c>
       <c r="H27" t="n">
-        <v>82.84362313637675</v>
+        <v>90.23827578282838</v>
       </c>
       <c r="I27" t="n">
-        <v>1.962754055188594</v>
+        <v>-12.2862539940138</v>
       </c>
       <c r="J27" t="n">
-        <v>12.20704447342378</v>
+        <v>-4.147358170156719</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.6446773294607908</v>
+        <v>-11.08340219298239</v>
       </c>
       <c r="L27" t="n">
-        <v>135.0816068649292</v>
+        <v>105.3988102674484</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1986</v>
+        <v>1976</v>
       </c>
       <c r="B28" t="n">
-        <v>37.71061179496347</v>
+        <v>43.41879626327474</v>
       </c>
       <c r="C28" t="n">
-        <v>80.79355754137686</v>
+        <v>91.2773327500002</v>
       </c>
       <c r="D28" t="n">
-        <v>2.895024033035791</v>
+        <v>-11.82799145558623</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.1188303460950237</v>
+        <v>-5.056570012751585</v>
       </c>
       <c r="F28" t="n">
-        <v>121.2803630232811</v>
+        <v>117.8115675449371</v>
       </c>
       <c r="G28" t="n">
-        <v>38.96269685331959</v>
+        <v>44.28383270214893</v>
       </c>
       <c r="H28" t="n">
-        <v>83.47610235817838</v>
+        <v>93.09585895678916</v>
       </c>
       <c r="I28" t="n">
-        <v>2.991145951053311</v>
+        <v>-12.06364155389236</v>
       </c>
       <c r="J28" t="n">
-        <v>10.65317729503711</v>
+        <v>-1.753394251620526</v>
       </c>
       <c r="K28" t="n">
-        <v>2.491585288917348</v>
+        <v>-12.18208663383597</v>
       </c>
       <c r="L28" t="n">
-        <v>138.5747077465057</v>
+        <v>111.3805692195892</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1987</v>
+        <v>1977</v>
       </c>
       <c r="B29" t="n">
-        <v>37.7361678445486</v>
+        <v>44.72658105213805</v>
       </c>
       <c r="C29" t="n">
-        <v>81.05221390576605</v>
+        <v>93.56549419247013</v>
       </c>
       <c r="D29" t="n">
-        <v>3.921929946438994</v>
+        <v>-11.48569512141521</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2137538335464981</v>
+        <v>-4.729431718880839</v>
       </c>
       <c r="F29" t="n">
-        <v>122.9240655303001</v>
+        <v>122.0769484043121</v>
       </c>
       <c r="G29" t="n">
-        <v>39.14637564117176</v>
+        <v>45.80248529777142</v>
       </c>
       <c r="H29" t="n">
-        <v>84.08115061323279</v>
+        <v>95.81622541489722</v>
       </c>
       <c r="I29" t="n">
-        <v>4.068493217279361</v>
+        <v>-11.7619851452553</v>
       </c>
       <c r="J29" t="n">
-        <v>15.65577074704103</v>
+        <v>-0.2118483720625231</v>
       </c>
       <c r="K29" t="n">
-        <v>-1.02089989699337</v>
+        <v>-12.45164430140703</v>
       </c>
       <c r="L29" t="n">
-        <v>141.9308903217316</v>
+        <v>117.1932328939438</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1988</v>
+        <v>1978</v>
       </c>
       <c r="B30" t="n">
-        <v>37.70821977079174</v>
+        <v>45.93568975917675</v>
       </c>
       <c r="C30" t="n">
-        <v>81.30826869889769</v>
+        <v>95.70340917614995</v>
       </c>
       <c r="D30" t="n">
-        <v>4.986040124720872</v>
+        <v>-11.06943143176876</v>
       </c>
       <c r="E30" t="n">
-        <v>0.4749751821399926</v>
+        <v>-4.4349846098049</v>
       </c>
       <c r="F30" t="n">
-        <v>124.4775037765503</v>
+        <v>126.1346828937531</v>
       </c>
       <c r="G30" t="n">
-        <v>39.26979423973023</v>
+        <v>47.22713539426721</v>
       </c>
       <c r="H30" t="n">
-        <v>84.67541032705108</v>
+        <v>98.39403493341582</v>
       </c>
       <c r="I30" t="n">
-        <v>5.192522239421445</v>
+        <v>-11.38063975323812</v>
       </c>
       <c r="J30" t="n">
-        <v>16.74875078235079</v>
+        <v>8.826165671292136</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.7213138331366693</v>
+        <v>-20.24291594750403</v>
       </c>
       <c r="L30" t="n">
-        <v>145.1651637554169</v>
+        <v>122.823780298233</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1989</v>
+        <v>1979</v>
       </c>
       <c r="B31" t="n">
-        <v>37.63306922278267</v>
+        <v>47.04213945251506</v>
       </c>
       <c r="C31" t="n">
-        <v>81.57682547474236</v>
+        <v>97.68922300568309</v>
       </c>
       <c r="D31" t="n">
-        <v>6.085434319992491</v>
+        <v>-10.57974019666463</v>
       </c>
       <c r="E31" t="n">
-        <v>0.6614613701129457</v>
+        <v>-4.172561373243113</v>
       </c>
       <c r="F31" t="n">
-        <v>125.9567903876305</v>
+        <v>129.9790608882904</v>
       </c>
       <c r="G31" t="n">
-        <v>39.33915982804758</v>
+        <v>48.55233167199075</v>
       </c>
       <c r="H31" t="n">
-        <v>85.27510091238689</v>
+        <v>100.8253368437607</v>
       </c>
       <c r="I31" t="n">
-        <v>6.361316742997482</v>
+        <v>-10.91938124009984</v>
       </c>
       <c r="J31" t="n">
-        <v>17.87438333782273</v>
+        <v>12.34901270354981</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.5551970177726133</v>
+        <v>-22.54527676867589</v>
       </c>
       <c r="L31" t="n">
-        <v>148.2947638034821</v>
+        <v>128.2620232105255</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1990</v>
+        <v>1980</v>
       </c>
       <c r="B32" t="n">
-        <v>37.51706709036858</v>
+        <v>48.0427965694126</v>
       </c>
       <c r="C32" t="n">
-        <v>81.87206625962428</v>
+        <v>99.52222942956075</v>
       </c>
       <c r="D32" t="n">
-        <v>7.218587216502891</v>
+        <v>-10.01749156270915</v>
       </c>
       <c r="E32" t="n">
-        <v>0.7709029786740729</v>
+        <v>-3.94115564254777</v>
       </c>
       <c r="F32" t="n">
-        <v>127.3786235451698</v>
+        <v>133.6063787937164</v>
       </c>
       <c r="G32" t="n">
-        <v>39.36096207950109</v>
+        <v>49.77357746657807</v>
       </c>
       <c r="H32" t="n">
-        <v>85.89592804931095</v>
+        <v>103.1075988468288</v>
       </c>
       <c r="I32" t="n">
-        <v>7.573367529288659</v>
+        <v>-10.37837985965088</v>
       </c>
       <c r="J32" t="n">
-        <v>17.15004722638063</v>
+        <v>5.789237996461569</v>
       </c>
       <c r="K32" t="n">
-        <v>1.358855081033823</v>
+        <v>-14.79142719809661</v>
       </c>
       <c r="L32" t="n">
-        <v>151.3391599655151</v>
+        <v>133.500607252121</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1991</v>
+        <v>1981</v>
       </c>
       <c r="B33" t="n">
-        <v>37.36659926070372</v>
+        <v>48.9353906170622</v>
       </c>
       <c r="C33" t="n">
-        <v>82.2072009042118</v>
+        <v>101.2028859588783</v>
       </c>
       <c r="D33" t="n">
-        <v>8.38438764590081</v>
+        <v>-9.383859888729356</v>
       </c>
       <c r="E33" t="n">
-        <v>0.8021023946623345</v>
+        <v>-3.739477140626114</v>
       </c>
       <c r="F33" t="n">
-        <v>128.7602902054787</v>
+        <v>137.0149395465851</v>
       </c>
       <c r="G33" t="n">
-        <v>39.34194435857267</v>
+        <v>50.88735708958646</v>
       </c>
       <c r="H33" t="n">
-        <v>86.55299620077325</v>
+        <v>105.2397320496818</v>
       </c>
       <c r="I33" t="n">
-        <v>8.827619284921825</v>
+        <v>-9.758169353815722</v>
       </c>
       <c r="J33" t="n">
-        <v>14.41333063084411</v>
+        <v>7.177473332790324</v>
       </c>
       <c r="K33" t="n">
-        <v>5.184158810776802</v>
+        <v>-15.01137622390231</v>
       </c>
       <c r="L33" t="n">
-        <v>154.3200492858887</v>
+        <v>138.5350168943405</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1992</v>
+        <v>1982</v>
       </c>
       <c r="B34" t="n">
-        <v>37.18807371396998</v>
+        <v>49.71852863810011</v>
       </c>
       <c r="C34" t="n">
-        <v>82.59442842984855</v>
+        <v>102.732821302214</v>
       </c>
       <c r="D34" t="n">
-        <v>9.582156841162433</v>
+        <v>-8.680294063244625</v>
       </c>
       <c r="E34" t="n">
-        <v>0.7550054456373303</v>
+        <v>-3.566003024438842</v>
       </c>
       <c r="F34" t="n">
-        <v>130.1196644306183</v>
+        <v>140.2050528526306</v>
       </c>
       <c r="G34" t="n">
-        <v>39.28907739495488</v>
+        <v>51.89116012575058</v>
       </c>
       <c r="H34" t="n">
-        <v>87.26074160042742</v>
+        <v>107.2221046436626</v>
       </c>
       <c r="I34" t="n">
-        <v>10.12351714258332</v>
+        <v>-9.059611004442655</v>
       </c>
       <c r="J34" t="n">
-        <v>13.18193450379734</v>
+        <v>7.100672079553606</v>
       </c>
       <c r="K34" t="n">
-        <v>7.406090718786961</v>
+        <v>-13.79075014757894</v>
       </c>
       <c r="L34" t="n">
-        <v>157.2613613605499</v>
+        <v>143.3635756969452</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1993</v>
+        <v>1983</v>
       </c>
       <c r="B35" t="n">
-        <v>36.98790954798916</v>
+        <v>50.39169842513177</v>
       </c>
       <c r="C35" t="n">
-        <v>83.04491049241632</v>
+        <v>104.1148435435144</v>
       </c>
       <c r="D35" t="n">
-        <v>10.8116637764354</v>
+        <v>-7.908485023284301</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6307220218393894</v>
+        <v>-3.419023904361545</v>
       </c>
       <c r="F35" t="n">
-        <v>131.4752058386803</v>
+        <v>143.1790330410004</v>
       </c>
       <c r="G35" t="n">
-        <v>39.20953391717236</v>
+        <v>52.7834929539832</v>
       </c>
       <c r="H35" t="n">
-        <v>88.03288086276724</v>
+        <v>109.0565565824107</v>
       </c>
       <c r="I35" t="n">
-        <v>11.46105045469524</v>
+        <v>-8.283853820156629</v>
       </c>
       <c r="J35" t="n">
-        <v>10.53469710115306</v>
+        <v>8.676275893439007</v>
       </c>
       <c r="K35" t="n">
-        <v>10.95109099444283</v>
+        <v>-14.24502041395939</v>
       </c>
       <c r="L35" t="n">
-        <v>160.1892533302307</v>
+        <v>147.9874511957169</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1994</v>
+        <v>1984</v>
       </c>
       <c r="B36" t="n">
-        <v>36.77252929020101</v>
+        <v>50.95527169742758</v>
       </c>
       <c r="C36" t="n">
-        <v>83.56875065539455</v>
+        <v>105.3529431326325</v>
       </c>
       <c r="D36" t="n">
-        <v>12.07314060156116</v>
+        <v>-7.070330436326387</v>
       </c>
       <c r="E36" t="n">
-        <v>0.4315434077688067</v>
+        <v>-3.296681991618783</v>
       </c>
       <c r="F36" t="n">
-        <v>132.8459639549255</v>
+        <v>145.9412024021149</v>
       </c>
       <c r="G36" t="n">
-        <v>39.11066735850467</v>
+        <v>53.56388736524139</v>
       </c>
       <c r="H36" t="n">
-        <v>88.88237147505414</v>
+        <v>110.7464054565702</v>
       </c>
       <c r="I36" t="n">
-        <v>12.84079706113505</v>
+        <v>-7.432290526782602</v>
       </c>
       <c r="J36" t="n">
-        <v>14.38907876825045</v>
+        <v>10.19609489014616</v>
       </c>
       <c r="K36" t="n">
-        <v>7.909199747456077</v>
+        <v>-14.663440256159</v>
       </c>
       <c r="L36" t="n">
-        <v>163.1321144104004</v>
+        <v>152.4106569290161</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1995</v>
+        <v>1985</v>
       </c>
       <c r="B37" t="n">
-        <v>36.54835200856295</v>
+        <v>51.41050401810343</v>
       </c>
       <c r="C37" t="n">
-        <v>84.17498847128414</v>
+        <v>106.4522903415958</v>
       </c>
       <c r="D37" t="n">
-        <v>13.36729509409701</v>
+        <v>-6.167896770337384</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1609373330268866</v>
+        <v>-3.197009262716954</v>
       </c>
       <c r="F37" t="n">
-        <v>134.251572906971</v>
+        <v>148.4978883266449</v>
       </c>
       <c r="G37" t="n">
-        <v>38.99999225307309</v>
+        <v>54.23290528689068</v>
       </c>
       <c r="H37" t="n">
-        <v>89.82139324677243</v>
+        <v>112.2964477771975</v>
       </c>
       <c r="I37" t="n">
-        <v>14.26396476076907</v>
+        <v>-6.506510055751178</v>
       </c>
       <c r="J37" t="n">
-        <v>16.11645711097677</v>
+        <v>12.55866140380141</v>
       </c>
       <c r="K37" t="n">
-        <v>6.91875398972152</v>
+        <v>-15.94144780203101</v>
       </c>
       <c r="L37" t="n">
-        <v>166.1205613613129</v>
+        <v>156.6400566101074</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="B38" t="n">
-        <v>36.32179043256151</v>
+        <v>51.75952868407051</v>
       </c>
       <c r="C38" t="n">
-        <v>84.87160657781986</v>
+        <v>107.4192343144029</v>
       </c>
       <c r="D38" t="n">
-        <v>14.69532515082411</v>
+        <v>-5.20337919366051</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.1764667429048501</v>
+        <v>-3.117959307208487</v>
       </c>
       <c r="F38" t="n">
-        <v>135.7122554183006</v>
+        <v>150.8574244976044</v>
       </c>
       <c r="G38" t="n">
-        <v>38.88516981348979</v>
+        <v>54.7921351312046</v>
       </c>
       <c r="H38" t="n">
-        <v>90.86134782506865</v>
+        <v>113.7129597560783</v>
       </c>
       <c r="I38" t="n">
-        <v>15.73243518970284</v>
+        <v>-5.508246755069248</v>
       </c>
       <c r="J38" t="n">
-        <v>19.29991270224928</v>
+        <v>10.82435430705965</v>
       </c>
       <c r="K38" t="n">
-        <v>4.408576772193296</v>
+        <v>-13.1358356895098</v>
       </c>
       <c r="L38" t="n">
-        <v>169.1874423027039</v>
+        <v>160.6853667497635</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1997</v>
+        <v>1987</v>
       </c>
       <c r="B39" t="n">
-        <v>36.09924980912688</v>
+        <v>52.005348788113</v>
       </c>
       <c r="C39" t="n">
-        <v>85.6655400753896</v>
+        <v>108.2612986727404</v>
       </c>
       <c r="D39" t="n">
-        <v>16.05893035312515</v>
+        <v>-4.179059098986004</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.5748985618641953</v>
+        <v>-3.057436279424152</v>
       </c>
       <c r="F39" t="n">
-        <v>137.2488216757774</v>
+        <v>153.0301520824432</v>
       </c>
       <c r="G39" t="n">
-        <v>38.77399697719627</v>
+        <v>55.24418493636018</v>
       </c>
       <c r="H39" t="n">
-        <v>92.01286479624437</v>
+        <v>115.0036937487946</v>
       </c>
       <c r="I39" t="n">
-        <v>17.24880489930991</v>
+        <v>-4.439326321317392</v>
       </c>
       <c r="J39" t="n">
-        <v>21.28907576483529</v>
+        <v>16.38424778279656</v>
       </c>
       <c r="K39" t="n">
-        <v>3.043093799367906</v>
+        <v>-17.63364205985724</v>
       </c>
       <c r="L39" t="n">
-        <v>172.3678362369537</v>
+        <v>164.5591580867767</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1998</v>
+        <v>1988</v>
       </c>
       <c r="B40" t="n">
-        <v>35.88712985688779</v>
+        <v>52.15182797415758</v>
       </c>
       <c r="C40" t="n">
-        <v>86.56270617655886</v>
+        <v>108.9871733004609</v>
       </c>
       <c r="D40" t="n">
-        <v>17.46032460410036</v>
+        <v>-3.097259747333005</v>
       </c>
       <c r="E40" t="n">
-        <v>-1.027492678810596</v>
+        <v>-3.013324893679517</v>
       </c>
       <c r="F40" t="n">
-        <v>138.8826679587364</v>
+        <v>155.028416633606</v>
       </c>
       <c r="G40" t="n">
-        <v>38.67440060583528</v>
+        <v>55.59267410989249</v>
       </c>
       <c r="H40" t="n">
-        <v>93.28583226208926</v>
+        <v>116.1778722397462</v>
       </c>
       <c r="I40" t="n">
-        <v>18.81642781520172</v>
+        <v>-3.301609137315249</v>
       </c>
       <c r="J40" t="n">
-        <v>20.17153856923074</v>
+        <v>17.5950674260159</v>
       </c>
       <c r="K40" t="n">
-        <v>4.750852604637618</v>
+        <v>-17.78714535489203</v>
       </c>
       <c r="L40" t="n">
-        <v>175.6990518569946</v>
+        <v>168.2768592834473</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1999</v>
+        <v>1989</v>
       </c>
       <c r="B41" t="n">
-        <v>35.6918297195195</v>
+        <v>52.20367738905199</v>
       </c>
       <c r="C41" t="n">
-        <v>87.5680304102724</v>
+        <v>109.6067079503459</v>
       </c>
       <c r="D41" t="n">
-        <v>18.90224923951075</v>
+        <v>-1.960300053749089</v>
       </c>
       <c r="E41" t="n">
-        <v>-1.526331001783277</v>
+        <v>-2.983514097675808</v>
       </c>
       <c r="F41" t="n">
-        <v>140.6357783675194</v>
+        <v>156.866571187973</v>
       </c>
       <c r="G41" t="n">
-        <v>38.59443687368142</v>
+        <v>55.84222010936139</v>
       </c>
       <c r="H41" t="n">
-        <v>94.68942467731159</v>
+        <v>117.2461829692733</v>
       </c>
       <c r="I41" t="n">
-        <v>20.4394582955752</v>
+        <v>-2.096930954998332</v>
       </c>
       <c r="J41" t="n">
-        <v>21.7276702831632</v>
+        <v>18.84206386944151</v>
       </c>
       <c r="K41" t="n">
-        <v>3.76963622448611</v>
+        <v>-17.97677239177482</v>
       </c>
       <c r="L41" t="n">
-        <v>179.2206263542175</v>
+        <v>171.8567636013031</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="B42" t="n">
-        <v>35.51975583605706</v>
+        <v>52.16644167936234</v>
       </c>
       <c r="C42" t="n">
-        <v>88.68548387644834</v>
+        <v>110.1309012681358</v>
       </c>
       <c r="D42" t="n">
-        <v>20.38798519919897</v>
+        <v>-0.7704466043620857</v>
       </c>
       <c r="E42" t="n">
-        <v>-2.062500028624839</v>
+        <v>-2.965920314693676</v>
       </c>
       <c r="F42" t="n">
-        <v>142.5307248830795</v>
+        <v>158.5609760284424</v>
       </c>
       <c r="G42" t="n">
-        <v>38.54229680382326</v>
+        <v>55.99842297360951</v>
       </c>
       <c r="H42" t="n">
-        <v>96.23214352973977</v>
+        <v>118.2207678565452</v>
       </c>
       <c r="I42" t="n">
-        <v>22.122893535822</v>
+        <v>-0.8270411674775481</v>
       </c>
       <c r="J42" t="n">
-        <v>26.62762764498752</v>
+        <v>18.02951935293441</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.5506349038073566</v>
+        <v>-16.10164392920865</v>
       </c>
       <c r="L42" t="n">
-        <v>182.9743266105652</v>
+        <v>175.3200250864029</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2001</v>
+        <v>1991</v>
       </c>
       <c r="B43" t="n">
-        <v>35.37733296577623</v>
+        <v>52.04648281914834</v>
       </c>
       <c r="C43" t="n">
-        <v>89.91812070085572</v>
+        <v>110.5718933673599</v>
       </c>
       <c r="D43" t="n">
-        <v>21.92136649076343</v>
+        <v>0.4701357523780564</v>
       </c>
       <c r="E43" t="n">
-        <v>-2.626154518948582</v>
+        <v>-2.958518261747059</v>
       </c>
       <c r="F43" t="n">
-        <v>144.5906656384468</v>
+        <v>160.1299936771393</v>
       </c>
       <c r="G43" t="n">
-        <v>38.52631843076895</v>
+        <v>56.06784966289666</v>
       </c>
       <c r="H43" t="n">
-        <v>97.92185731379864</v>
+        <v>119.1152208268359</v>
       </c>
       <c r="I43" t="n">
-        <v>23.87261772044125</v>
+        <v>0.5064607492706077</v>
       </c>
       <c r="J43" t="n">
-        <v>22.51197264230167</v>
+        <v>14.97623727424066</v>
       </c>
       <c r="K43" t="n">
-        <v>4.171385236988815</v>
+        <v>-11.97510171846696</v>
       </c>
       <c r="L43" t="n">
-        <v>187.0041513442993</v>
+        <v>178.6906667947769</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2002</v>
+        <v>1992</v>
       </c>
       <c r="B44" t="n">
-        <v>35.2710187148443</v>
+        <v>51.8509662037881</v>
       </c>
       <c r="C44" t="n">
-        <v>91.26811576546687</v>
+        <v>110.9429562214854</v>
       </c>
       <c r="D44" t="n">
-        <v>23.50679434422921</v>
+        <v>1.759434645404824</v>
       </c>
       <c r="E44" t="n">
-        <v>-3.206582475301033</v>
+        <v>-2.959358876937472</v>
       </c>
       <c r="F44" t="n">
-        <v>146.8393463492393</v>
+        <v>161.5939981937408</v>
       </c>
       <c r="G44" t="n">
-        <v>38.55500553267243</v>
+        <v>56.05801853675138</v>
       </c>
       <c r="H44" t="n">
-        <v>99.76583712375761</v>
+        <v>119.9445786977767</v>
       </c>
       <c r="I44" t="n">
-        <v>25.69544682914755</v>
+        <v>1.902190589441716</v>
       </c>
       <c r="J44" t="n">
-        <v>27.73643980695459</v>
+        <v>13.59792620902363</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.3963986593687281</v>
+        <v>-9.507132167682787</v>
       </c>
       <c r="L44" t="n">
-        <v>191.3563306331635</v>
+        <v>181.9955818653107</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2003</v>
+        <v>1993</v>
       </c>
       <c r="B45" t="n">
-        <v>35.20732046136307</v>
+        <v>51.58784272178254</v>
       </c>
       <c r="C45" t="n">
-        <v>92.73679486039016</v>
+        <v>111.2584829980165</v>
       </c>
       <c r="D45" t="n">
-        <v>25.1492507253371</v>
+        <v>3.09564234000029</v>
       </c>
       <c r="E45" t="n">
-        <v>-3.792266329473307</v>
+        <v>-2.966602421066405</v>
       </c>
       <c r="F45" t="n">
-        <v>149.301099717617</v>
+        <v>162.9753656387329</v>
       </c>
       <c r="G45" t="n">
-        <v>38.63705233192732</v>
+        <v>55.97738310537027</v>
       </c>
       <c r="H45" t="n">
-        <v>101.770778041692</v>
+        <v>120.7253181740935</v>
       </c>
       <c r="I45" t="n">
-        <v>27.59917266211605</v>
+        <v>3.359046396996022</v>
       </c>
       <c r="J45" t="n">
-        <v>28.58353428039268</v>
+        <v>10.64330366658101</v>
       </c>
       <c r="K45" t="n">
-        <v>-0.5112171237910381</v>
+        <v>-5.440514127808003</v>
       </c>
       <c r="L45" t="n">
-        <v>196.079320192337</v>
+        <v>185.2645372152328</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2004</v>
+        <v>1994</v>
       </c>
       <c r="B46" t="n">
-        <v>35.1928167723481</v>
+        <v>51.26583665133312</v>
       </c>
       <c r="C46" t="n">
-        <v>94.32466335839256</v>
+        <v>111.5339829316722</v>
       </c>
       <c r="D46" t="n">
-        <v>26.85431442569104</v>
+        <v>4.477208539092099</v>
       </c>
       <c r="E46" t="n">
-        <v>-4.370947872452668</v>
+        <v>-2.978547611385743</v>
       </c>
       <c r="F46" t="n">
-        <v>152.000846683979</v>
+        <v>164.2984805107117</v>
       </c>
       <c r="G46" t="n">
-        <v>38.78137783272454</v>
+        <v>55.83532094044448</v>
       </c>
       <c r="H46" t="n">
-        <v>103.942814021087</v>
+        <v>121.4753555103452</v>
       </c>
       <c r="I46" t="n">
-        <v>29.59261035904922</v>
+        <v>4.876276132928482</v>
       </c>
       <c r="J46" t="n">
-        <v>33.18634592045535</v>
+        <v>14.92454472067721</v>
       </c>
       <c r="K46" t="n">
-        <v>-4.279339129486154</v>
+        <v>-8.581323168233551</v>
       </c>
       <c r="L46" t="n">
-        <v>201.22380900383</v>
+        <v>188.5301741361618</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2005</v>
+        <v>1995</v>
       </c>
       <c r="B47" t="n">
-        <v>35.23418059817782</v>
+        <v>50.89443145034392</v>
       </c>
       <c r="C47" t="n">
-        <v>96.03141448261972</v>
+        <v>111.786076729326</v>
       </c>
       <c r="D47" t="n">
-        <v>28.62817624732453</v>
+        <v>5.902894323115618</v>
       </c>
       <c r="E47" t="n">
-        <v>-4.929677285344049</v>
+        <v>-2.993668902169119</v>
       </c>
       <c r="F47" t="n">
-        <v>154.964094042778</v>
+        <v>165.5897336006165</v>
       </c>
       <c r="G47" t="n">
-        <v>38.99716536776136</v>
+        <v>55.64212414864494</v>
       </c>
       <c r="H47" t="n">
-        <v>106.2874994536535</v>
+        <v>122.2140533298182</v>
       </c>
       <c r="I47" t="n">
-        <v>31.68564457412327</v>
+        <v>6.4535464765647</v>
       </c>
       <c r="J47" t="n">
-        <v>37.1998620319838</v>
+        <v>16.83727956424859</v>
       </c>
       <c r="K47" t="n">
-        <v>-7.327457594666733</v>
+        <v>-9.318986761311347</v>
       </c>
       <c r="L47" t="n">
-        <v>206.8427138328552</v>
+        <v>191.8280167579651</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2006</v>
+        <v>1996</v>
       </c>
       <c r="B48" t="n">
-        <v>35.33820622605195</v>
+        <v>50.48386104688534</v>
       </c>
       <c r="C48" t="n">
-        <v>97.85593171878809</v>
+        <v>112.0324906192857</v>
       </c>
       <c r="D48" t="n">
-        <v>30.47765552076696</v>
+        <v>7.371826295495705</v>
       </c>
       <c r="E48" t="n">
-        <v>-5.454857294552156</v>
+        <v>-3.010658115704217</v>
       </c>
       <c r="F48" t="n">
-        <v>158.2169361710548</v>
+        <v>166.8775198459625</v>
       </c>
       <c r="G48" t="n">
-        <v>39.2939107908675</v>
+        <v>55.40899666687305</v>
       </c>
       <c r="H48" t="n">
-        <v>108.80977451766</v>
+        <v>122.9622253642676</v>
       </c>
       <c r="I48" t="n">
-        <v>33.88927750002561</v>
+        <v>8.091011467140733</v>
       </c>
       <c r="J48" t="n">
-        <v>39.69275712450992</v>
+        <v>20.36876189910278</v>
       </c>
       <c r="K48" t="n">
-        <v>-8.694536175281058</v>
+        <v>-11.63452775936845</v>
       </c>
       <c r="L48" t="n">
-        <v>212.991183757782</v>
+        <v>195.1964676380157</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2007</v>
+        <v>1997</v>
       </c>
       <c r="B49" t="n">
-        <v>35.51183888957578</v>
+        <v>50.04510574404886</v>
       </c>
       <c r="C49" t="n">
-        <v>99.79626703674111</v>
+        <v>112.2920622610239</v>
       </c>
       <c r="D49" t="n">
-        <v>32.41021770580462</v>
+        <v>8.883551258478132</v>
       </c>
       <c r="E49" t="n">
-        <v>-5.932267828822575</v>
+        <v>-3.028476164338251</v>
       </c>
       <c r="F49" t="n">
-        <v>161.786055803299</v>
+        <v>168.1922430992126</v>
       </c>
       <c r="G49" t="n">
-        <v>39.68147723019083</v>
+        <v>55.14806027179576</v>
       </c>
       <c r="H49" t="n">
-        <v>111.5138900688956</v>
+        <v>123.7421587095277</v>
       </c>
       <c r="I49" t="n">
-        <v>36.21567781712181</v>
+        <v>9.789381258094297</v>
       </c>
       <c r="J49" t="n">
-        <v>42.52924426710228</v>
+        <v>22.56964543602227</v>
       </c>
       <c r="K49" t="n">
-        <v>-10.21369207419799</v>
+        <v>-12.57242837750452</v>
       </c>
       <c r="L49" t="n">
-        <v>219.7265973091125</v>
+        <v>198.6768172979355</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2008</v>
+        <v>1998</v>
       </c>
       <c r="B50" t="n">
-        <v>35.76220646011388</v>
+        <v>49.58989124420783</v>
       </c>
       <c r="C50" t="n">
-        <v>101.8495973124623</v>
+        <v>112.5847444948703</v>
       </c>
       <c r="D50" t="n">
-        <v>34.43399221694381</v>
+        <v>10.438090626186</v>
       </c>
       <c r="E50" t="n">
-        <v>-6.347074759489921</v>
+        <v>-3.04641452902149</v>
       </c>
       <c r="F50" t="n">
-        <v>165.6987212300301</v>
+        <v>169.5663118362427</v>
       </c>
       <c r="G50" t="n">
-        <v>40.1701566951564</v>
+        <v>54.87236737703771</v>
       </c>
       <c r="H50" t="n">
-        <v>114.4032957793948</v>
+        <v>124.5776368120997</v>
       </c>
       <c r="I50" t="n">
-        <v>38.67823045362577</v>
+        <v>11.54998991093354</v>
       </c>
       <c r="J50" t="n">
-        <v>41.26485909291869</v>
+        <v>21.31366972624049</v>
       </c>
       <c r="K50" t="n">
-        <v>-7.407980505287512</v>
+        <v>-10.00042139085614</v>
       </c>
       <c r="L50" t="n">
-        <v>227.1085615158081</v>
+        <v>202.3132424354553</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2009</v>
+        <v>1999</v>
       </c>
       <c r="B51" t="n">
-        <v>36.09665393760542</v>
+        <v>49.13069846472295</v>
       </c>
       <c r="C51" t="n">
-        <v>104.0121596041666</v>
+        <v>112.9316185654122</v>
       </c>
       <c r="D51" t="n">
-        <v>36.55779117055905</v>
+        <v>12.0359944177073</v>
       </c>
       <c r="E51" t="n">
-        <v>-6.683815434300698</v>
+        <v>-3.064169668896461</v>
       </c>
       <c r="F51" t="n">
-        <v>169.9827892780304</v>
+        <v>171.0341417789459</v>
       </c>
       <c r="G51" t="n">
-        <v>40.77073842495055</v>
+        <v>54.59592996620321</v>
       </c>
       <c r="H51" t="n">
-        <v>117.4804888997698</v>
+        <v>125.4939768990721</v>
       </c>
       <c r="I51" t="n">
-        <v>41.29158740821798</v>
+        <v>13.37486192618625</v>
       </c>
       <c r="J51" t="n">
-        <v>43.50071802861427</v>
+        <v>23.03030070738717</v>
       </c>
       <c r="K51" t="n">
-        <v>-7.844618710496704</v>
+        <v>-10.34225618345713</v>
       </c>
       <c r="L51" t="n">
-        <v>235.1989140510559</v>
+        <v>206.1528133153915</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="B52" t="n">
-        <v>36.52277887251248</v>
+        <v>48.68077941386195</v>
       </c>
       <c r="C52" t="n">
-        <v>106.2791537116574</v>
+        <v>113.3549127382047</v>
       </c>
       <c r="D52" t="n">
-        <v>38.79112815264403</v>
+        <v>13.67839433664197</v>
       </c>
       <c r="E52" t="n">
-        <v>-6.926357989468926</v>
+        <v>-3.081933216079811</v>
       </c>
       <c r="F52" t="n">
-        <v>174.666702747345</v>
+        <v>172.6321532726288</v>
       </c>
       <c r="G52" t="n">
-        <v>41.49458234716073</v>
+        <v>54.33375954058786</v>
       </c>
       <c r="H52" t="n">
-        <v>120.7468114862955</v>
+        <v>126.5180764486311</v>
       </c>
       <c r="I52" t="n">
-        <v>44.07171938060208</v>
+        <v>15.26677669784425</v>
       </c>
       <c r="J52" t="n">
-        <v>47.79824615604387</v>
+        <v>28.46245436568747</v>
       </c>
       <c r="K52" t="n">
-        <v>-10.04963542257715</v>
+        <v>-14.33557530966292</v>
       </c>
       <c r="L52" t="n">
-        <v>244.061723947525</v>
+        <v>210.2454917430878</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="B53" t="n">
-        <v>37.04846928523311</v>
+        <v>48.25418449863953</v>
       </c>
       <c r="C53" t="n">
-        <v>108.6446134231781</v>
+        <v>113.8780286235422</v>
       </c>
       <c r="D53" t="n">
-        <v>41.1442387652895</v>
+        <v>15.36705557367523</v>
       </c>
       <c r="E53" t="n">
-        <v>-7.057828678233349</v>
+        <v>-3.100494310404699</v>
       </c>
       <c r="F53" t="n">
-        <v>179.7794927954674</v>
+        <v>174.3987743854523</v>
       </c>
       <c r="G53" t="n">
-        <v>42.35369782390887</v>
+        <v>54.10192536380669</v>
       </c>
       <c r="H53" t="n">
-        <v>124.2021928542878</v>
+        <v>127.6784732594958</v>
       </c>
       <c r="I53" t="n">
-        <v>47.03596908265261</v>
+        <v>17.22933052017255</v>
       </c>
       <c r="J53" t="n">
-        <v>48.23811911783717</v>
+        <v>23.8717334560006</v>
       </c>
       <c r="K53" t="n">
-        <v>-8.066692288110232</v>
+        <v>-8.237323071201072</v>
       </c>
       <c r="L53" t="n">
-        <v>253.7632865905762</v>
+        <v>214.6441395282745</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2012</v>
+        <v>2002</v>
       </c>
       <c r="B54" t="n">
-        <v>37.68194098452431</v>
+        <v>47.8658030594471</v>
       </c>
       <c r="C54" t="n">
-        <v>111.101244405763</v>
+        <v>114.5255778820094</v>
       </c>
       <c r="D54" t="n">
-        <v>43.62810007811899</v>
+        <v>17.10442650467566</v>
       </c>
       <c r="E54" t="n">
-        <v>-7.060508140391924</v>
+        <v>-3.121367968211601</v>
       </c>
       <c r="F54" t="n">
-        <v>185.3507773280144</v>
+        <v>176.3744394779205</v>
       </c>
       <c r="G54" t="n">
-        <v>43.36082611602388</v>
+        <v>53.91763241755898</v>
       </c>
       <c r="H54" t="n">
-        <v>127.8448406341554</v>
+        <v>129.0054196517231</v>
       </c>
       <c r="I54" t="n">
-        <v>50.20310556817477</v>
+        <v>19.26699484905515</v>
       </c>
       <c r="J54" t="n">
-        <v>51.2475175541022</v>
+        <v>29.66037361892228</v>
       </c>
       <c r="K54" t="n">
-        <v>-8.284156855869981</v>
+        <v>-12.44590503242247</v>
       </c>
       <c r="L54" t="n">
-        <v>264.3721330165863</v>
+        <v>219.404515504837</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2013</v>
+        <v>2003</v>
       </c>
       <c r="B55" t="n">
-        <v>38.43177634961764</v>
+        <v>47.5314162424393</v>
       </c>
       <c r="C55" t="n">
-        <v>113.6402216585881</v>
+        <v>115.3234273333192</v>
       </c>
       <c r="D55" t="n">
-        <v>46.25445188540107</v>
+        <v>18.89368606130011</v>
       </c>
       <c r="E55" t="n">
-        <v>-6.915688775671669</v>
+        <v>-3.146941626270639</v>
       </c>
       <c r="F55" t="n">
-        <v>191.4107611179352</v>
+        <v>178.601588010788</v>
       </c>
       <c r="G55" t="n">
-        <v>44.52952543831268</v>
+        <v>53.79932028891323</v>
       </c>
       <c r="H55" t="n">
-        <v>131.670862546845</v>
+        <v>130.5309728680209</v>
       </c>
       <c r="I55" t="n">
-        <v>53.5933799449962</v>
+        <v>21.38517107644035</v>
       </c>
       <c r="J55" t="n">
-        <v>53.8084524036118</v>
+        <v>30.58334824800995</v>
       </c>
       <c r="K55" t="n">
-        <v>-7.643199719141691</v>
+        <v>-11.71352812908183</v>
       </c>
       <c r="L55" t="n">
-        <v>275.959020614624</v>
+        <v>224.5852843523026</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2014</v>
+        <v>2004</v>
       </c>
       <c r="B56" t="n">
-        <v>39.30696215735033</v>
+        <v>47.26776662169039</v>
       </c>
       <c r="C56" t="n">
-        <v>116.2509439752739</v>
+        <v>116.298752267085</v>
       </c>
       <c r="D56" t="n">
-        <v>49.03581660781452</v>
+        <v>20.73878794553105</v>
       </c>
       <c r="E56" t="n">
-        <v>-6.603486279276233</v>
+        <v>-3.180639666642882</v>
       </c>
       <c r="F56" t="n">
-        <v>197.9902364611626</v>
+        <v>181.1246671676636</v>
       </c>
       <c r="G56" t="n">
-        <v>45.87425774419418</v>
+        <v>53.76678538193717</v>
       </c>
       <c r="H56" t="n">
-        <v>135.6738214868723</v>
+        <v>132.2890946673591</v>
       </c>
       <c r="I56" t="n">
-        <v>57.22858156168326</v>
+        <v>23.59024003552544</v>
       </c>
       <c r="J56" t="n">
-        <v>55.53933021340457</v>
+        <v>35.6769086651295</v>
       </c>
       <c r="K56" t="n">
-        <v>-5.719055257100351</v>
+        <v>-15.07501394225012</v>
       </c>
       <c r="L56" t="n">
-        <v>288.596935749054</v>
+        <v>230.2480148077011</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2015</v>
+        <v>2005</v>
       </c>
       <c r="B57" t="n">
-        <v>40.31692718529091</v>
+        <v>47.09264302816779</v>
       </c>
       <c r="C57" t="n">
-        <v>118.9207411146118</v>
+        <v>117.480103914318</v>
       </c>
       <c r="D57" t="n">
-        <v>51.98552097167747</v>
+        <v>22.64450101703293</v>
       </c>
       <c r="E57" t="n">
-        <v>-6.102605796944154</v>
+        <v>-3.227119919204974</v>
       </c>
       <c r="F57" t="n">
-        <v>205.1205834746361</v>
+        <v>183.9901280403137</v>
       </c>
       <c r="G57" t="n">
-        <v>47.41047671287962</v>
+        <v>53.841327845168</v>
       </c>
       <c r="H57" t="n">
-        <v>139.844214847546</v>
+        <v>134.3157738322697</v>
       </c>
       <c r="I57" t="n">
-        <v>61.1320976945343</v>
+        <v>25.88960662961849</v>
       </c>
       <c r="J57" t="n">
-        <v>58.11351133572528</v>
+        <v>40.11432605607294</v>
       </c>
       <c r="K57" t="n">
-        <v>-4.139203970125514</v>
+        <v>-17.70384826026199</v>
       </c>
       <c r="L57" t="n">
-        <v>302.3610966205597</v>
+        <v>236.4571861028671</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2016</v>
+        <v>2006</v>
       </c>
       <c r="B58" t="n">
-        <v>41.47157749352299</v>
+        <v>47.02498777341092</v>
       </c>
       <c r="C58" t="n">
-        <v>121.6345254686473</v>
+        <v>118.8974853507911</v>
       </c>
       <c r="D58" t="n">
-        <v>55.11771615559132</v>
+        <v>24.61644567445737</v>
       </c>
       <c r="E58" t="n">
-        <v>-5.390051048017519</v>
+        <v>-3.292487686369931</v>
       </c>
       <c r="F58" t="n">
-        <v>212.8337680697441</v>
+        <v>187.2464311122894</v>
       </c>
       <c r="G58" t="n">
-        <v>49.15471372923957</v>
+        <v>54.04592785700545</v>
       </c>
       <c r="H58" t="n">
-        <v>144.1688655305442</v>
+        <v>136.6491565422924</v>
       </c>
       <c r="I58" t="n">
-        <v>65.32897282387464</v>
+        <v>28.29173828663637</v>
       </c>
       <c r="J58" t="n">
-        <v>59.59933730424572</v>
+        <v>42.86257787642446</v>
       </c>
       <c r="K58" t="n">
-        <v>-0.9229382675275346</v>
+        <v>-18.56921235950075</v>
       </c>
       <c r="L58" t="n">
-        <v>317.3289511203766</v>
+        <v>243.280188202858</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="B59" t="n">
-        <v>42.78133110546195</v>
+        <v>47.08501560449325</v>
       </c>
       <c r="C59" t="n">
-        <v>124.3743836727143</v>
+        <v>120.5824360802454</v>
       </c>
       <c r="D59" t="n">
-        <v>58.44739909389794</v>
+        <v>26.66112491157562</v>
       </c>
       <c r="E59" t="n">
-        <v>-4.440768403076255</v>
+        <v>-3.384537013108073</v>
       </c>
       <c r="F59" t="n">
-        <v>221.162345468998</v>
+        <v>190.9440395832062</v>
       </c>
       <c r="G59" t="n">
-        <v>51.12466315781803</v>
+        <v>54.40544225001144</v>
       </c>
       <c r="H59" t="n">
-        <v>148.6302157138101</v>
+        <v>139.329692861001</v>
       </c>
       <c r="I59" t="n">
-        <v>69.84597051830852</v>
+        <v>30.80619753598741</v>
       </c>
       <c r="J59" t="n">
-        <v>64.24728210828241</v>
+        <v>45.99261463244734</v>
       </c>
       <c r="K59" t="n">
-        <v>-0.2679534758343678</v>
+        <v>-19.74661975144733</v>
       </c>
       <c r="L59" t="n">
-        <v>333.5801780223846</v>
+        <v>250.7873275279999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2018</v>
+        <v>2008</v>
       </c>
       <c r="B60" t="n">
-        <v>44.25714870948202</v>
+        <v>47.29435722448402</v>
       </c>
       <c r="C60" t="n">
-        <v>127.1190980533219</v>
+        <v>122.56813113794</v>
       </c>
       <c r="D60" t="n">
-        <v>61.99043204845722</v>
+        <v>28.78595062029484</v>
       </c>
       <c r="E60" t="n">
-        <v>-3.227223373600978</v>
+        <v>-3.513011746161901</v>
       </c>
       <c r="F60" t="n">
-        <v>230.1394554376602</v>
+        <v>195.135427236557</v>
       </c>
       <c r="G60" t="n">
-        <v>53.33926304455639</v>
+        <v>54.94683115953134</v>
       </c>
       <c r="H60" t="n">
-        <v>153.2055093192255</v>
+        <v>142.4002947161137</v>
       </c>
       <c r="I60" t="n">
-        <v>74.71163546895963</v>
+        <v>33.44366772958512</v>
       </c>
       <c r="J60" t="n">
-        <v>66.24644729424173</v>
+        <v>44.57081588627711</v>
       </c>
       <c r="K60" t="n">
-        <v>3.693827803009441</v>
+        <v>-16.30978241841004</v>
       </c>
       <c r="L60" t="n">
-        <v>351.1966829299927</v>
+        <v>259.0518270730972</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="B61" t="n">
-        <v>45.9105630603154</v>
+        <v>47.67621764358495</v>
       </c>
       <c r="C61" t="n">
-        <v>129.843586020921</v>
+        <v>124.8894795741657</v>
       </c>
       <c r="D61" t="n">
-        <v>65.76356302988859</v>
+        <v>30.99926336910197</v>
       </c>
       <c r="E61" t="n">
-        <v>-1.718884760985354</v>
+        <v>-3.689891207046159</v>
       </c>
       <c r="F61" t="n">
-        <v>239.7988273501396</v>
+        <v>199.8750693798065</v>
       </c>
       <c r="G61" t="n">
-        <v>55.8187734274934</v>
+        <v>55.69940719029634</v>
       </c>
       <c r="H61" t="n">
-        <v>157.8658423246366</v>
+        <v>145.9064984682495</v>
       </c>
       <c r="I61" t="n">
-        <v>79.95635818553201</v>
+        <v>36.21597262397714</v>
       </c>
       <c r="J61" t="n">
-        <v>70.19190504927502</v>
+        <v>47.03664975972345</v>
       </c>
       <c r="K61" t="n">
-        <v>6.429727395432963</v>
+        <v>-16.70869591276795</v>
       </c>
       <c r="L61" t="n">
-        <v>370.26260638237</v>
+        <v>268.1498321294785</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B62" t="n">
+        <v>48.25555099846269</v>
+      </c>
+      <c r="C62" t="n">
+        <v>127.5832369732572</v>
+      </c>
+      <c r="D62" t="n">
+        <v>33.31034718308678</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-3.929684442602642</v>
+      </c>
+      <c r="F62" t="n">
+        <v>205.219450712204</v>
+      </c>
+      <c r="G62" t="n">
+        <v>56.69510274449478</v>
+      </c>
+      <c r="H62" t="n">
+        <v>149.8966352887459</v>
+      </c>
+      <c r="I62" t="n">
+        <v>39.13608936016629</v>
+      </c>
+      <c r="J62" t="n">
+        <v>51.79409696649518</v>
+      </c>
+      <c r="K62" t="n">
+        <v>-19.36151335965039</v>
+      </c>
+      <c r="L62" t="n">
+        <v>278.1604110002518</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B63" t="n">
+        <v>49.05924876730899</v>
+      </c>
+      <c r="C63" t="n">
+        <v>130.6881168659624</v>
+      </c>
+      <c r="D63" t="n">
+        <v>35.72943753948903</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-4.249741185837195</v>
+      </c>
+      <c r="F63" t="n">
+        <v>211.2270619869232</v>
+      </c>
+      <c r="G63" t="n">
+        <v>57.96875442641294</v>
+      </c>
+      <c r="H63" t="n">
+        <v>154.4220008134642</v>
+      </c>
+      <c r="I63" t="n">
+        <v>42.21815544596463</v>
+      </c>
+      <c r="J63" t="n">
+        <v>52.27105579789969</v>
+      </c>
+      <c r="K63" t="n">
+        <v>-17.71440683427397</v>
+      </c>
+      <c r="L63" t="n">
+        <v>289.1655596494675</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B64" t="n">
+        <v>50.1163403321729</v>
+      </c>
+      <c r="C64" t="n">
+        <v>134.2449047580234</v>
+      </c>
+      <c r="D64" t="n">
+        <v>38.26772383272469</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-4.670570580788436</v>
+      </c>
+      <c r="F64" t="n">
+        <v>217.9583983421326</v>
+      </c>
+      <c r="G64" t="n">
+        <v>59.55839941089679</v>
+      </c>
+      <c r="H64" t="n">
+        <v>159.5370213280196</v>
+      </c>
+      <c r="I64" t="n">
+        <v>45.47747033141144</v>
+      </c>
+      <c r="J64" t="n">
+        <v>55.60557743227463</v>
+      </c>
+      <c r="K64" t="n">
+        <v>-18.92826656206598</v>
+      </c>
+      <c r="L64" t="n">
+        <v>301.2502019405365</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B65" t="n">
+        <v>51.45819434188304</v>
+      </c>
+      <c r="C65" t="n">
+        <v>138.2965679683175</v>
+      </c>
+      <c r="D65" t="n">
+        <v>40.93734633312958</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-5.216146481312315</v>
+      </c>
+      <c r="F65" t="n">
+        <v>225.4759621620178</v>
+      </c>
+      <c r="G65" t="n">
+        <v>61.50556918294664</v>
+      </c>
+      <c r="H65" t="n">
+        <v>165.2994093113018</v>
+      </c>
+      <c r="I65" t="n">
+        <v>48.93049239796567</v>
+      </c>
+      <c r="J65" t="n">
+        <v>58.44698626930573</v>
+      </c>
+      <c r="K65" t="n">
+        <v>-19.68025977668552</v>
+      </c>
+      <c r="L65" t="n">
+        <v>314.5021973848343</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B66" t="n">
+        <v>53.11872651526772</v>
+      </c>
+      <c r="C66" t="n">
+        <v>142.8883630176093</v>
+      </c>
+      <c r="D66" t="n">
+        <v>43.75138815837494</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-5.914214614469721</v>
+      </c>
+      <c r="F66" t="n">
+        <v>233.8442630767822</v>
+      </c>
+      <c r="G66" t="n">
+        <v>63.85558497553357</v>
+      </c>
+      <c r="H66" t="n">
+        <v>171.7703078605112</v>
+      </c>
+      <c r="I66" t="n">
+        <v>52.59483175941089</v>
+      </c>
+      <c r="J66" t="n">
+        <v>60.37123775425429</v>
+      </c>
+      <c r="K66" t="n">
+        <v>-19.57962156563711</v>
+      </c>
+      <c r="L66" t="n">
+        <v>329.0123407840729</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B67" t="n">
+        <v>55.13459581075188</v>
+      </c>
+      <c r="C67" t="n">
+        <v>148.0679299506539</v>
+      </c>
+      <c r="D67" t="n">
+        <v>46.72386268460033</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-6.796572629126871</v>
+      </c>
+      <c r="F67" t="n">
+        <v>243.1298158168793</v>
+      </c>
+      <c r="G67" t="n">
+        <v>66.65783263269665</v>
+      </c>
+      <c r="H67" t="n">
+        <v>179.0144127799302</v>
+      </c>
+      <c r="I67" t="n">
+        <v>56.48924006759153</v>
+      </c>
+      <c r="J67" t="n">
+        <v>63.23930339311442</v>
+      </c>
+      <c r="K67" t="n">
+        <v>-20.52642592777612</v>
+      </c>
+      <c r="L67" t="n">
+        <v>344.8743629455566</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B68" t="n">
+        <v>57.5453925367602</v>
+      </c>
+      <c r="C68" t="n">
+        <v>153.8853770685802</v>
+      </c>
+      <c r="D68" t="n">
+        <v>49.86969790073072</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-7.899325624128352</v>
+      </c>
+      <c r="F68" t="n">
+        <v>253.4011418819427</v>
+      </c>
+      <c r="G68" t="n">
+        <v>69.96601966877631</v>
+      </c>
+      <c r="H68" t="n">
+        <v>187.1000760284935</v>
+      </c>
+      <c r="I68" t="n">
+        <v>60.63359915339104</v>
+      </c>
+      <c r="J68" t="n">
+        <v>64.90295637812815</v>
+      </c>
+      <c r="K68" t="n">
+        <v>-20.41771172511932</v>
+      </c>
+      <c r="L68" t="n">
+        <v>362.1849395036697</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B69" t="n">
+        <v>60.39380575182461</v>
+      </c>
+      <c r="C69" t="n">
+        <v>160.393350830883</v>
+      </c>
+      <c r="D69" t="n">
+        <v>53.20471783040207</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-9.263106779671581</v>
+      </c>
+      <c r="F69" t="n">
+        <v>264.7287676334381</v>
+      </c>
+      <c r="G69" t="n">
+        <v>73.83839763840827</v>
+      </c>
+      <c r="H69" t="n">
+        <v>196.0993825405622</v>
+      </c>
+      <c r="I69" t="n">
+        <v>65.04890795496605</v>
+      </c>
+      <c r="J69" t="n">
+        <v>70.09594646713768</v>
+      </c>
+      <c r="K69" t="n">
+        <v>-24.03894344277957</v>
+      </c>
+      <c r="L69" t="n">
+        <v>381.0436911582947</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B70" t="n">
+        <v>63.72576647907754</v>
+      </c>
+      <c r="C70" t="n">
+        <v>167.6470871312497</v>
+      </c>
+      <c r="D70" t="n">
+        <v>56.7456231732864</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-10.93324867425387</v>
+      </c>
+      <c r="F70" t="n">
+        <v>277.1852281093597</v>
+      </c>
+      <c r="G70" t="n">
+        <v>78.33794430743886</v>
+      </c>
+      <c r="H70" t="n">
+        <v>206.0881947854493</v>
+      </c>
+      <c r="I70" t="n">
+        <v>69.75726952298511</v>
+      </c>
+      <c r="J70" t="n">
+        <v>72.34753371217349</v>
+      </c>
+      <c r="K70" t="n">
+        <v>-24.97776032216449</v>
+      </c>
+      <c r="L70" t="n">
+        <v>401.5531820058823</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B71" t="n">
+        <v>67.59055938167194</v>
+      </c>
+      <c r="C71" t="n">
+        <v>175.7044451656469</v>
+      </c>
+      <c r="D71" t="n">
+        <v>60.50997062655751</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-12.95991244117982</v>
+      </c>
+      <c r="F71" t="n">
+        <v>290.8450627326965</v>
+      </c>
+      <c r="G71" t="n">
+        <v>83.53249969231707</v>
+      </c>
+      <c r="H71" t="n">
+        <v>217.1461761229041</v>
+      </c>
+      <c r="I71" t="n">
+        <v>74.78188002858336</v>
+      </c>
+      <c r="J71" t="n">
+        <v>76.77952375327426</v>
+      </c>
+      <c r="K71" t="n">
+        <v>-28.42114706381466</v>
+      </c>
+      <c r="L71" t="n">
+        <v>423.8189325332642</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
         <v>2020</v>
       </c>
-      <c r="B62" t="n">
-        <v>47.75370372563103</v>
-      </c>
-      <c r="C62" t="n">
-        <v>132.5182336147943</v>
-      </c>
-      <c r="D62" t="n">
-        <v>69.78444452063586</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.1183943354186283</v>
-      </c>
-      <c r="F62" t="n">
-        <v>250.1747761964798</v>
-      </c>
-      <c r="G62" t="n">
-        <v>58.58484741858675</v>
-      </c>
-      <c r="H62" t="n">
-        <v>162.5750442543452</v>
-      </c>
-      <c r="I62" t="n">
-        <v>85.61243873190821</v>
-      </c>
-      <c r="J62" t="n">
-        <v>17.64928148140623</v>
-      </c>
-      <c r="K62" t="n">
-        <v>66.4427033851311</v>
-      </c>
-      <c r="L62" t="n">
-        <v>390.8643152713776</v>
+      <c r="B72" t="n">
+        <v>72.04090080854958</v>
+      </c>
+      <c r="C72" t="n">
+        <v>184.6259214860905</v>
+      </c>
+      <c r="D72" t="n">
+        <v>64.51615328974488</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-15.39815836560443</v>
+      </c>
+      <c r="F72" t="n">
+        <v>305.7848172187805</v>
+      </c>
+      <c r="G72" t="n">
+        <v>89.49484841248733</v>
+      </c>
+      <c r="H72" t="n">
+        <v>229.35677748289</v>
+      </c>
+      <c r="I72" t="n">
+        <v>80.14701779155557</v>
+      </c>
+      <c r="J72" t="n">
+        <v>18.10464973948521</v>
+      </c>
+      <c r="K72" t="n">
+        <v>30.84611915788671</v>
+      </c>
+      <c r="L72" t="n">
+        <v>447.9494125843048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comet 4 is released in 1958, improve code readability
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,2700 +497,2358 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1950</v>
+        <v>1959</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9132065475827132</v>
+        <v>3.287775717876018</v>
       </c>
       <c r="C2" t="n">
-        <v>3.659758381057158</v>
+        <v>9.786162772295205</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.8713571247171499</v>
+        <v>-1.29223141872433</v>
       </c>
       <c r="E2" t="n">
-        <v>-3.318826059919425</v>
+        <v>-2.711080156945702</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3827817440032959</v>
+        <v>9.07062691450119</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9446767031497476</v>
+        <v>3.268379091711916</v>
       </c>
       <c r="H2" t="n">
-        <v>3.785877894648572</v>
+        <v>9.728428134301744</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.9013851006902512</v>
+        <v>-1.284607744879967</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>3.881585382408192</v>
       </c>
       <c r="K2" t="n">
-        <v>-7.226075872993079</v>
+        <v>-7.499935681412978</v>
       </c>
       <c r="L2" t="n">
-        <v>-3.39690637588501</v>
+        <v>8.093849182128906</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1951</v>
+        <v>1960</v>
       </c>
       <c r="B3" t="n">
-        <v>1.926302743666822</v>
+        <v>6.530406661456213</v>
       </c>
       <c r="C3" t="n">
-        <v>7.255034025449946</v>
+        <v>18.70883181645124</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.707475598112461</v>
+        <v>-2.553181581318139</v>
       </c>
       <c r="E3" t="n">
-        <v>-6.003424359557163</v>
+        <v>-4.846801086805379</v>
       </c>
       <c r="F3" t="n">
-        <v>1.470436811447144</v>
+        <v>17.83925580978394</v>
       </c>
       <c r="G3" t="n">
-        <v>1.957779554059642</v>
+        <v>6.466233179737721</v>
       </c>
       <c r="H3" t="n">
-        <v>7.373585136464739</v>
+        <v>18.52498248840961</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.735376656670808</v>
+        <v>-2.528091788288898</v>
       </c>
       <c r="J3" t="n">
-        <v>4.2390532078429</v>
+        <v>1.824230879717734</v>
       </c>
       <c r="K3" t="n">
-        <v>-17.47535272126495</v>
+        <v>-8.379235557916008</v>
       </c>
       <c r="L3" t="n">
-        <v>-5.640311479568481</v>
+        <v>15.90811920166016</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1952</v>
+        <v>1961</v>
       </c>
       <c r="B4" t="n">
-        <v>3.036678858962268</v>
+        <v>9.701232617198457</v>
       </c>
       <c r="C4" t="n">
-        <v>10.81432212542889</v>
+        <v>26.87535072580666</v>
       </c>
       <c r="D4" t="n">
-        <v>-2.515621244020234</v>
+        <v>-3.761301023962913</v>
       </c>
       <c r="E4" t="n">
-        <v>-8.132291933669265</v>
+        <v>-6.512522790882109</v>
       </c>
       <c r="F4" t="n">
-        <v>3.20308780670166</v>
+        <v>26.3027595281601</v>
       </c>
       <c r="G4" t="n">
-        <v>3.039026839022135</v>
+        <v>9.574483258347476</v>
       </c>
       <c r="H4" t="n">
-        <v>10.82268383040028</v>
+        <v>26.52421663720102</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.517566338906282</v>
+        <v>-3.712158558047018</v>
       </c>
       <c r="J4" t="n">
-        <v>2.504873567786579</v>
+        <v>-5.805430925972427</v>
       </c>
       <c r="K4" t="n">
-        <v>-20.66482333348338</v>
+        <v>-3.103212767486079</v>
       </c>
       <c r="L4" t="n">
-        <v>-6.815805435180664</v>
+        <v>23.47789764404297</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1953</v>
+        <v>1962</v>
       </c>
       <c r="B5" t="n">
-        <v>4.242105846552328</v>
+        <v>12.77970038436918</v>
       </c>
       <c r="C5" t="n">
-        <v>14.36025604106698</v>
+        <v>34.36376826569427</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.301010623425174</v>
+        <v>-4.898700532087598</v>
       </c>
       <c r="E5" t="n">
-        <v>-9.778489783481245</v>
+        <v>-7.786007439207694</v>
       </c>
       <c r="F5" t="n">
-        <v>5.522861480712891</v>
+        <v>34.45876067876816</v>
       </c>
       <c r="G5" t="n">
-        <v>4.190458154857925</v>
+        <v>12.58013834999703</v>
       </c>
       <c r="H5" t="n">
-        <v>14.18541974431015</v>
+        <v>33.8271591670817</v>
       </c>
       <c r="I5" t="n">
-        <v>-3.260820777832996</v>
+        <v>-4.822204635113438</v>
       </c>
       <c r="J5" t="n">
-        <v>2.754397577499184</v>
+        <v>-9.471529693604062</v>
       </c>
       <c r="K5" t="n">
-        <v>-24.87568064239963</v>
+        <v>-1.279651292609282</v>
       </c>
       <c r="L5" t="n">
-        <v>-7.006225943565369</v>
+        <v>30.83391189575195</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1954</v>
+        <v>1963</v>
       </c>
       <c r="B6" t="n">
-        <v>5.54017307698284</v>
+        <v>15.7499354102431</v>
       </c>
       <c r="C6" t="n">
-        <v>17.90972156307743</v>
+        <v>41.23390560325821</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.066986731430564</v>
+        <v>-5.950719837917978</v>
       </c>
       <c r="E6" t="n">
-        <v>-11.00901464767389</v>
+        <v>-8.727488107498619</v>
       </c>
       <c r="F6" t="n">
-        <v>8.373893260955811</v>
+        <v>42.30563306808472</v>
       </c>
       <c r="G6" t="n">
-        <v>5.415212565089421</v>
+        <v>15.47452387356712</v>
       </c>
       <c r="H6" t="n">
-        <v>17.50576162476995</v>
+        <v>40.51286815075157</v>
       </c>
       <c r="I6" t="n">
-        <v>-3.975254444954764</v>
+        <v>-5.846662465478001</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.6335383784258507</v>
+        <v>-9.41995883779421</v>
       </c>
       <c r="K6" t="n">
-        <v>-24.60383321145709</v>
+        <v>-2.717928771583583</v>
       </c>
       <c r="L6" t="n">
-        <v>-6.291651844978333</v>
+        <v>38.00284194946289</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1955</v>
+        <v>1964</v>
       </c>
       <c r="B7" t="n">
-        <v>6.927884744528988</v>
+        <v>18.5997301928843</v>
       </c>
       <c r="C7" t="n">
-        <v>21.47422453556341</v>
+        <v>47.53376641035477</v>
       </c>
       <c r="D7" t="n">
-        <v>-4.815227479649375</v>
+        <v>-6.905583369059036</v>
       </c>
       <c r="E7" t="n">
-        <v>-11.88455836370596</v>
+        <v>-9.385411474650912</v>
       </c>
       <c r="F7" t="n">
-        <v>11.70232343673706</v>
+        <v>49.84250175952911</v>
       </c>
       <c r="G7" t="n">
-        <v>6.716501754055951</v>
+        <v>18.25203096223686</v>
       </c>
       <c r="H7" t="n">
-        <v>20.81900494577425</v>
+        <v>46.64518072447325</v>
       </c>
       <c r="I7" t="n">
-        <v>-4.668305695874026</v>
+        <v>-6.776491925274968</v>
       </c>
       <c r="J7" t="n">
-        <v>1.168090994400017</v>
+        <v>-4.848951698943281</v>
       </c>
       <c r="K7" t="n">
-        <v>-28.78469619032701</v>
+        <v>-8.264329402823893</v>
       </c>
       <c r="L7" t="n">
-        <v>-4.749404191970825</v>
+        <v>45.00743865966797</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1956</v>
+        <v>1965</v>
       </c>
       <c r="B8" t="n">
-        <v>8.40139856721728</v>
+        <v>21.31980888105314</v>
       </c>
       <c r="C8" t="n">
-        <v>25.06041422771064</v>
+        <v>53.30345069934519</v>
       </c>
       <c r="D8" t="n">
-        <v>-5.545971051685223</v>
+        <v>-7.75411014039513</v>
       </c>
       <c r="E8" t="n">
-        <v>-12.45954363037343</v>
+        <v>-9.799907320214082</v>
       </c>
       <c r="F8" t="n">
-        <v>15.45629811286926</v>
+        <v>57.06924211978912</v>
       </c>
       <c r="G8" t="n">
-        <v>8.096816413395338</v>
+        <v>20.90924317868946</v>
       </c>
       <c r="H8" t="n">
-        <v>24.15188038300883</v>
+        <v>52.27696079050585</v>
       </c>
       <c r="I8" t="n">
-        <v>-5.344908836336008</v>
+        <v>-7.604785552461046</v>
       </c>
       <c r="J8" t="n">
-        <v>2.2225897486764</v>
+        <v>-4.864077674873918</v>
       </c>
       <c r="K8" t="n">
-        <v>-31.58041740162329</v>
+        <v>-8.85037449430175</v>
       </c>
       <c r="L8" t="n">
-        <v>-2.454039692878723</v>
+        <v>51.86696624755859</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1957</v>
+        <v>1966</v>
       </c>
       <c r="B9" t="n">
-        <v>9.955882984948611</v>
+        <v>23.90328056158642</v>
       </c>
       <c r="C9" t="n">
-        <v>28.67069356924484</v>
+        <v>58.57763885641797</v>
       </c>
       <c r="D9" t="n">
-        <v>-6.258244443995435</v>
+        <v>-8.489456348967874</v>
       </c>
       <c r="E9" t="n">
-        <v>-12.78236147001551</v>
+        <v>-10.00498235614589</v>
       </c>
       <c r="F9" t="n">
-        <v>19.5859706401825</v>
+        <v>63.98648071289062</v>
       </c>
       <c r="G9" t="n">
-        <v>9.557372116552234</v>
+        <v>23.44429346452527</v>
       </c>
       <c r="H9" t="n">
-        <v>27.52307230761696</v>
+        <v>57.45284009324688</v>
       </c>
       <c r="I9" t="n">
-        <v>-6.00774145678839</v>
+        <v>-8.326443120921592</v>
       </c>
       <c r="J9" t="n">
-        <v>1.261131954599775</v>
+        <v>-1.150778178179403</v>
       </c>
       <c r="K9" t="n">
-        <v>-31.81118503775665</v>
+        <v>-12.82261077551686</v>
       </c>
       <c r="L9" t="n">
-        <v>0.522649884223938</v>
+        <v>58.5973014831543</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1958</v>
+        <v>1967</v>
       </c>
       <c r="B10" t="n">
-        <v>11.58547278164227</v>
+        <v>26.34522486175173</v>
       </c>
       <c r="C10" t="n">
-        <v>32.30385724495742</v>
+        <v>63.38723034862433</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.950084751527919</v>
+        <v>-9.106878348521736</v>
       </c>
       <c r="E10" t="n">
-        <v>-12.89574413638464</v>
+        <v>-10.02998132323815</v>
       </c>
       <c r="F10" t="n">
-        <v>24.04350113868713</v>
+        <v>70.59559553861618</v>
       </c>
       <c r="G10" t="n">
-        <v>11.09778071124175</v>
+        <v>25.85641107825495</v>
       </c>
       <c r="H10" t="n">
-        <v>30.94402193062482</v>
+        <v>62.21113289435372</v>
       </c>
       <c r="I10" t="n">
-        <v>-6.657519977882894</v>
+        <v>-8.937907778532463</v>
       </c>
       <c r="J10" t="n">
-        <v>-4.463098459022535</v>
+        <v>-2.704144401693035</v>
       </c>
       <c r="K10" t="n">
-        <v>-26.80954303636678</v>
+        <v>-11.2142529312992</v>
       </c>
       <c r="L10" t="n">
-        <v>4.11164116859436</v>
+        <v>65.21123886108398</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1959</v>
+        <v>1968</v>
       </c>
       <c r="B11" t="n">
-        <v>13.283295499332</v>
+        <v>28.6423718859642</v>
       </c>
       <c r="C11" t="n">
-        <v>35.95571210172286</v>
+        <v>67.76045412170247</v>
       </c>
       <c r="D11" t="n">
-        <v>-7.618745887949796</v>
+        <v>-9.603510695911197</v>
       </c>
       <c r="E11" t="n">
-        <v>-12.83720712287984</v>
+        <v>-9.900600530947969</v>
       </c>
       <c r="F11" t="n">
-        <v>28.78305459022522</v>
+        <v>76.8987147808075</v>
       </c>
       <c r="G11" t="n">
-        <v>12.71590745495737</v>
+        <v>28.14558690183997</v>
       </c>
       <c r="H11" t="n">
-        <v>34.41988530523852</v>
+        <v>66.58518915904075</v>
       </c>
       <c r="I11" t="n">
-        <v>-7.293315701580117</v>
+        <v>-9.436943488153414</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.633307727389012</v>
+        <v>-11.09546896465161</v>
       </c>
       <c r="K11" t="n">
-        <v>-30.9624864489178</v>
+        <v>-2.479708975507327</v>
       </c>
       <c r="L11" t="n">
-        <v>8.24668288230896</v>
+        <v>71.71865463256836</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1960</v>
+        <v>1969</v>
       </c>
       <c r="B12" t="n">
-        <v>15.04154844148763</v>
+        <v>30.79285094055618</v>
       </c>
       <c r="C12" t="n">
-        <v>39.61965934872611</v>
+        <v>71.72363405344993</v>
       </c>
       <c r="D12" t="n">
-        <v>-8.260887452244436</v>
+        <v>-9.978154986526937</v>
       </c>
       <c r="E12" t="n">
-        <v>-12.63951830740596</v>
+        <v>-9.639612067625507</v>
       </c>
       <c r="F12" t="n">
-        <v>33.76080203056335</v>
+        <v>82.89871793985367</v>
       </c>
       <c r="G12" t="n">
-        <v>14.40787127605117</v>
+        <v>30.31235022635374</v>
       </c>
       <c r="H12" t="n">
-        <v>37.95054439494837</v>
+        <v>70.60443734592823</v>
       </c>
       <c r="I12" t="n">
-        <v>-7.912869044093752</v>
+        <v>-9.822452917669969</v>
       </c>
       <c r="J12" t="n">
-        <v>-2.837581849060681</v>
+        <v>-15.00504323302865</v>
       </c>
       <c r="K12" t="n">
-        <v>-28.74366571893092</v>
+        <v>2.037577780076798</v>
       </c>
       <c r="L12" t="n">
-        <v>12.86429905891418</v>
+        <v>78.12686920166016</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1961</v>
+        <v>1970</v>
       </c>
       <c r="B13" t="n">
-        <v>16.85161134246109</v>
+        <v>32.79599045058048</v>
       </c>
       <c r="C13" t="n">
-        <v>43.28722115030608</v>
+        <v>75.30172754410268</v>
       </c>
       <c r="D13" t="n">
-        <v>-8.872743211879946</v>
+        <v>-10.23107750683918</v>
       </c>
       <c r="E13" t="n">
-        <v>-12.33116706256447</v>
+        <v>-9.267405251199236</v>
       </c>
       <c r="F13" t="n">
-        <v>38.93492221832275</v>
+        <v>88.59923523664474</v>
       </c>
       <c r="G13" t="n">
-        <v>16.16814827838056</v>
+        <v>32.35760411355236</v>
       </c>
       <c r="H13" t="n">
-        <v>41.53158982213902</v>
+        <v>74.29516399604661</v>
       </c>
       <c r="I13" t="n">
-        <v>-8.512884908768523</v>
+        <v>-10.09431796610103</v>
       </c>
       <c r="J13" t="n">
-        <v>-10.47486073079117</v>
+        <v>-8.12051075134662</v>
       </c>
       <c r="K13" t="n">
-        <v>-20.80820234464976</v>
+        <v>-3.997086273254832</v>
       </c>
       <c r="L13" t="n">
-        <v>17.90379011631012</v>
+        <v>84.44085311889648</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1962</v>
+        <v>1971</v>
       </c>
       <c r="B14" t="n">
-        <v>18.70417874389799</v>
+        <v>34.65215557271623</v>
       </c>
       <c r="C14" t="n">
-        <v>46.94850765564462</v>
+        <v>78.51871050458566</v>
       </c>
       <c r="D14" t="n">
-        <v>-9.450269589119602</v>
+        <v>-10.36381565401408</v>
       </c>
       <c r="E14" t="n">
-        <v>-11.93681732121097</v>
+        <v>-8.802402393483575</v>
       </c>
       <c r="F14" t="n">
-        <v>44.26559948921204</v>
+        <v>94.00464802980423</v>
       </c>
       <c r="G14" t="n">
-        <v>17.98974078822075</v>
+        <v>34.28250646856244</v>
       </c>
       <c r="H14" t="n">
-        <v>45.15522946413149</v>
+        <v>77.68111842647022</v>
       </c>
       <c r="I14" t="n">
-        <v>-9.089300450709716</v>
+        <v>-10.25326047761006</v>
       </c>
       <c r="J14" t="n">
-        <v>-14.12907762420487</v>
+        <v>-10.20713390738528</v>
       </c>
       <c r="K14" t="n">
-        <v>-16.61935347943198</v>
+        <v>-0.8398508408478751</v>
       </c>
       <c r="L14" t="n">
-        <v>23.30723869800568</v>
+        <v>90.66337966918945</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1963</v>
+        <v>1972</v>
       </c>
       <c r="B15" t="n">
-        <v>20.58940038901413</v>
+        <v>36.3626154266025</v>
       </c>
       <c r="C15" t="n">
-        <v>50.59262524499342</v>
+        <v>81.39784891148379</v>
       </c>
       <c r="D15" t="n">
-        <v>-9.98927463016631</v>
+        <v>-10.37899366083637</v>
       </c>
       <c r="E15" t="n">
-        <v>-11.47772724781402</v>
+        <v>-8.261381921165473</v>
       </c>
       <c r="F15" t="n">
-        <v>49.71502375602722</v>
+        <v>99.12008875608444</v>
       </c>
       <c r="G15" t="n">
-        <v>19.86438115526018</v>
+        <v>36.08841008996086</v>
       </c>
       <c r="H15" t="n">
-        <v>48.81109563773504</v>
+        <v>80.78403925283232</v>
       </c>
       <c r="I15" t="n">
-        <v>-9.637520033078319</v>
+        <v>-10.30072713854741</v>
       </c>
       <c r="J15" t="n">
-        <v>-14.15300565806115</v>
+        <v>-2.705326252567289</v>
       </c>
       <c r="K15" t="n">
-        <v>-15.86544142873715</v>
+        <v>-7.071023942401141</v>
       </c>
       <c r="L15" t="n">
-        <v>29.01950967311859</v>
+        <v>96.79537200927734</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1964</v>
+        <v>1973</v>
       </c>
       <c r="B16" t="n">
-        <v>22.49702815821988</v>
+        <v>37.92943213781416</v>
       </c>
       <c r="C16" t="n">
-        <v>54.2080289306336</v>
+        <v>83.96189282841624</v>
       </c>
       <c r="D16" t="n">
-        <v>-10.48552928578224</v>
+        <v>-10.28014687447044</v>
       </c>
       <c r="E16" t="n">
-        <v>-10.97213610232662</v>
+        <v>-7.659738115067753</v>
       </c>
       <c r="F16" t="n">
-        <v>55.24739170074463</v>
+        <v>103.9514399766922</v>
       </c>
       <c r="G16" t="n">
-        <v>21.78275606097747</v>
+        <v>37.77682290969266</v>
       </c>
       <c r="H16" t="n">
-        <v>52.48694460610187</v>
+        <v>83.62407180305505</v>
       </c>
       <c r="I16" t="n">
-        <v>-10.15261771448583</v>
+        <v>-10.23878466072075</v>
       </c>
       <c r="J16" t="n">
-        <v>-9.815174003880767</v>
+        <v>-1.439771096366358</v>
       </c>
       <c r="K16" t="n">
-        <v>-19.31365356712857</v>
+        <v>-6.886191647310986</v>
       </c>
       <c r="L16" t="n">
-        <v>34.98825538158417</v>
+        <v>102.8361473083496</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1965</v>
+        <v>1974</v>
       </c>
       <c r="B17" t="n">
-        <v>24.4165571001426</v>
+        <v>39.3553676988036</v>
       </c>
       <c r="C17" t="n">
-        <v>57.78282169562615</v>
+        <v>86.23320884275344</v>
       </c>
       <c r="D17" t="n">
-        <v>-10.93486213972361</v>
+        <v>-10.07155601962034</v>
       </c>
       <c r="E17" t="n">
-        <v>-10.43560940468711</v>
+        <v>-7.011684058485308</v>
       </c>
       <c r="F17" t="n">
-        <v>60.82890725135803</v>
+        <v>108.5053364634514</v>
       </c>
       <c r="G17" t="n">
-        <v>23.73472976500977</v>
+        <v>39.34939158179957</v>
       </c>
       <c r="H17" t="n">
-        <v>56.16924828428904</v>
+        <v>86.22011432030808</v>
       </c>
       <c r="I17" t="n">
-        <v>-10.62950836350554</v>
+        <v>-10.07002665270789</v>
       </c>
       <c r="J17" t="n">
-        <v>-9.947676938802596</v>
+        <v>2.590839508003053</v>
       </c>
       <c r="K17" t="n">
-        <v>-18.16287460944032</v>
+        <v>-9.306646424639137</v>
       </c>
       <c r="L17" t="n">
-        <v>41.16391813755035</v>
+        <v>108.7836723327637</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1966</v>
+        <v>1975</v>
       </c>
       <c r="B18" t="n">
-        <v>26.3373609947235</v>
+        <v>40.64380373658872</v>
       </c>
       <c r="C18" t="n">
-        <v>61.30501233306438</v>
+        <v>88.23387128081097</v>
       </c>
       <c r="D18" t="n">
-        <v>-11.33323947708277</v>
+        <v>-9.758092927895738</v>
       </c>
       <c r="E18" t="n">
-        <v>-9.881355129849389</v>
+        <v>-6.330419453700728</v>
       </c>
       <c r="F18" t="n">
-        <v>66.42777872085571</v>
+        <v>112.7891626358032</v>
       </c>
       <c r="G18" t="n">
-        <v>25.7095613207795</v>
+        <v>40.80789114757954</v>
       </c>
       <c r="H18" t="n">
-        <v>59.84369406501386</v>
+        <v>88.59008960117285</v>
       </c>
       <c r="I18" t="n">
-        <v>-11.06309076894655</v>
+        <v>-9.797488359856867</v>
       </c>
       <c r="J18" t="n">
-        <v>-6.474974139409201</v>
+        <v>2.33069353240279</v>
       </c>
       <c r="K18" t="n">
-        <v>-20.51545786387407</v>
+        <v>-7.296458443270964</v>
       </c>
       <c r="L18" t="n">
-        <v>47.49973261356354</v>
+        <v>114.6347274780273</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1967</v>
+        <v>1976</v>
       </c>
       <c r="B19" t="n">
-        <v>28.24882167714172</v>
+        <v>41.79867314540072</v>
       </c>
       <c r="C19" t="n">
-        <v>64.76273235275475</v>
+        <v>89.98571335156966</v>
       </c>
       <c r="D19" t="n">
-        <v>-11.67683227374706</v>
+        <v>-9.345075457364823</v>
       </c>
       <c r="E19" t="n">
-        <v>-9.320499611068836</v>
+        <v>-5.628255915799549</v>
       </c>
       <c r="F19" t="n">
-        <v>72.01422214508057</v>
+        <v>116.811055123806</v>
       </c>
       <c r="G19" t="n">
-        <v>27.69611096696993</v>
+        <v>42.15423301085286</v>
       </c>
       <c r="H19" t="n">
-        <v>63.49559787895399</v>
+        <v>90.75117564317399</v>
       </c>
       <c r="I19" t="n">
-        <v>-11.44836574398019</v>
+        <v>-9.424569219300814</v>
       </c>
       <c r="J19" t="n">
-        <v>-8.107181697624965</v>
+        <v>4.870918216642175</v>
       </c>
       <c r="K19" t="n">
-        <v>-17.68443294114585</v>
+        <v>-7.966625815430711</v>
       </c>
       <c r="L19" t="n">
-        <v>53.95172846317291</v>
+        <v>120.3851318359375</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1968</v>
+        <v>1977</v>
       </c>
       <c r="B20" t="n">
-        <v>30.14044713605225</v>
+        <v>42.82439902002932</v>
       </c>
       <c r="C20" t="n">
-        <v>68.14441819647351</v>
+        <v>91.51035611139656</v>
       </c>
       <c r="D20" t="n">
-        <v>-11.96207126203547</v>
+        <v>-8.838134815904917</v>
       </c>
       <c r="E20" t="n">
-        <v>-8.762335887201722</v>
+        <v>-4.91672028919956</v>
       </c>
       <c r="F20" t="n">
-        <v>77.56045818328857</v>
+        <v>120.5799000263214</v>
       </c>
       <c r="G20" t="n">
-        <v>29.68303042512066</v>
+        <v>43.39050992500383</v>
       </c>
       <c r="H20" t="n">
-        <v>67.11024655664758</v>
+        <v>92.72006393446566</v>
       </c>
       <c r="I20" t="n">
-        <v>-11.78053277098685</v>
+        <v>-8.954969251726855</v>
       </c>
       <c r="J20" t="n">
-        <v>-16.38043429366912</v>
+        <v>6.536811392335045</v>
       </c>
       <c r="K20" t="n">
-        <v>-8.153574470182335</v>
+        <v>-7.662180709550332</v>
       </c>
       <c r="L20" t="n">
-        <v>60.47873544692993</v>
+        <v>126.0302352905273</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1969</v>
+        <v>1978</v>
       </c>
       <c r="B21" t="n">
-        <v>32.00197962039925</v>
+        <v>43.72584141117991</v>
       </c>
       <c r="C21" t="n">
-        <v>71.43896901844505</v>
+        <v>92.82921174212258</v>
       </c>
       <c r="D21" t="n">
-        <v>-12.18569172383114</v>
+        <v>-8.243093719922783</v>
       </c>
       <c r="E21" t="n">
-        <v>-8.214541220585673</v>
+        <v>-4.206623899760764</v>
       </c>
       <c r="F21" t="n">
-        <v>83.04071569442749</v>
+        <v>124.1053355336189</v>
       </c>
       <c r="G21" t="n">
-        <v>31.65893568603431</v>
+        <v>44.51898747030223</v>
       </c>
       <c r="H21" t="n">
-        <v>70.67318186122054</v>
+        <v>94.51304722906809</v>
       </c>
       <c r="I21" t="n">
-        <v>-12.05506769114672</v>
+        <v>-8.392615766564544</v>
       </c>
       <c r="J21" t="n">
-        <v>-20.32256507200328</v>
+        <v>15.81244382095472</v>
       </c>
       <c r="K21" t="n">
-        <v>-2.912101828553709</v>
+        <v>-14.88699382675854</v>
       </c>
       <c r="L21" t="n">
-        <v>67.04238295555115</v>
+        <v>131.564868927002</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1970</v>
+        <v>1979</v>
       </c>
       <c r="B22" t="n">
-        <v>33.82349471824228</v>
+        <v>44.50824951378353</v>
       </c>
       <c r="C22" t="n">
-        <v>74.63587563724801</v>
+        <v>93.96346889096168</v>
       </c>
       <c r="D22" t="n">
-        <v>-12.34476848431023</v>
+        <v>-7.565855728136039</v>
       </c>
       <c r="E22" t="n">
-        <v>-7.683372995066158</v>
+        <v>-3.508112120140211</v>
       </c>
       <c r="F22" t="n">
-        <v>88.43122887611389</v>
+        <v>127.397750556469</v>
       </c>
       <c r="G22" t="n">
-        <v>33.61256566596752</v>
+        <v>45.54214815887436</v>
       </c>
       <c r="H22" t="n">
-        <v>74.17043365246779</v>
+        <v>96.1461811799344</v>
       </c>
       <c r="I22" t="n">
-        <v>-12.26778441336672</v>
+        <v>-7.741605798555009</v>
       </c>
       <c r="J22" t="n">
-        <v>-13.7668364805827</v>
+        <v>19.47768039525441</v>
       </c>
       <c r="K22" t="n">
-        <v>-8.14127090438244</v>
+        <v>-16.44065454585972</v>
       </c>
       <c r="L22" t="n">
-        <v>73.60710752010345</v>
+        <v>136.9837493896484</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1971</v>
+        <v>1980</v>
       </c>
       <c r="B23" t="n">
-        <v>35.5954897028445</v>
+        <v>45.17721810844344</v>
       </c>
       <c r="C23" t="n">
-        <v>77.72533143444505</v>
+        <v>94.93406744126439</v>
       </c>
       <c r="D23" t="n">
-        <v>-12.43674276247808</v>
+        <v>-6.812305806546762</v>
       </c>
       <c r="E23" t="n">
-        <v>-7.173840871759708</v>
+        <v>-2.830695255436765</v>
       </c>
       <c r="F23" t="n">
-        <v>93.71023750305176</v>
+        <v>130.4682844877243</v>
       </c>
       <c r="G23" t="n">
-        <v>35.53292272943708</v>
+        <v>46.46272063681739</v>
       </c>
       <c r="H23" t="n">
-        <v>77.58871191367038</v>
+        <v>97.6353843623645</v>
       </c>
       <c r="I23" t="n">
-        <v>-12.41488242679537</v>
+        <v>-7.006147674307445</v>
       </c>
       <c r="J23" t="n">
-        <v>-15.93806109752243</v>
+        <v>12.90550033846501</v>
       </c>
       <c r="K23" t="n">
-        <v>-4.628540094924908</v>
+        <v>-7.715719382089457</v>
       </c>
       <c r="L23" t="n">
-        <v>80.14015102386475</v>
+        <v>142.28173828125</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1972</v>
+        <v>1981</v>
       </c>
       <c r="B24" t="n">
-        <v>37.30896248773059</v>
+        <v>45.73864838069303</v>
       </c>
       <c r="C24" t="n">
-        <v>80.69832548398503</v>
+        <v>95.7616552211873</v>
       </c>
       <c r="D24" t="n">
-        <v>-12.45944104503199</v>
+        <v>-5.988220659365505</v>
       </c>
       <c r="E24" t="n">
-        <v>-6.689858569139695</v>
+        <v>-2.183255144148269</v>
       </c>
       <c r="F24" t="n">
-        <v>98.85798835754395</v>
+        <v>133.3288277983665</v>
       </c>
       <c r="G24" t="n">
-        <v>37.40939877704282</v>
+        <v>47.28369971684863</v>
       </c>
       <c r="H24" t="n">
-        <v>80.91556659241809</v>
+        <v>98.99648350296098</v>
       </c>
       <c r="I24" t="n">
-        <v>-12.49298204810542</v>
+        <v>-6.190502726249947</v>
       </c>
       <c r="J24" t="n">
-        <v>-8.742404792191639</v>
+        <v>14.40157809806334</v>
       </c>
       <c r="K24" t="n">
-        <v>-10.47801079349186</v>
+        <v>-7.037240952462851</v>
       </c>
       <c r="L24" t="n">
-        <v>86.611567735672</v>
+        <v>147.4540176391602</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1973</v>
+        <v>1982</v>
       </c>
       <c r="B25" t="n">
-        <v>38.95548189732101</v>
+        <v>46.19871154651913</v>
       </c>
       <c r="C25" t="n">
-        <v>83.54672036647345</v>
+        <v>96.46654011660897</v>
       </c>
       <c r="D25" t="n">
-        <v>-12.41108725429237</v>
+        <v>-5.099190240288324</v>
       </c>
       <c r="E25" t="n">
-        <v>-6.234380256847068</v>
+        <v>-1.574039325729025</v>
       </c>
       <c r="F25" t="n">
-        <v>103.856734752655</v>
+        <v>135.9920220971107</v>
       </c>
       <c r="G25" t="n">
-        <v>39.23188669989649</v>
+        <v>48.00837196622741</v>
       </c>
       <c r="H25" t="n">
-        <v>84.13951792984568</v>
+        <v>100.2452532804912</v>
       </c>
       <c r="I25" t="n">
-        <v>-12.49914890711216</v>
+        <v>-5.298931801070181</v>
       </c>
       <c r="J25" t="n">
-        <v>-7.62358808821358</v>
+        <v>14.40912540349908</v>
       </c>
       <c r="K25" t="n">
-        <v>-10.25444368212303</v>
+        <v>-4.867488587917009</v>
       </c>
       <c r="L25" t="n">
-        <v>92.9942239522934</v>
+        <v>152.4963302612305</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1974</v>
+        <v>1983</v>
       </c>
       <c r="B26" t="n">
-        <v>40.52724824140295</v>
+        <v>46.56381547429721</v>
       </c>
       <c r="C26" t="n">
-        <v>86.26331700729254</v>
+        <v>97.06863271900603</v>
       </c>
       <c r="D26" t="n">
-        <v>-12.29030828541107</v>
+        <v>-4.150548066005355</v>
       </c>
       <c r="E26" t="n">
-        <v>-5.809521384747434</v>
+        <v>-1.010639877683182</v>
       </c>
       <c r="F26" t="n">
-        <v>108.690735578537</v>
+        <v>138.4712602496147</v>
       </c>
       <c r="G26" t="n">
-        <v>40.99087792164252</v>
+        <v>48.64035764407589</v>
       </c>
       <c r="H26" t="n">
-        <v>87.25016501242401</v>
+        <v>101.3974684716311</v>
       </c>
       <c r="I26" t="n">
-        <v>-12.43090879365356</v>
+        <v>-4.335644325814884</v>
       </c>
       <c r="J26" t="n">
-        <v>-3.786208066921161</v>
+        <v>16.09349069215158</v>
       </c>
       <c r="K26" t="n">
-        <v>-12.76012271064543</v>
+        <v>-4.390288418323014</v>
       </c>
       <c r="L26" t="n">
-        <v>99.26380336284637</v>
+        <v>157.4053840637207</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1975</v>
+        <v>1984</v>
       </c>
       <c r="B27" t="n">
-        <v>42.01714762070976</v>
+        <v>46.84057382730781</v>
       </c>
       <c r="C27" t="n">
-        <v>88.84191003242972</v>
+        <v>97.58738308757701</v>
       </c>
       <c r="D27" t="n">
-        <v>-12.0961339575979</v>
+        <v>-3.147310280131603</v>
       </c>
       <c r="E27" t="n">
-        <v>-5.416667916275223</v>
+        <v>-0.4999613291578342</v>
       </c>
       <c r="F27" t="n">
-        <v>113.3462557792664</v>
+        <v>140.7806853055954</v>
       </c>
       <c r="G27" t="n">
-        <v>42.67754884177296</v>
+        <v>49.18361698267464</v>
       </c>
       <c r="H27" t="n">
-        <v>90.23827578282838</v>
+        <v>102.468865770443</v>
       </c>
       <c r="I27" t="n">
-        <v>-12.2862539940138</v>
+        <v>-3.304743957969658</v>
       </c>
       <c r="J27" t="n">
-        <v>-4.147358170156719</v>
+        <v>17.7211766480359</v>
       </c>
       <c r="K27" t="n">
-        <v>-11.08340219298239</v>
+        <v>-3.889956550361585</v>
       </c>
       <c r="L27" t="n">
-        <v>105.3988102674484</v>
+        <v>162.1789588928223</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1976</v>
+        <v>1985</v>
       </c>
       <c r="B28" t="n">
-        <v>43.41879626327474</v>
+        <v>47.03577707884672</v>
       </c>
       <c r="C28" t="n">
-        <v>91.2773327500002</v>
+        <v>98.04171739125935</v>
       </c>
       <c r="D28" t="n">
-        <v>-11.82799145558623</v>
+        <v>-2.094123271162404</v>
       </c>
       <c r="E28" t="n">
-        <v>-5.056570012751585</v>
+        <v>-0.04818004446369173</v>
       </c>
       <c r="F28" t="n">
-        <v>117.8115675449371</v>
+        <v>142.93519115448</v>
       </c>
       <c r="G28" t="n">
-        <v>44.28383270214893</v>
+        <v>49.64246273230685</v>
       </c>
       <c r="H28" t="n">
-        <v>93.09585895678916</v>
+        <v>103.4751120120388</v>
       </c>
       <c r="I28" t="n">
-        <v>-12.06364155389236</v>
+        <v>-2.210177930541487</v>
       </c>
       <c r="J28" t="n">
-        <v>-1.753394251620526</v>
+        <v>20.20619646387262</v>
       </c>
       <c r="K28" t="n">
-        <v>-12.18208663383597</v>
+        <v>-4.297492203458074</v>
       </c>
       <c r="L28" t="n">
-        <v>111.3805692195892</v>
+        <v>166.8161010742188</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1977</v>
+        <v>1986</v>
       </c>
       <c r="B29" t="n">
-        <v>44.72658105213805</v>
+        <v>47.15636603396955</v>
       </c>
       <c r="C29" t="n">
-        <v>93.56549419247013</v>
+        <v>98.44996934260989</v>
       </c>
       <c r="D29" t="n">
-        <v>-11.48569512141521</v>
+        <v>-0.995218325147218</v>
       </c>
       <c r="E29" t="n">
-        <v>-4.729431718880839</v>
+        <v>0.339306785275852</v>
       </c>
       <c r="F29" t="n">
-        <v>122.0769484043121</v>
+        <v>144.9504238367081</v>
       </c>
       <c r="G29" t="n">
-        <v>45.80248529777142</v>
+        <v>50.0215932416729</v>
       </c>
       <c r="H29" t="n">
-        <v>95.81622541489722</v>
+        <v>104.4318028569822</v>
       </c>
       <c r="I29" t="n">
-        <v>-11.7619851452553</v>
+        <v>-1.055687925810735</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.2118483720625231</v>
+        <v>18.52428465227898</v>
       </c>
       <c r="K29" t="n">
-        <v>-12.45164430140703</v>
+        <v>-0.6044612394299946</v>
       </c>
       <c r="L29" t="n">
-        <v>117.1932328939438</v>
+        <v>171.3175315856934</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1978</v>
+        <v>1987</v>
       </c>
       <c r="B30" t="n">
-        <v>45.93568975917675</v>
+        <v>47.20940673566313</v>
       </c>
       <c r="C30" t="n">
-        <v>95.70340917614995</v>
+        <v>98.8298135782418</v>
       </c>
       <c r="D30" t="n">
-        <v>-11.06943143176876</v>
+        <v>0.1456270783391486</v>
       </c>
       <c r="E30" t="n">
-        <v>-4.4349846098049</v>
+        <v>0.6579318865111148</v>
       </c>
       <c r="F30" t="n">
-        <v>126.1346828937531</v>
+        <v>146.8427792787552</v>
       </c>
       <c r="G30" t="n">
-        <v>47.22713539426721</v>
+        <v>50.32610392498084</v>
       </c>
       <c r="H30" t="n">
-        <v>98.39403493341582</v>
+        <v>105.354415845006</v>
       </c>
       <c r="I30" t="n">
-        <v>-11.38063975323812</v>
+        <v>0.1552411687743352</v>
       </c>
       <c r="J30" t="n">
-        <v>8.826165671292136</v>
+        <v>24.26636351898214</v>
       </c>
       <c r="K30" t="n">
-        <v>-20.24291594750403</v>
+        <v>-4.416230445292111</v>
       </c>
       <c r="L30" t="n">
-        <v>122.823780298233</v>
+        <v>175.6858940124512</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1979</v>
+        <v>1988</v>
       </c>
       <c r="B31" t="n">
-        <v>47.04213945251506</v>
+        <v>47.2020675024537</v>
       </c>
       <c r="C31" t="n">
-        <v>97.68922300568309</v>
+        <v>99.19820400074011</v>
       </c>
       <c r="D31" t="n">
-        <v>-10.57974019666463</v>
+        <v>1.325122727644967</v>
       </c>
       <c r="E31" t="n">
-        <v>-4.172561373243113</v>
+        <v>0.9040100159683107</v>
       </c>
       <c r="F31" t="n">
-        <v>129.9790608882904</v>
+        <v>148.6294042468071</v>
       </c>
       <c r="G31" t="n">
-        <v>48.55233167199075</v>
+        <v>50.56147831552182</v>
       </c>
       <c r="H31" t="n">
-        <v>100.8253368437607</v>
+        <v>106.2582235462759</v>
       </c>
       <c r="I31" t="n">
-        <v>-10.91938124009984</v>
+        <v>1.419432825813049</v>
       </c>
       <c r="J31" t="n">
-        <v>12.34901270354981</v>
+        <v>25.58340215356819</v>
       </c>
       <c r="K31" t="n">
-        <v>-22.54527676867589</v>
+        <v>-3.896690741325479</v>
       </c>
       <c r="L31" t="n">
-        <v>128.2620232105255</v>
+        <v>179.9258460998535</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1980</v>
+        <v>1989</v>
       </c>
       <c r="B32" t="n">
-        <v>48.0427965694126</v>
+        <v>47.14159825754578</v>
       </c>
       <c r="C32" t="n">
-        <v>99.52222942956075</v>
+        <v>99.57131178683964</v>
       </c>
       <c r="D32" t="n">
-        <v>-10.01749156270915</v>
+        <v>2.540492374706781</v>
       </c>
       <c r="E32" t="n">
-        <v>-3.94115564254777</v>
+        <v>1.074794583318678</v>
       </c>
       <c r="F32" t="n">
-        <v>133.6063787937164</v>
+        <v>150.3281970024109</v>
       </c>
       <c r="G32" t="n">
-        <v>49.77357746657807</v>
+        <v>50.73361346102855</v>
       </c>
       <c r="H32" t="n">
-        <v>103.1075988468288</v>
+        <v>107.1582769935571</v>
       </c>
       <c r="I32" t="n">
-        <v>-10.37837985965088</v>
+        <v>2.734068485224377</v>
       </c>
       <c r="J32" t="n">
-        <v>5.789237996461569</v>
+        <v>26.93766980463741</v>
       </c>
       <c r="K32" t="n">
-        <v>-14.79142719809661</v>
+        <v>-3.519134115541181</v>
       </c>
       <c r="L32" t="n">
-        <v>133.500607252121</v>
+        <v>184.0444946289062</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1981</v>
+        <v>1990</v>
       </c>
       <c r="B33" t="n">
-        <v>48.9353906170622</v>
+        <v>47.03531076804186</v>
       </c>
       <c r="C33" t="n">
-        <v>101.2028859588783</v>
+        <v>99.96447293459201</v>
       </c>
       <c r="D33" t="n">
-        <v>-9.383859888729356</v>
+        <v>3.789498888982585</v>
       </c>
       <c r="E33" t="n">
-        <v>-3.739477140626114</v>
+        <v>1.168524114812065</v>
       </c>
       <c r="F33" t="n">
-        <v>137.0149395465851</v>
+        <v>151.9578067064285</v>
       </c>
       <c r="G33" t="n">
-        <v>50.88735708958646</v>
+        <v>50.84880065221385</v>
       </c>
       <c r="H33" t="n">
-        <v>105.2397320496818</v>
+        <v>108.0693094943552</v>
       </c>
       <c r="I33" t="n">
-        <v>-9.758169353815722</v>
+        <v>4.096740734380042</v>
       </c>
       <c r="J33" t="n">
-        <v>7.177473332790324</v>
+        <v>26.18919868546218</v>
       </c>
       <c r="K33" t="n">
-        <v>-15.01137622390231</v>
+        <v>-1.15259692969255</v>
       </c>
       <c r="L33" t="n">
-        <v>138.5350168943405</v>
+        <v>188.0514526367188</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1982</v>
+        <v>1991</v>
       </c>
       <c r="B34" t="n">
-        <v>49.71852863810011</v>
+        <v>46.8905618726435</v>
       </c>
       <c r="C34" t="n">
-        <v>102.732821302214</v>
+        <v>100.3921421339615</v>
       </c>
       <c r="D34" t="n">
-        <v>-8.680294063244625</v>
+        <v>5.070462918739533</v>
       </c>
       <c r="E34" t="n">
-        <v>-3.566003024438842</v>
+        <v>1.184465957250538</v>
       </c>
       <c r="F34" t="n">
-        <v>140.2050528526306</v>
+        <v>153.5376328825951</v>
       </c>
       <c r="G34" t="n">
-        <v>51.89116012575058</v>
+        <v>50.91375236377912</v>
       </c>
       <c r="H34" t="n">
-        <v>107.2221046436626</v>
+        <v>109.0057457140399</v>
       </c>
       <c r="I34" t="n">
-        <v>-9.059611004442655</v>
+        <v>5.505506505031679</v>
       </c>
       <c r="J34" t="n">
-        <v>7.100672079553606</v>
+        <v>23.14716753175523</v>
       </c>
       <c r="K34" t="n">
-        <v>-13.79075014757894</v>
+        <v>3.38717465663434</v>
       </c>
       <c r="L34" t="n">
-        <v>143.3635756969452</v>
+        <v>191.9593467712402</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1983</v>
+        <v>1992</v>
       </c>
       <c r="B35" t="n">
-        <v>50.39169842513177</v>
+        <v>46.71473821057894</v>
       </c>
       <c r="C35" t="n">
-        <v>104.1148435435144</v>
+        <v>100.8678554297609</v>
       </c>
       <c r="D35" t="n">
-        <v>-7.908485023284301</v>
+        <v>6.382281023679034</v>
       </c>
       <c r="E35" t="n">
-        <v>-3.419023904361545</v>
+        <v>1.122952184011197</v>
       </c>
       <c r="F35" t="n">
-        <v>143.1790330410004</v>
+        <v>155.0878268480301</v>
       </c>
       <c r="G35" t="n">
-        <v>52.7834929539832</v>
+        <v>50.93557003417359</v>
       </c>
       <c r="H35" t="n">
-        <v>109.0565565824107</v>
+        <v>109.9816013370272</v>
       </c>
       <c r="I35" t="n">
-        <v>-8.283853820156629</v>
+        <v>6.958941321558391</v>
       </c>
       <c r="J35" t="n">
-        <v>8.676275893439007</v>
+        <v>21.81074045488691</v>
       </c>
       <c r="K35" t="n">
-        <v>-14.24502041395939</v>
+        <v>6.096941255430121</v>
       </c>
       <c r="L35" t="n">
-        <v>147.9874511957169</v>
+        <v>195.7837944030762</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1984</v>
+        <v>1993</v>
       </c>
       <c r="B36" t="n">
-        <v>50.95527169742758</v>
+        <v>46.51524342192354</v>
       </c>
       <c r="C36" t="n">
-        <v>105.3529431326325</v>
+        <v>101.4042027670032</v>
       </c>
       <c r="D36" t="n">
-        <v>-7.070330436326387</v>
+        <v>7.724439592141614</v>
       </c>
       <c r="E36" t="n">
-        <v>-3.296681991618783</v>
+        <v>0.9854040248207738</v>
       </c>
       <c r="F36" t="n">
-        <v>145.9412024021149</v>
+        <v>156.6292898058891</v>
       </c>
       <c r="G36" t="n">
-        <v>53.56388736524139</v>
+        <v>50.92176606520668</v>
       </c>
       <c r="H36" t="n">
-        <v>110.7464054565702</v>
+        <v>111.0105142198692</v>
       </c>
       <c r="I36" t="n">
-        <v>-7.432290526782602</v>
+        <v>8.45619794629444</v>
       </c>
       <c r="J36" t="n">
-        <v>10.19609489014616</v>
+        <v>18.85663057594003</v>
       </c>
       <c r="K36" t="n">
-        <v>-14.663440256159</v>
+        <v>10.29879835821694</v>
       </c>
       <c r="L36" t="n">
-        <v>152.4106569290161</v>
+        <v>199.5439071655273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1985</v>
+        <v>1994</v>
       </c>
       <c r="B37" t="n">
-        <v>51.41050401810343</v>
+        <v>46.29948752242535</v>
       </c>
       <c r="C37" t="n">
-        <v>106.4522903415958</v>
+        <v>102.012810275515</v>
       </c>
       <c r="D37" t="n">
-        <v>-6.167896770337384</v>
+        <v>9.09702885589531</v>
       </c>
       <c r="E37" t="n">
-        <v>-3.197009262716954</v>
+        <v>0.7743479796673114</v>
       </c>
       <c r="F37" t="n">
-        <v>148.4978883266449</v>
+        <v>158.183674633503</v>
       </c>
       <c r="G37" t="n">
-        <v>54.23290528689068</v>
+        <v>50.88023851770513</v>
       </c>
       <c r="H37" t="n">
-        <v>112.2964477771975</v>
+        <v>112.1056926637815</v>
       </c>
       <c r="I37" t="n">
-        <v>-6.506510055751178</v>
+        <v>9.997065254042214</v>
       </c>
       <c r="J37" t="n">
-        <v>12.55866140380141</v>
+        <v>23.30701491396057</v>
       </c>
       <c r="K37" t="n">
-        <v>-15.94144780203101</v>
+        <v>6.972344454953951</v>
       </c>
       <c r="L37" t="n">
-        <v>156.6400566101074</v>
+        <v>203.2623558044434</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1986</v>
+        <v>1995</v>
       </c>
       <c r="B38" t="n">
-        <v>51.75952868407051</v>
+        <v>46.07487919583082</v>
       </c>
       <c r="C38" t="n">
-        <v>107.4192343144029</v>
+        <v>102.7043342335696</v>
       </c>
       <c r="D38" t="n">
-        <v>-5.20337919366051</v>
+        <v>10.50075463468881</v>
       </c>
       <c r="E38" t="n">
-        <v>-3.117959307208487</v>
+        <v>0.4934173414512557</v>
       </c>
       <c r="F38" t="n">
-        <v>150.8574244976044</v>
+        <v>159.7733854055405</v>
       </c>
       <c r="G38" t="n">
-        <v>54.7921351312046</v>
+        <v>50.81927671840951</v>
       </c>
       <c r="H38" t="n">
-        <v>113.7129597560783</v>
+        <v>113.2799493496681</v>
       </c>
       <c r="I38" t="n">
-        <v>-5.508246755069248</v>
+        <v>11.58203265741084</v>
       </c>
       <c r="J38" t="n">
-        <v>10.82435430705965</v>
+        <v>25.33350780415606</v>
       </c>
       <c r="K38" t="n">
-        <v>-13.1358356895098</v>
+        <v>5.950962230121121</v>
       </c>
       <c r="L38" t="n">
-        <v>160.6853667497635</v>
+        <v>206.9657287597656</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1987</v>
+        <v>1996</v>
       </c>
       <c r="B39" t="n">
-        <v>52.005348788113</v>
+        <v>45.84882013917341</v>
       </c>
       <c r="C39" t="n">
-        <v>108.2612986727404</v>
+        <v>103.4884644379322</v>
       </c>
       <c r="D39" t="n">
-        <v>-4.179059098986004</v>
+        <v>11.93694952311474</v>
       </c>
       <c r="E39" t="n">
-        <v>-3.057436279424152</v>
+        <v>0.1473421016953438</v>
       </c>
       <c r="F39" t="n">
-        <v>153.0301520824432</v>
+        <v>161.4215762019157</v>
       </c>
       <c r="G39" t="n">
-        <v>55.24418493636018</v>
+        <v>50.74755089516047</v>
       </c>
       <c r="H39" t="n">
-        <v>115.0036937487946</v>
+        <v>114.545720046541</v>
       </c>
       <c r="I39" t="n">
-        <v>-4.439326321317392</v>
+        <v>13.21235642745915</v>
       </c>
       <c r="J39" t="n">
-        <v>16.38424778279656</v>
+        <v>29.01916569179815</v>
       </c>
       <c r="K39" t="n">
-        <v>-17.63364205985724</v>
+        <v>3.159941283523629</v>
       </c>
       <c r="L39" t="n">
-        <v>164.5591580867767</v>
+        <v>210.6847343444824</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1988</v>
+        <v>1997</v>
       </c>
       <c r="B40" t="n">
-        <v>52.15182797415758</v>
+        <v>45.62870305311761</v>
       </c>
       <c r="C40" t="n">
-        <v>108.9871733004609</v>
+        <v>104.3739399767987</v>
       </c>
       <c r="D40" t="n">
-        <v>-3.097259747333005</v>
+        <v>13.4075849002903</v>
       </c>
       <c r="E40" t="n">
-        <v>-3.013324893679517</v>
+        <v>-0.2580756899302159</v>
       </c>
       <c r="F40" t="n">
-        <v>155.028416633606</v>
+        <v>163.1521522402763</v>
       </c>
       <c r="G40" t="n">
-        <v>55.59267410989249</v>
+        <v>50.67411623152266</v>
       </c>
       <c r="H40" t="n">
-        <v>116.1778722397462</v>
+        <v>115.9151326253812</v>
       </c>
       <c r="I40" t="n">
-        <v>-3.301609137315249</v>
+        <v>14.89013428302773</v>
       </c>
       <c r="J40" t="n">
-        <v>17.5950674260159</v>
+        <v>31.34075395482911</v>
       </c>
       <c r="K40" t="n">
-        <v>-17.78714535489203</v>
+        <v>1.634387899135788</v>
       </c>
       <c r="L40" t="n">
-        <v>168.2768592834473</v>
+        <v>214.4545249938965</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1989</v>
+        <v>1998</v>
       </c>
       <c r="B41" t="n">
-        <v>52.20367738905199</v>
+        <v>45.42191227554903</v>
       </c>
       <c r="C41" t="n">
-        <v>109.6067079503459</v>
+        <v>105.3685687342527</v>
       </c>
       <c r="D41" t="n">
-        <v>-1.960300053749089</v>
+        <v>14.91528190449989</v>
       </c>
       <c r="E41" t="n">
-        <v>-2.983514097675808</v>
+        <v>-0.7159922634379825</v>
       </c>
       <c r="F41" t="n">
-        <v>156.866571187973</v>
+        <v>164.9897706508636</v>
       </c>
       <c r="G41" t="n">
-        <v>55.84222010936139</v>
+        <v>50.60840381654495</v>
       </c>
       <c r="H41" t="n">
-        <v>117.2461829692733</v>
+        <v>117.4000566890483</v>
       </c>
       <c r="I41" t="n">
-        <v>-2.096930954998332</v>
+        <v>16.6183802452296</v>
       </c>
       <c r="J41" t="n">
-        <v>18.84206386944151</v>
+        <v>30.11614444334076</v>
       </c>
       <c r="K41" t="n">
-        <v>-17.97677239177482</v>
+        <v>3.571879918141136</v>
       </c>
       <c r="L41" t="n">
-        <v>171.8567636013031</v>
+        <v>218.3148651123047</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1990</v>
+        <v>1999</v>
       </c>
       <c r="B42" t="n">
-        <v>52.16644167936234</v>
+        <v>45.23582748092343</v>
       </c>
       <c r="C42" t="n">
-        <v>110.1309012681358</v>
+        <v>106.4792581623213</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.7704466043620857</v>
+        <v>16.46332455231387</v>
       </c>
       <c r="E42" t="n">
-        <v>-2.965920314693676</v>
+        <v>-1.218571685998931</v>
       </c>
       <c r="F42" t="n">
-        <v>158.5609760284424</v>
+        <v>166.9598385095596</v>
       </c>
       <c r="G42" t="n">
-        <v>55.99842297360951</v>
+        <v>50.56023167381345</v>
       </c>
       <c r="H42" t="n">
-        <v>118.2207678565452</v>
+        <v>119.0122135692798</v>
       </c>
       <c r="I42" t="n">
-        <v>-0.8270411674775481</v>
+        <v>18.40111146053868</v>
       </c>
       <c r="J42" t="n">
-        <v>18.02951935293441</v>
+        <v>31.93853057554702</v>
       </c>
       <c r="K42" t="n">
-        <v>-16.10164392920865</v>
+        <v>2.398375672481222</v>
       </c>
       <c r="L42" t="n">
-        <v>175.3200250864029</v>
+        <v>222.3104629516602</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="B43" t="n">
-        <v>52.04648281914834</v>
+        <v>45.07783093998246</v>
       </c>
       <c r="C43" t="n">
-        <v>110.5718933673599</v>
+        <v>107.7120490501449</v>
       </c>
       <c r="D43" t="n">
-        <v>0.4701357523780564</v>
+        <v>18.05567280178439</v>
       </c>
       <c r="E43" t="n">
-        <v>-2.958518261747059</v>
+        <v>-1.757038761932087</v>
       </c>
       <c r="F43" t="n">
-        <v>160.1299936771393</v>
+        <v>169.0885140299797</v>
       </c>
       <c r="G43" t="n">
-        <v>56.06784966289666</v>
+        <v>50.53981088906968</v>
       </c>
       <c r="H43" t="n">
-        <v>119.1152208268359</v>
+        <v>120.763277113232</v>
       </c>
       <c r="I43" t="n">
-        <v>0.5064607492706077</v>
+        <v>20.24343828992268</v>
       </c>
       <c r="J43" t="n">
-        <v>14.97623727424066</v>
+        <v>37.56957490439125</v>
       </c>
       <c r="K43" t="n">
-        <v>-11.97510171846696</v>
+        <v>-2.624897888510105</v>
       </c>
       <c r="L43" t="n">
-        <v>178.6906667947769</v>
+        <v>226.4912033081055</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1992</v>
+        <v>2001</v>
       </c>
       <c r="B44" t="n">
-        <v>51.8509662037881</v>
+        <v>44.95531854101138</v>
       </c>
       <c r="C44" t="n">
-        <v>110.9429562214854</v>
+        <v>109.0721523489197</v>
       </c>
       <c r="D44" t="n">
-        <v>1.759434645404824</v>
+        <v>19.69697675108842</v>
       </c>
       <c r="E44" t="n">
-        <v>-2.959358876937472</v>
+        <v>-2.321741435174644</v>
       </c>
       <c r="F44" t="n">
-        <v>161.5939981937408</v>
+        <v>171.4027062058449</v>
       </c>
       <c r="G44" t="n">
-        <v>56.05801853675138</v>
+        <v>50.55775402981955</v>
       </c>
       <c r="H44" t="n">
-        <v>119.9445786977767</v>
+        <v>122.6649755563188</v>
       </c>
       <c r="I44" t="n">
-        <v>1.902190589441716</v>
+        <v>22.15165942610622</v>
       </c>
       <c r="J44" t="n">
-        <v>13.59792620902363</v>
+        <v>32.92363347830938</v>
       </c>
       <c r="K44" t="n">
-        <v>-9.507132167682787</v>
+        <v>2.614308136887423</v>
       </c>
       <c r="L44" t="n">
-        <v>181.9955818653107</v>
+        <v>230.9123306274414</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1993</v>
+        <v>2002</v>
       </c>
       <c r="B45" t="n">
-        <v>51.58784272178254</v>
+        <v>44.87571357744274</v>
       </c>
       <c r="C45" t="n">
-        <v>111.2584829980165</v>
+        <v>110.5639838687215</v>
       </c>
       <c r="D45" t="n">
-        <v>3.09564234000029</v>
+        <v>21.39259400557647</v>
       </c>
       <c r="E45" t="n">
-        <v>-2.966602421066405</v>
+        <v>-2.902216223526494</v>
       </c>
       <c r="F45" t="n">
-        <v>162.9753656387329</v>
+        <v>173.9300752282143</v>
       </c>
       <c r="G45" t="n">
-        <v>55.97738310537027</v>
+        <v>50.62510994666669</v>
       </c>
       <c r="H45" t="n">
-        <v>120.7253181740935</v>
+        <v>124.7292442455792</v>
       </c>
       <c r="I45" t="n">
-        <v>3.359046396996022</v>
+        <v>24.1333749870686</v>
       </c>
       <c r="J45" t="n">
-        <v>10.64330366658101</v>
+        <v>38.91716652057909</v>
       </c>
       <c r="K45" t="n">
-        <v>-5.440514127808003</v>
+        <v>-2.770049966251001</v>
       </c>
       <c r="L45" t="n">
-        <v>185.2645372152328</v>
+        <v>235.6348457336426</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1994</v>
+        <v>2003</v>
       </c>
       <c r="B46" t="n">
-        <v>51.26583665133312</v>
+        <v>44.84648486869106</v>
       </c>
       <c r="C46" t="n">
-        <v>111.5339829316722</v>
+        <v>112.1911987995452</v>
       </c>
       <c r="D46" t="n">
-        <v>4.477208539092099</v>
+        <v>23.14860675855028</v>
       </c>
       <c r="E46" t="n">
-        <v>-2.978547611385743</v>
+        <v>-3.487257524068923</v>
       </c>
       <c r="F46" t="n">
-        <v>164.2984805107117</v>
+        <v>176.6990329027176</v>
       </c>
       <c r="G46" t="n">
-        <v>55.83532094044448</v>
+        <v>50.7533837118781</v>
       </c>
       <c r="H46" t="n">
-        <v>121.4753555103452</v>
+        <v>126.968322677708</v>
       </c>
       <c r="I46" t="n">
-        <v>4.876276132928482</v>
+        <v>26.19759663777564</v>
       </c>
       <c r="J46" t="n">
-        <v>14.92454472067721</v>
+        <v>39.92424316958314</v>
       </c>
       <c r="K46" t="n">
-        <v>-8.581323168233551</v>
+        <v>-3.117903038985844</v>
       </c>
       <c r="L46" t="n">
-        <v>188.5301741361618</v>
+        <v>240.725643157959</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1995</v>
+        <v>2004</v>
       </c>
       <c r="B47" t="n">
-        <v>50.89443145034392</v>
+        <v>44.87516786538301</v>
       </c>
       <c r="C47" t="n">
-        <v>111.786076729326</v>
+        <v>113.9567131572675</v>
       </c>
       <c r="D47" t="n">
-        <v>5.902894323115618</v>
+        <v>24.97184156382364</v>
       </c>
       <c r="E47" t="n">
-        <v>-2.993668902169119</v>
+        <v>-4.064982142290773</v>
       </c>
       <c r="F47" t="n">
-        <v>165.5897336006165</v>
+        <v>179.7387404441833</v>
       </c>
       <c r="G47" t="n">
-        <v>55.64212414864494</v>
+        <v>50.95458500720858</v>
       </c>
       <c r="H47" t="n">
-        <v>122.2140533298182</v>
+        <v>129.3948814884174</v>
       </c>
       <c r="I47" t="n">
-        <v>6.4535464765647</v>
+        <v>28.35487607684153</v>
       </c>
       <c r="J47" t="n">
-        <v>16.83727956424859</v>
+        <v>45.20217687485608</v>
       </c>
       <c r="K47" t="n">
-        <v>-9.318986761311347</v>
+        <v>-7.648664985653667</v>
       </c>
       <c r="L47" t="n">
-        <v>191.8280167579651</v>
+        <v>246.2578544616699</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1996</v>
+        <v>2005</v>
       </c>
       <c r="B48" t="n">
-        <v>50.48386104688534</v>
+        <v>44.96938955512552</v>
       </c>
       <c r="C48" t="n">
-        <v>112.0324906192857</v>
+        <v>115.8627216103943</v>
       </c>
       <c r="D48" t="n">
-        <v>7.371826295495705</v>
+        <v>26.86989228150882</v>
       </c>
       <c r="E48" t="n">
-        <v>-3.010658115704217</v>
+        <v>-4.622892705413292</v>
       </c>
       <c r="F48" t="n">
-        <v>166.8775198459625</v>
+        <v>183.0791107416153</v>
       </c>
       <c r="G48" t="n">
-        <v>55.40899666687305</v>
+        <v>51.24127346917766</v>
       </c>
       <c r="H48" t="n">
-        <v>122.9622253642676</v>
+        <v>132.0221035165181</v>
       </c>
       <c r="I48" t="n">
-        <v>8.091011467140733</v>
+        <v>30.61743804185594</v>
       </c>
       <c r="J48" t="n">
-        <v>20.36876189910278</v>
+        <v>49.8075767719444</v>
       </c>
       <c r="K48" t="n">
-        <v>-11.63452775936845</v>
+        <v>-11.3773490138516</v>
       </c>
       <c r="L48" t="n">
-        <v>195.1964676380157</v>
+        <v>252.3110427856445</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1997</v>
+        <v>2006</v>
       </c>
       <c r="B49" t="n">
-        <v>50.04510574404886</v>
+        <v>45.1368965545372</v>
       </c>
       <c r="C49" t="n">
-        <v>112.2920622610239</v>
+        <v>117.9107008684596</v>
       </c>
       <c r="D49" t="n">
-        <v>8.883551258478132</v>
+        <v>28.85114207998197</v>
       </c>
       <c r="E49" t="n">
-        <v>-3.028476164338251</v>
+        <v>-5.14793150241421</v>
       </c>
       <c r="F49" t="n">
-        <v>168.1922430992126</v>
+        <v>186.7508080005646</v>
       </c>
       <c r="G49" t="n">
-        <v>55.14806027179576</v>
+        <v>51.62662618039512</v>
       </c>
       <c r="H49" t="n">
-        <v>123.7421587095277</v>
+        <v>134.86376204552</v>
       </c>
       <c r="I49" t="n">
-        <v>9.789381258094297</v>
+        <v>32.99932518047636</v>
       </c>
       <c r="J49" t="n">
-        <v>22.56964543602227</v>
+        <v>52.68795298427746</v>
       </c>
       <c r="K49" t="n">
-        <v>-12.57242837750452</v>
+        <v>-13.20615454984861</v>
       </c>
       <c r="L49" t="n">
-        <v>198.6768172979355</v>
+        <v>258.9715118408203</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1998</v>
+        <v>2007</v>
       </c>
       <c r="B50" t="n">
-        <v>49.58989124420783</v>
+        <v>45.38558619326406</v>
       </c>
       <c r="C50" t="n">
-        <v>112.5847444948703</v>
+        <v>120.1013883374548</v>
       </c>
       <c r="D50" t="n">
-        <v>10.438090626186</v>
+        <v>30.92479043727737</v>
       </c>
       <c r="E50" t="n">
-        <v>-3.04641452902149</v>
+        <v>-5.626517701703619</v>
       </c>
       <c r="F50" t="n">
-        <v>169.5663118362427</v>
+        <v>190.7852472662926</v>
       </c>
       <c r="G50" t="n">
-        <v>54.87236737703771</v>
+        <v>52.12450824492436</v>
       </c>
       <c r="H50" t="n">
-        <v>124.5776368120997</v>
+        <v>137.9342282804235</v>
       </c>
       <c r="I50" t="n">
-        <v>11.54998991093354</v>
+        <v>35.51655116354232</v>
       </c>
       <c r="J50" t="n">
-        <v>21.31366972624049</v>
+        <v>55.96482992367342</v>
       </c>
       <c r="K50" t="n">
-        <v>-10.00042139085614</v>
+        <v>-15.20760571070816</v>
       </c>
       <c r="L50" t="n">
-        <v>202.3132424354553</v>
+        <v>266.3325119018555</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1999</v>
+        <v>2008</v>
       </c>
       <c r="B51" t="n">
-        <v>49.13069846472295</v>
+        <v>45.72354072753397</v>
       </c>
       <c r="C51" t="n">
-        <v>112.9316185654122</v>
+        <v>122.4347512322841</v>
       </c>
       <c r="D51" t="n">
-        <v>12.0359944177073</v>
+        <v>33.10088024399156</v>
       </c>
       <c r="E51" t="n">
-        <v>-3.064169668896461</v>
+        <v>-6.044578256875894</v>
       </c>
       <c r="F51" t="n">
-        <v>171.0341417789459</v>
+        <v>195.2145939469337</v>
       </c>
       <c r="G51" t="n">
-        <v>54.59592996620321</v>
+        <v>52.7495645221261</v>
       </c>
       <c r="H51" t="n">
-        <v>125.4939768990721</v>
+        <v>141.2484621075878</v>
       </c>
       <c r="I51" t="n">
-        <v>13.37486192618625</v>
+        <v>38.18726613002993</v>
       </c>
       <c r="J51" t="n">
-        <v>23.03030070738717</v>
+        <v>54.6056108063263</v>
       </c>
       <c r="K51" t="n">
-        <v>-10.34225618345713</v>
+        <v>-12.29637002725173</v>
       </c>
       <c r="L51" t="n">
-        <v>206.1528133153915</v>
+        <v>274.4945335388184</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2000</v>
+        <v>2009</v>
       </c>
       <c r="B52" t="n">
-        <v>48.68077941386195</v>
+        <v>46.15906335828793</v>
       </c>
       <c r="C52" t="n">
-        <v>113.3549127382047</v>
+        <v>124.9099284344037</v>
       </c>
       <c r="D52" t="n">
-        <v>13.67839433664197</v>
+        <v>35.39032686421503</v>
       </c>
       <c r="E52" t="n">
-        <v>-3.081933216079811</v>
+        <v>-6.387554247364527</v>
       </c>
       <c r="F52" t="n">
-        <v>172.6321532726288</v>
+        <v>200.0717644095421</v>
       </c>
       <c r="G52" t="n">
-        <v>54.33375954058786</v>
+        <v>53.51732175708143</v>
       </c>
       <c r="H52" t="n">
-        <v>126.5180764486311</v>
+        <v>144.8219340758725</v>
       </c>
       <c r="I52" t="n">
-        <v>15.26677669784425</v>
+        <v>41.03193115465174</v>
       </c>
       <c r="J52" t="n">
-        <v>28.46245436568747</v>
+        <v>57.23129051485344</v>
       </c>
       <c r="K52" t="n">
-        <v>-14.33557530966292</v>
+        <v>-13.03689904176571</v>
       </c>
       <c r="L52" t="n">
-        <v>210.2454917430878</v>
+        <v>283.5655784606934</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2001</v>
+        <v>2010</v>
       </c>
       <c r="B53" t="n">
-        <v>48.25418449863953</v>
+        <v>46.70071742995661</v>
       </c>
       <c r="C53" t="n">
-        <v>113.8780286235422</v>
+        <v>127.5251409894099</v>
       </c>
       <c r="D53" t="n">
-        <v>15.36705557367523</v>
+        <v>37.80494913567291</v>
       </c>
       <c r="E53" t="n">
-        <v>-3.100494310404699</v>
+        <v>-6.640381217320495</v>
       </c>
       <c r="F53" t="n">
-        <v>174.3987743854523</v>
+        <v>205.390426337719</v>
       </c>
       <c r="G53" t="n">
-        <v>54.10192536380669</v>
+        <v>54.44430555578766</v>
       </c>
       <c r="H53" t="n">
-        <v>127.6784732594958</v>
+        <v>148.6704728355773</v>
       </c>
       <c r="I53" t="n">
-        <v>17.22933052017255</v>
+        <v>44.07350283966503</v>
       </c>
       <c r="J53" t="n">
-        <v>23.8717334560006</v>
+        <v>62.21298671394278</v>
       </c>
       <c r="K53" t="n">
-        <v>-8.237323071201072</v>
+        <v>-15.73983758608603</v>
       </c>
       <c r="L53" t="n">
-        <v>214.6441395282745</v>
+        <v>293.6614303588867</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2002</v>
+        <v>2011</v>
       </c>
       <c r="B54" t="n">
-        <v>47.8658030594471</v>
+        <v>47.35736575322517</v>
       </c>
       <c r="C54" t="n">
-        <v>114.5255778820094</v>
+        <v>130.2775831136213</v>
       </c>
       <c r="D54" t="n">
-        <v>17.10442650467566</v>
+        <v>40.35750217214488</v>
       </c>
       <c r="E54" t="n">
-        <v>-3.121367968211601</v>
+        <v>-6.787452247773508</v>
       </c>
       <c r="F54" t="n">
-        <v>176.3744394779205</v>
+        <v>211.2049987912178</v>
       </c>
       <c r="G54" t="n">
-        <v>53.91763241755898</v>
+        <v>55.54816204423015</v>
       </c>
       <c r="H54" t="n">
-        <v>129.0054196517231</v>
+        <v>152.8100261158055</v>
       </c>
       <c r="I54" t="n">
-        <v>19.26699484905515</v>
+        <v>47.33762181875586</v>
       </c>
       <c r="J54" t="n">
-        <v>29.66037361892228</v>
+        <v>62.85457849953008</v>
       </c>
       <c r="K54" t="n">
-        <v>-12.44590503242247</v>
+        <v>-13.64454665092902</v>
       </c>
       <c r="L54" t="n">
-        <v>219.404515504837</v>
+        <v>304.9058418273926</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="B55" t="n">
-        <v>47.5314162424393</v>
+        <v>48.13821235603202</v>
       </c>
       <c r="C55" t="n">
-        <v>115.3234273333192</v>
+        <v>133.1632727971445</v>
       </c>
       <c r="D55" t="n">
-        <v>18.89368606130011</v>
+        <v>43.0617099800015</v>
       </c>
       <c r="E55" t="n">
-        <v>-3.146941626270639</v>
+        <v>-6.812544119326809</v>
       </c>
       <c r="F55" t="n">
-        <v>178.601588010788</v>
+        <v>217.5506510138512</v>
       </c>
       <c r="G55" t="n">
-        <v>53.79932028891323</v>
+        <v>56.84780325697707</v>
       </c>
       <c r="H55" t="n">
-        <v>130.5309728680209</v>
+        <v>157.2563492187649</v>
       </c>
       <c r="I55" t="n">
-        <v>21.38517107644035</v>
+        <v>50.85281519693546</v>
       </c>
       <c r="J55" t="n">
-        <v>30.58334824800995</v>
+        <v>66.44078362199606</v>
       </c>
       <c r="K55" t="n">
-        <v>-11.71352812908183</v>
+        <v>-13.96692701488836</v>
       </c>
       <c r="L55" t="n">
-        <v>224.5852843523026</v>
+        <v>317.4308242797852</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2004</v>
+        <v>2013</v>
       </c>
       <c r="B56" t="n">
-        <v>47.26776662169039</v>
+        <v>49.05284335810448</v>
       </c>
       <c r="C56" t="n">
-        <v>116.298752267085</v>
+        <v>136.1768739085894</v>
       </c>
       <c r="D56" t="n">
-        <v>20.73878794553105</v>
+        <v>45.93229996533801</v>
       </c>
       <c r="E56" t="n">
-        <v>-3.180639666642882</v>
+        <v>-6.698714679331808</v>
       </c>
       <c r="F56" t="n">
-        <v>181.1246671676636</v>
+        <v>224.4633025527</v>
       </c>
       <c r="G56" t="n">
-        <v>53.76678538193717</v>
+        <v>58.36357028728237</v>
       </c>
       <c r="H56" t="n">
-        <v>132.2890946673591</v>
+        <v>162.0246250323269</v>
       </c>
       <c r="I56" t="n">
-        <v>23.59024003552544</v>
+        <v>54.650716124912</v>
       </c>
       <c r="J56" t="n">
-        <v>35.6769086651295</v>
+        <v>69.5622093905431</v>
       </c>
       <c r="K56" t="n">
-        <v>-15.07501394225012</v>
+        <v>-13.22409904551354</v>
       </c>
       <c r="L56" t="n">
-        <v>230.2480148077011</v>
+        <v>331.3770217895508</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="B57" t="n">
-        <v>47.09264302816779</v>
+        <v>50.11126919750051</v>
       </c>
       <c r="C57" t="n">
-        <v>117.480103914318</v>
+        <v>139.3114734954626</v>
       </c>
       <c r="D57" t="n">
-        <v>22.64450101703293</v>
+        <v>48.9850378316325</v>
       </c>
       <c r="E57" t="n">
-        <v>-3.227119919204974</v>
+        <v>-6.428154822691305</v>
       </c>
       <c r="F57" t="n">
-        <v>183.9901280403137</v>
+        <v>231.9796257019043</v>
       </c>
       <c r="G57" t="n">
-        <v>53.841327845168</v>
+        <v>60.11738503598414</v>
       </c>
       <c r="H57" t="n">
-        <v>134.3157738322697</v>
+        <v>167.1289038609056</v>
       </c>
       <c r="I57" t="n">
-        <v>25.88960662961849</v>
+        <v>58.76627009226472</v>
       </c>
       <c r="J57" t="n">
-        <v>40.11432605607294</v>
+        <v>71.79291328163136</v>
       </c>
       <c r="K57" t="n">
-        <v>-17.70384826026199</v>
+        <v>-10.91167725735813</v>
       </c>
       <c r="L57" t="n">
-        <v>236.4571861028671</v>
+        <v>346.8937950134277</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="B58" t="n">
-        <v>47.02498777341092</v>
+        <v>51.32396452152532</v>
       </c>
       <c r="C58" t="n">
-        <v>118.8974853507911</v>
+        <v>142.5583260100778</v>
       </c>
       <c r="D58" t="n">
-        <v>24.61644567445737</v>
+        <v>52.23676193206015</v>
       </c>
       <c r="E58" t="n">
-        <v>-3.292487686369931</v>
+        <v>-5.982009524000297</v>
       </c>
       <c r="F58" t="n">
-        <v>187.2464311122894</v>
+        <v>240.1370429396629</v>
       </c>
       <c r="G58" t="n">
-        <v>54.04592785700545</v>
+        <v>62.13293861197647</v>
       </c>
       <c r="H58" t="n">
-        <v>136.6491565422924</v>
+        <v>172.581518228106</v>
       </c>
       <c r="I58" t="n">
-        <v>28.29173828663637</v>
+        <v>63.237973774452</v>
       </c>
       <c r="J58" t="n">
-        <v>42.86257787642446</v>
+        <v>75.03934725812121</v>
       </c>
       <c r="K58" t="n">
-        <v>-18.56921235950075</v>
+        <v>-8.852148508642074</v>
       </c>
       <c r="L58" t="n">
-        <v>243.280188202858</v>
+        <v>364.1396293640137</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="B59" t="n">
-        <v>47.08501560449325</v>
+        <v>52.70190793960818</v>
       </c>
       <c r="C59" t="n">
-        <v>120.5824360802454</v>
+        <v>145.9065426299362</v>
       </c>
       <c r="D59" t="n">
-        <v>26.66112491157562</v>
+        <v>55.70541808095835</v>
       </c>
       <c r="E59" t="n">
-        <v>-3.384537013108073</v>
+        <v>-5.340142258710372</v>
       </c>
       <c r="F59" t="n">
-        <v>190.9440395832062</v>
+        <v>248.9737263917923</v>
       </c>
       <c r="G59" t="n">
-        <v>54.40544225001144</v>
+        <v>64.4358653823173</v>
       </c>
       <c r="H59" t="n">
-        <v>139.329692861001</v>
+        <v>178.3922955896653</v>
       </c>
       <c r="I59" t="n">
-        <v>30.80619753598741</v>
+        <v>68.10810008327421</v>
       </c>
       <c r="J59" t="n">
-        <v>45.99261463244734</v>
+        <v>77.11425735621886</v>
       </c>
       <c r="K59" t="n">
-        <v>-19.74661975144733</v>
+        <v>-4.768268960792042</v>
       </c>
       <c r="L59" t="n">
-        <v>250.7873275279999</v>
+        <v>383.2822494506836</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2008</v>
+        <v>2017</v>
       </c>
       <c r="B60" t="n">
-        <v>47.29435722448402</v>
+        <v>54.25661901033149</v>
       </c>
       <c r="C60" t="n">
-        <v>122.56813113794</v>
+        <v>149.3427338288177</v>
       </c>
       <c r="D60" t="n">
-        <v>28.78595062029484</v>
+        <v>59.41009393395692</v>
       </c>
       <c r="E60" t="n">
-        <v>-3.513011746161901</v>
+        <v>-4.480846139961756</v>
       </c>
       <c r="F60" t="n">
-        <v>195.135427236557</v>
+        <v>258.5286006331444</v>
       </c>
       <c r="G60" t="n">
-        <v>54.94683115953134</v>
+        <v>67.05395488035725</v>
       </c>
       <c r="H60" t="n">
-        <v>142.4002947161137</v>
+        <v>184.5677286666146</v>
       </c>
       <c r="I60" t="n">
-        <v>33.44366772958512</v>
+        <v>73.42296351578348</v>
       </c>
       <c r="J60" t="n">
-        <v>44.57081588627711</v>
+        <v>82.87369440697557</v>
       </c>
       <c r="K60" t="n">
-        <v>-16.30978241841004</v>
+        <v>-3.419234108891089</v>
       </c>
       <c r="L60" t="n">
-        <v>259.0518270730972</v>
+        <v>404.4991073608398</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="B61" t="n">
-        <v>47.67621764358495</v>
+        <v>56.00019356269804</v>
       </c>
       <c r="C61" t="n">
-        <v>124.8894795741657</v>
+        <v>152.8505933518282</v>
       </c>
       <c r="D61" t="n">
-        <v>30.99926336910197</v>
+        <v>63.37105085965031</v>
       </c>
       <c r="E61" t="n">
-        <v>-3.689891207046159</v>
+        <v>-3.380496993918385</v>
       </c>
       <c r="F61" t="n">
-        <v>199.8750693798065</v>
+        <v>268.8413407802582</v>
       </c>
       <c r="G61" t="n">
-        <v>55.69940719029634</v>
+        <v>70.01733025438254</v>
       </c>
       <c r="H61" t="n">
-        <v>145.9064984682495</v>
+        <v>191.1098836169391</v>
       </c>
       <c r="I61" t="n">
-        <v>36.21597262397714</v>
+        <v>79.23315107187345</v>
       </c>
       <c r="J61" t="n">
-        <v>47.03664975972345</v>
+        <v>85.69813204886388</v>
       </c>
       <c r="K61" t="n">
-        <v>-16.70869591276795</v>
+        <v>1.918885667853147</v>
       </c>
       <c r="L61" t="n">
-        <v>268.1498321294785</v>
+        <v>427.9773826599121</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="B62" t="n">
-        <v>48.25555099846269</v>
+        <v>57.94533492154776</v>
       </c>
       <c r="C62" t="n">
-        <v>127.5832369732572</v>
+        <v>156.4104148620967</v>
       </c>
       <c r="D62" t="n">
-        <v>33.31034718308678</v>
+        <v>67.60975576902612</v>
       </c>
       <c r="E62" t="n">
-        <v>-3.929684442602642</v>
+        <v>-2.01313240565981</v>
       </c>
       <c r="F62" t="n">
-        <v>205.219450712204</v>
+        <v>279.9523731470108</v>
       </c>
       <c r="G62" t="n">
-        <v>56.69510274449478</v>
+        <v>73.3586644289912</v>
       </c>
       <c r="H62" t="n">
-        <v>149.8966352887459</v>
+        <v>198.015235438756</v>
       </c>
       <c r="I62" t="n">
-        <v>39.13608936016629</v>
+        <v>85.59379960959868</v>
       </c>
       <c r="J62" t="n">
-        <v>51.79409696649518</v>
+        <v>90.85487544283967</v>
       </c>
       <c r="K62" t="n">
-        <v>-19.36151335965039</v>
+        <v>6.091823273173759</v>
       </c>
       <c r="L62" t="n">
-        <v>278.1604110002518</v>
+        <v>453.9143981933594</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="B63" t="n">
-        <v>49.05924876730899</v>
+        <v>60.10538266207905</v>
       </c>
       <c r="C63" t="n">
-        <v>130.6881168659624</v>
+        <v>159.9985284350011</v>
       </c>
       <c r="D63" t="n">
-        <v>35.72943753948903</v>
+        <v>72.14891068456605</v>
       </c>
       <c r="E63" t="n">
-        <v>-4.249741185837195</v>
+        <v>-0.3499479079355297</v>
       </c>
       <c r="F63" t="n">
-        <v>211.2270619869232</v>
+        <v>291.9028738737106</v>
       </c>
       <c r="G63" t="n">
-        <v>57.96875442641294</v>
+        <v>77.11339268122182</v>
       </c>
       <c r="H63" t="n">
-        <v>154.4220008134642</v>
+        <v>205.2732851064607</v>
       </c>
       <c r="I63" t="n">
-        <v>42.21815544596463</v>
+        <v>92.56487580190534</v>
       </c>
       <c r="J63" t="n">
-        <v>52.27105579789969</v>
+        <v>30.77892531005693</v>
       </c>
       <c r="K63" t="n">
-        <v>-17.71440683427397</v>
+        <v>76.78746543629268</v>
       </c>
       <c r="L63" t="n">
-        <v>289.1655596494675</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>2012</v>
-      </c>
-      <c r="B64" t="n">
-        <v>50.1163403321729</v>
-      </c>
-      <c r="C64" t="n">
-        <v>134.2449047580234</v>
-      </c>
-      <c r="D64" t="n">
-        <v>38.26772383272469</v>
-      </c>
-      <c r="E64" t="n">
-        <v>-4.670570580788436</v>
-      </c>
-      <c r="F64" t="n">
-        <v>217.9583983421326</v>
-      </c>
-      <c r="G64" t="n">
-        <v>59.55839941089679</v>
-      </c>
-      <c r="H64" t="n">
-        <v>159.5370213280196</v>
-      </c>
-      <c r="I64" t="n">
-        <v>45.47747033141144</v>
-      </c>
-      <c r="J64" t="n">
-        <v>55.60557743227463</v>
-      </c>
-      <c r="K64" t="n">
-        <v>-18.92826656206598</v>
-      </c>
-      <c r="L64" t="n">
-        <v>301.2502019405365</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B65" t="n">
-        <v>51.45819434188304</v>
-      </c>
-      <c r="C65" t="n">
-        <v>138.2965679683175</v>
-      </c>
-      <c r="D65" t="n">
-        <v>40.93734633312958</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-5.216146481312315</v>
-      </c>
-      <c r="F65" t="n">
-        <v>225.4759621620178</v>
-      </c>
-      <c r="G65" t="n">
-        <v>61.50556918294664</v>
-      </c>
-      <c r="H65" t="n">
-        <v>165.2994093113018</v>
-      </c>
-      <c r="I65" t="n">
-        <v>48.93049239796567</v>
-      </c>
-      <c r="J65" t="n">
-        <v>58.44698626930573</v>
-      </c>
-      <c r="K65" t="n">
-        <v>-19.68025977668552</v>
-      </c>
-      <c r="L65" t="n">
-        <v>314.5021973848343</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B66" t="n">
-        <v>53.11872651526772</v>
-      </c>
-      <c r="C66" t="n">
-        <v>142.8883630176093</v>
-      </c>
-      <c r="D66" t="n">
-        <v>43.75138815837494</v>
-      </c>
-      <c r="E66" t="n">
-        <v>-5.914214614469721</v>
-      </c>
-      <c r="F66" t="n">
-        <v>233.8442630767822</v>
-      </c>
-      <c r="G66" t="n">
-        <v>63.85558497553357</v>
-      </c>
-      <c r="H66" t="n">
-        <v>171.7703078605112</v>
-      </c>
-      <c r="I66" t="n">
-        <v>52.59483175941089</v>
-      </c>
-      <c r="J66" t="n">
-        <v>60.37123775425429</v>
-      </c>
-      <c r="K66" t="n">
-        <v>-19.57962156563711</v>
-      </c>
-      <c r="L66" t="n">
-        <v>329.0123407840729</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B67" t="n">
-        <v>55.13459581075188</v>
-      </c>
-      <c r="C67" t="n">
-        <v>148.0679299506539</v>
-      </c>
-      <c r="D67" t="n">
-        <v>46.72386268460033</v>
-      </c>
-      <c r="E67" t="n">
-        <v>-6.796572629126871</v>
-      </c>
-      <c r="F67" t="n">
-        <v>243.1298158168793</v>
-      </c>
-      <c r="G67" t="n">
-        <v>66.65783263269665</v>
-      </c>
-      <c r="H67" t="n">
-        <v>179.0144127799302</v>
-      </c>
-      <c r="I67" t="n">
-        <v>56.48924006759153</v>
-      </c>
-      <c r="J67" t="n">
-        <v>63.23930339311442</v>
-      </c>
-      <c r="K67" t="n">
-        <v>-20.52642592777612</v>
-      </c>
-      <c r="L67" t="n">
-        <v>344.8743629455566</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>2016</v>
-      </c>
-      <c r="B68" t="n">
-        <v>57.5453925367602</v>
-      </c>
-      <c r="C68" t="n">
-        <v>153.8853770685802</v>
-      </c>
-      <c r="D68" t="n">
-        <v>49.86969790073072</v>
-      </c>
-      <c r="E68" t="n">
-        <v>-7.899325624128352</v>
-      </c>
-      <c r="F68" t="n">
-        <v>253.4011418819427</v>
-      </c>
-      <c r="G68" t="n">
-        <v>69.96601966877631</v>
-      </c>
-      <c r="H68" t="n">
-        <v>187.1000760284935</v>
-      </c>
-      <c r="I68" t="n">
-        <v>60.63359915339104</v>
-      </c>
-      <c r="J68" t="n">
-        <v>64.90295637812815</v>
-      </c>
-      <c r="K68" t="n">
-        <v>-20.41771172511932</v>
-      </c>
-      <c r="L68" t="n">
-        <v>362.1849395036697</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B69" t="n">
-        <v>60.39380575182461</v>
-      </c>
-      <c r="C69" t="n">
-        <v>160.393350830883</v>
-      </c>
-      <c r="D69" t="n">
-        <v>53.20471783040207</v>
-      </c>
-      <c r="E69" t="n">
-        <v>-9.263106779671581</v>
-      </c>
-      <c r="F69" t="n">
-        <v>264.7287676334381</v>
-      </c>
-      <c r="G69" t="n">
-        <v>73.83839763840827</v>
-      </c>
-      <c r="H69" t="n">
-        <v>196.0993825405622</v>
-      </c>
-      <c r="I69" t="n">
-        <v>65.04890795496605</v>
-      </c>
-      <c r="J69" t="n">
-        <v>70.09594646713768</v>
-      </c>
-      <c r="K69" t="n">
-        <v>-24.03894344277957</v>
-      </c>
-      <c r="L69" t="n">
-        <v>381.0436911582947</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B70" t="n">
-        <v>63.72576647907754</v>
-      </c>
-      <c r="C70" t="n">
-        <v>167.6470871312497</v>
-      </c>
-      <c r="D70" t="n">
-        <v>56.7456231732864</v>
-      </c>
-      <c r="E70" t="n">
-        <v>-10.93324867425387</v>
-      </c>
-      <c r="F70" t="n">
-        <v>277.1852281093597</v>
-      </c>
-      <c r="G70" t="n">
-        <v>78.33794430743886</v>
-      </c>
-      <c r="H70" t="n">
-        <v>206.0881947854493</v>
-      </c>
-      <c r="I70" t="n">
-        <v>69.75726952298511</v>
-      </c>
-      <c r="J70" t="n">
-        <v>72.34753371217349</v>
-      </c>
-      <c r="K70" t="n">
-        <v>-24.97776032216449</v>
-      </c>
-      <c r="L70" t="n">
-        <v>401.5531820058823</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B71" t="n">
-        <v>67.59055938167194</v>
-      </c>
-      <c r="C71" t="n">
-        <v>175.7044451656469</v>
-      </c>
-      <c r="D71" t="n">
-        <v>60.50997062655751</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-12.95991244117982</v>
-      </c>
-      <c r="F71" t="n">
-        <v>290.8450627326965</v>
-      </c>
-      <c r="G71" t="n">
-        <v>83.53249969231707</v>
-      </c>
-      <c r="H71" t="n">
-        <v>217.1461761229041</v>
-      </c>
-      <c r="I71" t="n">
-        <v>74.78188002858336</v>
-      </c>
-      <c r="J71" t="n">
-        <v>76.77952375327426</v>
-      </c>
-      <c r="K71" t="n">
-        <v>-28.42114706381466</v>
-      </c>
-      <c r="L71" t="n">
-        <v>423.8189325332642</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B72" t="n">
-        <v>72.04090080854958</v>
-      </c>
-      <c r="C72" t="n">
-        <v>184.6259214860905</v>
-      </c>
-      <c r="D72" t="n">
-        <v>64.51615328974488</v>
-      </c>
-      <c r="E72" t="n">
-        <v>-15.39815836560443</v>
-      </c>
-      <c r="F72" t="n">
-        <v>305.7848172187805</v>
-      </c>
-      <c r="G72" t="n">
-        <v>89.49484841248733</v>
-      </c>
-      <c r="H72" t="n">
-        <v>229.35677748289</v>
-      </c>
-      <c r="I72" t="n">
-        <v>80.14701779155557</v>
-      </c>
-      <c r="J72" t="n">
-        <v>18.10464973948521</v>
-      </c>
-      <c r="K72" t="n">
-        <v>30.84611915788671</v>
-      </c>
-      <c r="L72" t="n">
-        <v>447.9494125843048</v>
+        <v>482.5179443359375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add s-shaped curves for the future and add comet 1
</commit_message>
<xml_diff>
--- a/test_env/Dashboard.xlsx
+++ b/test_env/Dashboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,32 +466,62 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>deltaC_Structural_Ops</t>
+          <t>deltaC_Structural_Ops_x</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>deltaC_Engine_Ops</t>
+          <t>deltaC_Engine_Ops_x</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>deltaC_Aerodyn_Ops</t>
+          <t>deltaC_Aerodyn_Ops_x</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>deltaC_SLF_Ops</t>
+          <t>deltaC_SLF_Ops_x</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>deltaC_Res_Ops</t>
+          <t>deltaC_Res_Ops_x</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>deltaC_Tot_Ops</t>
+          <t>deltaC_Tot_Ops_x</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Structural_Ops_y</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Engine_Ops_y</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Aerodyn_Ops_y</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_SLF_Ops_y</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Res_Ops_y</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>deltaC_Tot_Ops_y</t>
         </is>
       </c>
     </row>
@@ -500,37 +530,55 @@
         <v>1959</v>
       </c>
       <c r="B2" t="n">
-        <v>3.287775717876018</v>
+        <v>3.285089589726697</v>
       </c>
       <c r="C2" t="n">
-        <v>9.786162772295205</v>
+        <v>7.917333575563769</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.29223141872433</v>
+        <v>-0.1515240078130952</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.711080156945702</v>
+        <v>-1.883540341807358</v>
       </c>
       <c r="F2" t="n">
-        <v>9.07062691450119</v>
+        <v>9.167358815670013</v>
       </c>
       <c r="G2" t="n">
-        <v>3.268379091711916</v>
+        <v>3.268607284596178</v>
       </c>
       <c r="H2" t="n">
-        <v>9.728428134301744</v>
+        <v>7.877609877244966</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.284607744879967</v>
+        <v>-0.1507637652494876</v>
       </c>
       <c r="J2" t="n">
-        <v>3.881585382408192</v>
+        <v>3.881856388353055</v>
       </c>
       <c r="K2" t="n">
-        <v>-7.499935681412978</v>
+        <v>-6.80400656228846</v>
       </c>
       <c r="L2" t="n">
-        <v>8.093849182128906</v>
+        <v>8.07330322265625</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3.268607284596178</v>
+      </c>
+      <c r="N2" t="n">
+        <v>7.877609877244966</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.1507637652494876</v>
+      </c>
+      <c r="P2" t="n">
+        <v>3.881856388353055</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-6.80400656228846</v>
+      </c>
+      <c r="R2" t="n">
+        <v>8.07330322265625</v>
       </c>
     </row>
     <row r="3">
@@ -538,37 +586,55 @@
         <v>1960</v>
       </c>
       <c r="B3" t="n">
-        <v>6.530406661456213</v>
+        <v>6.527665142616208</v>
       </c>
       <c r="C3" t="n">
-        <v>18.70883181645124</v>
+        <v>15.27822125418597</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.553181581318139</v>
+        <v>-0.2907253787696981</v>
       </c>
       <c r="E3" t="n">
-        <v>-4.846801086805379</v>
+        <v>-3.494333605427194</v>
       </c>
       <c r="F3" t="n">
-        <v>17.83925580978394</v>
+        <v>18.02082741260529</v>
       </c>
       <c r="G3" t="n">
-        <v>6.466233179737721</v>
+        <v>6.466614902938057</v>
       </c>
       <c r="H3" t="n">
-        <v>18.52498248840961</v>
+        <v>15.13533110142148</v>
       </c>
       <c r="I3" t="n">
-        <v>-2.528091788288898</v>
+        <v>-0.2880063584666288</v>
       </c>
       <c r="J3" t="n">
-        <v>1.824230879717734</v>
+        <v>1.82433857011958</v>
       </c>
       <c r="K3" t="n">
-        <v>-8.379235557916008</v>
+        <v>-7.253070086129674</v>
       </c>
       <c r="L3" t="n">
-        <v>15.90811920166016</v>
+        <v>15.88520812988281</v>
+      </c>
+      <c r="M3" t="n">
+        <v>6.466614902938057</v>
+      </c>
+      <c r="N3" t="n">
+        <v>15.13533110142148</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-0.2880063584666288</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.82433857011958</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-7.253070086129674</v>
+      </c>
+      <c r="R3" t="n">
+        <v>15.88520812988281</v>
       </c>
     </row>
     <row r="4">
@@ -576,37 +642,55 @@
         <v>1961</v>
       </c>
       <c r="B4" t="n">
-        <v>9.701232617198457</v>
+        <v>9.700115708522628</v>
       </c>
       <c r="C4" t="n">
-        <v>26.87535072580666</v>
+        <v>22.11945623784456</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.761301023962913</v>
+        <v>-0.4128944739495893</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.512522790882109</v>
+        <v>-4.848520803277733</v>
       </c>
       <c r="F4" t="n">
-        <v>26.3027595281601</v>
+        <v>26.55815666913986</v>
       </c>
       <c r="G4" t="n">
-        <v>9.574483258347476</v>
+        <v>9.575565174314939</v>
       </c>
       <c r="H4" t="n">
-        <v>26.52421663720102</v>
+        <v>21.83544002880217</v>
       </c>
       <c r="I4" t="n">
-        <v>-3.712158558047018</v>
+        <v>-0.4075928642732594</v>
       </c>
       <c r="J4" t="n">
-        <v>-5.805430925972427</v>
+        <v>-5.806086921853121</v>
       </c>
       <c r="K4" t="n">
-        <v>-3.103212767486079</v>
+        <v>-1.729864784666508</v>
       </c>
       <c r="L4" t="n">
-        <v>23.47789764404297</v>
+        <v>23.46746063232422</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9.575565174314939</v>
+      </c>
+      <c r="N4" t="n">
+        <v>21.83544002880217</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.4075928642732594</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-5.806086921853121</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1.729864784666508</v>
+      </c>
+      <c r="R4" t="n">
+        <v>23.46746063232422</v>
       </c>
     </row>
     <row r="5">
@@ -614,37 +698,55 @@
         <v>1962</v>
       </c>
       <c r="B5" t="n">
-        <v>12.77970038436918</v>
+        <v>12.78120558623636</v>
       </c>
       <c r="C5" t="n">
-        <v>34.36376826569427</v>
+        <v>28.47129925499688</v>
       </c>
       <c r="D5" t="n">
-        <v>-4.898700532087598</v>
+        <v>-0.5136931372627452</v>
       </c>
       <c r="E5" t="n">
-        <v>-7.786007439207694</v>
+        <v>-5.960994335463104</v>
       </c>
       <c r="F5" t="n">
-        <v>34.45876067876816</v>
+        <v>34.77781736850739</v>
       </c>
       <c r="G5" t="n">
-        <v>12.58013834999703</v>
+        <v>12.58277725562216</v>
       </c>
       <c r="H5" t="n">
-        <v>33.8271591670817</v>
+        <v>28.02928208036742</v>
       </c>
       <c r="I5" t="n">
-        <v>-4.822204635113438</v>
+        <v>-0.5057180467294402</v>
       </c>
       <c r="J5" t="n">
-        <v>-9.471529693604062</v>
+        <v>-9.473516492020927</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.279651292609282</v>
+        <v>0.2149077467061016</v>
       </c>
       <c r="L5" t="n">
-        <v>30.83391189575195</v>
+        <v>30.84773254394531</v>
+      </c>
+      <c r="M5" t="n">
+        <v>12.58277725562216</v>
+      </c>
+      <c r="N5" t="n">
+        <v>28.02928208036742</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-0.5057180467294402</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-9.473516492020927</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.2149077467061016</v>
+      </c>
+      <c r="R5" t="n">
+        <v>30.84773254394531</v>
       </c>
     </row>
     <row r="6">
@@ -652,37 +754,55 @@
         <v>1963</v>
       </c>
       <c r="B6" t="n">
-        <v>15.7499354102431</v>
+        <v>15.75457001144973</v>
       </c>
       <c r="C6" t="n">
-        <v>41.23390560325821</v>
+        <v>34.35976712425025</v>
       </c>
       <c r="D6" t="n">
-        <v>-5.950719837917978</v>
+        <v>-0.589114392502195</v>
       </c>
       <c r="E6" t="n">
-        <v>-8.727488107498619</v>
+        <v>-6.846222305938113</v>
       </c>
       <c r="F6" t="n">
-        <v>42.30563306808472</v>
+        <v>42.67900043725967</v>
       </c>
       <c r="G6" t="n">
-        <v>15.47452387356712</v>
+        <v>15.4796783129725</v>
       </c>
       <c r="H6" t="n">
-        <v>40.51286815075157</v>
+        <v>33.76024490706483</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.846662465478001</v>
+        <v>-0.5788353016838091</v>
       </c>
       <c r="J6" t="n">
-        <v>-9.41995883779421</v>
+        <v>-9.423096532565259</v>
       </c>
       <c r="K6" t="n">
-        <v>-2.717928771583583</v>
+        <v>-1.188041739792167</v>
       </c>
       <c r="L6" t="n">
-        <v>38.00284194946289</v>
+        <v>38.04994964599609</v>
+      </c>
+      <c r="M6" t="n">
+        <v>15.4796783129725</v>
+      </c>
+      <c r="N6" t="n">
+        <v>33.76024490706483</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-0.5788353016838091</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-9.423096532565259</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1.188041739792167</v>
+      </c>
+      <c r="R6" t="n">
+        <v>38.04994964599609</v>
       </c>
     </row>
     <row r="7">
@@ -690,37 +810,55 @@
         <v>1964</v>
       </c>
       <c r="B7" t="n">
-        <v>18.5997301928843</v>
+        <v>18.60765189109595</v>
       </c>
       <c r="C7" t="n">
-        <v>47.53376641035477</v>
+        <v>39.80805953410769</v>
       </c>
       <c r="D7" t="n">
-        <v>-6.905583369059036</v>
+        <v>-0.6354564433106036</v>
       </c>
       <c r="E7" t="n">
-        <v>-9.385411474650912</v>
+        <v>-7.518637559789163</v>
       </c>
       <c r="F7" t="n">
-        <v>49.84250175952911</v>
+        <v>50.26161742210388</v>
       </c>
       <c r="G7" t="n">
-        <v>18.25203096223686</v>
+        <v>18.26062739650845</v>
       </c>
       <c r="H7" t="n">
-        <v>46.64518072447325</v>
+        <v>39.06565679456893</v>
       </c>
       <c r="I7" t="n">
-        <v>-6.776491925274968</v>
+        <v>-0.6236054611252716</v>
       </c>
       <c r="J7" t="n">
-        <v>-4.848951698943281</v>
+        <v>-4.851235475057074</v>
       </c>
       <c r="K7" t="n">
-        <v>-8.264329402823893</v>
+        <v>-6.756995165295422</v>
       </c>
       <c r="L7" t="n">
-        <v>45.00743865966797</v>
+        <v>45.09444808959961</v>
+      </c>
+      <c r="M7" t="n">
+        <v>18.26062739650845</v>
+      </c>
+      <c r="N7" t="n">
+        <v>39.06565679456893</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-0.6236054611252716</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-4.851235475057074</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-6.756995165295422</v>
+      </c>
+      <c r="R7" t="n">
+        <v>45.09444808959961</v>
       </c>
     </row>
     <row r="8">
@@ -728,37 +866,55 @@
         <v>1965</v>
       </c>
       <c r="B8" t="n">
-        <v>21.31980888105314</v>
+        <v>21.33093031941356</v>
       </c>
       <c r="C8" t="n">
-        <v>53.30345069934519</v>
+        <v>44.83747991657093</v>
       </c>
       <c r="D8" t="n">
-        <v>-7.75411014039513</v>
+        <v>-0.6493055392363891</v>
       </c>
       <c r="E8" t="n">
-        <v>-9.799907320214082</v>
+        <v>-7.992804862496705</v>
       </c>
       <c r="F8" t="n">
-        <v>57.06924211978912</v>
+        <v>57.5262998342514</v>
       </c>
       <c r="G8" t="n">
-        <v>20.90924317868946</v>
+        <v>20.92208559628607</v>
       </c>
       <c r="H8" t="n">
-        <v>52.27696079050585</v>
+        <v>43.97809090785335</v>
       </c>
       <c r="I8" t="n">
-        <v>-7.604785552461046</v>
+        <v>-0.6368604588090885</v>
       </c>
       <c r="J8" t="n">
-        <v>-4.864077674873918</v>
+        <v>-4.867065177023756</v>
       </c>
       <c r="K8" t="n">
-        <v>-8.85037449430175</v>
+        <v>-7.397963667378841</v>
       </c>
       <c r="L8" t="n">
-        <v>51.86696624755859</v>
+        <v>51.99828720092773</v>
+      </c>
+      <c r="M8" t="n">
+        <v>20.92208559628607</v>
+      </c>
+      <c r="N8" t="n">
+        <v>43.97809090785335</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-0.6368604588090885</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-4.867065177023756</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-7.397963667378841</v>
+      </c>
+      <c r="R8" t="n">
+        <v>51.99828720092773</v>
       </c>
     </row>
     <row r="9">
@@ -766,37 +922,55 @@
         <v>1966</v>
       </c>
       <c r="B9" t="n">
-        <v>23.90328056158642</v>
+        <v>23.9173478862259</v>
       </c>
       <c r="C9" t="n">
-        <v>58.57763885641797</v>
+        <v>49.46805008299789</v>
       </c>
       <c r="D9" t="n">
-        <v>-8.489456348967874</v>
+        <v>-0.6275245697092844</v>
       </c>
       <c r="E9" t="n">
-        <v>-10.00498235614589</v>
+        <v>-8.283473415631612</v>
       </c>
       <c r="F9" t="n">
-        <v>63.98648071289062</v>
+        <v>64.4743999838829</v>
       </c>
       <c r="G9" t="n">
-        <v>23.44429346452527</v>
+        <v>23.46200814081557</v>
       </c>
       <c r="H9" t="n">
-        <v>57.45284009324688</v>
+        <v>48.52627470564889</v>
       </c>
       <c r="I9" t="n">
-        <v>-8.326443120921592</v>
+        <v>-0.6155777234632293</v>
       </c>
       <c r="J9" t="n">
-        <v>-1.150778178179403</v>
+        <v>-1.151647712963453</v>
       </c>
       <c r="K9" t="n">
-        <v>-12.82261077551686</v>
+        <v>-11.44570493201044</v>
       </c>
       <c r="L9" t="n">
-        <v>58.5973014831543</v>
+        <v>58.77535247802734</v>
+      </c>
+      <c r="M9" t="n">
+        <v>23.46200814081557</v>
+      </c>
+      <c r="N9" t="n">
+        <v>48.52627470564889</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-0.6155777234632293</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-1.151647712963453</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-11.44570493201044</v>
+      </c>
+      <c r="R9" t="n">
+        <v>58.77535247802734</v>
       </c>
     </row>
     <row r="10">
@@ -804,37 +978,55 @@
         <v>1967</v>
       </c>
       <c r="B10" t="n">
-        <v>26.34522486175173</v>
+        <v>26.36187690686668</v>
       </c>
       <c r="C10" t="n">
-        <v>63.38723034862433</v>
+        <v>53.71893211224084</v>
       </c>
       <c r="D10" t="n">
-        <v>-9.106878348521736</v>
+        <v>-0.5672451271150242</v>
       </c>
       <c r="E10" t="n">
-        <v>-10.02998132323815</v>
+        <v>-8.405574163541715</v>
       </c>
       <c r="F10" t="n">
-        <v>70.59559553861618</v>
+        <v>71.10798972845078</v>
       </c>
       <c r="G10" t="n">
-        <v>25.85641107825495</v>
+        <v>25.87943278348967</v>
       </c>
       <c r="H10" t="n">
-        <v>62.21113289435372</v>
+        <v>52.73583128056641</v>
       </c>
       <c r="I10" t="n">
-        <v>-8.937907778532463</v>
+        <v>-0.5568640727212982</v>
       </c>
       <c r="J10" t="n">
-        <v>-2.704144401693035</v>
+        <v>-2.706552080547493</v>
       </c>
       <c r="K10" t="n">
-        <v>-11.2142529312992</v>
+        <v>-9.915007853414238</v>
       </c>
       <c r="L10" t="n">
-        <v>65.21123886108398</v>
+        <v>65.43684005737305</v>
+      </c>
+      <c r="M10" t="n">
+        <v>25.87943278348967</v>
+      </c>
+      <c r="N10" t="n">
+        <v>52.73583128056641</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-0.5568640727212982</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-2.706552080547493</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-9.915007853414238</v>
+      </c>
+      <c r="R10" t="n">
+        <v>65.43684005737305</v>
       </c>
     </row>
     <row r="11">
@@ -842,37 +1034,55 @@
         <v>1968</v>
       </c>
       <c r="B11" t="n">
-        <v>28.6423718859642</v>
+        <v>28.66118522427448</v>
       </c>
       <c r="C11" t="n">
-        <v>67.76045412170247</v>
+        <v>57.60871884509036</v>
       </c>
       <c r="D11" t="n">
-        <v>-9.603510695911197</v>
+        <v>-0.4658616566786193</v>
       </c>
       <c r="E11" t="n">
-        <v>-9.900600530947969</v>
+        <v>-8.374180390286323</v>
       </c>
       <c r="F11" t="n">
-        <v>76.8987147808075</v>
+        <v>77.4298620223999</v>
       </c>
       <c r="G11" t="n">
-        <v>28.14558690183997</v>
+        <v>28.17413997763602</v>
       </c>
       <c r="H11" t="n">
-        <v>66.58518915904075</v>
+        <v>56.62976237630243</v>
       </c>
       <c r="I11" t="n">
-        <v>-9.436943488153414</v>
+        <v>-0.4579451764737369</v>
       </c>
       <c r="J11" t="n">
-        <v>-11.09546896465161</v>
+        <v>-11.1067250726676</v>
       </c>
       <c r="K11" t="n">
-        <v>-2.479708975507327</v>
+        <v>-1.248127978820547</v>
       </c>
       <c r="L11" t="n">
-        <v>71.71865463256836</v>
+        <v>71.99110412597656</v>
+      </c>
+      <c r="M11" t="n">
+        <v>28.17413997763602</v>
+      </c>
+      <c r="N11" t="n">
+        <v>56.62976237630243</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-0.4579451764737369</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-11.1067250726676</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-1.248127978820547</v>
+      </c>
+      <c r="R11" t="n">
+        <v>71.99110412597656</v>
       </c>
     </row>
     <row r="12">
@@ -880,37 +1090,55 @@
         <v>1969</v>
       </c>
       <c r="B12" t="n">
-        <v>30.79285094055618</v>
+        <v>30.81337381365908</v>
       </c>
       <c r="C12" t="n">
-        <v>71.72363405344993</v>
+        <v>61.15563855919169</v>
       </c>
       <c r="D12" t="n">
-        <v>-9.978154986526937</v>
+        <v>-0.3210266219853034</v>
       </c>
       <c r="E12" t="n">
-        <v>-9.639612067625507</v>
+        <v>-8.204456741046446</v>
       </c>
       <c r="F12" t="n">
-        <v>82.89871793985367</v>
+        <v>83.44352900981903</v>
       </c>
       <c r="G12" t="n">
-        <v>30.31235022635374</v>
+        <v>30.34646838321208</v>
       </c>
       <c r="H12" t="n">
-        <v>70.60443734592823</v>
+        <v>60.22896626688065</v>
       </c>
       <c r="I12" t="n">
-        <v>-9.822452917669969</v>
+        <v>-0.3161622058382942</v>
       </c>
       <c r="J12" t="n">
-        <v>-15.00504323302865</v>
+        <v>-15.02193218941645</v>
       </c>
       <c r="K12" t="n">
-        <v>2.037577780076798</v>
+        <v>3.20697279447843</v>
       </c>
       <c r="L12" t="n">
-        <v>78.12686920166016</v>
+        <v>78.44431304931641</v>
+      </c>
+      <c r="M12" t="n">
+        <v>30.34646838321208</v>
+      </c>
+      <c r="N12" t="n">
+        <v>60.22896626688065</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-0.3161622058382942</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-15.02193218941645</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>3.20697279447843</v>
+      </c>
+      <c r="R12" t="n">
+        <v>78.44431304931641</v>
       </c>
     </row>
     <row r="13">
@@ -918,37 +1146,55 @@
         <v>1970</v>
       </c>
       <c r="B13" t="n">
-        <v>32.79599045058048</v>
+        <v>32.81776820229656</v>
       </c>
       <c r="C13" t="n">
-        <v>75.30172754410268</v>
+        <v>64.37769946729797</v>
       </c>
       <c r="D13" t="n">
-        <v>-10.23107750683918</v>
+        <v>-0.1306460758431862</v>
       </c>
       <c r="E13" t="n">
-        <v>-9.267405251199236</v>
+        <v>-7.911596827496915</v>
       </c>
       <c r="F13" t="n">
-        <v>88.59923523664474</v>
+        <v>89.15322476625443</v>
       </c>
       <c r="G13" t="n">
-        <v>32.35760411355236</v>
+        <v>32.39712616181473</v>
       </c>
       <c r="H13" t="n">
-        <v>74.29516399604661</v>
+        <v>63.55253772264421</v>
       </c>
       <c r="I13" t="n">
-        <v>-10.09431796610103</v>
+        <v>-0.1289715185855182</v>
       </c>
       <c r="J13" t="n">
-        <v>-8.12051075134662</v>
+        <v>-8.130429253557205</v>
       </c>
       <c r="K13" t="n">
-        <v>-3.997086273254832</v>
+        <v>-2.889985402355284</v>
       </c>
       <c r="L13" t="n">
-        <v>84.44085311889648</v>
+        <v>84.80027770996094</v>
+      </c>
+      <c r="M13" t="n">
+        <v>32.39712616181473</v>
+      </c>
+      <c r="N13" t="n">
+        <v>63.55253772264421</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-0.1289715185855182</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-8.130429253557205</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-2.889985402355284</v>
+      </c>
+      <c r="R13" t="n">
+        <v>84.80027770996094</v>
       </c>
     </row>
     <row r="14">
@@ -956,37 +1202,55 @@
         <v>1971</v>
       </c>
       <c r="B14" t="n">
-        <v>34.65215557271623</v>
+        <v>34.6747493852001</v>
       </c>
       <c r="C14" t="n">
-        <v>78.51871050458566</v>
+        <v>67.29278654184215</v>
       </c>
       <c r="D14" t="n">
-        <v>-10.36381565401408</v>
+        <v>0.1071249848437823</v>
       </c>
       <c r="E14" t="n">
-        <v>-8.802402393483575</v>
+        <v>-7.510759189454845</v>
       </c>
       <c r="F14" t="n">
-        <v>94.00464802980423</v>
+        <v>94.56390172243118</v>
       </c>
       <c r="G14" t="n">
-        <v>34.28250646856244</v>
+        <v>34.32712583492241</v>
       </c>
       <c r="H14" t="n">
-        <v>77.68111842647022</v>
+        <v>66.61815852634052</v>
       </c>
       <c r="I14" t="n">
-        <v>-10.25326047761006</v>
+        <v>0.1060510284860549</v>
       </c>
       <c r="J14" t="n">
-        <v>-10.20713390738528</v>
+        <v>-10.22041868662738</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.8398508408478751</v>
+        <v>0.2301794882846444</v>
       </c>
       <c r="L14" t="n">
-        <v>90.66337966918945</v>
+        <v>91.06109619140625</v>
+      </c>
+      <c r="M14" t="n">
+        <v>34.32712583492241</v>
+      </c>
+      <c r="N14" t="n">
+        <v>66.61815852634052</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.1060510284860549</v>
+      </c>
+      <c r="P14" t="n">
+        <v>-10.22041868662738</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.2301794882846444</v>
+      </c>
+      <c r="R14" t="n">
+        <v>91.06109619140625</v>
       </c>
     </row>
     <row r="15">
@@ -994,37 +1258,55 @@
         <v>1972</v>
       </c>
       <c r="B15" t="n">
-        <v>36.3626154266025</v>
+        <v>36.3856160611831</v>
       </c>
       <c r="C15" t="n">
-        <v>81.39784891148379</v>
+        <v>69.9187280404974</v>
       </c>
       <c r="D15" t="n">
-        <v>-10.37899366083637</v>
+        <v>0.3938879173339767</v>
       </c>
       <c r="E15" t="n">
-        <v>-8.261381921165473</v>
+        <v>-7.016997659273258</v>
       </c>
       <c r="F15" t="n">
-        <v>99.12008875608444</v>
+        <v>99.68123435974121</v>
       </c>
       <c r="G15" t="n">
-        <v>36.08841008996086</v>
+        <v>36.13767956899571</v>
       </c>
       <c r="H15" t="n">
-        <v>80.78403925283232</v>
+        <v>69.44229240341997</v>
       </c>
       <c r="I15" t="n">
-        <v>-10.30072713854741</v>
+        <v>0.391203911973876</v>
       </c>
       <c r="J15" t="n">
-        <v>-2.705326252567289</v>
+        <v>-2.709019677828298</v>
       </c>
       <c r="K15" t="n">
-        <v>-7.071023942401141</v>
+        <v>-6.035174089862043</v>
       </c>
       <c r="L15" t="n">
-        <v>96.79537200927734</v>
+        <v>97.22698211669922</v>
+      </c>
+      <c r="M15" t="n">
+        <v>36.13767956899571</v>
+      </c>
+      <c r="N15" t="n">
+        <v>69.44229240341997</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.391203911973876</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-2.709019677828298</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-6.035174089862043</v>
+      </c>
+      <c r="R15" t="n">
+        <v>97.22698211669922</v>
       </c>
     </row>
     <row r="16">
@@ -1032,37 +1314,55 @@
         <v>1973</v>
       </c>
       <c r="B16" t="n">
-        <v>37.92943213781416</v>
+        <v>37.95246917470779</v>
       </c>
       <c r="C16" t="n">
-        <v>83.96189282841624</v>
+        <v>72.27333596157473</v>
       </c>
       <c r="D16" t="n">
-        <v>-10.28014687447044</v>
+        <v>0.7310064961529686</v>
       </c>
       <c r="E16" t="n">
-        <v>-7.659738115067753</v>
+        <v>-6.445195760052371</v>
       </c>
       <c r="F16" t="n">
-        <v>103.9514399766922</v>
+        <v>104.5116158723831</v>
       </c>
       <c r="G16" t="n">
-        <v>37.77682290969266</v>
+        <v>37.83019332237346</v>
       </c>
       <c r="H16" t="n">
-        <v>83.62407180305505</v>
+        <v>72.04048460966227</v>
       </c>
       <c r="I16" t="n">
-        <v>-10.23878466072075</v>
+        <v>0.728651328114558</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.439771096366358</v>
+        <v>-1.44180517774439</v>
       </c>
       <c r="K16" t="n">
-        <v>-6.886191647310986</v>
+        <v>-5.860694858773082</v>
       </c>
       <c r="L16" t="n">
-        <v>102.8361473083496</v>
+        <v>103.2968292236328</v>
+      </c>
+      <c r="M16" t="n">
+        <v>37.83019332237346</v>
+      </c>
+      <c r="N16" t="n">
+        <v>72.04048460966227</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.728651328114558</v>
+      </c>
+      <c r="P16" t="n">
+        <v>-1.44180517774439</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-5.860694858773082</v>
+      </c>
+      <c r="R16" t="n">
+        <v>103.2968292236328</v>
       </c>
     </row>
     <row r="17">
@@ -1070,37 +1370,55 @@
         <v>1974</v>
       </c>
       <c r="B17" t="n">
-        <v>39.3553676988036</v>
+        <v>39.37811591648713</v>
       </c>
       <c r="C17" t="n">
-        <v>86.23320884275344</v>
+        <v>74.37442665739427</v>
       </c>
       <c r="D17" t="n">
-        <v>-10.07155601962034</v>
+        <v>1.119614283418739</v>
       </c>
       <c r="E17" t="n">
-        <v>-7.011684058485308</v>
+        <v>-5.809995054054589</v>
       </c>
       <c r="F17" t="n">
-        <v>108.5053364634514</v>
+        <v>109.0621618032455</v>
       </c>
       <c r="G17" t="n">
-        <v>39.34939158179957</v>
+        <v>39.40622500318553</v>
       </c>
       <c r="H17" t="n">
-        <v>86.22011432030808</v>
+        <v>74.42751698836619</v>
       </c>
       <c r="I17" t="n">
-        <v>-10.07002665270789</v>
+        <v>1.120413492172864</v>
       </c>
       <c r="J17" t="n">
-        <v>2.590839508003053</v>
+        <v>2.594581529609554</v>
       </c>
       <c r="K17" t="n">
-        <v>-9.306646424639137</v>
+        <v>-8.280537092679841</v>
       </c>
       <c r="L17" t="n">
-        <v>108.7836723327637</v>
+        <v>109.2681999206543</v>
+      </c>
+      <c r="M17" t="n">
+        <v>39.40622500318553</v>
+      </c>
+      <c r="N17" t="n">
+        <v>74.42751698836619</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1.120413492172864</v>
+      </c>
+      <c r="P17" t="n">
+        <v>2.594581529609554</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>-8.280537092679841</v>
+      </c>
+      <c r="R17" t="n">
+        <v>109.2681999206543</v>
       </c>
     </row>
     <row r="18">
@@ -1108,37 +1426,55 @@
         <v>1975</v>
       </c>
       <c r="B18" t="n">
-        <v>40.64380373658872</v>
+        <v>40.66598646208161</v>
       </c>
       <c r="C18" t="n">
-        <v>88.23387128081097</v>
+        <v>76.23982484094809</v>
       </c>
       <c r="D18" t="n">
-        <v>-9.758092927895738</v>
+        <v>1.560623083942938</v>
       </c>
       <c r="E18" t="n">
-        <v>-6.330419453700728</v>
+        <v>-5.125729171041698</v>
       </c>
       <c r="F18" t="n">
-        <v>112.7891626358032</v>
+        <v>113.3407052159309</v>
       </c>
       <c r="G18" t="n">
-        <v>40.80789114757954</v>
+        <v>40.86750459450587</v>
       </c>
       <c r="H18" t="n">
-        <v>88.59008960117285</v>
+        <v>76.61762723687978</v>
       </c>
       <c r="I18" t="n">
-        <v>-9.797488359856867</v>
+        <v>1.568356668608039</v>
       </c>
       <c r="J18" t="n">
-        <v>2.33069353240279</v>
+        <v>2.3340982807496</v>
       </c>
       <c r="K18" t="n">
-        <v>-7.296458443270964</v>
+        <v>-6.249811359600706</v>
       </c>
       <c r="L18" t="n">
-        <v>114.6347274780273</v>
+        <v>115.1377754211426</v>
+      </c>
+      <c r="M18" t="n">
+        <v>40.86750459450587</v>
+      </c>
+      <c r="N18" t="n">
+        <v>76.61762723687978</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.568356668608039</v>
+      </c>
+      <c r="P18" t="n">
+        <v>2.3340982807496</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-6.249811359600706</v>
+      </c>
+      <c r="R18" t="n">
+        <v>115.1377754211426</v>
       </c>
     </row>
     <row r="19">
@@ -1146,37 +1482,55 @@
         <v>1976</v>
       </c>
       <c r="B19" t="n">
-        <v>41.79867314540072</v>
+        <v>41.82006369806206</v>
       </c>
       <c r="C19" t="n">
-        <v>89.98571335156966</v>
+        <v>77.88735795456604</v>
       </c>
       <c r="D19" t="n">
-        <v>-9.345075457364823</v>
+        <v>2.054732986683434</v>
       </c>
       <c r="E19" t="n">
-        <v>-5.628255915799549</v>
+        <v>-4.406352341719376</v>
       </c>
       <c r="F19" t="n">
-        <v>116.811055123806</v>
+        <v>117.3558022975922</v>
       </c>
       <c r="G19" t="n">
-        <v>42.15423301085286</v>
+        <v>42.21592290370524</v>
       </c>
       <c r="H19" t="n">
-        <v>90.75117564317399</v>
+        <v>78.62462195952186</v>
       </c>
       <c r="I19" t="n">
-        <v>-9.424569219300814</v>
+        <v>2.074182621523541</v>
       </c>
       <c r="J19" t="n">
-        <v>4.870918216642175</v>
+        <v>4.878046471233227</v>
       </c>
       <c r="K19" t="n">
-        <v>-7.966625815430711</v>
+        <v>-6.891376250905751</v>
       </c>
       <c r="L19" t="n">
-        <v>120.3851318359375</v>
+        <v>120.9013977050781</v>
+      </c>
+      <c r="M19" t="n">
+        <v>42.21592290370524</v>
+      </c>
+      <c r="N19" t="n">
+        <v>78.62462195952186</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2.074182621523541</v>
+      </c>
+      <c r="P19" t="n">
+        <v>4.878046471233227</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-6.891376250905751</v>
+      </c>
+      <c r="R19" t="n">
+        <v>120.9013977050781</v>
       </c>
     </row>
     <row r="20">
@@ -1184,37 +1538,55 @@
         <v>1977</v>
       </c>
       <c r="B20" t="n">
-        <v>42.82439902002932</v>
+        <v>42.84482031128956</v>
       </c>
       <c r="C20" t="n">
-        <v>91.51035611139656</v>
+        <v>79.33483567952138</v>
       </c>
       <c r="D20" t="n">
-        <v>-8.838134815904917</v>
+        <v>2.602443888905089</v>
       </c>
       <c r="E20" t="n">
-        <v>-4.91672028919956</v>
+        <v>-3.665372765992267</v>
       </c>
       <c r="F20" t="n">
-        <v>120.5799000263214</v>
+        <v>121.1167271137238</v>
       </c>
       <c r="G20" t="n">
-        <v>43.39050992500383</v>
+        <v>43.45356893499627</v>
       </c>
       <c r="H20" t="n">
-        <v>92.72006393446566</v>
+        <v>80.4620424616019</v>
       </c>
       <c r="I20" t="n">
-        <v>-8.954969251726855</v>
+        <v>2.639419983661343</v>
       </c>
       <c r="J20" t="n">
-        <v>6.536811392335045</v>
+        <v>6.546311277347238</v>
       </c>
       <c r="K20" t="n">
-        <v>-7.662180709550332</v>
+        <v>-6.546842077772761</v>
       </c>
       <c r="L20" t="n">
-        <v>126.0302352905273</v>
+        <v>126.554500579834</v>
+      </c>
+      <c r="M20" t="n">
+        <v>43.45356893499627</v>
+      </c>
+      <c r="N20" t="n">
+        <v>80.4620424616019</v>
+      </c>
+      <c r="O20" t="n">
+        <v>2.639419983661343</v>
+      </c>
+      <c r="P20" t="n">
+        <v>6.546311277347238</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-6.546842077772761</v>
+      </c>
+      <c r="R20" t="n">
+        <v>126.554500579834</v>
       </c>
     </row>
     <row r="21">
@@ -1222,37 +1594,55 @@
         <v>1978</v>
       </c>
       <c r="B21" t="n">
-        <v>43.72584141117991</v>
+        <v>43.74516469305438</v>
       </c>
       <c r="C21" t="n">
-        <v>92.82921174212258</v>
+        <v>80.60002339414352</v>
       </c>
       <c r="D21" t="n">
-        <v>-8.243093719922783</v>
+        <v>3.204068572933717</v>
       </c>
       <c r="E21" t="n">
-        <v>-4.206623899760764</v>
+        <v>-2.91578082003992</v>
       </c>
       <c r="F21" t="n">
-        <v>124.1053355336189</v>
+        <v>124.6334758400917</v>
       </c>
       <c r="G21" t="n">
-        <v>44.51898747030223</v>
+        <v>44.58272495099982</v>
       </c>
       <c r="H21" t="n">
-        <v>94.51304722906809</v>
+        <v>82.14321969613675</v>
       </c>
       <c r="I21" t="n">
-        <v>-8.392615766564544</v>
+        <v>3.265414793007436</v>
       </c>
       <c r="J21" t="n">
-        <v>15.81244382095472</v>
+        <v>15.83508237115742</v>
       </c>
       <c r="K21" t="n">
-        <v>-14.88699382675854</v>
+        <v>-13.73433976052018</v>
       </c>
       <c r="L21" t="n">
-        <v>131.564868927002</v>
+        <v>132.0921020507812</v>
+      </c>
+      <c r="M21" t="n">
+        <v>44.58272495099982</v>
+      </c>
+      <c r="N21" t="n">
+        <v>82.14321969613675</v>
+      </c>
+      <c r="O21" t="n">
+        <v>3.265414793007436</v>
+      </c>
+      <c r="P21" t="n">
+        <v>15.83508237115742</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-13.73433976052018</v>
+      </c>
+      <c r="R21" t="n">
+        <v>132.0921020507812</v>
       </c>
     </row>
     <row r="22">
@@ -1260,37 +1650,55 @@
         <v>1979</v>
       </c>
       <c r="B22" t="n">
-        <v>44.50824951378353</v>
+        <v>44.52639147266762</v>
       </c>
       <c r="C22" t="n">
-        <v>93.96346889096168</v>
+        <v>81.70060840990136</v>
       </c>
       <c r="D22" t="n">
-        <v>-7.565855728136039</v>
+        <v>3.859747490002989</v>
       </c>
       <c r="E22" t="n">
-        <v>-3.508112120140211</v>
+        <v>-2.169983530466105</v>
       </c>
       <c r="F22" t="n">
-        <v>127.397750556469</v>
+        <v>127.9167638421059</v>
       </c>
       <c r="G22" t="n">
-        <v>45.54214815887436</v>
+        <v>45.60591598733066</v>
       </c>
       <c r="H22" t="n">
-        <v>96.1461811799344</v>
+        <v>83.68140691443578</v>
       </c>
       <c r="I22" t="n">
-        <v>-7.741605798555009</v>
+        <v>3.953325520875423</v>
       </c>
       <c r="J22" t="n">
-        <v>19.47768039525441</v>
+        <v>19.50495290602528</v>
       </c>
       <c r="K22" t="n">
-        <v>-16.44065454585972</v>
+        <v>-15.2363277996144</v>
       </c>
       <c r="L22" t="n">
-        <v>136.9837493896484</v>
+        <v>137.5092735290527</v>
+      </c>
+      <c r="M22" t="n">
+        <v>45.60591598733066</v>
+      </c>
+      <c r="N22" t="n">
+        <v>83.68140691443578</v>
+      </c>
+      <c r="O22" t="n">
+        <v>3.953325520875423</v>
+      </c>
+      <c r="P22" t="n">
+        <v>19.50495290602528</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-15.2363277996144</v>
+      </c>
+      <c r="R22" t="n">
+        <v>137.5092735290527</v>
       </c>
     </row>
     <row r="23">
@@ -1298,37 +1706,55 @@
         <v>1980</v>
       </c>
       <c r="B23" t="n">
-        <v>45.17721810844344</v>
+        <v>45.19413762102163</v>
       </c>
       <c r="C23" t="n">
-        <v>94.93406744126439</v>
+        <v>82.65415930531636</v>
       </c>
       <c r="D23" t="n">
-        <v>-6.812305806546762</v>
+        <v>4.569465115906025</v>
       </c>
       <c r="E23" t="n">
-        <v>-2.830695255436765</v>
+        <v>-1.439734281261501</v>
       </c>
       <c r="F23" t="n">
-        <v>130.4682844877243</v>
+        <v>130.9780277609825</v>
       </c>
       <c r="G23" t="n">
-        <v>46.46272063681739</v>
+        <v>46.52592551370476</v>
       </c>
       <c r="H23" t="n">
-        <v>97.6353843623645</v>
+        <v>85.08982495659589</v>
       </c>
       <c r="I23" t="n">
-        <v>-7.006147674307445</v>
+        <v>4.704118826270682</v>
       </c>
       <c r="J23" t="n">
-        <v>12.90550033846501</v>
+        <v>12.92305612663846</v>
       </c>
       <c r="K23" t="n">
-        <v>-7.715719382089457</v>
+        <v>-6.441636818473446</v>
       </c>
       <c r="L23" t="n">
-        <v>142.28173828125</v>
+        <v>142.8012886047363</v>
+      </c>
+      <c r="M23" t="n">
+        <v>46.52592551370476</v>
+      </c>
+      <c r="N23" t="n">
+        <v>85.08982495659589</v>
+      </c>
+      <c r="O23" t="n">
+        <v>4.704118826270682</v>
+      </c>
+      <c r="P23" t="n">
+        <v>12.92305612663846</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-6.441636818473446</v>
+      </c>
+      <c r="R23" t="n">
+        <v>142.8012886047363</v>
       </c>
     </row>
     <row r="24">
@@ -1336,37 +1762,55 @@
         <v>1981</v>
       </c>
       <c r="B24" t="n">
-        <v>45.73864838069303</v>
+        <v>45.75434227135548</v>
       </c>
       <c r="C24" t="n">
-        <v>95.7616552211873</v>
+        <v>83.47807918717066</v>
       </c>
       <c r="D24" t="n">
-        <v>-5.988220659365505</v>
+        <v>5.333068000975798</v>
       </c>
       <c r="E24" t="n">
-        <v>-2.183255144148269</v>
+        <v>-0.7360663895480286</v>
       </c>
       <c r="F24" t="n">
-        <v>133.3288277983665</v>
+        <v>133.8294230699539</v>
       </c>
       <c r="G24" t="n">
-        <v>47.28369971684863</v>
+        <v>47.34580741366081</v>
       </c>
       <c r="H24" t="n">
-        <v>98.99648350296098</v>
+        <v>86.38168235526075</v>
       </c>
       <c r="I24" t="n">
-        <v>-6.190502726249947</v>
+        <v>5.518567155892303</v>
       </c>
       <c r="J24" t="n">
-        <v>14.40157809806334</v>
+        <v>14.42049474061643</v>
       </c>
       <c r="K24" t="n">
-        <v>-7.037240952462851</v>
+        <v>-5.702810362940063</v>
       </c>
       <c r="L24" t="n">
-        <v>147.4540176391602</v>
+        <v>147.9637413024902</v>
+      </c>
+      <c r="M24" t="n">
+        <v>47.34580741366081</v>
+      </c>
+      <c r="N24" t="n">
+        <v>86.38168235526075</v>
+      </c>
+      <c r="O24" t="n">
+        <v>5.518567155892303</v>
+      </c>
+      <c r="P24" t="n">
+        <v>14.42049474061643</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>-5.702810362940063</v>
+      </c>
+      <c r="R24" t="n">
+        <v>147.9637413024902</v>
       </c>
     </row>
     <row r="25">
@@ -1374,37 +1818,55 @@
         <v>1982</v>
       </c>
       <c r="B25" t="n">
-        <v>46.19871154651913</v>
+        <v>46.21321062375109</v>
       </c>
       <c r="C25" t="n">
-        <v>96.46654011660897</v>
+        <v>84.1895578111646</v>
       </c>
       <c r="D25" t="n">
-        <v>-5.099190240288324</v>
+        <v>6.150284497462599</v>
       </c>
       <c r="E25" t="n">
-        <v>-1.574039325729025</v>
+        <v>-0.0692255202498373</v>
       </c>
       <c r="F25" t="n">
-        <v>135.9920220971107</v>
+        <v>136.4838274121284</v>
       </c>
       <c r="G25" t="n">
-        <v>48.00837196622741</v>
+        <v>48.06893584694912</v>
       </c>
       <c r="H25" t="n">
-        <v>100.2452532804912</v>
+        <v>87.57025099069827</v>
       </c>
       <c r="I25" t="n">
-        <v>-5.298931801070181</v>
+        <v>6.397253663156519</v>
       </c>
       <c r="J25" t="n">
-        <v>14.40912540349908</v>
+        <v>14.42730291122327</v>
       </c>
       <c r="K25" t="n">
-        <v>-4.867488587917009</v>
+        <v>-3.470728122720528</v>
       </c>
       <c r="L25" t="n">
-        <v>152.4963302612305</v>
+        <v>152.9930152893066</v>
+      </c>
+      <c r="M25" t="n">
+        <v>48.06893584694912</v>
+      </c>
+      <c r="N25" t="n">
+        <v>87.57025099069827</v>
+      </c>
+      <c r="O25" t="n">
+        <v>6.397253663156519</v>
+      </c>
+      <c r="P25" t="n">
+        <v>14.42730291122327</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>-3.470728122720528</v>
+      </c>
+      <c r="R25" t="n">
+        <v>152.9930152893066</v>
       </c>
     </row>
     <row r="26">
@@ -1412,37 +1874,55 @@
         <v>1983</v>
       </c>
       <c r="B26" t="n">
-        <v>46.56381547429721</v>
+        <v>46.5771793046443</v>
       </c>
       <c r="C26" t="n">
-        <v>97.06863271900603</v>
+        <v>84.80552015959847</v>
       </c>
       <c r="D26" t="n">
-        <v>-4.150548066005355</v>
+        <v>7.020745866477421</v>
       </c>
       <c r="E26" t="n">
-        <v>-1.010639877683182</v>
+        <v>0.5513907994220091</v>
       </c>
       <c r="F26" t="n">
-        <v>138.4712602496147</v>
+        <v>138.9548361301422</v>
       </c>
       <c r="G26" t="n">
-        <v>48.64035764407589</v>
+        <v>48.69900621303332</v>
       </c>
       <c r="H26" t="n">
-        <v>101.3974684716311</v>
+        <v>88.66884201250899</v>
       </c>
       <c r="I26" t="n">
-        <v>-4.335644325814884</v>
+        <v>7.340576472771078</v>
       </c>
       <c r="J26" t="n">
-        <v>16.09349069215158</v>
+        <v>16.11289555837155</v>
       </c>
       <c r="K26" t="n">
-        <v>-4.390288418323014</v>
+        <v>-2.934982976411511</v>
       </c>
       <c r="L26" t="n">
-        <v>157.4053840637207</v>
+        <v>157.8863372802734</v>
+      </c>
+      <c r="M26" t="n">
+        <v>48.69900621303332</v>
+      </c>
+      <c r="N26" t="n">
+        <v>88.66884201250899</v>
+      </c>
+      <c r="O26" t="n">
+        <v>7.340576472771078</v>
+      </c>
+      <c r="P26" t="n">
+        <v>16.11289555837155</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>-2.934982976411511</v>
+      </c>
+      <c r="R26" t="n">
+        <v>157.8863372802734</v>
       </c>
     </row>
     <row r="27">
@@ -1450,37 +1930,55 @@
         <v>1984</v>
       </c>
       <c r="B27" t="n">
-        <v>46.84057382730781</v>
+        <v>46.85288629415884</v>
       </c>
       <c r="C27" t="n">
-        <v>97.58738308757701</v>
+        <v>85.34257125799654</v>
       </c>
       <c r="D27" t="n">
-        <v>-3.147310280131603</v>
+        <v>7.944009270958287</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.4999613291578342</v>
+        <v>1.117301284300588</v>
       </c>
       <c r="F27" t="n">
-        <v>140.7806853055954</v>
+        <v>141.2567681074142</v>
       </c>
       <c r="G27" t="n">
-        <v>49.18361698267464</v>
+        <v>49.24006492807237</v>
       </c>
       <c r="H27" t="n">
-        <v>102.468865770443</v>
+        <v>89.69081912027883</v>
       </c>
       <c r="I27" t="n">
-        <v>-3.304743957969658</v>
+        <v>8.348760625659924</v>
       </c>
       <c r="J27" t="n">
-        <v>17.7211766480359</v>
+        <v>17.74151519659493</v>
       </c>
       <c r="K27" t="n">
-        <v>-3.889956550361585</v>
+        <v>-2.379054768067007</v>
       </c>
       <c r="L27" t="n">
-        <v>162.1789588928223</v>
+        <v>162.6421051025391</v>
+      </c>
+      <c r="M27" t="n">
+        <v>49.24006492807237</v>
+      </c>
+      <c r="N27" t="n">
+        <v>89.69081912027883</v>
+      </c>
+      <c r="O27" t="n">
+        <v>8.348760625659924</v>
+      </c>
+      <c r="P27" t="n">
+        <v>17.74151519659493</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>-2.379054768067007</v>
+      </c>
+      <c r="R27" t="n">
+        <v>162.6421051025391</v>
       </c>
     </row>
     <row r="28">
@@ -1488,37 +1986,55 @@
         <v>1985</v>
       </c>
       <c r="B28" t="n">
-        <v>47.03577707884672</v>
+        <v>47.04714126856729</v>
       </c>
       <c r="C28" t="n">
-        <v>98.04171739125935</v>
+        <v>85.81694367746461</v>
       </c>
       <c r="D28" t="n">
-        <v>-2.094123271162404</v>
+        <v>8.919581842633105</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.04818004446369173</v>
+        <v>1.620993019017028</v>
       </c>
       <c r="F28" t="n">
-        <v>142.93519115448</v>
+        <v>143.404659807682</v>
       </c>
       <c r="G28" t="n">
-        <v>49.64246273230685</v>
+        <v>49.69652582987292</v>
       </c>
       <c r="H28" t="n">
-        <v>103.4751120120388</v>
+        <v>90.64958769253066</v>
       </c>
       <c r="I28" t="n">
-        <v>-2.210177930541487</v>
+        <v>9.421873837215196</v>
       </c>
       <c r="J28" t="n">
-        <v>20.20619646387262</v>
+        <v>20.22820199674432</v>
       </c>
       <c r="K28" t="n">
-        <v>-4.297492203458074</v>
+        <v>-2.736061335122862</v>
       </c>
       <c r="L28" t="n">
-        <v>166.8161010742188</v>
+        <v>167.2601280212402</v>
+      </c>
+      <c r="M28" t="n">
+        <v>49.69652582987292</v>
+      </c>
+      <c r="N28" t="n">
+        <v>90.64958769253066</v>
+      </c>
+      <c r="O28" t="n">
+        <v>9.421873837215196</v>
+      </c>
+      <c r="P28" t="n">
+        <v>20.22820199674432</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>-2.736061335122862</v>
+      </c>
+      <c r="R28" t="n">
+        <v>167.2601280212402</v>
       </c>
     </row>
     <row r="29">
@@ -1526,37 +2042,55 @@
         <v>1986</v>
       </c>
       <c r="B29" t="n">
-        <v>47.15636603396955</v>
+        <v>47.16689933881312</v>
       </c>
       <c r="C29" t="n">
-        <v>98.44996934260989</v>
+        <v>86.24444407367366</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.995218325147218</v>
+        <v>9.94694629445023</v>
       </c>
       <c r="E29" t="n">
-        <v>0.339306785275852</v>
+        <v>2.055979740389631</v>
       </c>
       <c r="F29" t="n">
-        <v>144.9504238367081</v>
+        <v>145.4142694473267</v>
       </c>
       <c r="G29" t="n">
-        <v>50.0215932416729</v>
+        <v>50.0731718515591</v>
       </c>
       <c r="H29" t="n">
-        <v>104.4318028569822</v>
+        <v>91.55854910711855</v>
       </c>
       <c r="I29" t="n">
-        <v>-1.055687925810735</v>
+        <v>10.55984510710406</v>
       </c>
       <c r="J29" t="n">
-        <v>18.52428465227898</v>
+        <v>18.54338552687326</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.6044612394299946</v>
+        <v>1.006808661251288</v>
       </c>
       <c r="L29" t="n">
-        <v>171.3175315856934</v>
+        <v>171.7417602539062</v>
+      </c>
+      <c r="M29" t="n">
+        <v>50.0731718515591</v>
+      </c>
+      <c r="N29" t="n">
+        <v>91.55854910711855</v>
+      </c>
+      <c r="O29" t="n">
+        <v>10.55984510710406</v>
+      </c>
+      <c r="P29" t="n">
+        <v>18.54338552687326</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>1.006808661251288</v>
+      </c>
+      <c r="R29" t="n">
+        <v>171.7417602539062</v>
       </c>
     </row>
     <row r="30">
@@ -1564,37 +2098,55 @@
         <v>1987</v>
       </c>
       <c r="B30" t="n">
-        <v>47.20940673566313</v>
+        <v>47.21923608892311</v>
       </c>
       <c r="C30" t="n">
-        <v>98.8298135782418</v>
+        <v>86.64040060798628</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1456270783391486</v>
+        <v>11.0255878482913</v>
       </c>
       <c r="E30" t="n">
-        <v>0.6579318865111148</v>
+        <v>2.416850185195571</v>
       </c>
       <c r="F30" t="n">
-        <v>146.8427792787552</v>
+        <v>147.3020747303963</v>
       </c>
       <c r="G30" t="n">
-        <v>50.32610392498084</v>
+        <v>50.37517897344573</v>
       </c>
       <c r="H30" t="n">
-        <v>105.354415845006</v>
+        <v>92.43109479236567</v>
       </c>
       <c r="I30" t="n">
-        <v>0.1552411687743352</v>
+        <v>11.76249357569371</v>
       </c>
       <c r="J30" t="n">
-        <v>24.26636351898214</v>
+        <v>24.2900266278548</v>
       </c>
       <c r="K30" t="n">
-        <v>-4.416230445292111</v>
+        <v>-2.768526787963445</v>
       </c>
       <c r="L30" t="n">
-        <v>175.6858940124512</v>
+        <v>176.0902671813965</v>
+      </c>
+      <c r="M30" t="n">
+        <v>50.37517897344573</v>
+      </c>
+      <c r="N30" t="n">
+        <v>92.43109479236567</v>
+      </c>
+      <c r="O30" t="n">
+        <v>11.76249357569371</v>
+      </c>
+      <c r="P30" t="n">
+        <v>24.2900266278548</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>-2.768526787963445</v>
+      </c>
+      <c r="R30" t="n">
+        <v>176.0902671813965</v>
       </c>
     </row>
     <row r="31">
@@ -1602,37 +2154,55 @@
         <v>1988</v>
       </c>
       <c r="B31" t="n">
-        <v>47.2020675024537</v>
+        <v>47.21132483714238</v>
       </c>
       <c r="C31" t="n">
-        <v>99.19820400074011</v>
+        <v>87.01961499282591</v>
       </c>
       <c r="D31" t="n">
-        <v>1.325122727644967</v>
+        <v>12.15502215842656</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9040100159683107</v>
+        <v>2.699312409932027</v>
       </c>
       <c r="F31" t="n">
-        <v>148.6294042468071</v>
+        <v>149.0852743983269</v>
       </c>
       <c r="G31" t="n">
-        <v>50.56147831552182</v>
+        <v>50.60811942325662</v>
       </c>
       <c r="H31" t="n">
-        <v>106.2582235462759</v>
+        <v>93.28056526509681</v>
       </c>
       <c r="I31" t="n">
-        <v>1.419432825813049</v>
+        <v>13.02956049439292</v>
       </c>
       <c r="J31" t="n">
-        <v>25.58340215356819</v>
+        <v>25.60700188420185</v>
       </c>
       <c r="K31" t="n">
-        <v>-3.896690741325479</v>
+        <v>-2.214211910698189</v>
       </c>
       <c r="L31" t="n">
-        <v>179.9258460998535</v>
+        <v>180.31103515625</v>
+      </c>
+      <c r="M31" t="n">
+        <v>50.60811942325662</v>
+      </c>
+      <c r="N31" t="n">
+        <v>93.28056526509681</v>
+      </c>
+      <c r="O31" t="n">
+        <v>13.02956049439292</v>
+      </c>
+      <c r="P31" t="n">
+        <v>25.60700188420185</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>-2.214211910698189</v>
+      </c>
+      <c r="R31" t="n">
+        <v>180.31103515625</v>
       </c>
     </row>
     <row r="32">
@@ -1640,37 +2210,55 @@
         <v>1989</v>
       </c>
       <c r="B32" t="n">
-        <v>47.14159825754578</v>
+        <v>47.15041586592794</v>
       </c>
       <c r="C32" t="n">
-        <v>99.57131178683964</v>
+        <v>87.39631754391758</v>
       </c>
       <c r="D32" t="n">
-        <v>2.540492374706781</v>
+        <v>13.33482420418356</v>
       </c>
       <c r="E32" t="n">
-        <v>1.074794583318678</v>
+        <v>2.900228827773887</v>
       </c>
       <c r="F32" t="n">
-        <v>150.3281970024109</v>
+        <v>150.781786441803</v>
       </c>
       <c r="G32" t="n">
-        <v>50.73361346102855</v>
+        <v>50.77795745377108</v>
       </c>
       <c r="H32" t="n">
-        <v>107.1582769935571</v>
+        <v>94.12019835583641</v>
       </c>
       <c r="I32" t="n">
-        <v>2.734068485224377</v>
+        <v>14.36074578894329</v>
       </c>
       <c r="J32" t="n">
-        <v>26.93766980463741</v>
+        <v>26.96121482248313</v>
       </c>
       <c r="K32" t="n">
-        <v>-3.519134115541181</v>
+        <v>-1.808380886365935</v>
       </c>
       <c r="L32" t="n">
-        <v>184.0444946289062</v>
+        <v>184.411735534668</v>
+      </c>
+      <c r="M32" t="n">
+        <v>50.77795745377108</v>
+      </c>
+      <c r="N32" t="n">
+        <v>94.12019835583641</v>
+      </c>
+      <c r="O32" t="n">
+        <v>14.36074578894329</v>
+      </c>
+      <c r="P32" t="n">
+        <v>26.96121482248313</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>-1.808380886365935</v>
+      </c>
+      <c r="R32" t="n">
+        <v>184.411735534668</v>
       </c>
     </row>
     <row r="33">
@@ -1678,37 +2266,55 @@
         <v>1990</v>
       </c>
       <c r="B33" t="n">
-        <v>47.03531076804186</v>
+        <v>47.04381743619871</v>
       </c>
       <c r="C33" t="n">
-        <v>99.96447293459201</v>
+        <v>87.78412782717889</v>
       </c>
       <c r="D33" t="n">
-        <v>3.789498888982585</v>
+        <v>14.56465822256371</v>
       </c>
       <c r="E33" t="n">
-        <v>1.168524114812065</v>
+        <v>3.017647237420661</v>
       </c>
       <c r="F33" t="n">
-        <v>151.9578067064285</v>
+        <v>152.410250723362</v>
       </c>
       <c r="G33" t="n">
-        <v>50.84880065221385</v>
+        <v>50.89105638313849</v>
       </c>
       <c r="H33" t="n">
-        <v>108.0693094943552</v>
+        <v>94.96310551022707</v>
       </c>
       <c r="I33" t="n">
-        <v>4.096740734380042</v>
+        <v>15.75575459646465</v>
       </c>
       <c r="J33" t="n">
-        <v>26.18919868546218</v>
+        <v>26.21096208457915</v>
       </c>
       <c r="K33" t="n">
-        <v>-1.15259692969255</v>
+        <v>0.5817474631883037</v>
       </c>
       <c r="L33" t="n">
-        <v>188.0514526367188</v>
+        <v>188.4026260375977</v>
+      </c>
+      <c r="M33" t="n">
+        <v>50.89105638313849</v>
+      </c>
+      <c r="N33" t="n">
+        <v>94.96310551022707</v>
+      </c>
+      <c r="O33" t="n">
+        <v>15.75575459646465</v>
+      </c>
+      <c r="P33" t="n">
+        <v>26.21096208457915</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.5817474631883037</v>
+      </c>
+      <c r="R33" t="n">
+        <v>188.4026260375977</v>
       </c>
     </row>
     <row r="34">
@@ -1716,37 +2322,55 @@
         <v>1991</v>
       </c>
       <c r="B34" t="n">
-        <v>46.8905618726435</v>
+        <v>46.89887867038714</v>
       </c>
       <c r="C34" t="n">
-        <v>100.3921421339615</v>
+        <v>88.19601900821053</v>
       </c>
       <c r="D34" t="n">
-        <v>5.070462918739533</v>
+        <v>15.8443079540689</v>
       </c>
       <c r="E34" t="n">
-        <v>1.184465957250538</v>
+        <v>3.050820364495287</v>
       </c>
       <c r="F34" t="n">
-        <v>153.5376328825951</v>
+        <v>153.9900259971619</v>
       </c>
       <c r="G34" t="n">
-        <v>50.91375236377912</v>
+        <v>50.95418879765953</v>
       </c>
       <c r="H34" t="n">
-        <v>109.0057457140399</v>
+        <v>95.8222612384952</v>
       </c>
       <c r="I34" t="n">
-        <v>5.505506505031679</v>
+        <v>17.21435313057179</v>
       </c>
       <c r="J34" t="n">
-        <v>23.14716753175523</v>
+        <v>23.16555132753959</v>
       </c>
       <c r="K34" t="n">
-        <v>3.38717465663434</v>
+        <v>5.14055102331201</v>
       </c>
       <c r="L34" t="n">
-        <v>191.9593467712402</v>
+        <v>192.2969055175781</v>
+      </c>
+      <c r="M34" t="n">
+        <v>50.95418879765953</v>
+      </c>
+      <c r="N34" t="n">
+        <v>95.8222612384952</v>
+      </c>
+      <c r="O34" t="n">
+        <v>17.21435313057179</v>
+      </c>
+      <c r="P34" t="n">
+        <v>23.16555132753959</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>5.14055102331201</v>
+      </c>
+      <c r="R34" t="n">
+        <v>192.2969055175781</v>
       </c>
     </row>
     <row r="35">
@@ -1754,37 +2378,55 @@
         <v>1992</v>
       </c>
       <c r="B35" t="n">
-        <v>46.71473821057894</v>
+        <v>46.72297499397698</v>
       </c>
       <c r="C35" t="n">
-        <v>100.8678554297609</v>
+        <v>88.64429151226896</v>
       </c>
       <c r="D35" t="n">
-        <v>6.382281023679034</v>
+        <v>17.17370767240946</v>
       </c>
       <c r="E35" t="n">
-        <v>1.122952184011197</v>
+        <v>3.000217816488501</v>
       </c>
       <c r="F35" t="n">
-        <v>155.0878268480301</v>
+        <v>155.5411919951439</v>
       </c>
       <c r="G35" t="n">
-        <v>50.93557003417359</v>
+        <v>50.97450274527767</v>
       </c>
       <c r="H35" t="n">
-        <v>109.9816013370272</v>
+        <v>96.7104231189867</v>
       </c>
       <c r="I35" t="n">
-        <v>6.958941321558391</v>
+        <v>18.73641841099977</v>
       </c>
       <c r="J35" t="n">
-        <v>21.81074045488691</v>
+        <v>21.82741152416063</v>
       </c>
       <c r="K35" t="n">
-        <v>6.096941255430121</v>
+        <v>7.861912382948294</v>
       </c>
       <c r="L35" t="n">
-        <v>195.7837944030762</v>
+        <v>196.110668182373</v>
+      </c>
+      <c r="M35" t="n">
+        <v>50.97450274527767</v>
+      </c>
+      <c r="N35" t="n">
+        <v>96.7104231189867</v>
+      </c>
+      <c r="O35" t="n">
+        <v>18.73641841099977</v>
+      </c>
+      <c r="P35" t="n">
+        <v>21.82741152416063</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>7.861912382948294</v>
+      </c>
+      <c r="R35" t="n">
+        <v>196.110668182373</v>
       </c>
     </row>
     <row r="36">
@@ -1792,37 +2434,55 @@
         <v>1993</v>
       </c>
       <c r="B36" t="n">
-        <v>46.51524342192354</v>
+        <v>46.52349552113176</v>
       </c>
       <c r="C36" t="n">
-        <v>101.4042027670032</v>
+        <v>89.1405538766796</v>
       </c>
       <c r="D36" t="n">
-        <v>7.724439592141614</v>
+        <v>18.55297321814709</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9854040248207738</v>
+        <v>2.867525440167192</v>
       </c>
       <c r="F36" t="n">
-        <v>156.6292898058891</v>
+        <v>157.0845480561256</v>
       </c>
       <c r="G36" t="n">
-        <v>50.92176606520668</v>
+        <v>50.95954843643019</v>
       </c>
       <c r="H36" t="n">
-        <v>111.0105142198692</v>
+        <v>97.64017776492226</v>
       </c>
       <c r="I36" t="n">
-        <v>8.45619794629444</v>
+        <v>20.32201421581745</v>
       </c>
       <c r="J36" t="n">
-        <v>18.85663057594003</v>
+        <v>18.8706215966307</v>
       </c>
       <c r="K36" t="n">
-        <v>10.29879835821694</v>
+        <v>12.07108708287911</v>
       </c>
       <c r="L36" t="n">
-        <v>199.5439071655273</v>
+        <v>199.8634490966797</v>
+      </c>
+      <c r="M36" t="n">
+        <v>50.95954843643019</v>
+      </c>
+      <c r="N36" t="n">
+        <v>97.64017776492226</v>
+      </c>
+      <c r="O36" t="n">
+        <v>20.32201421581745</v>
+      </c>
+      <c r="P36" t="n">
+        <v>18.8706215966307</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>12.07108708287911</v>
+      </c>
+      <c r="R36" t="n">
+        <v>199.8634490966797</v>
       </c>
     </row>
     <row r="37">
@@ -1830,37 +2490,55 @@
         <v>1994</v>
       </c>
       <c r="B37" t="n">
-        <v>46.29948752242535</v>
+        <v>46.30783275710031</v>
       </c>
       <c r="C37" t="n">
-        <v>102.012810275515</v>
+        <v>89.69570816598652</v>
       </c>
       <c r="D37" t="n">
-        <v>9.09702885589531</v>
+        <v>19.98243328271733</v>
       </c>
       <c r="E37" t="n">
-        <v>0.7743479796673114</v>
+        <v>2.655640648531637</v>
       </c>
       <c r="F37" t="n">
-        <v>158.183674633503</v>
+        <v>158.6416148543358</v>
       </c>
       <c r="G37" t="n">
-        <v>50.88023851770513</v>
+        <v>50.91724775335254</v>
       </c>
       <c r="H37" t="n">
-        <v>112.1056926637815</v>
+        <v>98.62388980835391</v>
       </c>
       <c r="I37" t="n">
-        <v>9.997065254042214</v>
+        <v>21.97145591994806</v>
       </c>
       <c r="J37" t="n">
-        <v>23.30701491396057</v>
+        <v>23.32396793769812</v>
       </c>
       <c r="K37" t="n">
-        <v>6.972344454953951</v>
+        <v>8.741670392170811</v>
       </c>
       <c r="L37" t="n">
-        <v>203.2623558044434</v>
+        <v>203.5782318115234</v>
+      </c>
+      <c r="M37" t="n">
+        <v>50.91724775335254</v>
+      </c>
+      <c r="N37" t="n">
+        <v>98.62388980835391</v>
+      </c>
+      <c r="O37" t="n">
+        <v>21.97145591994806</v>
+      </c>
+      <c r="P37" t="n">
+        <v>23.32396793769812</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>8.741670392170811</v>
+      </c>
+      <c r="R37" t="n">
+        <v>203.5782318115234</v>
       </c>
     </row>
     <row r="38">
@@ -1868,37 +2546,55 @@
         <v>1995</v>
       </c>
       <c r="B38" t="n">
-        <v>46.07487919583082</v>
+        <v>46.08337498408688</v>
       </c>
       <c r="C38" t="n">
-        <v>102.7043342335696</v>
+        <v>90.31994633891532</v>
       </c>
       <c r="D38" t="n">
-        <v>10.50075463468881</v>
+        <v>21.46266013691243</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4934173414512557</v>
+        <v>2.368650912941511</v>
       </c>
       <c r="F38" t="n">
-        <v>159.7733854055405</v>
+        <v>160.2346323728561</v>
       </c>
       <c r="G38" t="n">
-        <v>50.81927671840951</v>
+        <v>50.85590525765208</v>
       </c>
       <c r="H38" t="n">
-        <v>113.2799493496681</v>
+        <v>99.67374645355765</v>
       </c>
       <c r="I38" t="n">
-        <v>11.58203265741084</v>
+        <v>23.68539654217845</v>
       </c>
       <c r="J38" t="n">
-        <v>25.33350780415606</v>
+        <v>25.35176720186253</v>
       </c>
       <c r="K38" t="n">
-        <v>5.950962230121121</v>
+        <v>7.715037266917239</v>
       </c>
       <c r="L38" t="n">
-        <v>206.9657287597656</v>
+        <v>207.281852722168</v>
+      </c>
+      <c r="M38" t="n">
+        <v>50.85590525765208</v>
+      </c>
+      <c r="N38" t="n">
+        <v>99.67374645355765</v>
+      </c>
+      <c r="O38" t="n">
+        <v>23.68539654217845</v>
+      </c>
+      <c r="P38" t="n">
+        <v>25.35176720186253</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>7.715037266917239</v>
+      </c>
+      <c r="R38" t="n">
+        <v>207.281852722168</v>
       </c>
     </row>
     <row r="39">
@@ -1906,37 +2602,55 @@
         <v>1996</v>
       </c>
       <c r="B39" t="n">
-        <v>45.84882013917341</v>
+        <v>45.85750131437068</v>
       </c>
       <c r="C39" t="n">
-        <v>103.4884644379322</v>
+        <v>91.02275403993298</v>
       </c>
       <c r="D39" t="n">
-        <v>11.93694952311474</v>
+        <v>22.99450030601682</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1473421016953438</v>
+        <v>2.011805554603384</v>
       </c>
       <c r="F39" t="n">
-        <v>161.4215762019157</v>
+        <v>161.8865612149239</v>
       </c>
       <c r="G39" t="n">
-        <v>50.74755089516047</v>
+        <v>50.78419497134371</v>
       </c>
       <c r="H39" t="n">
-        <v>114.545720046541</v>
+        <v>100.8017697323607</v>
       </c>
       <c r="I39" t="n">
-        <v>13.21235642745915</v>
+        <v>25.46491093799375</v>
       </c>
       <c r="J39" t="n">
-        <v>29.01916569179815</v>
+        <v>29.04011999654393</v>
       </c>
       <c r="K39" t="n">
-        <v>3.159941283523629</v>
+        <v>4.91416946185559</v>
       </c>
       <c r="L39" t="n">
-        <v>210.6847343444824</v>
+        <v>211.0051651000977</v>
+      </c>
+      <c r="M39" t="n">
+        <v>50.78419497134371</v>
+      </c>
+      <c r="N39" t="n">
+        <v>100.8017697323607</v>
+      </c>
+      <c r="O39" t="n">
+        <v>25.46491093799375</v>
+      </c>
+      <c r="P39" t="n">
+        <v>29.04011999654393</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>4.91416946185559</v>
+      </c>
+      <c r="R39" t="n">
+        <v>211.0051651000977</v>
       </c>
     </row>
     <row r="40">
@@ -1944,37 +2658,55 @@
         <v>1997</v>
       </c>
       <c r="B40" t="n">
-        <v>45.62870305311761</v>
+        <v>45.63757956876405</v>
       </c>
       <c r="C40" t="n">
-        <v>104.3739399767987</v>
+        <v>91.81291831564671</v>
       </c>
       <c r="D40" t="n">
-        <v>13.4075849002903</v>
+        <v>24.57910415132275</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.2580756899302159</v>
+        <v>1.591480985430422</v>
       </c>
       <c r="F40" t="n">
-        <v>163.1521522402763</v>
+        <v>163.6210830211639</v>
       </c>
       <c r="G40" t="n">
-        <v>50.67411623152266</v>
+        <v>50.71115767968569</v>
       </c>
       <c r="H40" t="n">
-        <v>115.9151326253812</v>
+        <v>102.0198577955162</v>
       </c>
       <c r="I40" t="n">
-        <v>14.89013428302773</v>
+        <v>27.31158922144609</v>
       </c>
       <c r="J40" t="n">
-        <v>31.34075395482911</v>
+        <v>31.36366317287095</v>
       </c>
       <c r="K40" t="n">
-        <v>1.634387899135788</v>
+        <v>3.377019178820948</v>
       </c>
       <c r="L40" t="n">
-        <v>214.4545249938965</v>
+        <v>214.7832870483398</v>
+      </c>
+      <c r="M40" t="n">
+        <v>50.71115767968569</v>
+      </c>
+      <c r="N40" t="n">
+        <v>102.0198577955162</v>
+      </c>
+      <c r="O40" t="n">
+        <v>27.31158922144609</v>
+      </c>
+      <c r="P40" t="n">
+        <v>31.36366317287095</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>3.377019178820948</v>
+      </c>
+      <c r="R40" t="n">
+        <v>214.7832870483398</v>
       </c>
     </row>
     <row r="41">
@@ -1982,37 +2714,55 @@
         <v>1998</v>
       </c>
       <c r="B41" t="n">
-        <v>45.42191227554903</v>
+        <v>45.43096690292832</v>
       </c>
       <c r="C41" t="n">
-        <v>105.3685687342527</v>
+        <v>92.69854649715796</v>
       </c>
       <c r="D41" t="n">
-        <v>14.91528190449989</v>
+        <v>26.21795454777277</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.7159922634379825</v>
+        <v>1.115130316358332</v>
       </c>
       <c r="F41" t="n">
-        <v>164.9897706508636</v>
+        <v>165.4625982642174</v>
       </c>
       <c r="G41" t="n">
-        <v>50.60840381654495</v>
+        <v>50.6462009939</v>
       </c>
       <c r="H41" t="n">
-        <v>117.4000566890483</v>
+        <v>103.3398480769476</v>
       </c>
       <c r="I41" t="n">
-        <v>16.6183802452296</v>
+        <v>29.22763670235349</v>
       </c>
       <c r="J41" t="n">
-        <v>30.11614444334076</v>
+        <v>30.13863683466293</v>
       </c>
       <c r="K41" t="n">
-        <v>3.571879918141136</v>
+        <v>5.303526848923102</v>
       </c>
       <c r="L41" t="n">
-        <v>218.3148651123047</v>
+        <v>218.6558494567871</v>
+      </c>
+      <c r="M41" t="n">
+        <v>50.6462009939</v>
+      </c>
+      <c r="N41" t="n">
+        <v>103.3398480769476</v>
+      </c>
+      <c r="O41" t="n">
+        <v>29.22763670235349</v>
+      </c>
+      <c r="P41" t="n">
+        <v>30.13863683466293</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>5.303526848923102</v>
+      </c>
+      <c r="R41" t="n">
+        <v>218.6558494567871</v>
       </c>
     </row>
     <row r="42">
@@ -2020,37 +2770,55 @@
         <v>1999</v>
       </c>
       <c r="B42" t="n">
-        <v>45.23582748092343</v>
+        <v>45.24501441766186</v>
       </c>
       <c r="C42" t="n">
-        <v>106.4792581623213</v>
+        <v>93.68708614557811</v>
       </c>
       <c r="D42" t="n">
-        <v>16.46332455231387</v>
+        <v>27.91289431166486</v>
       </c>
       <c r="E42" t="n">
-        <v>-1.218571685998931</v>
+        <v>0.5912344136731917</v>
       </c>
       <c r="F42" t="n">
-        <v>166.9598385095596</v>
+        <v>167.436229288578</v>
       </c>
       <c r="G42" t="n">
-        <v>50.56023167381345</v>
+        <v>50.59910861118423</v>
       </c>
       <c r="H42" t="n">
-        <v>119.0122135692798</v>
+        <v>104.7736001050976</v>
       </c>
       <c r="I42" t="n">
-        <v>18.40111146053868</v>
+        <v>31.21598233764966</v>
       </c>
       <c r="J42" t="n">
-        <v>31.93853057554702</v>
+        <v>31.96308885409509</v>
       </c>
       <c r="K42" t="n">
-        <v>2.398375672481222</v>
+        <v>4.115517455254615</v>
       </c>
       <c r="L42" t="n">
-        <v>222.3104629516602</v>
+        <v>222.6672973632812</v>
+      </c>
+      <c r="M42" t="n">
+        <v>50.59910861118423</v>
+      </c>
+      <c r="N42" t="n">
+        <v>104.7736001050976</v>
+      </c>
+      <c r="O42" t="n">
+        <v>31.21598233764966</v>
+      </c>
+      <c r="P42" t="n">
+        <v>31.96308885409509</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>4.115517455254615</v>
+      </c>
+      <c r="R42" t="n">
+        <v>222.6672973632812</v>
       </c>
     </row>
     <row r="43">
@@ -2058,37 +2826,55 @@
         <v>2000</v>
       </c>
       <c r="B43" t="n">
-        <v>45.07783093998246</v>
+        <v>45.08707390593511</v>
       </c>
       <c r="C43" t="n">
-        <v>107.7120490501449</v>
+        <v>94.7853525488897</v>
       </c>
       <c r="D43" t="n">
-        <v>18.05567280178439</v>
+        <v>29.66615185453</v>
       </c>
       <c r="E43" t="n">
-        <v>-1.757038761932087</v>
+        <v>0.0292389614009565</v>
       </c>
       <c r="F43" t="n">
-        <v>169.0885140299797</v>
+        <v>169.5678172707558</v>
       </c>
       <c r="G43" t="n">
-        <v>50.53981088906968</v>
+        <v>50.58003863828593</v>
       </c>
       <c r="H43" t="n">
-        <v>120.763277113232</v>
+        <v>106.3330657533599</v>
       </c>
       <c r="I43" t="n">
-        <v>20.24343828992268</v>
+        <v>33.28038342390328</v>
       </c>
       <c r="J43" t="n">
-        <v>37.56957490439125</v>
+        <v>37.59947881273172</v>
       </c>
       <c r="K43" t="n">
-        <v>-2.624897888510105</v>
+        <v>-0.9259355308687347</v>
       </c>
       <c r="L43" t="n">
-        <v>226.4912033081055</v>
+        <v>226.8670310974121</v>
+      </c>
+      <c r="M43" t="n">
+        <v>50.58003863828593</v>
+      </c>
+      <c r="N43" t="n">
+        <v>106.3330657533599</v>
+      </c>
+      <c r="O43" t="n">
+        <v>33.28038342390328</v>
+      </c>
+      <c r="P43" t="n">
+        <v>37.59947881273172</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>-0.9259355308687347</v>
+      </c>
+      <c r="R43" t="n">
+        <v>226.8670310974121</v>
       </c>
     </row>
     <row r="44">
@@ -2096,37 +2882,55 @@
         <v>2001</v>
       </c>
       <c r="B44" t="n">
-        <v>44.95531854101138</v>
+        <v>44.96450906380728</v>
       </c>
       <c r="C44" t="n">
-        <v>109.0721523489197</v>
+        <v>95.99955694834173</v>
       </c>
       <c r="D44" t="n">
-        <v>19.69697675108842</v>
+        <v>31.4803651494206</v>
       </c>
       <c r="E44" t="n">
-        <v>-2.321741435174644</v>
+        <v>-0.5605064388981091</v>
       </c>
       <c r="F44" t="n">
-        <v>171.4027062058449</v>
+        <v>171.8839247226715</v>
       </c>
       <c r="G44" t="n">
-        <v>50.55775402981955</v>
+        <v>50.59954091891852</v>
       </c>
       <c r="H44" t="n">
-        <v>122.6649755563188</v>
+        <v>108.0303913273587</v>
       </c>
       <c r="I44" t="n">
-        <v>22.15165942610622</v>
+        <v>35.4255402246291</v>
       </c>
       <c r="J44" t="n">
-        <v>32.92363347830938</v>
+        <v>32.95084539616653</v>
       </c>
       <c r="K44" t="n">
-        <v>2.614308136887423</v>
+        <v>4.303355442253348</v>
       </c>
       <c r="L44" t="n">
-        <v>230.9123306274414</v>
+        <v>231.3096733093262</v>
+      </c>
+      <c r="M44" t="n">
+        <v>50.59954091891852</v>
+      </c>
+      <c r="N44" t="n">
+        <v>108.0303913273587</v>
+      </c>
+      <c r="O44" t="n">
+        <v>35.4255402246291</v>
+      </c>
+      <c r="P44" t="n">
+        <v>32.95084539616653</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>4.303355442253348</v>
+      </c>
+      <c r="R44" t="n">
+        <v>231.3096733093262</v>
       </c>
     </row>
     <row r="45">
@@ -2134,37 +2938,55 @@
         <v>2002</v>
       </c>
       <c r="B45" t="n">
-        <v>44.87571357744274</v>
+        <v>44.88470918285329</v>
       </c>
       <c r="C45" t="n">
-        <v>110.5639838687215</v>
+        <v>97.33533345779482</v>
       </c>
       <c r="D45" t="n">
-        <v>21.39259400557647</v>
+        <v>33.35860335811295</v>
       </c>
       <c r="E45" t="n">
-        <v>-2.902216223526494</v>
+        <v>-1.166812116429213</v>
       </c>
       <c r="F45" t="n">
-        <v>173.9300752282143</v>
+        <v>174.4118338823318</v>
       </c>
       <c r="G45" t="n">
-        <v>50.62510994666669</v>
+        <v>50.66859302930884</v>
       </c>
       <c r="H45" t="n">
-        <v>124.7292442455792</v>
+        <v>109.8780517492831</v>
       </c>
       <c r="I45" t="n">
-        <v>24.1333749870686</v>
+        <v>37.65722287945798</v>
       </c>
       <c r="J45" t="n">
-        <v>38.91716652057909</v>
+        <v>38.95059335418861</v>
       </c>
       <c r="K45" t="n">
-        <v>-2.770049966251001</v>
+        <v>-1.098991499299032</v>
       </c>
       <c r="L45" t="n">
-        <v>235.6348457336426</v>
+        <v>236.0554695129395</v>
+      </c>
+      <c r="M45" t="n">
+        <v>50.66859302930884</v>
+      </c>
+      <c r="N45" t="n">
+        <v>109.8780517492831</v>
+      </c>
+      <c r="O45" t="n">
+        <v>37.65722287945798</v>
+      </c>
+      <c r="P45" t="n">
+        <v>38.95059335418861</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>-1.098991499299032</v>
+      </c>
+      <c r="R45" t="n">
+        <v>236.0554695129395</v>
       </c>
     </row>
     <row r="46">
@@ -2172,37 +2994,55 @@
         <v>2003</v>
       </c>
       <c r="B46" t="n">
-        <v>44.84648486869106</v>
+        <v>44.85510739923663</v>
       </c>
       <c r="C46" t="n">
-        <v>112.1911987995452</v>
+        <v>98.79776953323213</v>
       </c>
       <c r="D46" t="n">
-        <v>23.14860675855028</v>
+        <v>35.30438607837005</v>
       </c>
       <c r="E46" t="n">
-        <v>-3.487257524068923</v>
+        <v>-1.777715522149379</v>
       </c>
       <c r="F46" t="n">
-        <v>176.6990329027176</v>
+        <v>177.1795474886894</v>
       </c>
       <c r="G46" t="n">
-        <v>50.7533837118781</v>
+        <v>50.79860683452164</v>
       </c>
       <c r="H46" t="n">
-        <v>126.968322677708</v>
+        <v>111.8889094607708</v>
       </c>
       <c r="I46" t="n">
-        <v>26.19759663777564</v>
+        <v>39.98237284255842</v>
       </c>
       <c r="J46" t="n">
-        <v>39.92424316958314</v>
+        <v>39.95981713161803</v>
       </c>
       <c r="K46" t="n">
-        <v>-3.117903038985844</v>
+        <v>-1.459437257017768</v>
       </c>
       <c r="L46" t="n">
-        <v>240.725643157959</v>
+        <v>241.1702690124512</v>
+      </c>
+      <c r="M46" t="n">
+        <v>50.79860683452164</v>
+      </c>
+      <c r="N46" t="n">
+        <v>111.8889094607708</v>
+      </c>
+      <c r="O46" t="n">
+        <v>39.98237284255842</v>
+      </c>
+      <c r="P46" t="n">
+        <v>39.95981713161803</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>-1.459437257017768</v>
+      </c>
+      <c r="R46" t="n">
+        <v>241.1702690124512</v>
       </c>
     </row>
     <row r="47">
@@ -2210,37 +3050,55 @@
         <v>2004</v>
       </c>
       <c r="B47" t="n">
-        <v>44.87516786538301</v>
+        <v>44.88320156873854</v>
       </c>
       <c r="C47" t="n">
-        <v>113.9567131572675</v>
+        <v>100.3914271003439</v>
       </c>
       <c r="D47" t="n">
-        <v>24.97184156382364</v>
+        <v>37.32169996645909</v>
       </c>
       <c r="E47" t="n">
-        <v>-4.064982142290773</v>
+        <v>-2.380539913503313</v>
       </c>
       <c r="F47" t="n">
-        <v>179.7387404441833</v>
+        <v>180.2157887220383</v>
       </c>
       <c r="G47" t="n">
-        <v>50.95458500720858</v>
+        <v>51.00148512463794</v>
       </c>
       <c r="H47" t="n">
-        <v>129.3948814884174</v>
+        <v>114.0763514398126</v>
       </c>
       <c r="I47" t="n">
-        <v>28.35487607684153</v>
+        <v>42.40923238843412</v>
       </c>
       <c r="J47" t="n">
-        <v>45.20217687485608</v>
+        <v>45.24378226596234</v>
       </c>
       <c r="K47" t="n">
-        <v>-7.648664985653667</v>
+        <v>-6.004899070409479</v>
       </c>
       <c r="L47" t="n">
-        <v>246.2578544616699</v>
+        <v>246.7259521484375</v>
+      </c>
+      <c r="M47" t="n">
+        <v>51.00148512463794</v>
+      </c>
+      <c r="N47" t="n">
+        <v>114.0763514398126</v>
+      </c>
+      <c r="O47" t="n">
+        <v>42.40923238843412</v>
+      </c>
+      <c r="P47" t="n">
+        <v>45.24378226596234</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>-6.004899070409479</v>
+      </c>
+      <c r="R47" t="n">
+        <v>246.7259521484375</v>
       </c>
     </row>
     <row r="48">
@@ -2248,37 +3106,55 @@
         <v>2005</v>
       </c>
       <c r="B48" t="n">
-        <v>44.96938955512552</v>
+        <v>44.9765785763455</v>
       </c>
       <c r="C48" t="n">
-        <v>115.8627216103943</v>
+        <v>102.1203629466639</v>
       </c>
       <c r="D48" t="n">
-        <v>26.86989228150882</v>
+        <v>39.41501241175467</v>
       </c>
       <c r="E48" t="n">
-        <v>-4.622892705413292</v>
+        <v>-2.961952969168827</v>
       </c>
       <c r="F48" t="n">
-        <v>183.0791107416153</v>
+        <v>183.5500009655952</v>
       </c>
       <c r="G48" t="n">
-        <v>51.24127346917766</v>
+        <v>51.28967191821799</v>
       </c>
       <c r="H48" t="n">
-        <v>132.0221035165181</v>
+        <v>116.4543875389047</v>
       </c>
       <c r="I48" t="n">
-        <v>30.61743804185594</v>
+        <v>44.94746197334355</v>
       </c>
       <c r="J48" t="n">
-        <v>49.8075767719444</v>
+        <v>49.85462098977081</v>
       </c>
       <c r="K48" t="n">
-        <v>-11.3773490138516</v>
+        <v>-9.745464167063204</v>
       </c>
       <c r="L48" t="n">
-        <v>252.3110427856445</v>
+        <v>252.8006782531738</v>
+      </c>
+      <c r="M48" t="n">
+        <v>51.28967191821799</v>
+      </c>
+      <c r="N48" t="n">
+        <v>116.4543875389047</v>
+      </c>
+      <c r="O48" t="n">
+        <v>44.94746197334355</v>
+      </c>
+      <c r="P48" t="n">
+        <v>49.85462098977081</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>-9.745464167063204</v>
+      </c>
+      <c r="R48" t="n">
+        <v>252.8006782531738</v>
       </c>
     </row>
     <row r="49">
@@ -2286,37 +3162,55 @@
         <v>2006</v>
       </c>
       <c r="B49" t="n">
-        <v>45.1368965545372</v>
+        <v>45.14294219361776</v>
       </c>
       <c r="C49" t="n">
-        <v>117.9107008684596</v>
+        <v>103.9881365441895</v>
       </c>
       <c r="D49" t="n">
-        <v>28.85114207998197</v>
+        <v>41.58928215604065</v>
       </c>
       <c r="E49" t="n">
-        <v>-5.14793150241421</v>
+        <v>-3.508013565185024</v>
       </c>
       <c r="F49" t="n">
-        <v>186.7508080005646</v>
+        <v>187.2123473286629</v>
       </c>
       <c r="G49" t="n">
-        <v>51.62662618039512</v>
+        <v>51.67620418911418</v>
       </c>
       <c r="H49" t="n">
-        <v>134.86376204552</v>
+        <v>119.0377037069319</v>
       </c>
       <c r="I49" t="n">
-        <v>32.99932518047636</v>
+        <v>47.60824466328397</v>
       </c>
       <c r="J49" t="n">
-        <v>52.68795298427746</v>
+        <v>52.73855015938382</v>
       </c>
       <c r="K49" t="n">
-        <v>-13.20615454984861</v>
+        <v>-11.58168736837205</v>
       </c>
       <c r="L49" t="n">
-        <v>258.9715118408203</v>
+        <v>259.4790153503418</v>
+      </c>
+      <c r="M49" t="n">
+        <v>51.67620418911418</v>
+      </c>
+      <c r="N49" t="n">
+        <v>119.0377037069319</v>
+      </c>
+      <c r="O49" t="n">
+        <v>47.60824466328397</v>
+      </c>
+      <c r="P49" t="n">
+        <v>52.73855015938382</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>-11.58168736837205</v>
+      </c>
+      <c r="R49" t="n">
+        <v>259.4790153503418</v>
       </c>
     </row>
     <row r="50">
@@ -2324,37 +3218,55 @@
         <v>2007</v>
       </c>
       <c r="B50" t="n">
-        <v>45.38558619326406</v>
+        <v>45.39014398459341</v>
       </c>
       <c r="C50" t="n">
-        <v>120.1013883374548</v>
+        <v>105.9978102634778</v>
       </c>
       <c r="D50" t="n">
-        <v>30.92479043727737</v>
+        <v>43.84996682640435</v>
       </c>
       <c r="E50" t="n">
-        <v>-5.626517701703619</v>
+        <v>-4.004208937730112</v>
       </c>
       <c r="F50" t="n">
-        <v>190.7852472662926</v>
+        <v>191.2337121367455</v>
       </c>
       <c r="G50" t="n">
-        <v>52.12450824492436</v>
+        <v>52.17479533071995</v>
       </c>
       <c r="H50" t="n">
-        <v>137.9342282804235</v>
+        <v>121.841738547439</v>
       </c>
       <c r="I50" t="n">
-        <v>35.51655116354232</v>
+        <v>50.40440156354354</v>
       </c>
       <c r="J50" t="n">
-        <v>55.96482992367342</v>
+        <v>56.01882190886992</v>
       </c>
       <c r="K50" t="n">
-        <v>-15.20760571070816</v>
+        <v>-13.58746624339464</v>
       </c>
       <c r="L50" t="n">
-        <v>266.3325119018555</v>
+        <v>266.8522911071777</v>
+      </c>
+      <c r="M50" t="n">
+        <v>52.17479533071995</v>
+      </c>
+      <c r="N50" t="n">
+        <v>121.841738547439</v>
+      </c>
+      <c r="O50" t="n">
+        <v>50.40440156354354</v>
+      </c>
+      <c r="P50" t="n">
+        <v>56.01882190886992</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>-13.58746624339464</v>
+      </c>
+      <c r="R50" t="n">
+        <v>266.8522911071777</v>
       </c>
     </row>
     <row r="51">
@@ -2362,37 +3274,55 @@
         <v>2008</v>
       </c>
       <c r="B51" t="n">
-        <v>45.72354072753397</v>
+        <v>45.72621660561527</v>
       </c>
       <c r="C51" t="n">
-        <v>122.4347512322841</v>
+        <v>108.1519377733008</v>
       </c>
       <c r="D51" t="n">
-        <v>33.10088024399156</v>
+        <v>46.2030272394938</v>
       </c>
       <c r="E51" t="n">
-        <v>-6.044578256875894</v>
+        <v>-4.435482057767636</v>
       </c>
       <c r="F51" t="n">
-        <v>195.2145939469337</v>
+        <v>195.6456995606422</v>
       </c>
       <c r="G51" t="n">
-        <v>52.7495645221261</v>
+        <v>52.79991986775892</v>
       </c>
       <c r="H51" t="n">
-        <v>141.2484621075878</v>
+        <v>124.8827056308849</v>
       </c>
       <c r="I51" t="n">
-        <v>38.18726613002993</v>
+        <v>53.35049162133343</v>
       </c>
       <c r="J51" t="n">
-        <v>54.6056108063263</v>
+        <v>54.65773791971473</v>
       </c>
       <c r="K51" t="n">
-        <v>-12.29637002725173</v>
+        <v>-10.67203713808066</v>
       </c>
       <c r="L51" t="n">
-        <v>274.4945335388184</v>
+        <v>275.0188179016113</v>
+      </c>
+      <c r="M51" t="n">
+        <v>52.79991986775892</v>
+      </c>
+      <c r="N51" t="n">
+        <v>124.8827056308849</v>
+      </c>
+      <c r="O51" t="n">
+        <v>53.35049162133343</v>
+      </c>
+      <c r="P51" t="n">
+        <v>54.65773791971473</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>-10.67203713808066</v>
+      </c>
+      <c r="R51" t="n">
+        <v>275.0188179016113</v>
       </c>
     </row>
     <row r="52">
@@ -2400,37 +3330,55 @@
         <v>2009</v>
       </c>
       <c r="B52" t="n">
-        <v>46.15906335828793</v>
+        <v>46.15940932655764</v>
       </c>
       <c r="C52" t="n">
-        <v>124.9099284344037</v>
+        <v>110.4525340745549</v>
       </c>
       <c r="D52" t="n">
-        <v>35.39032686421503</v>
+        <v>48.6549282288513</v>
       </c>
       <c r="E52" t="n">
-        <v>-6.387554247364527</v>
+        <v>-4.786237775097831</v>
       </c>
       <c r="F52" t="n">
-        <v>200.0717644095421</v>
+        <v>200.480633854866</v>
       </c>
       <c r="G52" t="n">
-        <v>53.51732175708143</v>
+        <v>53.56690930589938</v>
       </c>
       <c r="H52" t="n">
-        <v>144.8219340758725</v>
+        <v>128.1775690308574</v>
       </c>
       <c r="I52" t="n">
-        <v>41.03193115465174</v>
+        <v>56.46290032182886</v>
       </c>
       <c r="J52" t="n">
-        <v>57.23129051485344</v>
+        <v>57.28431926630478</v>
       </c>
       <c r="K52" t="n">
-        <v>-13.03689904176571</v>
+        <v>-11.40759910897246</v>
       </c>
       <c r="L52" t="n">
-        <v>283.5655784606934</v>
+        <v>284.084098815918</v>
+      </c>
+      <c r="M52" t="n">
+        <v>53.56690930589938</v>
+      </c>
+      <c r="N52" t="n">
+        <v>128.1775690308574</v>
+      </c>
+      <c r="O52" t="n">
+        <v>56.46290032182886</v>
+      </c>
+      <c r="P52" t="n">
+        <v>57.28431926630478</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>-11.40759910897246</v>
+      </c>
+      <c r="R52" t="n">
+        <v>284.084098815918</v>
       </c>
     </row>
     <row r="53">
@@ -2438,37 +3386,55 @@
         <v>2010</v>
       </c>
       <c r="B53" t="n">
-        <v>46.70071742995661</v>
+        <v>46.69822640111115</v>
       </c>
       <c r="C53" t="n">
-        <v>127.5251409894099</v>
+        <v>112.901032822723</v>
       </c>
       <c r="D53" t="n">
-        <v>37.80494913567291</v>
+        <v>51.21263677981118</v>
       </c>
       <c r="E53" t="n">
-        <v>-6.640381217320495</v>
+        <v>-5.04033581153714</v>
       </c>
       <c r="F53" t="n">
-        <v>205.390426337719</v>
+        <v>205.7715601921082</v>
       </c>
       <c r="G53" t="n">
-        <v>54.44430555578766</v>
+        <v>54.49207165358691</v>
       </c>
       <c r="H53" t="n">
-        <v>148.6704728355773</v>
+        <v>131.7440006713703</v>
       </c>
       <c r="I53" t="n">
-        <v>44.07350283966503</v>
+        <v>59.7599285464124</v>
       </c>
       <c r="J53" t="n">
-        <v>62.21298671394278</v>
+        <v>62.2675685226725</v>
       </c>
       <c r="K53" t="n">
-        <v>-15.73983758608603</v>
+        <v>-14.10242513745027</v>
       </c>
       <c r="L53" t="n">
-        <v>293.6614303588867</v>
+        <v>294.1611442565918</v>
+      </c>
+      <c r="M53" t="n">
+        <v>54.49207165358691</v>
+      </c>
+      <c r="N53" t="n">
+        <v>131.7440006713703</v>
+      </c>
+      <c r="O53" t="n">
+        <v>59.7599285464124</v>
+      </c>
+      <c r="P53" t="n">
+        <v>62.2675685226725</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>-14.10242513745027</v>
+      </c>
+      <c r="R53" t="n">
+        <v>294.1611442565918</v>
       </c>
     </row>
     <row r="54">
@@ -2476,37 +3442,55 @@
         <v>2011</v>
       </c>
       <c r="B54" t="n">
-        <v>47.35736575322517</v>
+        <v>47.35146548510519</v>
       </c>
       <c r="C54" t="n">
-        <v>130.2775831136213</v>
+        <v>115.4982241406916</v>
       </c>
       <c r="D54" t="n">
-        <v>40.35750217214488</v>
+        <v>53.88361648415351</v>
       </c>
       <c r="E54" t="n">
-        <v>-6.787452247773508</v>
+        <v>-5.181063354060399</v>
       </c>
       <c r="F54" t="n">
-        <v>211.2049987912178</v>
+        <v>211.5522427558899</v>
       </c>
       <c r="G54" t="n">
-        <v>55.54816204423015</v>
+        <v>55.59280879549629</v>
       </c>
       <c r="H54" t="n">
-        <v>152.8100261158055</v>
+        <v>135.6002528135604</v>
       </c>
       <c r="I54" t="n">
-        <v>47.33762181875586</v>
+        <v>63.26185594732377</v>
       </c>
       <c r="J54" t="n">
-        <v>62.85457849953008</v>
+        <v>62.90509771769028</v>
       </c>
       <c r="K54" t="n">
-        <v>-13.64454665092902</v>
+        <v>-11.9893869171371</v>
       </c>
       <c r="L54" t="n">
-        <v>304.9058418273926</v>
+        <v>305.3706283569336</v>
+      </c>
+      <c r="M54" t="n">
+        <v>55.59280879549629</v>
+      </c>
+      <c r="N54" t="n">
+        <v>135.6002528135604</v>
+      </c>
+      <c r="O54" t="n">
+        <v>63.26185594732377</v>
+      </c>
+      <c r="P54" t="n">
+        <v>62.90509771769028</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>-11.9893869171371</v>
+      </c>
+      <c r="R54" t="n">
+        <v>305.3706283569336</v>
       </c>
     </row>
     <row r="55">
@@ -2514,37 +3498,55 @@
         <v>2012</v>
       </c>
       <c r="B55" t="n">
-        <v>48.13821235603202</v>
+        <v>48.12825883009775</v>
       </c>
       <c r="C55" t="n">
-        <v>133.1632727971445</v>
+        <v>118.2441722632614</v>
       </c>
       <c r="D55" t="n">
-        <v>43.0617099800015</v>
+        <v>56.67581979337152</v>
       </c>
       <c r="E55" t="n">
-        <v>-6.812544119326809</v>
+        <v>-5.19108310633132</v>
       </c>
       <c r="F55" t="n">
-        <v>217.5506510138512</v>
+        <v>217.8571677803993</v>
       </c>
       <c r="G55" t="n">
-        <v>56.84780325697707</v>
+        <v>56.88776379849961</v>
       </c>
       <c r="H55" t="n">
-        <v>157.2563492187649</v>
+        <v>139.7650092850419</v>
       </c>
       <c r="I55" t="n">
-        <v>50.85281519693546</v>
+        <v>66.99100960360049</v>
       </c>
       <c r="J55" t="n">
-        <v>66.44078362199606</v>
+        <v>66.48748738707059</v>
       </c>
       <c r="K55" t="n">
-        <v>-13.96692701488836</v>
+        <v>-12.29004158910519</v>
       </c>
       <c r="L55" t="n">
-        <v>317.4308242797852</v>
+        <v>317.8412284851074</v>
+      </c>
+      <c r="M55" t="n">
+        <v>56.88776379849961</v>
+      </c>
+      <c r="N55" t="n">
+        <v>139.7650092850419</v>
+      </c>
+      <c r="O55" t="n">
+        <v>66.99100960360049</v>
+      </c>
+      <c r="P55" t="n">
+        <v>66.48748738707059</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>-12.29004158910519</v>
+      </c>
+      <c r="R55" t="n">
+        <v>317.8412284851074</v>
       </c>
     </row>
     <row r="56">
@@ -2552,37 +3554,55 @@
         <v>2013</v>
       </c>
       <c r="B56" t="n">
-        <v>49.05284335810448</v>
+        <v>49.03811291997128</v>
       </c>
       <c r="C56" t="n">
-        <v>136.1768739085894</v>
+        <v>121.1381110380687</v>
       </c>
       <c r="D56" t="n">
-        <v>45.93229996533801</v>
+        <v>59.59767700768653</v>
       </c>
       <c r="E56" t="n">
-        <v>-6.698714679331808</v>
+        <v>-5.05236051467665</v>
       </c>
       <c r="F56" t="n">
-        <v>224.4633025527</v>
+        <v>224.7215404510498</v>
       </c>
       <c r="G56" t="n">
-        <v>58.36357028728237</v>
+        <v>58.3969642683777</v>
       </c>
       <c r="H56" t="n">
-        <v>162.0246250323269</v>
+        <v>144.2571404281723</v>
       </c>
       <c r="I56" t="n">
-        <v>54.650716124912</v>
+        <v>70.97180555002123</v>
       </c>
       <c r="J56" t="n">
-        <v>69.5622093905431</v>
+        <v>69.60201085629782</v>
       </c>
       <c r="K56" t="n">
-        <v>-13.22409904551354</v>
+        <v>-11.51812419735148</v>
       </c>
       <c r="L56" t="n">
-        <v>331.3770217895508</v>
+        <v>331.7097969055176</v>
+      </c>
+      <c r="M56" t="n">
+        <v>58.3969642683777</v>
+      </c>
+      <c r="N56" t="n">
+        <v>144.2571404281723</v>
+      </c>
+      <c r="O56" t="n">
+        <v>70.97180555002123</v>
+      </c>
+      <c r="P56" t="n">
+        <v>69.60201085629782</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>-11.51812419735148</v>
+      </c>
+      <c r="R56" t="n">
+        <v>331.7097969055176</v>
       </c>
     </row>
     <row r="57">
@@ -2590,37 +3610,55 @@
         <v>2014</v>
       </c>
       <c r="B57" t="n">
-        <v>50.11126919750051</v>
+        <v>50.09094967665374</v>
       </c>
       <c r="C57" t="n">
-        <v>139.3114734954626</v>
+        <v>124.1783178351851</v>
       </c>
       <c r="D57" t="n">
-        <v>48.9850378316325</v>
+        <v>62.65808344851043</v>
       </c>
       <c r="E57" t="n">
-        <v>-6.428154822691305</v>
+        <v>-4.746063850497485</v>
       </c>
       <c r="F57" t="n">
-        <v>231.9796257019043</v>
+        <v>232.1812871098518</v>
       </c>
       <c r="G57" t="n">
-        <v>60.11738503598414</v>
+        <v>60.14199227157199</v>
       </c>
       <c r="H57" t="n">
-        <v>167.1289038609056</v>
+        <v>149.0954250168935</v>
       </c>
       <c r="I57" t="n">
-        <v>58.76627009226472</v>
+        <v>75.23079508049703</v>
       </c>
       <c r="J57" t="n">
-        <v>71.79291328163136</v>
+        <v>71.82229948140503</v>
       </c>
       <c r="K57" t="n">
-        <v>-10.91167725735813</v>
+        <v>-9.168815378199618</v>
       </c>
       <c r="L57" t="n">
-        <v>346.8937950134277</v>
+        <v>347.121696472168</v>
+      </c>
+      <c r="M57" t="n">
+        <v>60.14199227157199</v>
+      </c>
+      <c r="N57" t="n">
+        <v>149.0954250168935</v>
+      </c>
+      <c r="O57" t="n">
+        <v>75.23079508049703</v>
+      </c>
+      <c r="P57" t="n">
+        <v>71.82229948140503</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>-9.168815378199618</v>
+      </c>
+      <c r="R57" t="n">
+        <v>347.121696472168</v>
       </c>
     </row>
     <row r="58">
@@ -2628,37 +3666,55 @@
         <v>2015</v>
       </c>
       <c r="B58" t="n">
-        <v>51.32396452152532</v>
+        <v>51.29714537837557</v>
       </c>
       <c r="C58" t="n">
-        <v>142.5583260100778</v>
+        <v>127.3619610507244</v>
       </c>
       <c r="D58" t="n">
-        <v>52.23676193206015</v>
+        <v>65.86638414623286</v>
       </c>
       <c r="E58" t="n">
-        <v>-5.982009524000297</v>
+        <v>-4.252437227268366</v>
       </c>
       <c r="F58" t="n">
-        <v>240.1370429396629</v>
+        <v>240.2730533480644</v>
       </c>
       <c r="G58" t="n">
-        <v>62.13293861197647</v>
+        <v>62.14614621421309</v>
       </c>
       <c r="H58" t="n">
-        <v>172.581518228106</v>
+        <v>154.2981582153271</v>
       </c>
       <c r="I58" t="n">
-        <v>63.237973774452</v>
+        <v>79.79668087883253</v>
       </c>
       <c r="J58" t="n">
-        <v>75.03934725812121</v>
+        <v>75.05529831375557</v>
       </c>
       <c r="K58" t="n">
-        <v>-8.852148508642074</v>
+        <v>-7.065345664364642</v>
       </c>
       <c r="L58" t="n">
-        <v>364.1396293640137</v>
+        <v>364.2309379577637</v>
+      </c>
+      <c r="M58" t="n">
+        <v>62.14614621421309</v>
+      </c>
+      <c r="N58" t="n">
+        <v>154.2981582153271</v>
+      </c>
+      <c r="O58" t="n">
+        <v>79.79668087883253</v>
+      </c>
+      <c r="P58" t="n">
+        <v>75.05529831375557</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>-7.065345664364642</v>
+      </c>
+      <c r="R58" t="n">
+        <v>364.2309379577637</v>
       </c>
     </row>
     <row r="59">
@@ -2666,37 +3722,55 @@
         <v>2016</v>
       </c>
       <c r="B59" t="n">
-        <v>52.70190793960818</v>
+        <v>52.66756960748666</v>
       </c>
       <c r="C59" t="n">
-        <v>145.9065426299362</v>
+        <v>130.6849221509881</v>
       </c>
       <c r="D59" t="n">
-        <v>55.70541808095835</v>
+        <v>69.2323573237624</v>
       </c>
       <c r="E59" t="n">
-        <v>-5.340142258710372</v>
+        <v>-3.550642811065586</v>
       </c>
       <c r="F59" t="n">
-        <v>248.9737263917923</v>
+        <v>249.0342062711716</v>
       </c>
       <c r="G59" t="n">
-        <v>64.4358653823173</v>
+        <v>64.43463167122547</v>
       </c>
       <c r="H59" t="n">
-        <v>178.3922955896653</v>
+        <v>159.8827302368004</v>
       </c>
       <c r="I59" t="n">
-        <v>68.10810008327421</v>
+        <v>84.70034742695204</v>
       </c>
       <c r="J59" t="n">
-        <v>77.11425735621886</v>
+        <v>77.11278085272201</v>
       </c>
       <c r="K59" t="n">
-        <v>-4.768268960792042</v>
+        <v>-2.929947737748705</v>
       </c>
       <c r="L59" t="n">
-        <v>383.2822494506836</v>
+        <v>383.2005424499512</v>
+      </c>
+      <c r="M59" t="n">
+        <v>64.43463167122547</v>
+      </c>
+      <c r="N59" t="n">
+        <v>159.8827302368004</v>
+      </c>
+      <c r="O59" t="n">
+        <v>84.70034742695204</v>
+      </c>
+      <c r="P59" t="n">
+        <v>77.11278085272201</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>-2.929947737748705</v>
+      </c>
+      <c r="R59" t="n">
+        <v>383.2005424499512</v>
       </c>
     </row>
     <row r="60">
@@ -2704,37 +3778,55 @@
         <v>2017</v>
       </c>
       <c r="B60" t="n">
-        <v>54.25661901033149</v>
+        <v>54.21362075565683</v>
       </c>
       <c r="C60" t="n">
-        <v>149.3427338288177</v>
+        <v>134.1415888260336</v>
       </c>
       <c r="D60" t="n">
-        <v>59.41009393395692</v>
+        <v>72.76619613184045</v>
       </c>
       <c r="E60" t="n">
-        <v>-4.480846139961756</v>
+        <v>-2.618573718043692</v>
       </c>
       <c r="F60" t="n">
-        <v>258.5286006331444</v>
+        <v>258.5028319954872</v>
       </c>
       <c r="G60" t="n">
-        <v>67.05395488035725</v>
+        <v>67.03474407241391</v>
       </c>
       <c r="H60" t="n">
-        <v>184.5677286666146</v>
+        <v>165.8650898258233</v>
       </c>
       <c r="I60" t="n">
-        <v>73.42296351578348</v>
+        <v>89.97486732726713</v>
       </c>
       <c r="J60" t="n">
-        <v>82.87369440697557</v>
+        <v>82.84995121200141</v>
       </c>
       <c r="K60" t="n">
-        <v>-3.419234108891089</v>
+        <v>-1.52191653662689</v>
       </c>
       <c r="L60" t="n">
-        <v>404.4991073608398</v>
+        <v>404.2027359008789</v>
+      </c>
+      <c r="M60" t="n">
+        <v>67.03474407241391</v>
+      </c>
+      <c r="N60" t="n">
+        <v>165.8650898258233</v>
+      </c>
+      <c r="O60" t="n">
+        <v>89.97486732726713</v>
+      </c>
+      <c r="P60" t="n">
+        <v>82.84995121200141</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>-1.52191653662689</v>
+      </c>
+      <c r="R60" t="n">
+        <v>404.2027359008789</v>
       </c>
     </row>
     <row r="61">
@@ -2742,37 +3834,55 @@
         <v>2018</v>
       </c>
       <c r="B61" t="n">
-        <v>56.00019356269804</v>
+        <v>55.94726059988243</v>
       </c>
       <c r="C61" t="n">
-        <v>152.8505933518282</v>
+        <v>137.7246155308829</v>
       </c>
       <c r="D61" t="n">
-        <v>63.37105085965031</v>
+        <v>76.47848997840109</v>
       </c>
       <c r="E61" t="n">
-        <v>-3.380496993918385</v>
+        <v>-1.432627957616113</v>
       </c>
       <c r="F61" t="n">
-        <v>268.8413407802582</v>
+        <v>268.7177381515503</v>
       </c>
       <c r="G61" t="n">
-        <v>70.01733025438254</v>
+        <v>69.9760612804931</v>
       </c>
       <c r="H61" t="n">
-        <v>191.1098836169391</v>
+        <v>172.2591246271255</v>
       </c>
       <c r="I61" t="n">
-        <v>79.23315107187345</v>
+        <v>95.65550563130553</v>
       </c>
       <c r="J61" t="n">
-        <v>85.69813204886388</v>
+        <v>85.64762057222845</v>
       </c>
       <c r="K61" t="n">
-        <v>1.918885667853147</v>
+        <v>3.880865897880682</v>
       </c>
       <c r="L61" t="n">
-        <v>427.9773826599121</v>
+        <v>427.4191780090332</v>
+      </c>
+      <c r="M61" t="n">
+        <v>69.9760612804931</v>
+      </c>
+      <c r="N61" t="n">
+        <v>172.2591246271255</v>
+      </c>
+      <c r="O61" t="n">
+        <v>95.65550563130553</v>
+      </c>
+      <c r="P61" t="n">
+        <v>85.64762057222845</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>3.880865897880682</v>
+      </c>
+      <c r="R61" t="n">
+        <v>427.4191780090332</v>
       </c>
     </row>
     <row r="62">
@@ -2780,37 +3890,55 @@
         <v>2019</v>
       </c>
       <c r="B62" t="n">
-        <v>57.94533492154776</v>
+        <v>57.88104439479543</v>
       </c>
       <c r="C62" t="n">
-        <v>156.4104148620967</v>
+        <v>141.4246493435941</v>
       </c>
       <c r="D62" t="n">
-        <v>67.60975576902612</v>
+        <v>80.3802048610433</v>
       </c>
       <c r="E62" t="n">
-        <v>-2.01313240565981</v>
+        <v>0.03255343694797119</v>
       </c>
       <c r="F62" t="n">
-        <v>279.9523731470108</v>
+        <v>279.7184520363808</v>
       </c>
       <c r="G62" t="n">
-        <v>73.3586644289912</v>
+        <v>73.29064617532954</v>
       </c>
       <c r="H62" t="n">
-        <v>198.015235438756</v>
+        <v>179.075965955504</v>
       </c>
       <c r="I62" t="n">
-        <v>85.59379960959868</v>
+        <v>101.7797314400385</v>
       </c>
       <c r="J62" t="n">
-        <v>90.85487544283967</v>
+        <v>90.7706346077718</v>
       </c>
       <c r="K62" t="n">
-        <v>6.091823273173759</v>
+        <v>8.124300660467455</v>
       </c>
       <c r="L62" t="n">
-        <v>453.9143981933594</v>
+        <v>453.0412788391113</v>
+      </c>
+      <c r="M62" t="n">
+        <v>73.29064617532954</v>
+      </c>
+      <c r="N62" t="n">
+        <v>179.075965955504</v>
+      </c>
+      <c r="O62" t="n">
+        <v>101.7797314400385</v>
+      </c>
+      <c r="P62" t="n">
+        <v>90.7706346077718</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>8.124300660467455</v>
+      </c>
+      <c r="R62" t="n">
+        <v>453.0412788391113</v>
       </c>
     </row>
     <row r="63">
@@ -2818,37 +3946,55 @@
         <v>2020</v>
       </c>
       <c r="B63" t="n">
-        <v>60.10538266207905</v>
+        <v>60.02814874943347</v>
       </c>
       <c r="C63" t="n">
-        <v>159.9985284350011</v>
+        <v>145.2300231007811</v>
       </c>
       <c r="D63" t="n">
-        <v>72.14891068456605</v>
+        <v>84.48266371735011</v>
       </c>
       <c r="E63" t="n">
-        <v>-0.3499479079355297</v>
+        <v>1.80438576117065</v>
       </c>
       <c r="F63" t="n">
-        <v>291.9028738737106</v>
+        <v>291.5452213287354</v>
       </c>
       <c r="G63" t="n">
-        <v>77.11339268122182</v>
+        <v>77.01324006851262</v>
       </c>
       <c r="H63" t="n">
-        <v>205.2732851064607</v>
+        <v>186.3231645024143</v>
       </c>
       <c r="I63" t="n">
-        <v>92.56487580190534</v>
+        <v>108.3872116338272</v>
       </c>
       <c r="J63" t="n">
-        <v>30.77892531005693</v>
+        <v>30.73895054459787</v>
       </c>
       <c r="K63" t="n">
-        <v>76.78746543629268</v>
+        <v>78.80779991934918</v>
       </c>
       <c r="L63" t="n">
-        <v>482.5179443359375</v>
+        <v>481.2703666687012</v>
+      </c>
+      <c r="M63" t="n">
+        <v>77.01324006851262</v>
+      </c>
+      <c r="N63" t="n">
+        <v>186.3231645024143</v>
+      </c>
+      <c r="O63" t="n">
+        <v>108.3872116338272</v>
+      </c>
+      <c r="P63" t="n">
+        <v>30.73895054459787</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>78.80779991934918</v>
+      </c>
+      <c r="R63" t="n">
+        <v>481.2703666687012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>